<commit_message>
Inversion count resolved,sort array of 0,1,2 without sort algo
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -31,22 +31,22 @@
     <t xml:space="preserve">Done [yes or no] </t>
   </si>
   <si>
+    <t>&lt;-&gt;</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Reverse the array</t>
+  </si>
+  <si>
+    <t>&lt;YES-&gt;</t>
+  </si>
+  <si>
+    <t>Find the maximum and minimum element in an array</t>
+  </si>
+  <si>
     <t>&lt;-YES&gt;</t>
-  </si>
-  <si>
-    <t>Array</t>
-  </si>
-  <si>
-    <t>Reverse the array</t>
-  </si>
-  <si>
-    <t>&lt;YES-&gt;</t>
-  </si>
-  <si>
-    <t>Find the maximum and minimum element in an array</t>
-  </si>
-  <si>
-    <t>&lt;-&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Find the "Kth" max and min element of an array </t>
@@ -1425,10 +1425,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1503,7 +1503,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1523,16 +1523,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1546,26 +1569,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1579,16 +1587,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1596,14 +1597,6 @@
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1618,6 +1611,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1654,7 +1654,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1666,7 +1678,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1678,25 +1798,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1708,133 +1828,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1845,6 +1845,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1868,39 +1892,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1945,16 +1936,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1967,127 +1967,127 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2438,7 +2438,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2500,7 +2500,7 @@
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -2522,7 +2522,7 @@
       <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -2537,7 +2537,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" ht="21" spans="1:3">
@@ -2548,7 +2548,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" ht="21" spans="1:3">
@@ -2559,7 +2559,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" ht="21" spans="1:3">
@@ -2570,7 +2570,7 @@
         <v>17</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" ht="21" spans="1:3">
@@ -2581,7 +2581,7 @@
         <v>18</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" ht="21" spans="1:3">
@@ -2592,7 +2592,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" ht="21" spans="1:3">
@@ -2603,7 +2603,7 @@
         <v>20</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" ht="21" spans="1:3">
@@ -2614,7 +2614,7 @@
         <v>21</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" ht="21" spans="1:3">
@@ -2625,7 +2625,7 @@
         <v>22</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" ht="21" spans="1:3">
@@ -2636,7 +2636,7 @@
         <v>23</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" ht="21" spans="1:3">
@@ -2647,7 +2647,7 @@
         <v>24</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" ht="21" spans="1:3">
@@ -2658,7 +2658,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" ht="21" spans="1:3">
@@ -2669,7 +2669,7 @@
         <v>26</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" ht="21" spans="1:3">
@@ -2680,7 +2680,7 @@
         <v>27</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" ht="21" spans="1:3">
@@ -2691,7 +2691,7 @@
         <v>28</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" ht="21" spans="1:3">
@@ -2702,7 +2702,7 @@
         <v>29</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" ht="21" spans="1:3">
@@ -2713,7 +2713,7 @@
         <v>30</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" ht="21" spans="1:3">
@@ -2724,7 +2724,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" ht="21" spans="1:3">
@@ -2735,7 +2735,7 @@
         <v>32</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" ht="21" spans="1:3">
@@ -2746,7 +2746,7 @@
         <v>33</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" ht="21" spans="1:3">
@@ -2757,7 +2757,7 @@
         <v>34</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" ht="21" spans="1:3">
@@ -2768,7 +2768,7 @@
         <v>35</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" ht="21" spans="1:3">
@@ -2779,7 +2779,7 @@
         <v>36</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" ht="21" spans="1:3">
@@ -2790,7 +2790,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" ht="21" spans="1:3">
@@ -2801,7 +2801,7 @@
         <v>38</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" ht="21" spans="1:3">
@@ -2812,7 +2812,7 @@
         <v>39</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" ht="21" spans="1:3">
@@ -2823,7 +2823,7 @@
         <v>40</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" ht="21" spans="1:3">
@@ -2834,7 +2834,7 @@
         <v>41</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" ht="21" spans="1:3">
@@ -2845,7 +2845,7 @@
         <v>42</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" ht="21" spans="1:3">
@@ -2856,7 +2856,7 @@
         <v>43</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" ht="21" spans="1:3">
@@ -2867,20 +2867,20 @@
         <v>44</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" ht="21" spans="2:3">
       <c r="B42" s="9"/>
       <c r="C42" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" ht="21" spans="1:3">
       <c r="A43" s="6"/>
       <c r="B43" s="9"/>
       <c r="C43" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" ht="21" spans="1:3">
@@ -2891,7 +2891,7 @@
         <v>46</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" ht="21" spans="1:3">
@@ -2902,7 +2902,7 @@
         <v>47</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" ht="21" spans="1:3">
@@ -2913,7 +2913,7 @@
         <v>48</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" ht="21" spans="1:3">
@@ -2924,7 +2924,7 @@
         <v>49</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" ht="21" spans="1:3">
@@ -2935,7 +2935,7 @@
         <v>50</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" ht="21" spans="1:3">
@@ -2946,7 +2946,7 @@
         <v>51</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" ht="21" spans="1:3">
@@ -2957,7 +2957,7 @@
         <v>52</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" ht="21" spans="1:3">
@@ -2968,7 +2968,7 @@
         <v>53</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" ht="21" spans="1:3">
@@ -2979,7 +2979,7 @@
         <v>54</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" ht="21" spans="1:3">
@@ -2990,7 +2990,7 @@
         <v>55</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" ht="21" spans="1:3">
@@ -3006,7 +3006,7 @@
         <v>57</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" ht="21" spans="1:3">
@@ -3017,7 +3017,7 @@
         <v>58</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" ht="21" spans="1:3">
@@ -3028,7 +3028,7 @@
         <v>59</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" ht="21" spans="1:3">
@@ -3039,7 +3039,7 @@
         <v>60</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" ht="21" spans="1:3">
@@ -3050,7 +3050,7 @@
         <v>61</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" ht="21" spans="1:3">
@@ -3061,7 +3061,7 @@
         <v>62</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" ht="21" spans="1:3">
@@ -3072,7 +3072,7 @@
         <v>63</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" ht="21" spans="1:3">
@@ -3083,7 +3083,7 @@
         <v>64</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" ht="21" spans="1:3">
@@ -3094,7 +3094,7 @@
         <v>65</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" ht="21" spans="1:3">
@@ -3105,7 +3105,7 @@
         <v>66</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" ht="21" spans="1:3">
@@ -3116,7 +3116,7 @@
         <v>67</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" ht="21" spans="1:3">
@@ -3127,7 +3127,7 @@
         <v>68</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" ht="21" spans="1:3">
@@ -3138,7 +3138,7 @@
         <v>69</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" ht="21" spans="1:3">
@@ -3149,7 +3149,7 @@
         <v>70</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" ht="21" spans="1:3">
@@ -3160,7 +3160,7 @@
         <v>71</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" ht="21" spans="1:3">
@@ -3171,7 +3171,7 @@
         <v>72</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" ht="21" spans="1:3">
@@ -3182,7 +3182,7 @@
         <v>73</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" ht="21" spans="1:3">
@@ -3193,7 +3193,7 @@
         <v>74</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" ht="21" spans="1:3">
@@ -3204,7 +3204,7 @@
         <v>75</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" ht="21" spans="1:3">
@@ -3215,7 +3215,7 @@
         <v>76</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" ht="21" spans="1:3">
@@ -3226,7 +3226,7 @@
         <v>77</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" ht="21" spans="1:3">
@@ -3237,7 +3237,7 @@
         <v>78</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" ht="21" spans="1:3">
@@ -3248,7 +3248,7 @@
         <v>79</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" ht="21" spans="1:3">
@@ -3259,7 +3259,7 @@
         <v>80</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" ht="21" spans="1:3">
@@ -3270,7 +3270,7 @@
         <v>81</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" ht="21" spans="1:3">
@@ -3281,7 +3281,7 @@
         <v>82</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" ht="21" spans="1:3">
@@ -3292,7 +3292,7 @@
         <v>83</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" ht="21" spans="1:3">
@@ -3303,7 +3303,7 @@
         <v>84</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" ht="21" spans="1:3">
@@ -3314,7 +3314,7 @@
         <v>85</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" ht="21" spans="1:3">
@@ -3325,7 +3325,7 @@
         <v>86</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" ht="21" spans="1:3">
@@ -3336,7 +3336,7 @@
         <v>87</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" ht="21" spans="1:3">
@@ -3347,7 +3347,7 @@
         <v>88</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" ht="21" spans="1:3">
@@ -3358,7 +3358,7 @@
         <v>89</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="89" ht="21" spans="1:3">
@@ -3369,7 +3369,7 @@
         <v>90</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" ht="21" spans="1:3">
@@ -3380,7 +3380,7 @@
         <v>91</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" ht="21" spans="1:3">
@@ -3391,7 +3391,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" ht="21" spans="1:3">
@@ -3402,7 +3402,7 @@
         <v>93</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" ht="21" spans="1:3">
@@ -3413,7 +3413,7 @@
         <v>94</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" ht="21" spans="1:3">
@@ -3424,7 +3424,7 @@
         <v>95</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" ht="21" spans="1:3">
@@ -3435,7 +3435,7 @@
         <v>96</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" ht="21" spans="1:3">
@@ -3446,7 +3446,7 @@
         <v>97</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97" ht="21" spans="1:3">
@@ -3457,7 +3457,7 @@
         <v>98</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" ht="21" spans="1:3">
@@ -3468,7 +3468,7 @@
         <v>99</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100" ht="21" spans="1:3">
@@ -3484,7 +3484,7 @@
         <v>101</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102" ht="21" spans="1:3">
@@ -3495,7 +3495,7 @@
         <v>102</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" ht="21" spans="1:3">
@@ -3506,7 +3506,7 @@
         <v>103</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="104" ht="21" spans="1:3">
@@ -3517,7 +3517,7 @@
         <v>104</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105" ht="21" spans="1:3">
@@ -3528,7 +3528,7 @@
         <v>105</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="106" ht="21" spans="1:3">
@@ -3539,7 +3539,7 @@
         <v>106</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107" ht="21" spans="1:3">
@@ -3550,7 +3550,7 @@
         <v>107</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108" ht="21" spans="1:3">
@@ -3561,7 +3561,7 @@
         <v>108</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="109" ht="21" spans="1:3">
@@ -3572,7 +3572,7 @@
         <v>109</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110" ht="21" spans="1:3">
@@ -3583,7 +3583,7 @@
         <v>110</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111" ht="21" spans="1:3">
@@ -3594,7 +3594,7 @@
         <v>111</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112" ht="21" spans="1:3">
@@ -3605,7 +3605,7 @@
         <v>112</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113" ht="21" spans="1:3">
@@ -3616,7 +3616,7 @@
         <v>113</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114" ht="21" spans="1:3">
@@ -3627,7 +3627,7 @@
         <v>114</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115" ht="21" spans="1:3">
@@ -3638,7 +3638,7 @@
         <v>115</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" ht="21" spans="1:3">
@@ -3649,7 +3649,7 @@
         <v>116</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117" ht="21" spans="1:3">
@@ -3660,7 +3660,7 @@
         <v>117</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118" ht="21" spans="1:3">
@@ -3671,7 +3671,7 @@
         <v>118</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="119" ht="21" spans="1:3">
@@ -3682,7 +3682,7 @@
         <v>119</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120" ht="21" spans="1:3">
@@ -3693,7 +3693,7 @@
         <v>120</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121" ht="21" spans="1:3">
@@ -3704,7 +3704,7 @@
         <v>121</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="122" ht="21" spans="1:3">
@@ -3715,7 +3715,7 @@
         <v>122</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="123" ht="21" spans="1:3">
@@ -3726,7 +3726,7 @@
         <v>123</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124" ht="21" spans="1:3">
@@ -3737,7 +3737,7 @@
         <v>124</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125" ht="21" spans="1:3">
@@ -3748,7 +3748,7 @@
         <v>125</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" ht="21" spans="1:3">
@@ -3759,7 +3759,7 @@
         <v>126</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="127" ht="21" spans="1:3">
@@ -3770,7 +3770,7 @@
         <v>127</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" ht="21" spans="1:3">
@@ -3781,7 +3781,7 @@
         <v>128</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129" ht="21" spans="1:3">
@@ -3792,7 +3792,7 @@
         <v>129</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="130" ht="21" spans="1:3">
@@ -3803,7 +3803,7 @@
         <v>130</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="131" ht="21" spans="1:3">
@@ -3814,7 +3814,7 @@
         <v>131</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132" ht="21" spans="1:3">
@@ -3825,7 +3825,7 @@
         <v>132</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="133" ht="21" spans="1:3">
@@ -3836,7 +3836,7 @@
         <v>133</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134" ht="21" spans="1:3">
@@ -3847,7 +3847,7 @@
         <v>134</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="135" ht="21" spans="1:3">
@@ -3858,7 +3858,7 @@
         <v>135</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136" ht="21" spans="1:3">
@@ -3869,7 +3869,7 @@
         <v>136</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138" ht="21" spans="2:3">
@@ -3884,7 +3884,7 @@
         <v>138</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140" ht="21" spans="1:3">
@@ -3895,7 +3895,7 @@
         <v>139</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141" ht="21" spans="1:3">
@@ -3906,7 +3906,7 @@
         <v>140</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="142" ht="21" spans="1:3">
@@ -3917,7 +3917,7 @@
         <v>141</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="143" ht="21" spans="1:3">
@@ -3928,7 +3928,7 @@
         <v>142</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="144" ht="21" spans="1:3">
@@ -3939,7 +3939,7 @@
         <v>143</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="145" ht="21" spans="1:3">
@@ -3950,7 +3950,7 @@
         <v>144</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="146" ht="21" spans="1:3">
@@ -3961,7 +3961,7 @@
         <v>145</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="147" ht="21" spans="1:3">
@@ -3972,7 +3972,7 @@
         <v>146</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="148" ht="21" spans="1:3">
@@ -3983,7 +3983,7 @@
         <v>147</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="149" ht="21" spans="1:3">
@@ -3994,7 +3994,7 @@
         <v>148</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="150" ht="21" spans="1:3">
@@ -4005,7 +4005,7 @@
         <v>149</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="151" ht="21" spans="1:3">
@@ -4016,7 +4016,7 @@
         <v>150</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="152" ht="21" spans="1:3">
@@ -4027,7 +4027,7 @@
         <v>151</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="153" ht="21" spans="1:3">
@@ -4038,7 +4038,7 @@
         <v>152</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="154" ht="21" spans="1:3">
@@ -4049,7 +4049,7 @@
         <v>153</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="155" ht="21" spans="1:3">
@@ -4060,7 +4060,7 @@
         <v>154</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="156" ht="21" spans="1:3">
@@ -4071,7 +4071,7 @@
         <v>155</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="157" ht="21" spans="1:3">
@@ -4082,7 +4082,7 @@
         <v>156</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="158" ht="21" spans="1:3">
@@ -4093,7 +4093,7 @@
         <v>157</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="159" ht="21" spans="1:3">
@@ -4104,7 +4104,7 @@
         <v>158</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="160" ht="21" spans="1:3">
@@ -4115,7 +4115,7 @@
         <v>159</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="161" ht="21" spans="1:3">
@@ -4126,7 +4126,7 @@
         <v>160</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="162" ht="21" spans="1:3">
@@ -4137,7 +4137,7 @@
         <v>161</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="163" ht="21" spans="1:3">
@@ -4148,7 +4148,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="164" ht="21" spans="1:3">
@@ -4159,7 +4159,7 @@
         <v>163</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="165" ht="21" spans="1:3">
@@ -4170,7 +4170,7 @@
         <v>164</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="166" ht="21" spans="1:3">
@@ -4181,7 +4181,7 @@
         <v>165</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="167" ht="21" spans="1:3">
@@ -4192,7 +4192,7 @@
         <v>166</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="168" ht="21" spans="1:3">
@@ -4203,7 +4203,7 @@
         <v>167</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="169" ht="21" spans="1:3">
@@ -4214,7 +4214,7 @@
         <v>168</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="170" ht="21" spans="1:3">
@@ -4225,7 +4225,7 @@
         <v>169</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="171" ht="21" spans="1:3">
@@ -4236,7 +4236,7 @@
         <v>170</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="172" ht="21" spans="1:3">
@@ -4247,7 +4247,7 @@
         <v>171</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="173" ht="21" spans="1:3">
@@ -4258,7 +4258,7 @@
         <v>172</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="174" ht="21" spans="1:3">
@@ -4269,7 +4269,7 @@
         <v>173</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="176" ht="21" spans="2:3">
@@ -4284,7 +4284,7 @@
         <v>175</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="178" ht="21" spans="1:3">
@@ -4295,7 +4295,7 @@
         <v>176</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="179" ht="21" spans="1:3">
@@ -4306,7 +4306,7 @@
         <v>177</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="180" ht="21" spans="1:3">
@@ -4317,7 +4317,7 @@
         <v>178</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="181" ht="21" spans="1:3">
@@ -4328,7 +4328,7 @@
         <v>179</v>
       </c>
       <c r="C181" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="182" ht="21" spans="1:3">
@@ -4339,7 +4339,7 @@
         <v>180</v>
       </c>
       <c r="C182" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="183" ht="21" spans="1:3">
@@ -4350,7 +4350,7 @@
         <v>181</v>
       </c>
       <c r="C183" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="184" ht="21" spans="1:3">
@@ -4361,7 +4361,7 @@
         <v>182</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="185" ht="21" spans="1:3">
@@ -4372,7 +4372,7 @@
         <v>183</v>
       </c>
       <c r="C185" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="186" ht="21" spans="1:3">
@@ -4383,7 +4383,7 @@
         <v>184</v>
       </c>
       <c r="C186" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="187" ht="21" spans="1:3">
@@ -4394,7 +4394,7 @@
         <v>185</v>
       </c>
       <c r="C187" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="188" ht="21" spans="1:3">
@@ -4405,7 +4405,7 @@
         <v>186</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="189" ht="21" spans="1:3">
@@ -4416,7 +4416,7 @@
         <v>187</v>
       </c>
       <c r="C189" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="190" ht="21" spans="1:3">
@@ -4427,7 +4427,7 @@
         <v>188</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="191" ht="21" spans="1:3">
@@ -4438,7 +4438,7 @@
         <v>189</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="192" ht="21" spans="1:3">
@@ -4449,7 +4449,7 @@
         <v>190</v>
       </c>
       <c r="C192" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="193" ht="21" spans="1:3">
@@ -4460,7 +4460,7 @@
         <v>191</v>
       </c>
       <c r="C193" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="194" ht="21" spans="1:3">
@@ -4471,7 +4471,7 @@
         <v>192</v>
       </c>
       <c r="C194" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="195" ht="21" spans="1:3">
@@ -4482,7 +4482,7 @@
         <v>193</v>
       </c>
       <c r="C195" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="196" ht="21" spans="1:3">
@@ -4493,7 +4493,7 @@
         <v>194</v>
       </c>
       <c r="C196" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="197" ht="21" spans="1:3">
@@ -4504,7 +4504,7 @@
         <v>195</v>
       </c>
       <c r="C197" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="198" ht="21" spans="1:3">
@@ -4515,7 +4515,7 @@
         <v>196</v>
       </c>
       <c r="C198" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="199" ht="21" spans="1:3">
@@ -4526,7 +4526,7 @@
         <v>197</v>
       </c>
       <c r="C199" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="200" ht="21" spans="1:3">
@@ -4537,7 +4537,7 @@
         <v>198</v>
       </c>
       <c r="C200" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="201" ht="21" spans="1:3">
@@ -4548,7 +4548,7 @@
         <v>199</v>
       </c>
       <c r="C201" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="202" ht="21" spans="1:3">
@@ -4559,7 +4559,7 @@
         <v>200</v>
       </c>
       <c r="C202" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="203" ht="21" spans="1:3">
@@ -4570,7 +4570,7 @@
         <v>201</v>
       </c>
       <c r="C203" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="204" ht="21" spans="1:3">
@@ -4581,7 +4581,7 @@
         <v>202</v>
       </c>
       <c r="C204" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="205" ht="21" spans="1:3">
@@ -4592,7 +4592,7 @@
         <v>203</v>
       </c>
       <c r="C205" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="206" ht="21" spans="1:3">
@@ -4603,7 +4603,7 @@
         <v>204</v>
       </c>
       <c r="C206" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="207" ht="21" spans="1:3">
@@ -4614,7 +4614,7 @@
         <v>205</v>
       </c>
       <c r="C207" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="208" ht="21" spans="1:3">
@@ -4625,7 +4625,7 @@
         <v>206</v>
       </c>
       <c r="C208" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="209" ht="21" spans="1:3">
@@ -4636,7 +4636,7 @@
         <v>207</v>
       </c>
       <c r="C209" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="210" ht="21" spans="1:3">
@@ -4647,7 +4647,7 @@
         <v>208</v>
       </c>
       <c r="C210" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="211" ht="21" spans="1:3">
@@ -4658,7 +4658,7 @@
         <v>209</v>
       </c>
       <c r="C211" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="212" ht="21" spans="1:3">
@@ -4679,7 +4679,7 @@
         <v>211</v>
       </c>
       <c r="C214" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="215" ht="21" spans="1:3">
@@ -4690,7 +4690,7 @@
         <v>212</v>
       </c>
       <c r="C215" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="216" ht="21" spans="1:3">
@@ -4701,7 +4701,7 @@
         <v>213</v>
       </c>
       <c r="C216" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="217" ht="21" spans="1:3">
@@ -4712,7 +4712,7 @@
         <v>214</v>
       </c>
       <c r="C217" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="218" ht="21" spans="1:3">
@@ -4723,7 +4723,7 @@
         <v>215</v>
       </c>
       <c r="C218" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="219" ht="21" spans="1:3">
@@ -4734,7 +4734,7 @@
         <v>216</v>
       </c>
       <c r="C219" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="220" ht="21" spans="1:3">
@@ -4745,7 +4745,7 @@
         <v>217</v>
       </c>
       <c r="C220" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="221" ht="21" spans="1:3">
@@ -4756,7 +4756,7 @@
         <v>218</v>
       </c>
       <c r="C221" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="222" ht="21" spans="1:3">
@@ -4767,7 +4767,7 @@
         <v>219</v>
       </c>
       <c r="C222" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="223" ht="21" spans="1:3">
@@ -4778,7 +4778,7 @@
         <v>220</v>
       </c>
       <c r="C223" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="224" ht="21" spans="1:3">
@@ -4789,7 +4789,7 @@
         <v>221</v>
       </c>
       <c r="C224" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="225" ht="21" spans="1:3">
@@ -4800,7 +4800,7 @@
         <v>222</v>
       </c>
       <c r="C225" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="226" ht="21" spans="1:3">
@@ -4811,7 +4811,7 @@
         <v>223</v>
       </c>
       <c r="C226" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="227" ht="21" spans="1:3">
@@ -4822,7 +4822,7 @@
         <v>224</v>
       </c>
       <c r="C227" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="228" ht="21" spans="1:3">
@@ -4833,7 +4833,7 @@
         <v>225</v>
       </c>
       <c r="C228" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="229" ht="21" spans="1:3">
@@ -4844,7 +4844,7 @@
         <v>226</v>
       </c>
       <c r="C229" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="230" ht="21" spans="1:3">
@@ -4855,7 +4855,7 @@
         <v>227</v>
       </c>
       <c r="C230" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="231" ht="21" spans="1:3">
@@ -4866,7 +4866,7 @@
         <v>228</v>
       </c>
       <c r="C231" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="232" ht="21" spans="1:3">
@@ -4877,7 +4877,7 @@
         <v>229</v>
       </c>
       <c r="C232" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="233" ht="21" spans="1:3">
@@ -4888,7 +4888,7 @@
         <v>230</v>
       </c>
       <c r="C233" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="234" ht="21" spans="1:3">
@@ -4899,7 +4899,7 @@
         <v>231</v>
       </c>
       <c r="C234" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="235" ht="21" spans="1:3">
@@ -4910,7 +4910,7 @@
         <v>232</v>
       </c>
       <c r="C235" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="236" ht="21" spans="2:3">
@@ -4929,7 +4929,7 @@
         <v>234</v>
       </c>
       <c r="C238" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="239" ht="21" spans="1:3">
@@ -4940,7 +4940,7 @@
         <v>235</v>
       </c>
       <c r="C239" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="240" ht="21" spans="1:3">
@@ -4951,7 +4951,7 @@
         <v>236</v>
       </c>
       <c r="C240" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="241" ht="21" spans="1:3">
@@ -4962,7 +4962,7 @@
         <v>237</v>
       </c>
       <c r="C241" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="242" ht="21" spans="1:3">
@@ -4984,7 +4984,7 @@
         <v>240</v>
       </c>
       <c r="C243" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="244" ht="21" spans="1:3">
@@ -4995,7 +4995,7 @@
         <v>241</v>
       </c>
       <c r="C244" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="245" ht="21" spans="1:3">
@@ -5006,7 +5006,7 @@
         <v>242</v>
       </c>
       <c r="C245" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="246" ht="21" spans="1:3">
@@ -5017,7 +5017,7 @@
         <v>243</v>
       </c>
       <c r="C246" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="247" ht="21" spans="1:3">
@@ -5028,7 +5028,7 @@
         <v>244</v>
       </c>
       <c r="C247" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="248" ht="21" spans="1:3">
@@ -5039,7 +5039,7 @@
         <v>245</v>
       </c>
       <c r="C248" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="249" ht="21" spans="1:3">
@@ -5050,7 +5050,7 @@
         <v>246</v>
       </c>
       <c r="C249" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="250" ht="21" spans="1:3">
@@ -5061,7 +5061,7 @@
         <v>247</v>
       </c>
       <c r="C250" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="251" ht="21" spans="1:3">
@@ -5072,7 +5072,7 @@
         <v>248</v>
       </c>
       <c r="C251" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="252" ht="21" spans="1:3">
@@ -5083,7 +5083,7 @@
         <v>249</v>
       </c>
       <c r="C252" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="253" ht="21" spans="1:3">
@@ -5094,7 +5094,7 @@
         <v>250</v>
       </c>
       <c r="C253" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="254" ht="21" spans="1:3">
@@ -5105,7 +5105,7 @@
         <v>251</v>
       </c>
       <c r="C254" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="255" ht="21" spans="1:3">
@@ -5116,7 +5116,7 @@
         <v>252</v>
       </c>
       <c r="C255" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="256" ht="21" spans="1:3">
@@ -5127,7 +5127,7 @@
         <v>253</v>
       </c>
       <c r="C256" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="257" ht="21" spans="1:3">
@@ -5138,7 +5138,7 @@
         <v>254</v>
       </c>
       <c r="C257" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="258" ht="21" spans="1:3">
@@ -5149,7 +5149,7 @@
         <v>255</v>
       </c>
       <c r="C258" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="259" ht="21" spans="1:3">
@@ -5160,7 +5160,7 @@
         <v>256</v>
       </c>
       <c r="C259" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="260" ht="21" spans="1:3">
@@ -5171,7 +5171,7 @@
         <v>257</v>
       </c>
       <c r="C260" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="261" ht="21" spans="1:3">
@@ -5182,7 +5182,7 @@
         <v>258</v>
       </c>
       <c r="C261" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="262" ht="21" spans="1:3">
@@ -5193,7 +5193,7 @@
         <v>259</v>
       </c>
       <c r="C262" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="263" ht="21" spans="1:3">
@@ -5204,7 +5204,7 @@
         <v>260</v>
       </c>
       <c r="C263" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="264" ht="21" spans="1:3">
@@ -5215,7 +5215,7 @@
         <v>261</v>
       </c>
       <c r="C264" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="265" ht="21" spans="1:3">
@@ -5226,7 +5226,7 @@
         <v>262</v>
       </c>
       <c r="C265" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="266" ht="21" spans="1:3">
@@ -5237,7 +5237,7 @@
         <v>263</v>
       </c>
       <c r="C266" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="267" ht="21" spans="1:3">
@@ -5248,7 +5248,7 @@
         <v>264</v>
       </c>
       <c r="C267" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="268" ht="21" spans="1:3">
@@ -5259,7 +5259,7 @@
         <v>265</v>
       </c>
       <c r="C268" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="269" ht="21" spans="1:3">
@@ -5270,7 +5270,7 @@
         <v>266</v>
       </c>
       <c r="C269" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="270" ht="21" spans="1:3">
@@ -5281,7 +5281,7 @@
         <v>267</v>
       </c>
       <c r="C270" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="271" ht="21" spans="1:3">
@@ -5292,7 +5292,7 @@
         <v>90</v>
       </c>
       <c r="C271" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="272" ht="21" spans="1:3">
@@ -5303,7 +5303,7 @@
         <v>268</v>
       </c>
       <c r="C272" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="273" ht="21" spans="2:3">
@@ -5322,7 +5322,7 @@
         <v>270</v>
       </c>
       <c r="C275" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="276" ht="21" spans="1:3">
@@ -5333,7 +5333,7 @@
         <v>271</v>
       </c>
       <c r="C276" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="277" ht="21" spans="1:3">
@@ -5344,7 +5344,7 @@
         <v>272</v>
       </c>
       <c r="C277" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="278" ht="21" spans="1:3">
@@ -5355,7 +5355,7 @@
         <v>273</v>
       </c>
       <c r="C278" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="279" ht="21" spans="1:3">
@@ -5366,7 +5366,7 @@
         <v>274</v>
       </c>
       <c r="C279" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="280" ht="21" spans="1:3">
@@ -5377,7 +5377,7 @@
         <v>275</v>
       </c>
       <c r="C280" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="281" ht="21" spans="1:3">
@@ -5388,7 +5388,7 @@
         <v>276</v>
       </c>
       <c r="C281" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="282" ht="21" spans="1:3">
@@ -5399,7 +5399,7 @@
         <v>277</v>
       </c>
       <c r="C282" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="283" ht="21" spans="1:3">
@@ -5410,7 +5410,7 @@
         <v>278</v>
       </c>
       <c r="C283" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="284" ht="21" spans="1:3">
@@ -5421,7 +5421,7 @@
         <v>279</v>
       </c>
       <c r="C284" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="285" ht="21" spans="1:3">
@@ -5432,7 +5432,7 @@
         <v>280</v>
       </c>
       <c r="C285" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="286" ht="21" spans="1:3">
@@ -5443,7 +5443,7 @@
         <v>281</v>
       </c>
       <c r="C286" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="287" ht="21" spans="1:3">
@@ -5454,7 +5454,7 @@
         <v>282</v>
       </c>
       <c r="C287" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="288" ht="21" spans="1:3">
@@ -5465,7 +5465,7 @@
         <v>283</v>
       </c>
       <c r="C288" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="289" ht="21" spans="1:3">
@@ -5476,7 +5476,7 @@
         <v>284</v>
       </c>
       <c r="C289" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="290" ht="21" spans="1:3">
@@ -5487,7 +5487,7 @@
         <v>285</v>
       </c>
       <c r="C290" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="291" ht="21" spans="1:3">
@@ -5498,7 +5498,7 @@
         <v>286</v>
       </c>
       <c r="C291" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="292" ht="21" spans="1:3">
@@ -5509,7 +5509,7 @@
         <v>287</v>
       </c>
       <c r="C292" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="293" ht="21" spans="1:3">
@@ -5520,7 +5520,7 @@
         <v>288</v>
       </c>
       <c r="C293" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="294" ht="21" spans="2:3">
@@ -5539,7 +5539,7 @@
         <v>290</v>
       </c>
       <c r="C296" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="297" ht="21" spans="1:3">
@@ -5550,7 +5550,7 @@
         <v>291</v>
       </c>
       <c r="C297" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="298" ht="21" spans="1:3">
@@ -5561,7 +5561,7 @@
         <v>292</v>
       </c>
       <c r="C298" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="299" ht="21" spans="1:3">
@@ -5572,7 +5572,7 @@
         <v>293</v>
       </c>
       <c r="C299" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="300" ht="21" spans="1:3">
@@ -5583,7 +5583,7 @@
         <v>294</v>
       </c>
       <c r="C300" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="301" ht="21" spans="1:3">
@@ -5594,7 +5594,7 @@
         <v>295</v>
       </c>
       <c r="C301" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="302" ht="21" spans="1:3">
@@ -5605,7 +5605,7 @@
         <v>296</v>
       </c>
       <c r="C302" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="303" ht="21" spans="1:3">
@@ -5616,7 +5616,7 @@
         <v>297</v>
       </c>
       <c r="C303" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="304" ht="21" spans="1:3">
@@ -5627,7 +5627,7 @@
         <v>298</v>
       </c>
       <c r="C304" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="305" ht="21" spans="1:3">
@@ -5638,7 +5638,7 @@
         <v>299</v>
       </c>
       <c r="C305" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="306" ht="21" spans="1:3">
@@ -5649,7 +5649,7 @@
         <v>300</v>
       </c>
       <c r="C306" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="307" ht="21" spans="1:3">
@@ -5660,7 +5660,7 @@
         <v>301</v>
       </c>
       <c r="C307" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="308" ht="21" spans="1:3">
@@ -5671,7 +5671,7 @@
         <v>302</v>
       </c>
       <c r="C308" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="309" ht="21" spans="1:3">
@@ -5682,7 +5682,7 @@
         <v>303</v>
       </c>
       <c r="C309" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="310" ht="21" spans="1:3">
@@ -5693,7 +5693,7 @@
         <v>304</v>
       </c>
       <c r="C310" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="311" ht="21" spans="1:3">
@@ -5704,7 +5704,7 @@
         <v>305</v>
       </c>
       <c r="C311" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="312" ht="21" spans="1:3">
@@ -5715,7 +5715,7 @@
         <v>306</v>
       </c>
       <c r="C312" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="313" ht="21" spans="1:3">
@@ -5726,7 +5726,7 @@
         <v>307</v>
       </c>
       <c r="C313" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="314" ht="21" spans="1:3">
@@ -5737,7 +5737,7 @@
         <v>308</v>
       </c>
       <c r="C314" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="315" ht="21" spans="1:3">
@@ -5748,7 +5748,7 @@
         <v>309</v>
       </c>
       <c r="C315" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="316" ht="21" spans="1:3">
@@ -5759,7 +5759,7 @@
         <v>310</v>
       </c>
       <c r="C316" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="317" ht="21" spans="1:3">
@@ -5770,7 +5770,7 @@
         <v>311</v>
       </c>
       <c r="C317" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="318" ht="21" spans="1:3">
@@ -5781,7 +5781,7 @@
         <v>312</v>
       </c>
       <c r="C318" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="319" ht="21" spans="1:3">
@@ -5792,7 +5792,7 @@
         <v>313</v>
       </c>
       <c r="C319" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="320" ht="21" spans="1:3">
@@ -5803,7 +5803,7 @@
         <v>314</v>
       </c>
       <c r="C320" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="321" ht="21" spans="1:3">
@@ -5814,7 +5814,7 @@
         <v>315</v>
       </c>
       <c r="C321" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="322" ht="21" spans="1:3">
@@ -5825,7 +5825,7 @@
         <v>316</v>
       </c>
       <c r="C322" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="323" ht="21" spans="1:3">
@@ -5836,7 +5836,7 @@
         <v>317</v>
       </c>
       <c r="C323" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="324" ht="21" spans="1:3">
@@ -5847,7 +5847,7 @@
         <v>318</v>
       </c>
       <c r="C324" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="325" ht="21" spans="1:3">
@@ -5858,7 +5858,7 @@
         <v>319</v>
       </c>
       <c r="C325" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="326" ht="21" spans="1:3">
@@ -5869,7 +5869,7 @@
         <v>320</v>
       </c>
       <c r="C326" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="327" ht="21" spans="1:3">
@@ -5880,7 +5880,7 @@
         <v>321</v>
       </c>
       <c r="C327" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="328" ht="21" spans="1:3">
@@ -5891,7 +5891,7 @@
         <v>322</v>
       </c>
       <c r="C328" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="329" ht="21" spans="1:3">
@@ -5902,7 +5902,7 @@
         <v>323</v>
       </c>
       <c r="C329" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="330" ht="21" spans="1:3">
@@ -5913,7 +5913,7 @@
         <v>324</v>
       </c>
       <c r="C330" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="331" ht="21" spans="1:3">
@@ -5924,7 +5924,7 @@
         <v>325</v>
       </c>
       <c r="C331" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="332" ht="21" spans="1:3">
@@ -5935,7 +5935,7 @@
         <v>326</v>
       </c>
       <c r="C332" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="333" ht="21" spans="1:3">
@@ -5946,7 +5946,7 @@
         <v>327</v>
       </c>
       <c r="C333" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="334" ht="21" spans="2:3">
@@ -5965,7 +5965,7 @@
         <v>329</v>
       </c>
       <c r="C336" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="337" ht="21" spans="1:3">
@@ -5976,7 +5976,7 @@
         <v>330</v>
       </c>
       <c r="C337" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="338" ht="21" spans="1:3">
@@ -5987,7 +5987,7 @@
         <v>331</v>
       </c>
       <c r="C338" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="339" ht="21" spans="1:3">
@@ -5998,7 +5998,7 @@
         <v>332</v>
       </c>
       <c r="C339" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="340" ht="21" spans="1:3">
@@ -6009,7 +6009,7 @@
         <v>333</v>
       </c>
       <c r="C340" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="341" ht="21" spans="1:3">
@@ -6020,7 +6020,7 @@
         <v>334</v>
       </c>
       <c r="C341" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="342" ht="21" spans="1:3">
@@ -6031,7 +6031,7 @@
         <v>335</v>
       </c>
       <c r="C342" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="343" ht="21" spans="1:3">
@@ -6042,7 +6042,7 @@
         <v>336</v>
       </c>
       <c r="C343" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="344" ht="21" spans="1:3">
@@ -6053,7 +6053,7 @@
         <v>337</v>
       </c>
       <c r="C344" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="345" ht="21" spans="1:3">
@@ -6064,7 +6064,7 @@
         <v>338</v>
       </c>
       <c r="C345" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="346" ht="21" spans="1:3">
@@ -6075,7 +6075,7 @@
         <v>339</v>
       </c>
       <c r="C346" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="347" ht="21" spans="1:3">
@@ -6086,7 +6086,7 @@
         <v>340</v>
       </c>
       <c r="C347" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="348" ht="21" spans="1:3">
@@ -6097,7 +6097,7 @@
         <v>341</v>
       </c>
       <c r="C348" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="349" ht="21" spans="1:3">
@@ -6108,7 +6108,7 @@
         <v>342</v>
       </c>
       <c r="C349" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="350" ht="21" spans="1:3">
@@ -6119,7 +6119,7 @@
         <v>343</v>
       </c>
       <c r="C350" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="351" ht="21" spans="1:3">
@@ -6130,7 +6130,7 @@
         <v>344</v>
       </c>
       <c r="C351" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="352" ht="21" spans="1:3">
@@ -6141,7 +6141,7 @@
         <v>345</v>
       </c>
       <c r="C352" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="353" ht="21" spans="1:3">
@@ -6152,7 +6152,7 @@
         <v>346</v>
       </c>
       <c r="C353" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="354" ht="21" spans="2:3">
@@ -6171,7 +6171,7 @@
         <v>348</v>
       </c>
       <c r="C356" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="357" ht="21" spans="1:3">
@@ -6248,7 +6248,7 @@
         <v>355</v>
       </c>
       <c r="C363" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="364" ht="21" spans="1:3">
@@ -6259,7 +6259,7 @@
         <v>356</v>
       </c>
       <c r="C364" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="365" ht="21" spans="1:3">
@@ -6270,7 +6270,7 @@
         <v>357</v>
       </c>
       <c r="C365" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="366" ht="21" spans="1:3">
@@ -6281,7 +6281,7 @@
         <v>358</v>
       </c>
       <c r="C366" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="367" ht="21" spans="1:3">
@@ -6292,7 +6292,7 @@
         <v>359</v>
       </c>
       <c r="C367" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="368" ht="21" spans="1:3">
@@ -6303,7 +6303,7 @@
         <v>360</v>
       </c>
       <c r="C368" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="369" ht="21" spans="1:3">
@@ -6314,7 +6314,7 @@
         <v>361</v>
       </c>
       <c r="C369" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="370" ht="21" spans="1:3">
@@ -6325,7 +6325,7 @@
         <v>362</v>
       </c>
       <c r="C370" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="371" ht="21" spans="1:3">
@@ -6336,7 +6336,7 @@
         <v>363</v>
       </c>
       <c r="C371" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="372" ht="21" spans="1:3">
@@ -6347,7 +6347,7 @@
         <v>364</v>
       </c>
       <c r="C372" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="373" ht="21" spans="1:3">
@@ -6358,7 +6358,7 @@
         <v>365</v>
       </c>
       <c r="C373" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="374" ht="21" spans="1:3">
@@ -6369,7 +6369,7 @@
         <v>366</v>
       </c>
       <c r="C374" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="375" ht="21" spans="1:3">
@@ -6380,7 +6380,7 @@
         <v>367</v>
       </c>
       <c r="C375" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="376" ht="21" spans="1:3">
@@ -6391,7 +6391,7 @@
         <v>368</v>
       </c>
       <c r="C376" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="377" ht="21" spans="1:3">
@@ -6402,7 +6402,7 @@
         <v>369</v>
       </c>
       <c r="C377" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="378" ht="21" spans="1:3">
@@ -6413,7 +6413,7 @@
         <v>370</v>
       </c>
       <c r="C378" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="379" ht="21" spans="1:3">
@@ -6424,7 +6424,7 @@
         <v>371</v>
       </c>
       <c r="C379" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="380" ht="21" spans="1:3">
@@ -6435,7 +6435,7 @@
         <v>372</v>
       </c>
       <c r="C380" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="381" ht="21" spans="1:3">
@@ -6446,7 +6446,7 @@
         <v>373</v>
       </c>
       <c r="C381" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="382" ht="21" spans="1:3">
@@ -6457,7 +6457,7 @@
         <v>374</v>
       </c>
       <c r="C382" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="383" ht="21" spans="1:3">
@@ -6468,7 +6468,7 @@
         <v>375</v>
       </c>
       <c r="C383" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="384" ht="21" spans="1:3">
@@ -6479,7 +6479,7 @@
         <v>376</v>
       </c>
       <c r="C384" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="385" ht="21" spans="1:3">
@@ -6490,7 +6490,7 @@
         <v>377</v>
       </c>
       <c r="C385" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="386" ht="21" spans="1:3">
@@ -6501,7 +6501,7 @@
         <v>378</v>
       </c>
       <c r="C386" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="387" ht="21" spans="1:3">
@@ -6512,7 +6512,7 @@
         <v>379</v>
       </c>
       <c r="C387" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="388" ht="21" spans="1:3">
@@ -6523,7 +6523,7 @@
         <v>380</v>
       </c>
       <c r="C388" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="389" ht="21" spans="1:3">
@@ -6534,7 +6534,7 @@
         <v>381</v>
       </c>
       <c r="C389" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="390" ht="21" spans="1:3">
@@ -6545,7 +6545,7 @@
         <v>381</v>
       </c>
       <c r="C390" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="391" ht="21" spans="1:3">
@@ -6556,7 +6556,7 @@
         <v>382</v>
       </c>
       <c r="C391" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="392" ht="21" spans="1:3">
@@ -6567,7 +6567,7 @@
         <v>383</v>
       </c>
       <c r="C392" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="393" ht="21" spans="1:3">
@@ -6578,7 +6578,7 @@
         <v>384</v>
       </c>
       <c r="C393" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="394" ht="21" spans="1:3">
@@ -6589,7 +6589,7 @@
         <v>385</v>
       </c>
       <c r="C394" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="395" ht="21" spans="1:3">
@@ -6600,7 +6600,7 @@
         <v>386</v>
       </c>
       <c r="C395" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="396" ht="21" spans="1:3">
@@ -6611,7 +6611,7 @@
         <v>387</v>
       </c>
       <c r="C396" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="397" ht="21" spans="1:3">
@@ -6622,7 +6622,7 @@
         <v>388</v>
       </c>
       <c r="C397" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="398" ht="21" spans="1:3">
@@ -6633,7 +6633,7 @@
         <v>389</v>
       </c>
       <c r="C398" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="399" ht="21" spans="1:3">
@@ -6644,7 +6644,7 @@
         <v>390</v>
       </c>
       <c r="C399" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="400" ht="21" spans="2:3">
@@ -6663,7 +6663,7 @@
         <v>392</v>
       </c>
       <c r="C402" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="403" ht="21" spans="1:3">
@@ -6674,7 +6674,7 @@
         <v>393</v>
       </c>
       <c r="C403" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="404" ht="21" spans="1:3">
@@ -6685,7 +6685,7 @@
         <v>394</v>
       </c>
       <c r="C404" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="405" ht="21" spans="1:3">
@@ -6696,7 +6696,7 @@
         <v>92</v>
       </c>
       <c r="C405" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="406" ht="21" spans="1:3">
@@ -6707,7 +6707,7 @@
         <v>395</v>
       </c>
       <c r="C406" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="407" ht="21" spans="1:3">
@@ -6718,7 +6718,7 @@
         <v>396</v>
       </c>
       <c r="C407" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="408" ht="21" spans="2:3">
@@ -6737,7 +6737,7 @@
         <v>398</v>
       </c>
       <c r="C410" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="411" ht="21" spans="1:3">
@@ -6748,7 +6748,7 @@
         <v>399</v>
       </c>
       <c r="C411" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="412" ht="21" spans="1:3">
@@ -6759,7 +6759,7 @@
         <v>400</v>
       </c>
       <c r="C412" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="413" ht="21" spans="1:3">
@@ -6770,7 +6770,7 @@
         <v>401</v>
       </c>
       <c r="C413" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="414" ht="21" spans="1:3">
@@ -6781,7 +6781,7 @@
         <v>402</v>
       </c>
       <c r="C414" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="415" ht="21" spans="1:3">
@@ -6792,7 +6792,7 @@
         <v>403</v>
       </c>
       <c r="C415" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="416" ht="21" spans="1:3">
@@ -6803,7 +6803,7 @@
         <v>404</v>
       </c>
       <c r="C416" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="417" ht="21" spans="1:3">
@@ -6814,7 +6814,7 @@
         <v>277</v>
       </c>
       <c r="C417" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="418" ht="21" spans="1:3">
@@ -6825,7 +6825,7 @@
         <v>405</v>
       </c>
       <c r="C418" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="419" ht="21" spans="1:3">
@@ -6836,7 +6836,7 @@
         <v>406</v>
       </c>
       <c r="C419" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="420" ht="21" spans="1:3">
@@ -6847,7 +6847,7 @@
         <v>407</v>
       </c>
       <c r="C420" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="421" ht="21" spans="1:3">
@@ -6858,7 +6858,7 @@
         <v>408</v>
       </c>
       <c r="C421" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="422" ht="21" spans="1:3">
@@ -6869,7 +6869,7 @@
         <v>409</v>
       </c>
       <c r="C422" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="423" ht="21" spans="1:3">
@@ -6880,7 +6880,7 @@
         <v>410</v>
       </c>
       <c r="C423" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="424" ht="21" spans="1:3">
@@ -6891,7 +6891,7 @@
         <v>411</v>
       </c>
       <c r="C424" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="425" ht="21" spans="1:3">
@@ -6902,7 +6902,7 @@
         <v>412</v>
       </c>
       <c r="C425" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="426" ht="21" spans="1:3">
@@ -6913,7 +6913,7 @@
         <v>413</v>
       </c>
       <c r="C426" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="427" ht="21" spans="1:3">
@@ -6924,7 +6924,7 @@
         <v>414</v>
       </c>
       <c r="C427" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="428" ht="21" spans="1:3">
@@ -6935,7 +6935,7 @@
         <v>415</v>
       </c>
       <c r="C428" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="429" ht="21" spans="1:3">
@@ -6946,7 +6946,7 @@
         <v>416</v>
       </c>
       <c r="C429" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="430" ht="21" spans="1:3">
@@ -6957,7 +6957,7 @@
         <v>417</v>
       </c>
       <c r="C430" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="431" ht="21" spans="1:3">
@@ -6968,7 +6968,7 @@
         <v>418</v>
       </c>
       <c r="C431" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="432" ht="21" spans="1:3">
@@ -6979,7 +6979,7 @@
         <v>419</v>
       </c>
       <c r="C432" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="433" ht="21" spans="1:3">
@@ -6990,7 +6990,7 @@
         <v>420</v>
       </c>
       <c r="C433" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="434" ht="21" spans="1:3">
@@ -7001,7 +7001,7 @@
         <v>421</v>
       </c>
       <c r="C434" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="435" ht="21" spans="1:3">
@@ -7012,7 +7012,7 @@
         <v>422</v>
       </c>
       <c r="C435" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="436" ht="21" spans="1:3">
@@ -7023,7 +7023,7 @@
         <v>423</v>
       </c>
       <c r="C436" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="437" ht="21" spans="1:3">
@@ -7034,7 +7034,7 @@
         <v>424</v>
       </c>
       <c r="C437" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="438" ht="21" spans="1:3">
@@ -7045,7 +7045,7 @@
         <v>425</v>
       </c>
       <c r="C438" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="439" ht="21" spans="1:3">
@@ -7056,7 +7056,7 @@
         <v>426</v>
       </c>
       <c r="C439" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="440" ht="21" spans="1:3">
@@ -7067,7 +7067,7 @@
         <v>427</v>
       </c>
       <c r="C440" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="441" ht="21" spans="1:3">
@@ -7078,7 +7078,7 @@
         <v>428</v>
       </c>
       <c r="C441" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="442" ht="21" spans="1:3">
@@ -7089,7 +7089,7 @@
         <v>429</v>
       </c>
       <c r="C442" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="443" ht="21" spans="1:3">
@@ -7100,7 +7100,7 @@
         <v>430</v>
       </c>
       <c r="C443" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="444" ht="21" spans="1:3">
@@ -7111,7 +7111,7 @@
         <v>431</v>
       </c>
       <c r="C444" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="445" ht="21" spans="1:3">
@@ -7122,7 +7122,7 @@
         <v>432</v>
       </c>
       <c r="C445" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="446" ht="21" spans="1:3">
@@ -7133,7 +7133,7 @@
         <v>433</v>
       </c>
       <c r="C446" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="447" ht="21" spans="1:3">
@@ -7144,7 +7144,7 @@
         <v>434</v>
       </c>
       <c r="C447" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="448" ht="21" spans="1:3">
@@ -7155,7 +7155,7 @@
         <v>435</v>
       </c>
       <c r="C448" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="449" ht="21" spans="1:3">
@@ -7166,7 +7166,7 @@
         <v>436</v>
       </c>
       <c r="C449" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="450" ht="21" spans="1:3">
@@ -7177,7 +7177,7 @@
         <v>437</v>
       </c>
       <c r="C450" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="451" ht="21" spans="1:3">
@@ -7188,7 +7188,7 @@
         <v>438</v>
       </c>
       <c r="C451" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="452" ht="21" spans="1:3">
@@ -7199,7 +7199,7 @@
         <v>439</v>
       </c>
       <c r="C452" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="453" ht="21" spans="1:3">
@@ -7210,7 +7210,7 @@
         <v>440</v>
       </c>
       <c r="C453" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="454" ht="21" spans="1:3">
@@ -7221,7 +7221,7 @@
         <v>441</v>
       </c>
       <c r="C454" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="455" ht="21" spans="1:3">
@@ -7232,7 +7232,7 @@
         <v>442</v>
       </c>
       <c r="C455" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="456" ht="21" spans="1:3">
@@ -7243,7 +7243,7 @@
         <v>443</v>
       </c>
       <c r="C456" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="457" ht="21" spans="1:3">
@@ -7254,7 +7254,7 @@
         <v>444</v>
       </c>
       <c r="C457" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="458" ht="21" spans="1:3">
@@ -7265,7 +7265,7 @@
         <v>445</v>
       </c>
       <c r="C458" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="459" ht="21" spans="1:3">
@@ -7276,7 +7276,7 @@
         <v>446</v>
       </c>
       <c r="C459" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="460" ht="21" spans="1:3">
@@ -7287,7 +7287,7 @@
         <v>447</v>
       </c>
       <c r="C460" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="461" ht="21" spans="1:3">
@@ -7298,7 +7298,7 @@
         <v>448</v>
       </c>
       <c r="C461" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="462" ht="21" spans="1:3">
@@ -7309,7 +7309,7 @@
         <v>449</v>
       </c>
       <c r="C462" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="463" ht="21" spans="1:3">
@@ -7320,7 +7320,7 @@
         <v>450</v>
       </c>
       <c r="C463" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="464" ht="21" spans="1:3">
@@ -7331,7 +7331,7 @@
         <v>451</v>
       </c>
       <c r="C464" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="465" ht="21" spans="1:3">
@@ -7342,7 +7342,7 @@
         <v>452</v>
       </c>
       <c r="C465" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="466" ht="21" spans="1:3">
@@ -7353,7 +7353,7 @@
         <v>453</v>
       </c>
       <c r="C466" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="467" ht="21" spans="1:3">
@@ -7364,7 +7364,7 @@
         <v>454</v>
       </c>
       <c r="C467" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="468" ht="21" spans="1:3">
@@ -7375,7 +7375,7 @@
         <v>455</v>
       </c>
       <c r="C468" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="469" ht="21" spans="1:3">
@@ -7386,7 +7386,7 @@
         <v>456</v>
       </c>
       <c r="C469" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="470" ht="21" spans="2:3">
@@ -7406,7 +7406,7 @@
         <v>458</v>
       </c>
       <c r="C472" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="473" ht="21" spans="1:3">
@@ -7417,7 +7417,7 @@
         <v>459</v>
       </c>
       <c r="C473" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="474" ht="21" spans="1:3">
@@ -7428,7 +7428,7 @@
         <v>460</v>
       </c>
       <c r="C474" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="475" ht="21" spans="1:3">
@@ -7439,7 +7439,7 @@
         <v>461</v>
       </c>
       <c r="C475" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="476" ht="21" spans="1:3">
@@ -7450,7 +7450,7 @@
         <v>462</v>
       </c>
       <c r="C476" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="477" ht="21" spans="1:3">
@@ -7461,7 +7461,7 @@
         <v>463</v>
       </c>
       <c r="C477" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="478" ht="21" spans="1:3">
@@ -7472,7 +7472,7 @@
         <v>464</v>
       </c>
       <c r="C478" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="479" ht="21" spans="1:3">
@@ -7483,7 +7483,7 @@
         <v>465</v>
       </c>
       <c r="C479" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="480" ht="21" spans="1:3">
@@ -7494,7 +7494,7 @@
         <v>466</v>
       </c>
       <c r="C480" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="481" ht="21" spans="1:3">
@@ -7505,7 +7505,7 @@
         <v>467</v>
       </c>
       <c r="C481" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Union of two array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1425,10 +1425,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1503,16 +1503,24 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1523,10 +1531,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1546,16 +1555,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1594,15 +1602,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1617,14 +1617,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1632,7 +1632,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1654,19 +1654,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1678,7 +1672,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1696,7 +1702,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1708,25 +1774,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1738,85 +1816,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1828,13 +1828,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1845,6 +1845,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1859,15 +1883,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1896,28 +1911,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1939,155 +1937,157 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2438,7 +2438,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2533,18 +2533,18 @@
       <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" ht="21" spans="1:3">
       <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="5" t="s">

</xml_diff>

<commit_message>
Rotate array cyclically by one
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1426,9 +1426,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1502,25 +1502,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1531,11 +1517,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1555,25 +1561,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1586,7 +1585,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1608,6 +1607,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -1617,14 +1631,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1633,13 +1640,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1654,7 +1654,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1666,7 +1762,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1678,37 +1804,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1720,121 +1834,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1848,26 +1848,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1887,21 +1887,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1916,6 +1901,21 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1948,146 +1948,146 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2438,7 +2438,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2548,7 +2548,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Finding max sum subarray
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1425,9 +1425,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
@@ -1502,16 +1502,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1532,14 +1524,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1548,6 +1563,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1576,6 +1599,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -1585,25 +1616,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1622,24 +1638,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1654,7 +1654,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1666,13 +1744,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1690,91 +1798,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1792,19 +1816,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1816,25 +1828,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1845,6 +1845,56 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1872,35 +1922,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1919,175 +1945,149 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2438,7 +2438,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2555,18 +2555,18 @@
       <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" ht="21" spans="1:3">
       <c r="A14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="5" t="s">

</xml_diff>

<commit_message>
Basic declaration of class
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1425,10 +1425,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1503,21 +1503,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1530,16 +1524,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1553,32 +1554,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1624,7 +1602,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1644,6 +1637,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1654,7 +1654,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1666,13 +1792,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1684,157 +1828,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1848,26 +1848,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1883,17 +1874,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1931,163 +1922,172 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2438,7 +2438,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2577,7 +2577,7 @@
       <c r="A15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="5" t="s">

</xml_diff>

<commit_message>
Matrix chain multiplication memoaization
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1422,10 +1422,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1500,6 +1500,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1508,20 +1515,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1535,9 +1528,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1574,14 +1582,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -1613,7 +1613,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1628,15 +1636,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1651,13 +1651,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1669,31 +1693,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1705,49 +1735,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1765,13 +1753,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1783,13 +1771,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1801,31 +1789,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1945,53 +1945,53 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -2003,88 +2003,88 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2435,7 +2435,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A407" workbookViewId="0">
-      <selection activeCell="C415" sqref="C415"/>
+      <selection activeCell="C416" sqref="C416"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -6787,7 +6787,7 @@
         <v>402</v>
       </c>
       <c r="C415" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="416" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Tree code (any number of children of each parent
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1422,10 +1422,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1500,9 +1500,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1510,6 +1510,21 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1521,18 +1536,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1559,14 +1566,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -1579,6 +1578,14 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1599,21 +1606,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1627,16 +1635,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1651,7 +1651,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1663,25 +1675,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1699,25 +1723,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1729,7 +1753,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1741,19 +1777,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1765,31 +1795,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1801,37 +1831,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1846,16 +1846,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1871,15 +1880,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1909,25 +1909,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1942,149 +1933,158 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2435,7 +2435,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A407" workbookViewId="0">
-      <selection activeCell="C416" sqref="C416"/>
+      <selection activeCell="C417" sqref="C417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -6798,7 +6798,7 @@
         <v>403</v>
       </c>
       <c r="C416" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="417" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Diameter of BT LeetCode
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1422,9 +1422,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
@@ -1500,7 +1500,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1515,31 +1536,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1561,6 +1560,29 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1605,28 +1627,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1651,13 +1651,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1669,37 +1699,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1723,13 +1723,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1747,13 +1789,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1765,73 +1819,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1842,6 +1842,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1860,11 +1875,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1884,17 +1905,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1904,21 +1919,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1945,80 +1945,80 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -2027,64 +2027,64 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2434,8 +2434,8 @@
   <sheetPr/>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A407" workbookViewId="0">
-      <selection activeCell="C417" sqref="C417"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="B179" sqref="B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -4279,7 +4279,7 @@
         <v>174</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="178" ht="21" spans="1:3">
@@ -4290,14 +4290,14 @@
         <v>175</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="179" ht="21" spans="1:3">
       <c r="A179" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B179" s="8" t="s">
+      <c r="B179" s="7" t="s">
         <v>176</v>
       </c>
       <c r="C179" s="5" t="s">

</xml_diff>

<commit_message>
Mirror of Binary Tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1422,10 +1422,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1507,21 +1507,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1534,24 +1520,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1570,21 +1541,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1629,7 +1585,36 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1637,6 +1622,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1651,7 +1651,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1663,7 +1765,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1675,49 +1783,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1729,7 +1795,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1741,19 +1813,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1771,67 +1831,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1842,6 +1842,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1856,6 +1880,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1890,35 +1923,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1933,25 +1942,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1964,127 +1964,127 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2435,7 +2435,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="B179" sqref="B179"/>
+      <selection activeCell="C182" sqref="C182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -4301,7 +4301,7 @@
         <v>176</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="180" ht="21" spans="1:3">
@@ -4312,7 +4312,7 @@
         <v>177</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="181" ht="21" spans="1:3">
@@ -4323,7 +4323,7 @@
         <v>178</v>
       </c>
       <c r="C181" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="182" ht="21" spans="1:3">

</xml_diff>

<commit_message>
pre,in,post recursive approach for BT leetcode
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1424,8 +1424,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1502,14 +1502,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1523,6 +1523,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1585,7 +1592,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1599,22 +1606,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1628,7 +1620,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1651,31 +1651,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1687,13 +1675,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1711,13 +1699,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1735,19 +1723,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1765,7 +1741,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1777,7 +1753,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1789,13 +1771,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1807,31 +1825,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1894,6 +1894,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1904,21 +1919,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1945,146 +1945,146 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2435,7 +2435,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="C182" sqref="C182"/>
+      <selection activeCell="C185" sqref="C185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -4330,11 +4330,11 @@
       <c r="A182" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B182" s="8" t="s">
+      <c r="B182" s="7" t="s">
         <v>179</v>
       </c>
       <c r="C182" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="183" ht="21" spans="1:3">
@@ -4345,7 +4345,7 @@
         <v>180</v>
       </c>
       <c r="C183" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="184" ht="21" spans="1:3">
@@ -4356,7 +4356,7 @@
         <v>181</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="185" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Vertical Traversal of Binary Tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1422,9 +1422,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
@@ -1502,6 +1502,21 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1509,12 +1524,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1529,7 +1552,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1544,10 +1567,33 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1566,56 +1612,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1626,9 +1627,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1651,7 +1651,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1663,13 +1681,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1681,55 +1729,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1741,43 +1765,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1801,37 +1801,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1845,26 +1845,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1884,25 +1884,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1926,8 +1917,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1945,146 +1945,146 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2434,8 +2434,8 @@
   <sheetPr/>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="C185" sqref="C185"/>
+    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="B187" sqref="B187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -4367,7 +4367,7 @@
         <v>182</v>
       </c>
       <c r="C185" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="186" ht="21" spans="1:3">
@@ -4378,14 +4378,14 @@
         <v>183</v>
       </c>
       <c r="C186" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="187" ht="21" spans="1:3">
       <c r="A187" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B187" s="8" t="s">
+      <c r="B187" s="7" t="s">
         <v>184</v>
       </c>
       <c r="C187" s="5" t="s">

</xml_diff>

<commit_message>
Zig zag traversal of binary tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1422,10 +1422,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1507,45 +1507,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1559,31 +1521,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1591,7 +1529,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1612,16 +1550,72 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1634,9 +1628,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1651,7 +1651,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1663,19 +1675,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1687,13 +1687,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1705,49 +1711,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1765,7 +1735,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1777,7 +1747,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1789,7 +1783,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1801,7 +1807,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1819,13 +1825,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1842,6 +1842,60 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1869,60 +1923,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1945,7 +1945,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1964,127 +1964,127 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2434,8 +2434,8 @@
   <sheetPr/>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="B187" sqref="B187"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="C188" sqref="C188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -4389,7 +4389,7 @@
         <v>184</v>
       </c>
       <c r="C187" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="188" ht="21" spans="1:3">

</xml_diff>

<commit_message>
A binary tree is balanced or not
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1422,10 +1422,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1500,16 +1500,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1520,18 +1520,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1566,8 +1566,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1581,14 +1597,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -1597,24 +1605,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1623,20 +1637,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1651,37 +1651,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1705,7 +1717,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1717,121 +1825,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1842,30 +1842,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1908,15 +1884,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1934,6 +1901,39 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1945,146 +1945,146 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2434,8 +2434,8 @@
   <sheetPr/>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="C190" sqref="C190"/>
+    <sheetView tabSelected="1" topLeftCell="A186" workbookViewId="0">
+      <selection activeCell="C191" sqref="C191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -4422,7 +4422,7 @@
         <v>187</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="191" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Boundary Traversal of binary tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1423,9 +1423,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1500,20 +1500,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1521,30 +1507,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1558,6 +1521,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -1566,16 +1536,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1584,6 +1547,13 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1605,6 +1575,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -1621,7 +1607,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1634,9 +1628,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1651,19 +1651,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1681,19 +1687,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1705,13 +1717,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1723,31 +1747,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1765,13 +1771,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1783,55 +1819,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1860,15 +1860,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1880,6 +1871,50 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1902,189 +1937,154 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2434,8 +2434,8 @@
   <sheetPr/>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A186" workbookViewId="0">
-      <selection activeCell="C191" sqref="C191"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="C192" sqref="C192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -4433,7 +4433,7 @@
         <v>188</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="192" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Convert Binary tree into doubly linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="468">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -590,6 +590,9 @@
   </si>
   <si>
     <t>Convert Binary tree into Doubly Linked List</t>
+  </si>
+  <si>
+    <t>&lt;YES&gt;</t>
   </si>
   <si>
     <t>Convert Binary tree into Sum tree</t>
@@ -1423,9 +1426,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1507,7 +1510,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1521,34 +1554,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1564,6 +1574,14 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1583,24 +1601,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1628,8 +1630,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1657,7 +1660,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1669,19 +1708,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1693,145 +1834,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1842,6 +1845,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1856,6 +1874,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1879,42 +1906,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1942,149 +1934,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2435,7 +2438,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="C192" sqref="C192"/>
+      <selection activeCell="C195" sqref="C195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -4444,14 +4447,14 @@
         <v>189</v>
       </c>
       <c r="C192" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="193" ht="21" spans="1:3">
       <c r="A193" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B193" s="8" t="s">
+      <c r="B193" s="7" t="s">
         <v>190</v>
       </c>
       <c r="C193" s="5" t="s">
@@ -4466,7 +4469,7 @@
         <v>191</v>
       </c>
       <c r="C194" s="5" t="s">
-        <v>5</v>
+        <v>192</v>
       </c>
     </row>
     <row r="195" ht="21" spans="1:3">
@@ -4474,7 +4477,7 @@
         <v>173</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C195" s="5" t="s">
         <v>5</v>
@@ -4485,7 +4488,7 @@
         <v>173</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C196" s="5" t="s">
         <v>5</v>
@@ -4496,7 +4499,7 @@
         <v>173</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C197" s="5" t="s">
         <v>5</v>
@@ -4507,7 +4510,7 @@
         <v>173</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C198" s="5" t="s">
         <v>5</v>
@@ -4518,7 +4521,7 @@
         <v>173</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C199" s="5" t="s">
         <v>5</v>
@@ -4529,7 +4532,7 @@
         <v>173</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C200" s="5" t="s">
         <v>5</v>
@@ -4540,7 +4543,7 @@
         <v>173</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C201" s="5" t="s">
         <v>5</v>
@@ -4551,7 +4554,7 @@
         <v>173</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C202" s="5" t="s">
         <v>5</v>
@@ -4562,7 +4565,7 @@
         <v>173</v>
       </c>
       <c r="B203" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C203" s="5" t="s">
         <v>5</v>
@@ -4573,7 +4576,7 @@
         <v>173</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C204" s="5" t="s">
         <v>5</v>
@@ -4584,7 +4587,7 @@
         <v>173</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C205" s="5" t="s">
         <v>5</v>
@@ -4595,7 +4598,7 @@
         <v>173</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C206" s="5" t="s">
         <v>5</v>
@@ -4606,7 +4609,7 @@
         <v>173</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C207" s="5" t="s">
         <v>5</v>
@@ -4617,7 +4620,7 @@
         <v>173</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C208" s="5" t="s">
         <v>5</v>
@@ -4628,7 +4631,7 @@
         <v>173</v>
       </c>
       <c r="B209" s="8" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C209" s="5" t="s">
         <v>5</v>
@@ -4639,7 +4642,7 @@
         <v>173</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C210" s="5" t="s">
         <v>5</v>
@@ -4650,7 +4653,7 @@
         <v>173</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C211" s="5" t="s">
         <v>5</v>
@@ -4668,10 +4671,10 @@
     </row>
     <row r="214" ht="21" spans="1:3">
       <c r="A214" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B214" s="8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C214" s="5" t="s">
         <v>5</v>
@@ -4679,10 +4682,10 @@
     </row>
     <row r="215" ht="21" spans="1:3">
       <c r="A215" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B215" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C215" s="5" t="s">
         <v>5</v>
@@ -4690,10 +4693,10 @@
     </row>
     <row r="216" ht="21" spans="1:3">
       <c r="A216" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B216" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C216" s="5" t="s">
         <v>5</v>
@@ -4701,10 +4704,10 @@
     </row>
     <row r="217" ht="21" spans="1:3">
       <c r="A217" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C217" s="5" t="s">
         <v>5</v>
@@ -4712,10 +4715,10 @@
     </row>
     <row r="218" ht="21" spans="1:3">
       <c r="A218" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B218" s="8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C218" s="5" t="s">
         <v>5</v>
@@ -4723,10 +4726,10 @@
     </row>
     <row r="219" ht="21" spans="1:3">
       <c r="A219" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B219" s="8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C219" s="5" t="s">
         <v>5</v>
@@ -4734,10 +4737,10 @@
     </row>
     <row r="220" ht="21" spans="1:3">
       <c r="A220" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B220" s="11" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C220" s="5" t="s">
         <v>5</v>
@@ -4745,10 +4748,10 @@
     </row>
     <row r="221" ht="21" spans="1:3">
       <c r="A221" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B221" s="8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C221" s="5" t="s">
         <v>5</v>
@@ -4756,10 +4759,10 @@
     </row>
     <row r="222" ht="21" spans="1:3">
       <c r="A222" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B222" s="8" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C222" s="5" t="s">
         <v>5</v>
@@ -4767,10 +4770,10 @@
     </row>
     <row r="223" ht="21" spans="1:3">
       <c r="A223" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B223" s="8" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C223" s="5" t="s">
         <v>5</v>
@@ -4778,10 +4781,10 @@
     </row>
     <row r="224" ht="21" spans="1:3">
       <c r="A224" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B224" s="8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C224" s="5" t="s">
         <v>5</v>
@@ -4789,10 +4792,10 @@
     </row>
     <row r="225" ht="21" spans="1:3">
       <c r="A225" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B225" s="8" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C225" s="5" t="s">
         <v>5</v>
@@ -4800,10 +4803,10 @@
     </row>
     <row r="226" ht="21" spans="1:3">
       <c r="A226" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B226" s="8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C226" s="5" t="s">
         <v>5</v>
@@ -4811,10 +4814,10 @@
     </row>
     <row r="227" ht="21" spans="1:3">
       <c r="A227" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B227" s="8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C227" s="5" t="s">
         <v>5</v>
@@ -4822,10 +4825,10 @@
     </row>
     <row r="228" ht="21" spans="1:3">
       <c r="A228" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B228" s="8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C228" s="5" t="s">
         <v>5</v>
@@ -4833,10 +4836,10 @@
     </row>
     <row r="229" ht="21" spans="1:3">
       <c r="A229" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B229" s="8" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C229" s="5" t="s">
         <v>5</v>
@@ -4844,10 +4847,10 @@
     </row>
     <row r="230" ht="21" spans="1:3">
       <c r="A230" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B230" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C230" s="5" t="s">
         <v>5</v>
@@ -4855,10 +4858,10 @@
     </row>
     <row r="231" ht="21" spans="1:3">
       <c r="A231" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B231" s="8" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C231" s="5" t="s">
         <v>5</v>
@@ -4866,10 +4869,10 @@
     </row>
     <row r="232" ht="21" spans="1:3">
       <c r="A232" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B232" s="8" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C232" s="5" t="s">
         <v>5</v>
@@ -4877,10 +4880,10 @@
     </row>
     <row r="233" ht="21" spans="1:3">
       <c r="A233" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B233" s="8" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C233" s="5" t="s">
         <v>5</v>
@@ -4888,10 +4891,10 @@
     </row>
     <row r="234" ht="21" spans="1:3">
       <c r="A234" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B234" s="8" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C234" s="5" t="s">
         <v>5</v>
@@ -4899,10 +4902,10 @@
     </row>
     <row r="235" ht="21" spans="1:3">
       <c r="A235" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B235" s="8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C235" s="5" t="s">
         <v>5</v>
@@ -4918,10 +4921,10 @@
     </row>
     <row r="238" ht="21" spans="1:3">
       <c r="A238" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B238" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C238" s="5" t="s">
         <v>5</v>
@@ -4929,10 +4932,10 @@
     </row>
     <row r="239" ht="21" spans="1:3">
       <c r="A239" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B239" s="8" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C239" s="5" t="s">
         <v>5</v>
@@ -4940,10 +4943,10 @@
     </row>
     <row r="240" ht="21" spans="1:3">
       <c r="A240" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B240" s="8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C240" s="5" t="s">
         <v>5</v>
@@ -4951,10 +4954,10 @@
     </row>
     <row r="241" ht="21" spans="1:3">
       <c r="A241" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B241" s="8" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C241" s="5" t="s">
         <v>5</v>
@@ -4962,21 +4965,21 @@
     </row>
     <row r="242" ht="21" spans="1:3">
       <c r="A242" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B242" s="8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C242" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="243" ht="21" spans="1:3">
       <c r="A243" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B243" s="8" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C243" s="5" t="s">
         <v>5</v>
@@ -4984,10 +4987,10 @@
     </row>
     <row r="244" ht="21" spans="1:3">
       <c r="A244" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B244" s="8" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C244" s="5" t="s">
         <v>5</v>
@@ -4995,10 +4998,10 @@
     </row>
     <row r="245" ht="21" spans="1:3">
       <c r="A245" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B245" s="8" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C245" s="5" t="s">
         <v>5</v>
@@ -5006,10 +5009,10 @@
     </row>
     <row r="246" ht="21" spans="1:3">
       <c r="A246" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B246" s="8" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C246" s="5" t="s">
         <v>5</v>
@@ -5017,10 +5020,10 @@
     </row>
     <row r="247" ht="21" spans="1:3">
       <c r="A247" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B247" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C247" s="5" t="s">
         <v>5</v>
@@ -5028,10 +5031,10 @@
     </row>
     <row r="248" ht="21" spans="1:3">
       <c r="A248" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B248" s="8" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C248" s="5" t="s">
         <v>5</v>
@@ -5039,10 +5042,10 @@
     </row>
     <row r="249" ht="21" spans="1:3">
       <c r="A249" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B249" s="8" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C249" s="5" t="s">
         <v>5</v>
@@ -5050,10 +5053,10 @@
     </row>
     <row r="250" ht="21" spans="1:3">
       <c r="A250" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B250" s="8" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C250" s="5" t="s">
         <v>5</v>
@@ -5061,10 +5064,10 @@
     </row>
     <row r="251" ht="21" spans="1:3">
       <c r="A251" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B251" s="8" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C251" s="5" t="s">
         <v>5</v>
@@ -5072,10 +5075,10 @@
     </row>
     <row r="252" ht="21" spans="1:3">
       <c r="A252" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B252" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C252" s="5" t="s">
         <v>5</v>
@@ -5083,10 +5086,10 @@
     </row>
     <row r="253" ht="21" spans="1:3">
       <c r="A253" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B253" s="8" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C253" s="5" t="s">
         <v>5</v>
@@ -5094,10 +5097,10 @@
     </row>
     <row r="254" ht="21" spans="1:3">
       <c r="A254" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B254" s="8" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C254" s="5" t="s">
         <v>5</v>
@@ -5105,10 +5108,10 @@
     </row>
     <row r="255" ht="21" spans="1:3">
       <c r="A255" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B255" s="8" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C255" s="5" t="s">
         <v>5</v>
@@ -5116,10 +5119,10 @@
     </row>
     <row r="256" ht="21" spans="1:3">
       <c r="A256" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B256" s="8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C256" s="5" t="s">
         <v>5</v>
@@ -5127,10 +5130,10 @@
     </row>
     <row r="257" ht="21" spans="1:3">
       <c r="A257" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B257" s="8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C257" s="5" t="s">
         <v>5</v>
@@ -5138,10 +5141,10 @@
     </row>
     <row r="258" ht="21" spans="1:3">
       <c r="A258" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B258" s="8" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C258" s="5" t="s">
         <v>5</v>
@@ -5149,10 +5152,10 @@
     </row>
     <row r="259" ht="21" spans="1:3">
       <c r="A259" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B259" s="8" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C259" s="5" t="s">
         <v>5</v>
@@ -5160,10 +5163,10 @@
     </row>
     <row r="260" ht="21" spans="1:3">
       <c r="A260" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B260" s="8" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C260" s="5" t="s">
         <v>5</v>
@@ -5171,10 +5174,10 @@
     </row>
     <row r="261" ht="21" spans="1:3">
       <c r="A261" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B261" s="8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C261" s="5" t="s">
         <v>5</v>
@@ -5182,10 +5185,10 @@
     </row>
     <row r="262" ht="21" spans="1:3">
       <c r="A262" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B262" s="8" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C262" s="5" t="s">
         <v>5</v>
@@ -5193,10 +5196,10 @@
     </row>
     <row r="263" ht="21" spans="1:3">
       <c r="A263" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B263" s="8" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C263" s="5" t="s">
         <v>5</v>
@@ -5204,10 +5207,10 @@
     </row>
     <row r="264" ht="21" spans="1:3">
       <c r="A264" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B264" s="8" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C264" s="5" t="s">
         <v>5</v>
@@ -5215,10 +5218,10 @@
     </row>
     <row r="265" ht="21" spans="1:3">
       <c r="A265" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B265" s="8" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C265" s="5" t="s">
         <v>5</v>
@@ -5226,10 +5229,10 @@
     </row>
     <row r="266" ht="21" spans="1:3">
       <c r="A266" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B266" s="8" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C266" s="5" t="s">
         <v>5</v>
@@ -5237,10 +5240,10 @@
     </row>
     <row r="267" ht="21" spans="1:3">
       <c r="A267" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B267" s="8" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C267" s="5" t="s">
         <v>5</v>
@@ -5248,10 +5251,10 @@
     </row>
     <row r="268" ht="21" spans="1:3">
       <c r="A268" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B268" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C268" s="5" t="s">
         <v>5</v>
@@ -5259,10 +5262,10 @@
     </row>
     <row r="269" ht="21" spans="1:3">
       <c r="A269" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B269" s="8" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C269" s="5" t="s">
         <v>5</v>
@@ -5270,10 +5273,10 @@
     </row>
     <row r="270" ht="21" spans="1:3">
       <c r="A270" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B270" s="8" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C270" s="5" t="s">
         <v>5</v>
@@ -5281,7 +5284,7 @@
     </row>
     <row r="271" ht="21" spans="1:3">
       <c r="A271" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B271" s="8" t="s">
         <v>89</v>
@@ -5292,10 +5295,10 @@
     </row>
     <row r="272" ht="21" spans="1:3">
       <c r="A272" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B272" s="8" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C272" s="5" t="s">
         <v>5</v>
@@ -5311,10 +5314,10 @@
     </row>
     <row r="275" ht="21" spans="1:3">
       <c r="A275" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B275" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C275" s="5" t="s">
         <v>5</v>
@@ -5322,10 +5325,10 @@
     </row>
     <row r="276" ht="21" spans="1:3">
       <c r="A276" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B276" s="8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C276" s="5" t="s">
         <v>5</v>
@@ -5333,10 +5336,10 @@
     </row>
     <row r="277" ht="21" spans="1:3">
       <c r="A277" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B277" s="8" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C277" s="5" t="s">
         <v>5</v>
@@ -5344,10 +5347,10 @@
     </row>
     <row r="278" ht="21" spans="1:3">
       <c r="A278" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B278" s="8" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C278" s="5" t="s">
         <v>5</v>
@@ -5355,10 +5358,10 @@
     </row>
     <row r="279" ht="21" spans="1:3">
       <c r="A279" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B279" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C279" s="5" t="s">
         <v>5</v>
@@ -5366,10 +5369,10 @@
     </row>
     <row r="280" ht="21" spans="1:3">
       <c r="A280" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B280" s="8" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C280" s="5" t="s">
         <v>5</v>
@@ -5377,10 +5380,10 @@
     </row>
     <row r="281" ht="21" spans="1:3">
       <c r="A281" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B281" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C281" s="5" t="s">
         <v>5</v>
@@ -5388,10 +5391,10 @@
     </row>
     <row r="282" ht="21" spans="1:3">
       <c r="A282" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B282" s="8" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C282" s="5" t="s">
         <v>5</v>
@@ -5399,10 +5402,10 @@
     </row>
     <row r="283" ht="21" spans="1:3">
       <c r="A283" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B283" s="8" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C283" s="5" t="s">
         <v>5</v>
@@ -5410,10 +5413,10 @@
     </row>
     <row r="284" ht="21" spans="1:3">
       <c r="A284" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B284" s="8" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C284" s="5" t="s">
         <v>5</v>
@@ -5421,10 +5424,10 @@
     </row>
     <row r="285" ht="21" spans="1:3">
       <c r="A285" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B285" s="8" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C285" s="5" t="s">
         <v>5</v>
@@ -5432,10 +5435,10 @@
     </row>
     <row r="286" ht="21" spans="1:3">
       <c r="A286" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B286" s="8" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C286" s="5" t="s">
         <v>5</v>
@@ -5443,10 +5446,10 @@
     </row>
     <row r="287" ht="21" spans="1:3">
       <c r="A287" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B287" s="8" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C287" s="5" t="s">
         <v>5</v>
@@ -5454,10 +5457,10 @@
     </row>
     <row r="288" ht="21" spans="1:3">
       <c r="A288" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B288" s="8" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C288" s="5" t="s">
         <v>5</v>
@@ -5465,10 +5468,10 @@
     </row>
     <row r="289" ht="21" spans="1:3">
       <c r="A289" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B289" s="8" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C289" s="5" t="s">
         <v>5</v>
@@ -5476,10 +5479,10 @@
     </row>
     <row r="290" ht="21" spans="1:3">
       <c r="A290" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B290" s="8" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C290" s="5" t="s">
         <v>5</v>
@@ -5487,10 +5490,10 @@
     </row>
     <row r="291" ht="21" spans="1:3">
       <c r="A291" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B291" s="8" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C291" s="5" t="s">
         <v>5</v>
@@ -5498,10 +5501,10 @@
     </row>
     <row r="292" ht="21" spans="1:3">
       <c r="A292" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B292" s="8" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C292" s="5" t="s">
         <v>5</v>
@@ -5509,10 +5512,10 @@
     </row>
     <row r="293" ht="21" spans="1:3">
       <c r="A293" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B293" s="8" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C293" s="5" t="s">
         <v>5</v>
@@ -5528,10 +5531,10 @@
     </row>
     <row r="296" ht="21" spans="1:3">
       <c r="A296" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B296" s="8" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C296" s="5" t="s">
         <v>5</v>
@@ -5539,10 +5542,10 @@
     </row>
     <row r="297" ht="21" spans="1:3">
       <c r="A297" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B297" s="8" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C297" s="5" t="s">
         <v>5</v>
@@ -5550,10 +5553,10 @@
     </row>
     <row r="298" ht="21" spans="1:3">
       <c r="A298" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B298" s="8" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C298" s="5" t="s">
         <v>5</v>
@@ -5561,10 +5564,10 @@
     </row>
     <row r="299" ht="21" spans="1:3">
       <c r="A299" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B299" s="8" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C299" s="5" t="s">
         <v>5</v>
@@ -5572,10 +5575,10 @@
     </row>
     <row r="300" ht="21" spans="1:3">
       <c r="A300" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B300" s="8" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C300" s="5" t="s">
         <v>5</v>
@@ -5583,10 +5586,10 @@
     </row>
     <row r="301" ht="21" spans="1:3">
       <c r="A301" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B301" s="8" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C301" s="5" t="s">
         <v>5</v>
@@ -5594,10 +5597,10 @@
     </row>
     <row r="302" ht="21" spans="1:3">
       <c r="A302" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B302" s="8" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C302" s="5" t="s">
         <v>5</v>
@@ -5605,10 +5608,10 @@
     </row>
     <row r="303" ht="21" spans="1:3">
       <c r="A303" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B303" s="8" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C303" s="5" t="s">
         <v>5</v>
@@ -5616,10 +5619,10 @@
     </row>
     <row r="304" ht="21" spans="1:3">
       <c r="A304" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B304" s="8" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C304" s="5" t="s">
         <v>5</v>
@@ -5627,10 +5630,10 @@
     </row>
     <row r="305" ht="21" spans="1:3">
       <c r="A305" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B305" s="8" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C305" s="5" t="s">
         <v>5</v>
@@ -5638,10 +5641,10 @@
     </row>
     <row r="306" ht="21" spans="1:3">
       <c r="A306" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B306" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C306" s="5" t="s">
         <v>5</v>
@@ -5649,10 +5652,10 @@
     </row>
     <row r="307" ht="21" spans="1:3">
       <c r="A307" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B307" s="8" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C307" s="5" t="s">
         <v>5</v>
@@ -5660,10 +5663,10 @@
     </row>
     <row r="308" ht="21" spans="1:3">
       <c r="A308" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B308" s="8" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C308" s="5" t="s">
         <v>5</v>
@@ -5671,10 +5674,10 @@
     </row>
     <row r="309" ht="21" spans="1:3">
       <c r="A309" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B309" s="11" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C309" s="5" t="s">
         <v>5</v>
@@ -5682,10 +5685,10 @@
     </row>
     <row r="310" ht="21" spans="1:3">
       <c r="A310" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B310" s="8" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C310" s="5" t="s">
         <v>5</v>
@@ -5693,10 +5696,10 @@
     </row>
     <row r="311" ht="21" spans="1:3">
       <c r="A311" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B311" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C311" s="5" t="s">
         <v>5</v>
@@ -5704,10 +5707,10 @@
     </row>
     <row r="312" ht="21" spans="1:3">
       <c r="A312" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B312" s="8" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C312" s="5" t="s">
         <v>5</v>
@@ -5715,10 +5718,10 @@
     </row>
     <row r="313" ht="21" spans="1:3">
       <c r="A313" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B313" s="8" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C313" s="5" t="s">
         <v>5</v>
@@ -5726,10 +5729,10 @@
     </row>
     <row r="314" ht="21" spans="1:3">
       <c r="A314" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B314" s="8" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C314" s="5" t="s">
         <v>5</v>
@@ -5737,10 +5740,10 @@
     </row>
     <row r="315" ht="21" spans="1:3">
       <c r="A315" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B315" s="8" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C315" s="5" t="s">
         <v>5</v>
@@ -5748,10 +5751,10 @@
     </row>
     <row r="316" ht="21" spans="1:3">
       <c r="A316" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B316" s="8" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C316" s="5" t="s">
         <v>5</v>
@@ -5759,10 +5762,10 @@
     </row>
     <row r="317" ht="21" spans="1:3">
       <c r="A317" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B317" s="8" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C317" s="5" t="s">
         <v>5</v>
@@ -5770,10 +5773,10 @@
     </row>
     <row r="318" ht="21" spans="1:3">
       <c r="A318" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B318" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C318" s="5" t="s">
         <v>5</v>
@@ -5781,10 +5784,10 @@
     </row>
     <row r="319" ht="21" spans="1:3">
       <c r="A319" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B319" s="8" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C319" s="5" t="s">
         <v>5</v>
@@ -5792,10 +5795,10 @@
     </row>
     <row r="320" ht="21" spans="1:3">
       <c r="A320" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B320" s="8" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C320" s="5" t="s">
         <v>5</v>
@@ -5803,10 +5806,10 @@
     </row>
     <row r="321" ht="21" spans="1:3">
       <c r="A321" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B321" s="8" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C321" s="5" t="s">
         <v>5</v>
@@ -5814,10 +5817,10 @@
     </row>
     <row r="322" ht="21" spans="1:3">
       <c r="A322" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B322" s="8" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C322" s="5" t="s">
         <v>5</v>
@@ -5825,10 +5828,10 @@
     </row>
     <row r="323" ht="21" spans="1:3">
       <c r="A323" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B323" s="8" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C323" s="5" t="s">
         <v>5</v>
@@ -5836,10 +5839,10 @@
     </row>
     <row r="324" ht="21" spans="1:3">
       <c r="A324" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B324" s="8" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C324" s="5" t="s">
         <v>5</v>
@@ -5847,10 +5850,10 @@
     </row>
     <row r="325" ht="21" spans="1:3">
       <c r="A325" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B325" s="8" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C325" s="5" t="s">
         <v>5</v>
@@ -5858,10 +5861,10 @@
     </row>
     <row r="326" ht="21" spans="1:3">
       <c r="A326" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B326" s="8" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C326" s="5" t="s">
         <v>5</v>
@@ -5869,10 +5872,10 @@
     </row>
     <row r="327" ht="21" spans="1:3">
       <c r="A327" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B327" s="8" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C327" s="5" t="s">
         <v>5</v>
@@ -5880,10 +5883,10 @@
     </row>
     <row r="328" ht="21" spans="1:3">
       <c r="A328" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B328" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C328" s="5" t="s">
         <v>5</v>
@@ -5891,10 +5894,10 @@
     </row>
     <row r="329" ht="21" spans="1:3">
       <c r="A329" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B329" s="8" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C329" s="5" t="s">
         <v>5</v>
@@ -5902,10 +5905,10 @@
     </row>
     <row r="330" ht="21" spans="1:3">
       <c r="A330" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B330" s="8" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C330" s="5" t="s">
         <v>5</v>
@@ -5913,10 +5916,10 @@
     </row>
     <row r="331" ht="21" spans="1:3">
       <c r="A331" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B331" s="8" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C331" s="5" t="s">
         <v>5</v>
@@ -5924,10 +5927,10 @@
     </row>
     <row r="332" ht="21" spans="1:3">
       <c r="A332" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B332" s="8" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C332" s="5" t="s">
         <v>5</v>
@@ -5935,10 +5938,10 @@
     </row>
     <row r="333" ht="21" spans="1:3">
       <c r="A333" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B333" s="8" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C333" s="5" t="s">
         <v>5</v>
@@ -5954,10 +5957,10 @@
     </row>
     <row r="336" ht="21" spans="1:3">
       <c r="A336" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B336" s="8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C336" s="5" t="s">
         <v>5</v>
@@ -5965,10 +5968,10 @@
     </row>
     <row r="337" ht="21" spans="1:3">
       <c r="A337" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B337" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C337" s="5" t="s">
         <v>5</v>
@@ -5976,10 +5979,10 @@
     </row>
     <row r="338" ht="21" spans="1:3">
       <c r="A338" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B338" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C338" s="5" t="s">
         <v>5</v>
@@ -5987,10 +5990,10 @@
     </row>
     <row r="339" ht="21" spans="1:3">
       <c r="A339" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B339" s="8" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C339" s="5" t="s">
         <v>5</v>
@@ -5998,10 +6001,10 @@
     </row>
     <row r="340" ht="21" spans="1:3">
       <c r="A340" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B340" s="8" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C340" s="5" t="s">
         <v>5</v>
@@ -6009,10 +6012,10 @@
     </row>
     <row r="341" ht="21" spans="1:3">
       <c r="A341" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B341" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C341" s="5" t="s">
         <v>5</v>
@@ -6020,10 +6023,10 @@
     </row>
     <row r="342" ht="21" spans="1:3">
       <c r="A342" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B342" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C342" s="5" t="s">
         <v>5</v>
@@ -6031,10 +6034,10 @@
     </row>
     <row r="343" ht="21" spans="1:3">
       <c r="A343" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B343" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C343" s="5" t="s">
         <v>5</v>
@@ -6042,10 +6045,10 @@
     </row>
     <row r="344" ht="21" spans="1:3">
       <c r="A344" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B344" s="11" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C344" s="5" t="s">
         <v>5</v>
@@ -6053,10 +6056,10 @@
     </row>
     <row r="345" ht="21" spans="1:3">
       <c r="A345" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B345" s="8" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C345" s="5" t="s">
         <v>5</v>
@@ -6064,10 +6067,10 @@
     </row>
     <row r="346" ht="21" spans="1:3">
       <c r="A346" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B346" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C346" s="5" t="s">
         <v>5</v>
@@ -6075,10 +6078,10 @@
     </row>
     <row r="347" ht="21" spans="1:3">
       <c r="A347" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B347" s="8" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C347" s="5" t="s">
         <v>5</v>
@@ -6086,10 +6089,10 @@
     </row>
     <row r="348" ht="21" spans="1:3">
       <c r="A348" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B348" s="8" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C348" s="5" t="s">
         <v>5</v>
@@ -6097,10 +6100,10 @@
     </row>
     <row r="349" ht="21" spans="1:3">
       <c r="A349" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B349" s="8" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C349" s="5" t="s">
         <v>5</v>
@@ -6108,10 +6111,10 @@
     </row>
     <row r="350" ht="21" spans="1:3">
       <c r="A350" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B350" s="8" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C350" s="5" t="s">
         <v>5</v>
@@ -6119,10 +6122,10 @@
     </row>
     <row r="351" ht="21" spans="1:3">
       <c r="A351" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B351" s="8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C351" s="5" t="s">
         <v>5</v>
@@ -6130,10 +6133,10 @@
     </row>
     <row r="352" ht="21" spans="1:3">
       <c r="A352" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B352" s="8" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C352" s="5" t="s">
         <v>5</v>
@@ -6141,10 +6144,10 @@
     </row>
     <row r="353" ht="21" spans="1:3">
       <c r="A353" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B353" s="8" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C353" s="5" t="s">
         <v>5</v>
@@ -6160,10 +6163,10 @@
     </row>
     <row r="356" ht="21" spans="1:3">
       <c r="A356" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B356" s="8" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C356" s="5" t="s">
         <v>5</v>
@@ -6171,76 +6174,76 @@
     </row>
     <row r="357" ht="21" spans="1:3">
       <c r="A357" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B357" s="8" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C357" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="358" ht="21" spans="1:3">
       <c r="A358" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B358" s="8" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C358" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="359" ht="21" spans="1:3">
       <c r="A359" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B359" s="7" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C359" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="360" ht="21" spans="1:3">
       <c r="A360" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B360" s="7" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C360" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="361" ht="21" spans="1:3">
       <c r="A361" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B361" s="8" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C361" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="362" ht="21" spans="1:3">
       <c r="A362" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B362" s="8" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C362" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="363" ht="21" spans="1:3">
       <c r="A363" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B363" s="8" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C363" s="5" t="s">
         <v>5</v>
@@ -6248,10 +6251,10 @@
     </row>
     <row r="364" ht="21" spans="1:3">
       <c r="A364" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B364" s="8" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C364" s="5" t="s">
         <v>5</v>
@@ -6259,10 +6262,10 @@
     </row>
     <row r="365" ht="21" spans="1:3">
       <c r="A365" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B365" s="8" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C365" s="5" t="s">
         <v>5</v>
@@ -6270,10 +6273,10 @@
     </row>
     <row r="366" ht="21" spans="1:3">
       <c r="A366" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B366" s="8" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C366" s="5" t="s">
         <v>5</v>
@@ -6281,10 +6284,10 @@
     </row>
     <row r="367" ht="21" spans="1:3">
       <c r="A367" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B367" s="8" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C367" s="5" t="s">
         <v>5</v>
@@ -6292,10 +6295,10 @@
     </row>
     <row r="368" ht="21" spans="1:3">
       <c r="A368" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B368" s="8" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C368" s="5" t="s">
         <v>5</v>
@@ -6303,10 +6306,10 @@
     </row>
     <row r="369" ht="21" spans="1:3">
       <c r="A369" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B369" s="8" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C369" s="5" t="s">
         <v>5</v>
@@ -6314,10 +6317,10 @@
     </row>
     <row r="370" ht="21" spans="1:3">
       <c r="A370" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B370" s="8" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C370" s="5" t="s">
         <v>5</v>
@@ -6325,10 +6328,10 @@
     </row>
     <row r="371" ht="21" spans="1:3">
       <c r="A371" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B371" s="8" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C371" s="5" t="s">
         <v>5</v>
@@ -6336,10 +6339,10 @@
     </row>
     <row r="372" ht="21" spans="1:3">
       <c r="A372" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B372" s="8" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C372" s="5" t="s">
         <v>5</v>
@@ -6347,10 +6350,10 @@
     </row>
     <row r="373" ht="21" spans="1:3">
       <c r="A373" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B373" s="8" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C373" s="5" t="s">
         <v>5</v>
@@ -6358,10 +6361,10 @@
     </row>
     <row r="374" ht="21" spans="1:3">
       <c r="A374" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B374" s="8" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C374" s="5" t="s">
         <v>5</v>
@@ -6369,10 +6372,10 @@
     </row>
     <row r="375" ht="21" spans="1:3">
       <c r="A375" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B375" s="8" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C375" s="5" t="s">
         <v>5</v>
@@ -6380,10 +6383,10 @@
     </row>
     <row r="376" ht="21" spans="1:3">
       <c r="A376" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B376" s="8" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C376" s="5" t="s">
         <v>5</v>
@@ -6391,10 +6394,10 @@
     </row>
     <row r="377" ht="21" spans="1:3">
       <c r="A377" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B377" s="8" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C377" s="5" t="s">
         <v>5</v>
@@ -6402,10 +6405,10 @@
     </row>
     <row r="378" ht="21" spans="1:3">
       <c r="A378" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B378" s="8" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C378" s="5" t="s">
         <v>5</v>
@@ -6413,10 +6416,10 @@
     </row>
     <row r="379" ht="21" spans="1:3">
       <c r="A379" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B379" s="8" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C379" s="5" t="s">
         <v>5</v>
@@ -6424,10 +6427,10 @@
     </row>
     <row r="380" ht="21" spans="1:3">
       <c r="A380" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B380" s="8" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C380" s="5" t="s">
         <v>5</v>
@@ -6435,10 +6438,10 @@
     </row>
     <row r="381" ht="21" spans="1:3">
       <c r="A381" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B381" s="8" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C381" s="5" t="s">
         <v>5</v>
@@ -6446,10 +6449,10 @@
     </row>
     <row r="382" ht="21" spans="1:3">
       <c r="A382" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B382" s="8" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C382" s="5" t="s">
         <v>5</v>
@@ -6457,10 +6460,10 @@
     </row>
     <row r="383" ht="21" spans="1:3">
       <c r="A383" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B383" s="8" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C383" s="5" t="s">
         <v>5</v>
@@ -6468,10 +6471,10 @@
     </row>
     <row r="384" ht="21" spans="1:3">
       <c r="A384" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B384" s="8" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C384" s="5" t="s">
         <v>5</v>
@@ -6479,10 +6482,10 @@
     </row>
     <row r="385" ht="21" spans="1:3">
       <c r="A385" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B385" s="8" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C385" s="5" t="s">
         <v>5</v>
@@ -6490,10 +6493,10 @@
     </row>
     <row r="386" ht="21" spans="1:3">
       <c r="A386" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B386" s="8" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C386" s="5" t="s">
         <v>5</v>
@@ -6501,10 +6504,10 @@
     </row>
     <row r="387" ht="21" spans="1:3">
       <c r="A387" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B387" s="8" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C387" s="5" t="s">
         <v>5</v>
@@ -6512,10 +6515,10 @@
     </row>
     <row r="388" ht="21" spans="1:3">
       <c r="A388" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B388" s="8" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C388" s="5" t="s">
         <v>5</v>
@@ -6523,10 +6526,10 @@
     </row>
     <row r="389" ht="21" spans="1:3">
       <c r="A389" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B389" s="8" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C389" s="5" t="s">
         <v>5</v>
@@ -6534,10 +6537,10 @@
     </row>
     <row r="390" ht="21" spans="1:3">
       <c r="A390" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B390" s="8" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C390" s="5" t="s">
         <v>5</v>
@@ -6545,10 +6548,10 @@
     </row>
     <row r="391" ht="21" spans="1:3">
       <c r="A391" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B391" s="8" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C391" s="5" t="s">
         <v>5</v>
@@ -6556,10 +6559,10 @@
     </row>
     <row r="392" ht="21" spans="1:3">
       <c r="A392" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B392" s="8" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C392" s="5" t="s">
         <v>5</v>
@@ -6567,10 +6570,10 @@
     </row>
     <row r="393" ht="21" spans="1:3">
       <c r="A393" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B393" s="8" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C393" s="5" t="s">
         <v>5</v>
@@ -6578,10 +6581,10 @@
     </row>
     <row r="394" ht="21" spans="1:3">
       <c r="A394" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B394" s="8" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C394" s="5" t="s">
         <v>5</v>
@@ -6589,10 +6592,10 @@
     </row>
     <row r="395" ht="21" spans="1:3">
       <c r="A395" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B395" s="8" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C395" s="5" t="s">
         <v>5</v>
@@ -6600,10 +6603,10 @@
     </row>
     <row r="396" ht="21" spans="1:3">
       <c r="A396" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B396" s="8" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C396" s="5" t="s">
         <v>5</v>
@@ -6611,10 +6614,10 @@
     </row>
     <row r="397" ht="21" spans="1:3">
       <c r="A397" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B397" s="8" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C397" s="5" t="s">
         <v>5</v>
@@ -6622,10 +6625,10 @@
     </row>
     <row r="398" ht="21" spans="1:3">
       <c r="A398" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B398" s="8" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C398" s="5" t="s">
         <v>5</v>
@@ -6633,10 +6636,10 @@
     </row>
     <row r="399" ht="21" spans="1:3">
       <c r="A399" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B399" s="8" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C399" s="5" t="s">
         <v>5</v>
@@ -6652,10 +6655,10 @@
     </row>
     <row r="402" ht="21" spans="1:3">
       <c r="A402" s="10" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B402" s="8" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C402" s="5" t="s">
         <v>5</v>
@@ -6663,10 +6666,10 @@
     </row>
     <row r="403" ht="21" spans="1:3">
       <c r="A403" s="10" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B403" s="8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C403" s="5" t="s">
         <v>5</v>
@@ -6674,10 +6677,10 @@
     </row>
     <row r="404" ht="21" spans="1:3">
       <c r="A404" s="10" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B404" s="8" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C404" s="5" t="s">
         <v>5</v>
@@ -6685,7 +6688,7 @@
     </row>
     <row r="405" ht="21" spans="1:3">
       <c r="A405" s="10" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B405" s="8" t="s">
         <v>91</v>
@@ -6696,10 +6699,10 @@
     </row>
     <row r="406" ht="21" spans="1:3">
       <c r="A406" s="10" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B406" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C406" s="5" t="s">
         <v>5</v>
@@ -6707,10 +6710,10 @@
     </row>
     <row r="407" ht="21" spans="1:3">
       <c r="A407" s="10" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B407" s="8" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C407" s="5" t="s">
         <v>5</v>
@@ -6726,10 +6729,10 @@
     </row>
     <row r="410" ht="21" spans="1:3">
       <c r="A410" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B410" s="8" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C410" s="5" t="s">
         <v>8</v>
@@ -6737,10 +6740,10 @@
     </row>
     <row r="411" ht="21" spans="1:3">
       <c r="A411" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B411" s="8" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C411" s="5" t="s">
         <v>10</v>
@@ -6748,10 +6751,10 @@
     </row>
     <row r="412" ht="21" spans="1:3">
       <c r="A412" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B412" s="8" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C412" s="5" t="s">
         <v>10</v>
@@ -6759,10 +6762,10 @@
     </row>
     <row r="413" ht="21" spans="1:3">
       <c r="A413" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B413" s="8" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C413" s="5" t="s">
         <v>10</v>
@@ -6770,10 +6773,10 @@
     </row>
     <row r="414" ht="21" spans="1:3">
       <c r="A414" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B414" s="8" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C414" s="5" t="s">
         <v>10</v>
@@ -6781,10 +6784,10 @@
     </row>
     <row r="415" ht="21" spans="1:3">
       <c r="A415" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B415" s="8" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C415" s="5" t="s">
         <v>10</v>
@@ -6792,10 +6795,10 @@
     </row>
     <row r="416" ht="21" spans="1:3">
       <c r="A416" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B416" s="8" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C416" s="5" t="s">
         <v>10</v>
@@ -6803,10 +6806,10 @@
     </row>
     <row r="417" ht="21" spans="1:3">
       <c r="A417" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B417" s="8" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C417" s="5" t="s">
         <v>5</v>
@@ -6814,10 +6817,10 @@
     </row>
     <row r="418" ht="21" spans="1:3">
       <c r="A418" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B418" s="8" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C418" s="5" t="s">
         <v>5</v>
@@ -6825,10 +6828,10 @@
     </row>
     <row r="419" ht="21" spans="1:3">
       <c r="A419" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B419" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C419" s="5" t="s">
         <v>5</v>
@@ -6836,10 +6839,10 @@
     </row>
     <row r="420" ht="21" spans="1:3">
       <c r="A420" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B420" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C420" s="5" t="s">
         <v>5</v>
@@ -6847,10 +6850,10 @@
     </row>
     <row r="421" ht="21" spans="1:3">
       <c r="A421" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B421" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C421" s="5" t="s">
         <v>5</v>
@@ -6858,10 +6861,10 @@
     </row>
     <row r="422" ht="21" spans="1:3">
       <c r="A422" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B422" s="8" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C422" s="5" t="s">
         <v>5</v>
@@ -6869,10 +6872,10 @@
     </row>
     <row r="423" ht="21" spans="1:3">
       <c r="A423" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B423" s="8" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C423" s="5" t="s">
         <v>5</v>
@@ -6880,10 +6883,10 @@
     </row>
     <row r="424" ht="21" spans="1:3">
       <c r="A424" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B424" s="8" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C424" s="5" t="s">
         <v>5</v>
@@ -6891,10 +6894,10 @@
     </row>
     <row r="425" ht="21" spans="1:3">
       <c r="A425" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B425" s="8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C425" s="5" t="s">
         <v>5</v>
@@ -6902,10 +6905,10 @@
     </row>
     <row r="426" ht="21" spans="1:3">
       <c r="A426" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B426" s="8" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C426" s="5" t="s">
         <v>5</v>
@@ -6913,10 +6916,10 @@
     </row>
     <row r="427" ht="21" spans="1:3">
       <c r="A427" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B427" s="8" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C427" s="5" t="s">
         <v>5</v>
@@ -6924,10 +6927,10 @@
     </row>
     <row r="428" ht="21" spans="1:3">
       <c r="A428" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B428" s="8" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C428" s="5" t="s">
         <v>5</v>
@@ -6935,10 +6938,10 @@
     </row>
     <row r="429" ht="21" spans="1:3">
       <c r="A429" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B429" s="8" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C429" s="5" t="s">
         <v>5</v>
@@ -6946,10 +6949,10 @@
     </row>
     <row r="430" ht="21" spans="1:3">
       <c r="A430" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B430" s="8" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C430" s="5" t="s">
         <v>5</v>
@@ -6957,10 +6960,10 @@
     </row>
     <row r="431" ht="21" spans="1:3">
       <c r="A431" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B431" s="8" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C431" s="5" t="s">
         <v>5</v>
@@ -6968,10 +6971,10 @@
     </row>
     <row r="432" ht="21" spans="1:3">
       <c r="A432" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B432" s="8" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C432" s="5" t="s">
         <v>5</v>
@@ -6979,10 +6982,10 @@
     </row>
     <row r="433" ht="21" spans="1:3">
       <c r="A433" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B433" s="8" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C433" s="5" t="s">
         <v>5</v>
@@ -6990,10 +6993,10 @@
     </row>
     <row r="434" ht="21" spans="1:3">
       <c r="A434" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B434" s="8" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C434" s="5" t="s">
         <v>5</v>
@@ -7001,10 +7004,10 @@
     </row>
     <row r="435" ht="21" spans="1:3">
       <c r="A435" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B435" s="8" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C435" s="5" t="s">
         <v>5</v>
@@ -7012,10 +7015,10 @@
     </row>
     <row r="436" ht="21" spans="1:3">
       <c r="A436" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B436" s="8" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C436" s="5" t="s">
         <v>5</v>
@@ -7023,10 +7026,10 @@
     </row>
     <row r="437" ht="21" spans="1:3">
       <c r="A437" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B437" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C437" s="5" t="s">
         <v>5</v>
@@ -7034,10 +7037,10 @@
     </row>
     <row r="438" ht="21" spans="1:3">
       <c r="A438" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B438" s="8" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C438" s="5" t="s">
         <v>5</v>
@@ -7045,10 +7048,10 @@
     </row>
     <row r="439" ht="21" spans="1:3">
       <c r="A439" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B439" s="8" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C439" s="5" t="s">
         <v>5</v>
@@ -7056,10 +7059,10 @@
     </row>
     <row r="440" ht="21" spans="1:3">
       <c r="A440" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B440" s="8" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C440" s="5" t="s">
         <v>5</v>
@@ -7067,10 +7070,10 @@
     </row>
     <row r="441" ht="21" spans="1:3">
       <c r="A441" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B441" s="8" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C441" s="5" t="s">
         <v>5</v>
@@ -7078,10 +7081,10 @@
     </row>
     <row r="442" ht="21" spans="1:3">
       <c r="A442" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B442" s="8" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C442" s="5" t="s">
         <v>5</v>
@@ -7089,10 +7092,10 @@
     </row>
     <row r="443" ht="21" spans="1:3">
       <c r="A443" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B443" s="8" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C443" s="5" t="s">
         <v>5</v>
@@ -7100,10 +7103,10 @@
     </row>
     <row r="444" ht="21" spans="1:3">
       <c r="A444" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B444" s="8" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C444" s="5" t="s">
         <v>5</v>
@@ -7111,10 +7114,10 @@
     </row>
     <row r="445" ht="21" spans="1:3">
       <c r="A445" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B445" s="8" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C445" s="5" t="s">
         <v>5</v>
@@ -7122,10 +7125,10 @@
     </row>
     <row r="446" ht="21" spans="1:3">
       <c r="A446" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B446" s="8" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C446" s="5" t="s">
         <v>5</v>
@@ -7133,10 +7136,10 @@
     </row>
     <row r="447" ht="21" spans="1:3">
       <c r="A447" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B447" s="8" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C447" s="5" t="s">
         <v>5</v>
@@ -7144,10 +7147,10 @@
     </row>
     <row r="448" ht="21" spans="1:3">
       <c r="A448" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B448" s="8" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C448" s="5" t="s">
         <v>5</v>
@@ -7155,10 +7158,10 @@
     </row>
     <row r="449" ht="21" spans="1:3">
       <c r="A449" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B449" s="8" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C449" s="5" t="s">
         <v>5</v>
@@ -7166,10 +7169,10 @@
     </row>
     <row r="450" ht="21" spans="1:3">
       <c r="A450" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B450" s="8" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C450" s="5" t="s">
         <v>5</v>
@@ -7177,10 +7180,10 @@
     </row>
     <row r="451" ht="21" spans="1:3">
       <c r="A451" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B451" s="8" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C451" s="5" t="s">
         <v>5</v>
@@ -7188,10 +7191,10 @@
     </row>
     <row r="452" ht="21" spans="1:3">
       <c r="A452" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B452" s="8" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C452" s="5" t="s">
         <v>5</v>
@@ -7199,10 +7202,10 @@
     </row>
     <row r="453" ht="21" spans="1:3">
       <c r="A453" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B453" s="8" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C453" s="5" t="s">
         <v>5</v>
@@ -7210,10 +7213,10 @@
     </row>
     <row r="454" ht="21" spans="1:3">
       <c r="A454" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B454" s="8" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C454" s="5" t="s">
         <v>5</v>
@@ -7221,10 +7224,10 @@
     </row>
     <row r="455" ht="21" spans="1:3">
       <c r="A455" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B455" s="8" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C455" s="5" t="s">
         <v>5</v>
@@ -7232,10 +7235,10 @@
     </row>
     <row r="456" ht="21" spans="1:3">
       <c r="A456" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B456" s="8" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C456" s="5" t="s">
         <v>5</v>
@@ -7243,10 +7246,10 @@
     </row>
     <row r="457" ht="21" spans="1:3">
       <c r="A457" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B457" s="8" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C457" s="5" t="s">
         <v>5</v>
@@ -7254,10 +7257,10 @@
     </row>
     <row r="458" ht="21" spans="1:3">
       <c r="A458" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B458" s="8" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C458" s="5" t="s">
         <v>5</v>
@@ -7265,10 +7268,10 @@
     </row>
     <row r="459" ht="21" spans="1:3">
       <c r="A459" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B459" s="8" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C459" s="5" t="s">
         <v>5</v>
@@ -7276,10 +7279,10 @@
     </row>
     <row r="460" ht="21" spans="1:3">
       <c r="A460" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B460" s="8" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C460" s="5" t="s">
         <v>5</v>
@@ -7287,10 +7290,10 @@
     </row>
     <row r="461" ht="21" spans="1:3">
       <c r="A461" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B461" s="8" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C461" s="5" t="s">
         <v>5</v>
@@ -7298,10 +7301,10 @@
     </row>
     <row r="462" ht="21" spans="1:3">
       <c r="A462" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B462" s="8" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C462" s="5" t="s">
         <v>5</v>
@@ -7309,10 +7312,10 @@
     </row>
     <row r="463" ht="21" spans="1:3">
       <c r="A463" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B463" s="8" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C463" s="5" t="s">
         <v>5</v>
@@ -7320,10 +7323,10 @@
     </row>
     <row r="464" ht="21" spans="1:3">
       <c r="A464" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B464" s="8" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C464" s="5" t="s">
         <v>5</v>
@@ -7331,10 +7334,10 @@
     </row>
     <row r="465" ht="21" spans="1:3">
       <c r="A465" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B465" s="8" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C465" s="5" t="s">
         <v>5</v>
@@ -7342,10 +7345,10 @@
     </row>
     <row r="466" ht="21" spans="1:3">
       <c r="A466" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B466" s="8" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C466" s="5" t="s">
         <v>5</v>
@@ -7353,10 +7356,10 @@
     </row>
     <row r="467" ht="21" spans="1:3">
       <c r="A467" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B467" s="8" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C467" s="5" t="s">
         <v>5</v>
@@ -7364,10 +7367,10 @@
     </row>
     <row r="468" ht="21" spans="1:3">
       <c r="A468" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B468" s="8" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C468" s="5" t="s">
         <v>5</v>
@@ -7375,10 +7378,10 @@
     </row>
     <row r="469" ht="21" spans="1:3">
       <c r="A469" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B469" s="8" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C469" s="5" t="s">
         <v>5</v>
@@ -7395,10 +7398,10 @@
     </row>
     <row r="472" ht="21" spans="1:3">
       <c r="A472" s="6" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B472" s="8" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C472" s="5" t="s">
         <v>5</v>
@@ -7406,10 +7409,10 @@
     </row>
     <row r="473" ht="21" spans="1:3">
       <c r="A473" s="6" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B473" s="8" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C473" s="5" t="s">
         <v>5</v>
@@ -7417,10 +7420,10 @@
     </row>
     <row r="474" ht="21" spans="1:3">
       <c r="A474" s="6" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B474" s="8" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C474" s="5" t="s">
         <v>5</v>
@@ -7428,10 +7431,10 @@
     </row>
     <row r="475" ht="21" spans="1:3">
       <c r="A475" s="6" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B475" s="8" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C475" s="5" t="s">
         <v>5</v>
@@ -7439,10 +7442,10 @@
     </row>
     <row r="476" ht="21" spans="1:3">
       <c r="A476" s="6" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B476" s="8" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C476" s="5" t="s">
         <v>5</v>
@@ -7450,10 +7453,10 @@
     </row>
     <row r="477" ht="21" spans="1:3">
       <c r="A477" s="6" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B477" s="8" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C477" s="5" t="s">
         <v>5</v>
@@ -7461,10 +7464,10 @@
     </row>
     <row r="478" ht="21" spans="1:3">
       <c r="A478" s="6" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B478" s="8" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C478" s="5" t="s">
         <v>5</v>
@@ -7472,10 +7475,10 @@
     </row>
     <row r="479" ht="21" spans="1:3">
       <c r="A479" s="6" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B479" s="8" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C479" s="5" t="s">
         <v>5</v>
@@ -7483,10 +7486,10 @@
     </row>
     <row r="480" ht="21" spans="1:3">
       <c r="A480" s="6" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B480" s="8" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C480" s="5" t="s">
         <v>5</v>
@@ -7494,10 +7497,10 @@
     </row>
     <row r="481" ht="21" spans="1:3">
       <c r="A481" s="6" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B481" s="8" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C481" s="5" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Binary tree to sum tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1425,9 +1425,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
@@ -1505,28 +1505,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1538,9 +1517,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1548,7 +1548,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1602,7 +1617,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1617,21 +1632,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1639,7 +1639,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1651,48 +1651,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1708,25 +1666,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1738,43 +1702,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1792,19 +1732,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1822,19 +1834,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1878,6 +1878,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1911,21 +1926,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1948,146 +1948,146 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2438,7 +2438,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="C195" sqref="C195"/>
+      <selection activeCell="C194" sqref="C194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -4480,7 +4480,7 @@
         <v>193</v>
       </c>
       <c r="C195" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="196" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Construct Bt from preorder,inorder using map
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1425,10 +1425,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1502,6 +1502,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1509,24 +1517,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1539,23 +1531,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1570,22 +1555,31 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1601,23 +1595,30 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1630,16 +1631,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1654,7 +1654,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1666,13 +1726,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1684,115 +1810,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1804,37 +1828,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1848,17 +1848,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1873,21 +1878,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1917,11 +1907,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1934,160 +1945,149 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2438,7 +2438,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="C194" sqref="C194"/>
+      <selection activeCell="C197" sqref="C197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -4491,7 +4491,7 @@
         <v>194</v>
       </c>
       <c r="C196" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="197" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Minimize maximum difference between two heights
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1426,9 +1426,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1502,29 +1502,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1540,7 +1517,46 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1555,14 +1571,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -1570,9 +1578,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1587,37 +1602,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1639,7 +1631,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1660,7 +1660,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1672,19 +1684,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1696,7 +1696,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1708,37 +1750,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1756,13 +1774,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1774,19 +1792,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1798,43 +1834,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1845,21 +1845,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1874,24 +1859,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1911,12 +1878,25 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1940,154 +1920,174 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2441,7 +2441,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2573,7 +2573,7 @@
         <v>16</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Finding duplicate number in an array in O(n)
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1425,10 +1425,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1503,31 +1503,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1538,9 +1516,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1556,7 +1540,29 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1570,11 +1576,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1586,8 +1592,24 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1602,27 +1624,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1631,15 +1639,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1660,7 +1660,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1672,115 +1810,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1792,37 +1822,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1834,7 +1834,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1863,21 +1863,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1896,7 +1881,27 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1917,6 +1922,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1925,169 +1945,149 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2440,8 +2440,8 @@
   <sheetPr/>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2589,18 +2589,18 @@
       <c r="A16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>17</v>
+      <c r="C16" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17" ht="21" spans="1:3">
       <c r="A17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="8" t="s">

</xml_diff>

<commit_message>
Merge Intervals mistake solved
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -79,13 +79,13 @@
     <t>Kadane's Algo [V.V.V.V.V IMP]</t>
   </si>
   <si>
+    <t>Merge Intervals</t>
+  </si>
+  <si>
+    <t>Next Permutation</t>
+  </si>
+  <si>
     <t>&lt;-&gt;</t>
-  </si>
-  <si>
-    <t>Merge Intervals</t>
-  </si>
-  <si>
-    <t>Next Permutation</t>
   </si>
   <si>
     <t>Count Inversion</t>
@@ -1425,10 +1425,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1502,9 +1502,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1524,54 +1531,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1586,7 +1548,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1597,6 +1567,13 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1616,8 +1593,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1630,8 +1622,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1640,6 +1633,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1660,7 +1660,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1672,19 +1672,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1696,25 +1684,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1726,19 +1714,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1750,31 +1726,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1792,13 +1762,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1810,19 +1798,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1834,7 +1828,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1845,45 +1845,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1907,6 +1868,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1937,6 +1913,30 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1948,146 +1948,146 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2441,7 +2441,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2616,8 +2616,8 @@
       <c r="B18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>21</v>
+      <c r="C18" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="19" ht="21" spans="1:3">
@@ -2625,10 +2625,10 @@
         <v>6</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="9" t="s">
         <v>21</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="20" ht="21" spans="1:3">
@@ -2636,10 +2636,10 @@
         <v>6</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" ht="21" spans="1:3">
@@ -2650,7 +2650,7 @@
         <v>24</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" ht="21" spans="1:3">
@@ -2661,7 +2661,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" ht="21" spans="1:3">
@@ -2672,7 +2672,7 @@
         <v>26</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" ht="21" spans="1:3">
@@ -2683,7 +2683,7 @@
         <v>27</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" ht="21" spans="1:3">
@@ -2694,7 +2694,7 @@
         <v>28</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" ht="21" spans="1:3">
@@ -2705,7 +2705,7 @@
         <v>29</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" ht="21" spans="1:3">
@@ -2716,7 +2716,7 @@
         <v>30</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" ht="21" spans="1:3">
@@ -2727,7 +2727,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" ht="21" spans="1:3">
@@ -2738,7 +2738,7 @@
         <v>32</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" ht="21" spans="1:3">
@@ -2749,7 +2749,7 @@
         <v>33</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" ht="21" spans="1:3">
@@ -2760,7 +2760,7 @@
         <v>34</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" ht="21" spans="1:3">
@@ -2771,7 +2771,7 @@
         <v>35</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" ht="21" spans="1:3">
@@ -2782,7 +2782,7 @@
         <v>36</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" ht="21" spans="1:3">
@@ -2793,7 +2793,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" ht="21" spans="1:3">
@@ -2804,7 +2804,7 @@
         <v>38</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" ht="21" spans="1:3">
@@ -2815,7 +2815,7 @@
         <v>39</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" ht="21" spans="1:3">
@@ -2826,7 +2826,7 @@
         <v>40</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" ht="21" spans="1:3">
@@ -2837,7 +2837,7 @@
         <v>41</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" ht="21" spans="1:3">
@@ -2848,7 +2848,7 @@
         <v>42</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" ht="21" spans="1:3">
@@ -2859,7 +2859,7 @@
         <v>43</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" ht="21" spans="1:3">
@@ -2870,20 +2870,20 @@
         <v>44</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" ht="21" spans="2:3">
       <c r="B42" s="10"/>
       <c r="C42" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" ht="21" spans="1:3">
       <c r="A43" s="6"/>
       <c r="B43" s="10"/>
       <c r="C43" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" ht="21" spans="1:3">
@@ -2894,7 +2894,7 @@
         <v>46</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" ht="21" spans="1:3">
@@ -2905,7 +2905,7 @@
         <v>47</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" ht="21" spans="1:3">
@@ -2916,7 +2916,7 @@
         <v>48</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" ht="21" spans="1:3">
@@ -2927,7 +2927,7 @@
         <v>49</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" ht="21" spans="1:3">
@@ -2938,7 +2938,7 @@
         <v>50</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" ht="21" spans="1:3">
@@ -2949,7 +2949,7 @@
         <v>51</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" ht="21" spans="1:3">
@@ -2960,7 +2960,7 @@
         <v>52</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" ht="21" spans="1:3">
@@ -2971,7 +2971,7 @@
         <v>53</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" ht="21" spans="1:3">
@@ -2982,7 +2982,7 @@
         <v>54</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53" ht="21" spans="1:3">
@@ -2993,7 +2993,7 @@
         <v>55</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" ht="21" spans="1:3">
@@ -3009,7 +3009,7 @@
         <v>57</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" ht="21" spans="1:3">
@@ -3020,7 +3020,7 @@
         <v>58</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58" ht="21" spans="1:3">
@@ -3031,7 +3031,7 @@
         <v>59</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59" ht="21" spans="1:3">
@@ -3042,7 +3042,7 @@
         <v>60</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60" ht="21" spans="1:3">
@@ -3053,7 +3053,7 @@
         <v>61</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61" ht="21" spans="1:3">
@@ -3064,7 +3064,7 @@
         <v>62</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62" ht="21" spans="1:3">
@@ -3075,7 +3075,7 @@
         <v>63</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63" ht="21" spans="1:3">
@@ -3086,7 +3086,7 @@
         <v>64</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" ht="21" spans="1:3">
@@ -3097,7 +3097,7 @@
         <v>65</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65" ht="21" spans="1:3">
@@ -3108,7 +3108,7 @@
         <v>66</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="66" ht="21" spans="1:3">
@@ -3119,7 +3119,7 @@
         <v>67</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67" ht="21" spans="1:3">
@@ -3130,7 +3130,7 @@
         <v>68</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" ht="21" spans="1:3">
@@ -3141,7 +3141,7 @@
         <v>69</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="69" ht="21" spans="1:3">
@@ -3152,7 +3152,7 @@
         <v>70</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="70" ht="21" spans="1:3">
@@ -3163,7 +3163,7 @@
         <v>71</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71" ht="21" spans="1:3">
@@ -3174,7 +3174,7 @@
         <v>72</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="72" ht="21" spans="1:3">
@@ -3185,7 +3185,7 @@
         <v>73</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="73" ht="21" spans="1:3">
@@ -3196,7 +3196,7 @@
         <v>74</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="74" ht="21" spans="1:3">
@@ -3207,7 +3207,7 @@
         <v>75</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="75" ht="21" spans="1:3">
@@ -3218,7 +3218,7 @@
         <v>76</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="76" ht="21" spans="1:3">
@@ -3229,7 +3229,7 @@
         <v>77</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="77" ht="21" spans="1:3">
@@ -3240,7 +3240,7 @@
         <v>78</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="78" ht="21" spans="1:3">
@@ -3251,7 +3251,7 @@
         <v>79</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="79" ht="21" spans="1:3">
@@ -3262,7 +3262,7 @@
         <v>80</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="80" ht="21" spans="1:3">
@@ -3273,7 +3273,7 @@
         <v>81</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="81" ht="21" spans="1:3">
@@ -3284,7 +3284,7 @@
         <v>82</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="82" ht="21" spans="1:3">
@@ -3295,7 +3295,7 @@
         <v>83</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="83" ht="21" spans="1:3">
@@ -3306,7 +3306,7 @@
         <v>84</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="84" ht="21" spans="1:3">
@@ -3317,7 +3317,7 @@
         <v>85</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="85" ht="21" spans="1:3">
@@ -3328,7 +3328,7 @@
         <v>86</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="86" ht="21" spans="1:3">
@@ -3339,7 +3339,7 @@
         <v>87</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="87" ht="21" spans="1:3">
@@ -3350,7 +3350,7 @@
         <v>88</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="88" ht="21" spans="1:3">
@@ -3361,7 +3361,7 @@
         <v>89</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="89" ht="21" spans="1:3">
@@ -3372,7 +3372,7 @@
         <v>90</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="90" ht="21" spans="1:3">
@@ -3383,7 +3383,7 @@
         <v>91</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="91" ht="21" spans="1:3">
@@ -3394,7 +3394,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="92" ht="21" spans="1:3">
@@ -3405,7 +3405,7 @@
         <v>93</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="93" ht="21" spans="1:3">
@@ -3416,7 +3416,7 @@
         <v>94</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="94" ht="21" spans="1:3">
@@ -3427,7 +3427,7 @@
         <v>95</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="95" ht="21" spans="1:3">
@@ -3438,7 +3438,7 @@
         <v>96</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="96" ht="21" spans="1:3">
@@ -3449,7 +3449,7 @@
         <v>97</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="97" ht="21" spans="1:3">
@@ -3460,7 +3460,7 @@
         <v>98</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="98" ht="21" spans="1:3">
@@ -3471,7 +3471,7 @@
         <v>99</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="100" ht="21" spans="1:3">
@@ -3487,7 +3487,7 @@
         <v>101</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="102" ht="21" spans="1:3">
@@ -3498,7 +3498,7 @@
         <v>102</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="103" ht="21" spans="1:3">
@@ -3509,7 +3509,7 @@
         <v>103</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="104" ht="21" spans="1:3">
@@ -3520,7 +3520,7 @@
         <v>104</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="105" ht="21" spans="1:3">
@@ -3531,7 +3531,7 @@
         <v>105</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="106" ht="21" spans="1:3">
@@ -3542,7 +3542,7 @@
         <v>106</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="107" ht="21" spans="1:3">
@@ -3553,7 +3553,7 @@
         <v>107</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="108" ht="21" spans="1:3">
@@ -3564,7 +3564,7 @@
         <v>108</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="109" ht="21" spans="1:3">
@@ -3575,7 +3575,7 @@
         <v>109</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="110" ht="21" spans="1:3">
@@ -3586,7 +3586,7 @@
         <v>110</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="111" ht="21" spans="1:3">
@@ -3597,7 +3597,7 @@
         <v>111</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="112" ht="21" spans="1:3">
@@ -3608,7 +3608,7 @@
         <v>112</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="113" ht="21" spans="1:3">
@@ -3619,7 +3619,7 @@
         <v>113</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="114" ht="21" spans="1:3">
@@ -3630,7 +3630,7 @@
         <v>114</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="115" ht="21" spans="1:3">
@@ -3641,7 +3641,7 @@
         <v>115</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="116" ht="21" spans="1:3">
@@ -3652,7 +3652,7 @@
         <v>116</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="117" ht="21" spans="1:3">
@@ -3663,7 +3663,7 @@
         <v>117</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="118" ht="21" spans="1:3">
@@ -3674,7 +3674,7 @@
         <v>118</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="119" ht="21" spans="1:3">
@@ -3685,7 +3685,7 @@
         <v>119</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="120" ht="21" spans="1:3">
@@ -3696,7 +3696,7 @@
         <v>120</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="121" ht="21" spans="1:3">
@@ -3707,7 +3707,7 @@
         <v>121</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="122" ht="21" spans="1:3">
@@ -3718,7 +3718,7 @@
         <v>122</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="123" ht="21" spans="1:3">
@@ -3729,7 +3729,7 @@
         <v>123</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="124" ht="21" spans="1:3">
@@ -3740,7 +3740,7 @@
         <v>124</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="125" ht="21" spans="1:3">
@@ -3751,7 +3751,7 @@
         <v>125</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="126" ht="21" spans="1:3">
@@ -3762,7 +3762,7 @@
         <v>126</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="127" ht="21" spans="1:3">
@@ -3773,7 +3773,7 @@
         <v>127</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="128" ht="21" spans="1:3">
@@ -3784,7 +3784,7 @@
         <v>128</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="129" ht="21" spans="1:3">
@@ -3795,7 +3795,7 @@
         <v>129</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="130" ht="21" spans="1:3">
@@ -3806,7 +3806,7 @@
         <v>130</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="131" ht="21" spans="1:3">
@@ -3817,7 +3817,7 @@
         <v>131</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="132" ht="21" spans="1:3">
@@ -3828,7 +3828,7 @@
         <v>132</v>
       </c>
       <c r="C132" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="133" ht="21" spans="1:3">
@@ -3839,7 +3839,7 @@
         <v>133</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="134" ht="21" spans="1:3">
@@ -3850,7 +3850,7 @@
         <v>134</v>
       </c>
       <c r="C134" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="135" ht="21" spans="1:3">
@@ -3861,7 +3861,7 @@
         <v>135</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="136" ht="21" spans="1:3">
@@ -3872,7 +3872,7 @@
         <v>136</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="138" ht="21" spans="2:3">
@@ -3887,7 +3887,7 @@
         <v>138</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="140" ht="21" spans="1:3">
@@ -3898,7 +3898,7 @@
         <v>139</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="141" ht="21" spans="1:3">
@@ -3909,7 +3909,7 @@
         <v>140</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="142" ht="21" spans="1:3">
@@ -3920,7 +3920,7 @@
         <v>141</v>
       </c>
       <c r="C142" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="143" ht="21" spans="1:3">
@@ -3931,7 +3931,7 @@
         <v>142</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="144" ht="21" spans="1:3">
@@ -3942,7 +3942,7 @@
         <v>143</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="145" ht="21" spans="1:3">
@@ -3953,7 +3953,7 @@
         <v>144</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="146" ht="21" spans="1:3">
@@ -3964,7 +3964,7 @@
         <v>145</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="147" ht="21" spans="1:3">
@@ -3975,7 +3975,7 @@
         <v>146</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="148" ht="21" spans="1:3">
@@ -3986,7 +3986,7 @@
         <v>147</v>
       </c>
       <c r="C148" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="149" ht="21" spans="1:3">
@@ -3997,7 +3997,7 @@
         <v>148</v>
       </c>
       <c r="C149" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="150" ht="21" spans="1:3">
@@ -4008,7 +4008,7 @@
         <v>149</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="151" ht="21" spans="1:3">
@@ -4019,7 +4019,7 @@
         <v>150</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="152" ht="21" spans="1:3">
@@ -4030,7 +4030,7 @@
         <v>151</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="153" ht="21" spans="1:3">
@@ -4041,7 +4041,7 @@
         <v>152</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="154" ht="21" spans="1:3">
@@ -4052,7 +4052,7 @@
         <v>153</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="155" ht="21" spans="1:3">
@@ -4063,7 +4063,7 @@
         <v>154</v>
       </c>
       <c r="C155" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="156" ht="21" spans="1:3">
@@ -4074,7 +4074,7 @@
         <v>155</v>
       </c>
       <c r="C156" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="157" ht="21" spans="1:3">
@@ -4085,7 +4085,7 @@
         <v>156</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="158" ht="21" spans="1:3">
@@ -4096,7 +4096,7 @@
         <v>157</v>
       </c>
       <c r="C158" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="159" ht="21" spans="1:3">
@@ -4107,7 +4107,7 @@
         <v>158</v>
       </c>
       <c r="C159" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="160" ht="21" spans="1:3">
@@ -4118,7 +4118,7 @@
         <v>159</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="161" ht="21" spans="1:3">
@@ -4129,7 +4129,7 @@
         <v>160</v>
       </c>
       <c r="C161" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="162" ht="21" spans="1:3">
@@ -4140,7 +4140,7 @@
         <v>161</v>
       </c>
       <c r="C162" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="163" ht="21" spans="1:3">
@@ -4151,7 +4151,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="164" ht="21" spans="1:3">
@@ -4162,7 +4162,7 @@
         <v>163</v>
       </c>
       <c r="C164" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="165" ht="21" spans="1:3">
@@ -4173,7 +4173,7 @@
         <v>164</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="166" ht="21" spans="1:3">
@@ -4184,7 +4184,7 @@
         <v>165</v>
       </c>
       <c r="C166" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="167" ht="21" spans="1:3">
@@ -4195,7 +4195,7 @@
         <v>166</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="168" ht="21" spans="1:3">
@@ -4206,7 +4206,7 @@
         <v>167</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="169" ht="21" spans="1:3">
@@ -4217,7 +4217,7 @@
         <v>168</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="170" ht="21" spans="1:3">
@@ -4228,7 +4228,7 @@
         <v>169</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="171" ht="21" spans="1:3">
@@ -4239,7 +4239,7 @@
         <v>170</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="172" ht="21" spans="1:3">
@@ -4250,7 +4250,7 @@
         <v>171</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="173" ht="21" spans="1:3">
@@ -4261,7 +4261,7 @@
         <v>172</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="174" ht="21" spans="1:3">
@@ -4272,7 +4272,7 @@
         <v>173</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="176" ht="21" spans="2:3">
@@ -4463,7 +4463,7 @@
         <v>191</v>
       </c>
       <c r="C193" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="194" ht="21" spans="1:3">
@@ -4507,7 +4507,7 @@
         <v>196</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="198" ht="21" spans="1:3">
@@ -4518,7 +4518,7 @@
         <v>197</v>
       </c>
       <c r="C198" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="199" ht="21" spans="1:3">
@@ -4529,7 +4529,7 @@
         <v>198</v>
       </c>
       <c r="C199" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="200" ht="21" spans="1:3">
@@ -4540,7 +4540,7 @@
         <v>199</v>
       </c>
       <c r="C200" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="201" ht="21" spans="1:3">
@@ -4551,7 +4551,7 @@
         <v>200</v>
       </c>
       <c r="C201" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="202" ht="21" spans="1:3">
@@ -4562,7 +4562,7 @@
         <v>201</v>
       </c>
       <c r="C202" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="203" ht="21" spans="1:3">
@@ -4573,7 +4573,7 @@
         <v>202</v>
       </c>
       <c r="C203" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="204" ht="21" spans="1:3">
@@ -4584,7 +4584,7 @@
         <v>203</v>
       </c>
       <c r="C204" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="205" ht="21" spans="1:3">
@@ -4595,7 +4595,7 @@
         <v>204</v>
       </c>
       <c r="C205" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="206" ht="21" spans="1:3">
@@ -4606,7 +4606,7 @@
         <v>205</v>
       </c>
       <c r="C206" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="207" ht="21" spans="1:3">
@@ -4617,7 +4617,7 @@
         <v>206</v>
       </c>
       <c r="C207" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="208" ht="21" spans="1:3">
@@ -4628,7 +4628,7 @@
         <v>207</v>
       </c>
       <c r="C208" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="209" ht="21" spans="1:3">
@@ -4639,7 +4639,7 @@
         <v>208</v>
       </c>
       <c r="C209" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="210" ht="21" spans="1:3">
@@ -4650,7 +4650,7 @@
         <v>209</v>
       </c>
       <c r="C210" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="211" ht="21" spans="1:3">
@@ -4661,7 +4661,7 @@
         <v>210</v>
       </c>
       <c r="C211" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="212" ht="21" spans="1:3">
@@ -4682,7 +4682,7 @@
         <v>212</v>
       </c>
       <c r="C214" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="215" ht="21" spans="1:3">
@@ -4693,7 +4693,7 @@
         <v>213</v>
       </c>
       <c r="C215" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="216" ht="21" spans="1:3">
@@ -4704,7 +4704,7 @@
         <v>214</v>
       </c>
       <c r="C216" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="217" ht="21" spans="1:3">
@@ -4715,7 +4715,7 @@
         <v>215</v>
       </c>
       <c r="C217" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="218" ht="21" spans="1:3">
@@ -4726,7 +4726,7 @@
         <v>216</v>
       </c>
       <c r="C218" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="219" ht="21" spans="1:3">
@@ -4737,7 +4737,7 @@
         <v>217</v>
       </c>
       <c r="C219" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="220" ht="21" spans="1:3">
@@ -4748,7 +4748,7 @@
         <v>218</v>
       </c>
       <c r="C220" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="221" ht="21" spans="1:3">
@@ -4759,7 +4759,7 @@
         <v>219</v>
       </c>
       <c r="C221" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="222" ht="21" spans="1:3">
@@ -4770,7 +4770,7 @@
         <v>220</v>
       </c>
       <c r="C222" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="223" ht="21" spans="1:3">
@@ -4781,7 +4781,7 @@
         <v>221</v>
       </c>
       <c r="C223" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="224" ht="21" spans="1:3">
@@ -4792,7 +4792,7 @@
         <v>222</v>
       </c>
       <c r="C224" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="225" ht="21" spans="1:3">
@@ -4803,7 +4803,7 @@
         <v>223</v>
       </c>
       <c r="C225" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="226" ht="21" spans="1:3">
@@ -4814,7 +4814,7 @@
         <v>224</v>
       </c>
       <c r="C226" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="227" ht="21" spans="1:3">
@@ -4825,7 +4825,7 @@
         <v>225</v>
       </c>
       <c r="C227" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="228" ht="21" spans="1:3">
@@ -4836,7 +4836,7 @@
         <v>226</v>
       </c>
       <c r="C228" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="229" ht="21" spans="1:3">
@@ -4847,7 +4847,7 @@
         <v>227</v>
       </c>
       <c r="C229" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="230" ht="21" spans="1:3">
@@ -4858,7 +4858,7 @@
         <v>228</v>
       </c>
       <c r="C230" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="231" ht="21" spans="1:3">
@@ -4869,7 +4869,7 @@
         <v>229</v>
       </c>
       <c r="C231" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="232" ht="21" spans="1:3">
@@ -4880,7 +4880,7 @@
         <v>230</v>
       </c>
       <c r="C232" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="233" ht="21" spans="1:3">
@@ -4891,7 +4891,7 @@
         <v>231</v>
       </c>
       <c r="C233" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="234" ht="21" spans="1:3">
@@ -4902,7 +4902,7 @@
         <v>232</v>
       </c>
       <c r="C234" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="235" ht="21" spans="1:3">
@@ -4913,7 +4913,7 @@
         <v>233</v>
       </c>
       <c r="C235" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="236" ht="21" spans="2:3">
@@ -4932,7 +4932,7 @@
         <v>235</v>
       </c>
       <c r="C238" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="239" ht="21" spans="1:3">
@@ -4943,7 +4943,7 @@
         <v>236</v>
       </c>
       <c r="C239" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="240" ht="21" spans="1:3">
@@ -4954,7 +4954,7 @@
         <v>237</v>
       </c>
       <c r="C240" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="241" ht="21" spans="1:3">
@@ -4965,7 +4965,7 @@
         <v>238</v>
       </c>
       <c r="C241" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="242" ht="21" spans="1:3">
@@ -4987,7 +4987,7 @@
         <v>241</v>
       </c>
       <c r="C243" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="244" ht="21" spans="1:3">
@@ -4998,7 +4998,7 @@
         <v>242</v>
       </c>
       <c r="C244" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="245" ht="21" spans="1:3">
@@ -5009,7 +5009,7 @@
         <v>243</v>
       </c>
       <c r="C245" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="246" ht="21" spans="1:3">
@@ -5020,7 +5020,7 @@
         <v>244</v>
       </c>
       <c r="C246" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="247" ht="21" spans="1:3">
@@ -5031,7 +5031,7 @@
         <v>245</v>
       </c>
       <c r="C247" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="248" ht="21" spans="1:3">
@@ -5042,7 +5042,7 @@
         <v>246</v>
       </c>
       <c r="C248" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="249" ht="21" spans="1:3">
@@ -5053,7 +5053,7 @@
         <v>247</v>
       </c>
       <c r="C249" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="250" ht="21" spans="1:3">
@@ -5064,7 +5064,7 @@
         <v>248</v>
       </c>
       <c r="C250" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="251" ht="21" spans="1:3">
@@ -5075,7 +5075,7 @@
         <v>249</v>
       </c>
       <c r="C251" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="252" ht="21" spans="1:3">
@@ -5086,7 +5086,7 @@
         <v>250</v>
       </c>
       <c r="C252" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="253" ht="21" spans="1:3">
@@ -5097,7 +5097,7 @@
         <v>251</v>
       </c>
       <c r="C253" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="254" ht="21" spans="1:3">
@@ -5108,7 +5108,7 @@
         <v>252</v>
       </c>
       <c r="C254" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="255" ht="21" spans="1:3">
@@ -5119,7 +5119,7 @@
         <v>253</v>
       </c>
       <c r="C255" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="256" ht="21" spans="1:3">
@@ -5130,7 +5130,7 @@
         <v>254</v>
       </c>
       <c r="C256" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="257" ht="21" spans="1:3">
@@ -5141,7 +5141,7 @@
         <v>255</v>
       </c>
       <c r="C257" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="258" ht="21" spans="1:3">
@@ -5152,7 +5152,7 @@
         <v>256</v>
       </c>
       <c r="C258" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="259" ht="21" spans="1:3">
@@ -5163,7 +5163,7 @@
         <v>257</v>
       </c>
       <c r="C259" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="260" ht="21" spans="1:3">
@@ -5174,7 +5174,7 @@
         <v>258</v>
       </c>
       <c r="C260" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="261" ht="21" spans="1:3">
@@ -5185,7 +5185,7 @@
         <v>259</v>
       </c>
       <c r="C261" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="262" ht="21" spans="1:3">
@@ -5196,7 +5196,7 @@
         <v>260</v>
       </c>
       <c r="C262" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="263" ht="21" spans="1:3">
@@ -5207,7 +5207,7 @@
         <v>261</v>
       </c>
       <c r="C263" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="264" ht="21" spans="1:3">
@@ -5218,7 +5218,7 @@
         <v>262</v>
       </c>
       <c r="C264" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="265" ht="21" spans="1:3">
@@ -5229,7 +5229,7 @@
         <v>263</v>
       </c>
       <c r="C265" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="266" ht="21" spans="1:3">
@@ -5240,7 +5240,7 @@
         <v>264</v>
       </c>
       <c r="C266" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="267" ht="21" spans="1:3">
@@ -5251,7 +5251,7 @@
         <v>265</v>
       </c>
       <c r="C267" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="268" ht="21" spans="1:3">
@@ -5262,7 +5262,7 @@
         <v>266</v>
       </c>
       <c r="C268" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="269" ht="21" spans="1:3">
@@ -5273,7 +5273,7 @@
         <v>267</v>
       </c>
       <c r="C269" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="270" ht="21" spans="1:3">
@@ -5284,7 +5284,7 @@
         <v>268</v>
       </c>
       <c r="C270" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="271" ht="21" spans="1:3">
@@ -5295,7 +5295,7 @@
         <v>90</v>
       </c>
       <c r="C271" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="272" ht="21" spans="1:3">
@@ -5306,7 +5306,7 @@
         <v>269</v>
       </c>
       <c r="C272" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="273" ht="21" spans="2:3">
@@ -5325,7 +5325,7 @@
         <v>271</v>
       </c>
       <c r="C275" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="276" ht="21" spans="1:3">
@@ -5336,7 +5336,7 @@
         <v>272</v>
       </c>
       <c r="C276" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="277" ht="21" spans="1:3">
@@ -5347,7 +5347,7 @@
         <v>273</v>
       </c>
       <c r="C277" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="278" ht="21" spans="1:3">
@@ -5358,7 +5358,7 @@
         <v>274</v>
       </c>
       <c r="C278" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="279" ht="21" spans="1:3">
@@ -5369,7 +5369,7 @@
         <v>275</v>
       </c>
       <c r="C279" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="280" ht="21" spans="1:3">
@@ -5380,7 +5380,7 @@
         <v>276</v>
       </c>
       <c r="C280" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="281" ht="21" spans="1:3">
@@ -5391,7 +5391,7 @@
         <v>277</v>
       </c>
       <c r="C281" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="282" ht="21" spans="1:3">
@@ -5402,7 +5402,7 @@
         <v>278</v>
       </c>
       <c r="C282" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="283" ht="21" spans="1:3">
@@ -5413,7 +5413,7 @@
         <v>279</v>
       </c>
       <c r="C283" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="284" ht="21" spans="1:3">
@@ -5424,7 +5424,7 @@
         <v>280</v>
       </c>
       <c r="C284" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="285" ht="21" spans="1:3">
@@ -5435,7 +5435,7 @@
         <v>281</v>
       </c>
       <c r="C285" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="286" ht="21" spans="1:3">
@@ -5446,7 +5446,7 @@
         <v>282</v>
       </c>
       <c r="C286" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="287" ht="21" spans="1:3">
@@ -5457,7 +5457,7 @@
         <v>283</v>
       </c>
       <c r="C287" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="288" ht="21" spans="1:3">
@@ -5468,7 +5468,7 @@
         <v>284</v>
       </c>
       <c r="C288" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="289" ht="21" spans="1:3">
@@ -5479,7 +5479,7 @@
         <v>285</v>
       </c>
       <c r="C289" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="290" ht="21" spans="1:3">
@@ -5490,7 +5490,7 @@
         <v>286</v>
       </c>
       <c r="C290" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="291" ht="21" spans="1:3">
@@ -5501,7 +5501,7 @@
         <v>287</v>
       </c>
       <c r="C291" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="292" ht="21" spans="1:3">
@@ -5512,7 +5512,7 @@
         <v>288</v>
       </c>
       <c r="C292" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="293" ht="21" spans="1:3">
@@ -5523,7 +5523,7 @@
         <v>289</v>
       </c>
       <c r="C293" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="294" ht="21" spans="2:3">
@@ -5542,7 +5542,7 @@
         <v>291</v>
       </c>
       <c r="C296" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="297" ht="21" spans="1:3">
@@ -5553,7 +5553,7 @@
         <v>292</v>
       </c>
       <c r="C297" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="298" ht="21" spans="1:3">
@@ -5564,7 +5564,7 @@
         <v>293</v>
       </c>
       <c r="C298" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="299" ht="21" spans="1:3">
@@ -5575,7 +5575,7 @@
         <v>294</v>
       </c>
       <c r="C299" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="300" ht="21" spans="1:3">
@@ -5586,7 +5586,7 @@
         <v>295</v>
       </c>
       <c r="C300" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="301" ht="21" spans="1:3">
@@ -5597,7 +5597,7 @@
         <v>296</v>
       </c>
       <c r="C301" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="302" ht="21" spans="1:3">
@@ -5608,7 +5608,7 @@
         <v>297</v>
       </c>
       <c r="C302" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="303" ht="21" spans="1:3">
@@ -5619,7 +5619,7 @@
         <v>298</v>
       </c>
       <c r="C303" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="304" ht="21" spans="1:3">
@@ -5630,7 +5630,7 @@
         <v>299</v>
       </c>
       <c r="C304" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="305" ht="21" spans="1:3">
@@ -5641,7 +5641,7 @@
         <v>300</v>
       </c>
       <c r="C305" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="306" ht="21" spans="1:3">
@@ -5652,7 +5652,7 @@
         <v>301</v>
       </c>
       <c r="C306" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="307" ht="21" spans="1:3">
@@ -5663,7 +5663,7 @@
         <v>302</v>
       </c>
       <c r="C307" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="308" ht="21" spans="1:3">
@@ -5674,7 +5674,7 @@
         <v>303</v>
       </c>
       <c r="C308" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="309" ht="21" spans="1:3">
@@ -5685,7 +5685,7 @@
         <v>304</v>
       </c>
       <c r="C309" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="310" ht="21" spans="1:3">
@@ -5696,7 +5696,7 @@
         <v>305</v>
       </c>
       <c r="C310" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="311" ht="21" spans="1:3">
@@ -5707,7 +5707,7 @@
         <v>306</v>
       </c>
       <c r="C311" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="312" ht="21" spans="1:3">
@@ -5718,7 +5718,7 @@
         <v>307</v>
       </c>
       <c r="C312" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="313" ht="21" spans="1:3">
@@ -5729,7 +5729,7 @@
         <v>308</v>
       </c>
       <c r="C313" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="314" ht="21" spans="1:3">
@@ -5740,7 +5740,7 @@
         <v>309</v>
       </c>
       <c r="C314" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="315" ht="21" spans="1:3">
@@ -5751,7 +5751,7 @@
         <v>310</v>
       </c>
       <c r="C315" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="316" ht="21" spans="1:3">
@@ -5762,7 +5762,7 @@
         <v>311</v>
       </c>
       <c r="C316" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="317" ht="21" spans="1:3">
@@ -5773,7 +5773,7 @@
         <v>312</v>
       </c>
       <c r="C317" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="318" ht="21" spans="1:3">
@@ -5784,7 +5784,7 @@
         <v>313</v>
       </c>
       <c r="C318" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="319" ht="21" spans="1:3">
@@ -5795,7 +5795,7 @@
         <v>314</v>
       </c>
       <c r="C319" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="320" ht="21" spans="1:3">
@@ -5806,7 +5806,7 @@
         <v>315</v>
       </c>
       <c r="C320" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="321" ht="21" spans="1:3">
@@ -5817,7 +5817,7 @@
         <v>316</v>
       </c>
       <c r="C321" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="322" ht="21" spans="1:3">
@@ -5828,7 +5828,7 @@
         <v>317</v>
       </c>
       <c r="C322" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="323" ht="21" spans="1:3">
@@ -5839,7 +5839,7 @@
         <v>318</v>
       </c>
       <c r="C323" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="324" ht="21" spans="1:3">
@@ -5850,7 +5850,7 @@
         <v>319</v>
       </c>
       <c r="C324" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="325" ht="21" spans="1:3">
@@ -5861,7 +5861,7 @@
         <v>320</v>
       </c>
       <c r="C325" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="326" ht="21" spans="1:3">
@@ -5872,7 +5872,7 @@
         <v>321</v>
       </c>
       <c r="C326" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="327" ht="21" spans="1:3">
@@ -5883,7 +5883,7 @@
         <v>322</v>
       </c>
       <c r="C327" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="328" ht="21" spans="1:3">
@@ -5894,7 +5894,7 @@
         <v>323</v>
       </c>
       <c r="C328" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="329" ht="21" spans="1:3">
@@ -5905,7 +5905,7 @@
         <v>324</v>
       </c>
       <c r="C329" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="330" ht="21" spans="1:3">
@@ -5916,7 +5916,7 @@
         <v>325</v>
       </c>
       <c r="C330" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="331" ht="21" spans="1:3">
@@ -5927,7 +5927,7 @@
         <v>326</v>
       </c>
       <c r="C331" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="332" ht="21" spans="1:3">
@@ -5938,7 +5938,7 @@
         <v>327</v>
       </c>
       <c r="C332" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="333" ht="21" spans="1:3">
@@ -5949,7 +5949,7 @@
         <v>328</v>
       </c>
       <c r="C333" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="334" ht="21" spans="2:3">
@@ -5968,7 +5968,7 @@
         <v>330</v>
       </c>
       <c r="C336" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="337" ht="21" spans="1:3">
@@ -5979,7 +5979,7 @@
         <v>331</v>
       </c>
       <c r="C337" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="338" ht="21" spans="1:3">
@@ -5990,7 +5990,7 @@
         <v>332</v>
       </c>
       <c r="C338" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="339" ht="21" spans="1:3">
@@ -6001,7 +6001,7 @@
         <v>333</v>
       </c>
       <c r="C339" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="340" ht="21" spans="1:3">
@@ -6012,7 +6012,7 @@
         <v>334</v>
       </c>
       <c r="C340" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="341" ht="21" spans="1:3">
@@ -6023,7 +6023,7 @@
         <v>335</v>
       </c>
       <c r="C341" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="342" ht="21" spans="1:3">
@@ -6034,7 +6034,7 @@
         <v>336</v>
       </c>
       <c r="C342" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="343" ht="21" spans="1:3">
@@ -6045,7 +6045,7 @@
         <v>337</v>
       </c>
       <c r="C343" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="344" ht="21" spans="1:3">
@@ -6056,7 +6056,7 @@
         <v>338</v>
       </c>
       <c r="C344" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="345" ht="21" spans="1:3">
@@ -6067,7 +6067,7 @@
         <v>339</v>
       </c>
       <c r="C345" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="346" ht="21" spans="1:3">
@@ -6078,7 +6078,7 @@
         <v>340</v>
       </c>
       <c r="C346" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="347" ht="21" spans="1:3">
@@ -6089,7 +6089,7 @@
         <v>341</v>
       </c>
       <c r="C347" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="348" ht="21" spans="1:3">
@@ -6100,7 +6100,7 @@
         <v>342</v>
       </c>
       <c r="C348" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="349" ht="21" spans="1:3">
@@ -6111,7 +6111,7 @@
         <v>343</v>
       </c>
       <c r="C349" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="350" ht="21" spans="1:3">
@@ -6122,7 +6122,7 @@
         <v>344</v>
       </c>
       <c r="C350" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="351" ht="21" spans="1:3">
@@ -6133,7 +6133,7 @@
         <v>345</v>
       </c>
       <c r="C351" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="352" ht="21" spans="1:3">
@@ -6144,7 +6144,7 @@
         <v>346</v>
       </c>
       <c r="C352" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="353" ht="21" spans="1:3">
@@ -6155,7 +6155,7 @@
         <v>347</v>
       </c>
       <c r="C353" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="354" ht="21" spans="2:3">
@@ -6174,7 +6174,7 @@
         <v>349</v>
       </c>
       <c r="C356" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="357" ht="21" spans="1:3">
@@ -6251,7 +6251,7 @@
         <v>356</v>
       </c>
       <c r="C363" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="364" ht="21" spans="1:3">
@@ -6262,7 +6262,7 @@
         <v>357</v>
       </c>
       <c r="C364" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="365" ht="21" spans="1:3">
@@ -6273,7 +6273,7 @@
         <v>358</v>
       </c>
       <c r="C365" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="366" ht="21" spans="1:3">
@@ -6284,7 +6284,7 @@
         <v>359</v>
       </c>
       <c r="C366" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="367" ht="21" spans="1:3">
@@ -6295,7 +6295,7 @@
         <v>360</v>
       </c>
       <c r="C367" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="368" ht="21" spans="1:3">
@@ -6306,7 +6306,7 @@
         <v>361</v>
       </c>
       <c r="C368" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="369" ht="21" spans="1:3">
@@ -6317,7 +6317,7 @@
         <v>362</v>
       </c>
       <c r="C369" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="370" ht="21" spans="1:3">
@@ -6328,7 +6328,7 @@
         <v>363</v>
       </c>
       <c r="C370" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="371" ht="21" spans="1:3">
@@ -6339,7 +6339,7 @@
         <v>364</v>
       </c>
       <c r="C371" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="372" ht="21" spans="1:3">
@@ -6350,7 +6350,7 @@
         <v>365</v>
       </c>
       <c r="C372" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="373" ht="21" spans="1:3">
@@ -6361,7 +6361,7 @@
         <v>366</v>
       </c>
       <c r="C373" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="374" ht="21" spans="1:3">
@@ -6372,7 +6372,7 @@
         <v>367</v>
       </c>
       <c r="C374" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="375" ht="21" spans="1:3">
@@ -6383,7 +6383,7 @@
         <v>368</v>
       </c>
       <c r="C375" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="376" ht="21" spans="1:3">
@@ -6394,7 +6394,7 @@
         <v>369</v>
       </c>
       <c r="C376" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="377" ht="21" spans="1:3">
@@ -6405,7 +6405,7 @@
         <v>370</v>
       </c>
       <c r="C377" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="378" ht="21" spans="1:3">
@@ -6416,7 +6416,7 @@
         <v>371</v>
       </c>
       <c r="C378" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="379" ht="21" spans="1:3">
@@ -6427,7 +6427,7 @@
         <v>372</v>
       </c>
       <c r="C379" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="380" ht="21" spans="1:3">
@@ -6438,7 +6438,7 @@
         <v>373</v>
       </c>
       <c r="C380" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="381" ht="21" spans="1:3">
@@ -6449,7 +6449,7 @@
         <v>374</v>
       </c>
       <c r="C381" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="382" ht="21" spans="1:3">
@@ -6460,7 +6460,7 @@
         <v>375</v>
       </c>
       <c r="C382" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="383" ht="21" spans="1:3">
@@ -6471,7 +6471,7 @@
         <v>376</v>
       </c>
       <c r="C383" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="384" ht="21" spans="1:3">
@@ -6482,7 +6482,7 @@
         <v>377</v>
       </c>
       <c r="C384" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="385" ht="21" spans="1:3">
@@ -6493,7 +6493,7 @@
         <v>378</v>
       </c>
       <c r="C385" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="386" ht="21" spans="1:3">
@@ -6504,7 +6504,7 @@
         <v>379</v>
       </c>
       <c r="C386" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="387" ht="21" spans="1:3">
@@ -6515,7 +6515,7 @@
         <v>380</v>
       </c>
       <c r="C387" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="388" ht="21" spans="1:3">
@@ -6526,7 +6526,7 @@
         <v>381</v>
       </c>
       <c r="C388" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="389" ht="21" spans="1:3">
@@ -6537,7 +6537,7 @@
         <v>382</v>
       </c>
       <c r="C389" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="390" ht="21" spans="1:3">
@@ -6548,7 +6548,7 @@
         <v>382</v>
       </c>
       <c r="C390" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="391" ht="21" spans="1:3">
@@ -6559,7 +6559,7 @@
         <v>383</v>
       </c>
       <c r="C391" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="392" ht="21" spans="1:3">
@@ -6570,7 +6570,7 @@
         <v>384</v>
       </c>
       <c r="C392" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="393" ht="21" spans="1:3">
@@ -6581,7 +6581,7 @@
         <v>385</v>
       </c>
       <c r="C393" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="394" ht="21" spans="1:3">
@@ -6592,7 +6592,7 @@
         <v>386</v>
       </c>
       <c r="C394" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="395" ht="21" spans="1:3">
@@ -6603,7 +6603,7 @@
         <v>387</v>
       </c>
       <c r="C395" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="396" ht="21" spans="1:3">
@@ -6614,7 +6614,7 @@
         <v>388</v>
       </c>
       <c r="C396" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="397" ht="21" spans="1:3">
@@ -6625,7 +6625,7 @@
         <v>389</v>
       </c>
       <c r="C397" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="398" ht="21" spans="1:3">
@@ -6636,7 +6636,7 @@
         <v>390</v>
       </c>
       <c r="C398" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="399" ht="21" spans="1:3">
@@ -6647,7 +6647,7 @@
         <v>391</v>
       </c>
       <c r="C399" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="400" ht="21" spans="2:3">
@@ -6666,7 +6666,7 @@
         <v>393</v>
       </c>
       <c r="C402" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="403" ht="21" spans="1:3">
@@ -6677,7 +6677,7 @@
         <v>394</v>
       </c>
       <c r="C403" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="404" ht="21" spans="1:3">
@@ -6688,7 +6688,7 @@
         <v>395</v>
       </c>
       <c r="C404" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="405" ht="21" spans="1:3">
@@ -6699,7 +6699,7 @@
         <v>92</v>
       </c>
       <c r="C405" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="406" ht="21" spans="1:3">
@@ -6710,7 +6710,7 @@
         <v>396</v>
       </c>
       <c r="C406" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="407" ht="21" spans="1:3">
@@ -6721,7 +6721,7 @@
         <v>397</v>
       </c>
       <c r="C407" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="408" ht="21" spans="2:3">
@@ -6817,7 +6817,7 @@
         <v>278</v>
       </c>
       <c r="C417" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="418" ht="21" spans="1:3">
@@ -6828,7 +6828,7 @@
         <v>406</v>
       </c>
       <c r="C418" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="419" ht="21" spans="1:3">
@@ -6839,7 +6839,7 @@
         <v>407</v>
       </c>
       <c r="C419" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="420" ht="21" spans="1:3">
@@ -6850,7 +6850,7 @@
         <v>408</v>
       </c>
       <c r="C420" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="421" ht="21" spans="1:3">
@@ -6861,7 +6861,7 @@
         <v>409</v>
       </c>
       <c r="C421" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="422" ht="21" spans="1:3">
@@ -6872,7 +6872,7 @@
         <v>410</v>
       </c>
       <c r="C422" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="423" ht="21" spans="1:3">
@@ -6883,7 +6883,7 @@
         <v>411</v>
       </c>
       <c r="C423" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="424" ht="21" spans="1:3">
@@ -6894,7 +6894,7 @@
         <v>412</v>
       </c>
       <c r="C424" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="425" ht="21" spans="1:3">
@@ -6905,7 +6905,7 @@
         <v>413</v>
       </c>
       <c r="C425" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="426" ht="21" spans="1:3">
@@ -6916,7 +6916,7 @@
         <v>414</v>
       </c>
       <c r="C426" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="427" ht="21" spans="1:3">
@@ -6927,7 +6927,7 @@
         <v>415</v>
       </c>
       <c r="C427" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="428" ht="21" spans="1:3">
@@ -6938,7 +6938,7 @@
         <v>416</v>
       </c>
       <c r="C428" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="429" ht="21" spans="1:3">
@@ -6949,7 +6949,7 @@
         <v>417</v>
       </c>
       <c r="C429" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="430" ht="21" spans="1:3">
@@ -6960,7 +6960,7 @@
         <v>418</v>
       </c>
       <c r="C430" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="431" ht="21" spans="1:3">
@@ -6971,7 +6971,7 @@
         <v>419</v>
       </c>
       <c r="C431" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="432" ht="21" spans="1:3">
@@ -6982,7 +6982,7 @@
         <v>420</v>
       </c>
       <c r="C432" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="433" ht="21" spans="1:3">
@@ -6993,7 +6993,7 @@
         <v>421</v>
       </c>
       <c r="C433" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="434" ht="21" spans="1:3">
@@ -7004,7 +7004,7 @@
         <v>422</v>
       </c>
       <c r="C434" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="435" ht="21" spans="1:3">
@@ -7015,7 +7015,7 @@
         <v>423</v>
       </c>
       <c r="C435" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="436" ht="21" spans="1:3">
@@ -7026,7 +7026,7 @@
         <v>424</v>
       </c>
       <c r="C436" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="437" ht="21" spans="1:3">
@@ -7037,7 +7037,7 @@
         <v>425</v>
       </c>
       <c r="C437" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="438" ht="21" spans="1:3">
@@ -7048,7 +7048,7 @@
         <v>17</v>
       </c>
       <c r="C438" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="439" ht="21" spans="1:3">
@@ -7059,7 +7059,7 @@
         <v>426</v>
       </c>
       <c r="C439" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="440" ht="21" spans="1:3">
@@ -7070,7 +7070,7 @@
         <v>427</v>
       </c>
       <c r="C440" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="441" ht="21" spans="1:3">
@@ -7081,7 +7081,7 @@
         <v>428</v>
       </c>
       <c r="C441" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="442" ht="21" spans="1:3">
@@ -7092,7 +7092,7 @@
         <v>429</v>
       </c>
       <c r="C442" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="443" ht="21" spans="1:3">
@@ -7103,7 +7103,7 @@
         <v>430</v>
       </c>
       <c r="C443" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="444" ht="21" spans="1:3">
@@ -7114,7 +7114,7 @@
         <v>431</v>
       </c>
       <c r="C444" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="445" ht="21" spans="1:3">
@@ -7125,7 +7125,7 @@
         <v>432</v>
       </c>
       <c r="C445" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="446" ht="21" spans="1:3">
@@ -7136,7 +7136,7 @@
         <v>433</v>
       </c>
       <c r="C446" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="447" ht="21" spans="1:3">
@@ -7147,7 +7147,7 @@
         <v>434</v>
       </c>
       <c r="C447" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="448" ht="21" spans="1:3">
@@ -7158,7 +7158,7 @@
         <v>435</v>
       </c>
       <c r="C448" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="449" ht="21" spans="1:3">
@@ -7169,7 +7169,7 @@
         <v>436</v>
       </c>
       <c r="C449" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="450" ht="21" spans="1:3">
@@ -7180,7 +7180,7 @@
         <v>437</v>
       </c>
       <c r="C450" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="451" ht="21" spans="1:3">
@@ -7191,7 +7191,7 @@
         <v>438</v>
       </c>
       <c r="C451" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="452" ht="21" spans="1:3">
@@ -7202,7 +7202,7 @@
         <v>439</v>
       </c>
       <c r="C452" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="453" ht="21" spans="1:3">
@@ -7213,7 +7213,7 @@
         <v>440</v>
       </c>
       <c r="C453" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="454" ht="21" spans="1:3">
@@ -7224,7 +7224,7 @@
         <v>441</v>
       </c>
       <c r="C454" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="455" ht="21" spans="1:3">
@@ -7235,7 +7235,7 @@
         <v>442</v>
       </c>
       <c r="C455" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="456" ht="21" spans="1:3">
@@ -7246,7 +7246,7 @@
         <v>443</v>
       </c>
       <c r="C456" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="457" ht="21" spans="1:3">
@@ -7257,7 +7257,7 @@
         <v>444</v>
       </c>
       <c r="C457" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="458" ht="21" spans="1:3">
@@ -7268,7 +7268,7 @@
         <v>445</v>
       </c>
       <c r="C458" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="459" ht="21" spans="1:3">
@@ -7279,7 +7279,7 @@
         <v>446</v>
       </c>
       <c r="C459" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="460" ht="21" spans="1:3">
@@ -7290,7 +7290,7 @@
         <v>447</v>
       </c>
       <c r="C460" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="461" ht="21" spans="1:3">
@@ -7301,7 +7301,7 @@
         <v>448</v>
       </c>
       <c r="C461" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="462" ht="21" spans="1:3">
@@ -7312,7 +7312,7 @@
         <v>449</v>
       </c>
       <c r="C462" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="463" ht="21" spans="1:3">
@@ -7323,7 +7323,7 @@
         <v>450</v>
       </c>
       <c r="C463" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="464" ht="21" spans="1:3">
@@ -7334,7 +7334,7 @@
         <v>451</v>
       </c>
       <c r="C464" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="465" ht="21" spans="1:3">
@@ -7345,7 +7345,7 @@
         <v>452</v>
       </c>
       <c r="C465" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="466" ht="21" spans="1:3">
@@ -7356,7 +7356,7 @@
         <v>453</v>
       </c>
       <c r="C466" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="467" ht="21" spans="1:3">
@@ -7367,7 +7367,7 @@
         <v>454</v>
       </c>
       <c r="C467" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="468" ht="21" spans="1:3">
@@ -7378,7 +7378,7 @@
         <v>455</v>
       </c>
       <c r="C468" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="469" ht="21" spans="1:3">
@@ -7389,7 +7389,7 @@
         <v>456</v>
       </c>
       <c r="C469" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="470" ht="21" spans="2:3">
@@ -7409,7 +7409,7 @@
         <v>458</v>
       </c>
       <c r="C472" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="473" ht="21" spans="1:3">
@@ -7420,7 +7420,7 @@
         <v>459</v>
       </c>
       <c r="C473" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="474" ht="21" spans="1:3">
@@ -7431,7 +7431,7 @@
         <v>460</v>
       </c>
       <c r="C474" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="475" ht="21" spans="1:3">
@@ -7442,7 +7442,7 @@
         <v>461</v>
       </c>
       <c r="C475" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="476" ht="21" spans="1:3">
@@ -7453,7 +7453,7 @@
         <v>462</v>
       </c>
       <c r="C476" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="477" ht="21" spans="1:3">
@@ -7464,7 +7464,7 @@
         <v>463</v>
       </c>
       <c r="C477" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="478" ht="21" spans="1:3">
@@ -7475,7 +7475,7 @@
         <v>464</v>
       </c>
       <c r="C478" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="479" ht="21" spans="1:3">
@@ -7486,7 +7486,7 @@
         <v>465</v>
       </c>
       <c r="C479" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="480" ht="21" spans="1:3">
@@ -7497,7 +7497,7 @@
         <v>466</v>
       </c>
       <c r="C480" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="481" ht="21" spans="1:3">
@@ -7508,7 +7508,7 @@
         <v>467</v>
       </c>
       <c r="C481" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Count inversions in array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335"/>
+    <workbookView windowWidth="23040" windowHeight="8892"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -85,13 +85,13 @@
     <t>Next Permutation</t>
   </si>
   <si>
+    <t>Count Inversion</t>
+  </si>
+  <si>
+    <t>Best time to buy and Sell stock</t>
+  </si>
+  <si>
     <t>&lt;-&gt;</t>
-  </si>
-  <si>
-    <t>Count Inversion</t>
-  </si>
-  <si>
-    <t>Best time to buy and Sell stock</t>
   </si>
   <si>
     <t>find all pairs on integer array whose sum is equal to given number</t>
@@ -1425,10 +1425,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1502,6 +1502,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1509,9 +1517,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1521,6 +1535,21 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1539,6 +1568,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -1547,33 +1591,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1593,30 +1615,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1630,16 +1638,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1660,7 +1660,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1672,7 +1672,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1690,13 +1690,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1708,13 +1714,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1726,43 +1744,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1780,7 +1786,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1792,31 +1798,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1828,13 +1828,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1845,6 +1845,26 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1873,21 +1893,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1911,15 +1916,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1935,159 +1931,163 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2441,7 +2441,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2638,8 +2638,8 @@
       <c r="B20" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>23</v>
+      <c r="C20" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="21" ht="21" spans="1:3">
@@ -2647,10 +2647,10 @@
         <v>6</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="9" t="s">
         <v>23</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="22" ht="21" spans="1:3">
@@ -2658,10 +2658,10 @@
         <v>6</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" ht="21" spans="1:3">
@@ -2672,7 +2672,7 @@
         <v>26</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" ht="21" spans="1:3">
@@ -2683,7 +2683,7 @@
         <v>27</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" ht="21" spans="1:3">
@@ -2694,7 +2694,7 @@
         <v>28</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" ht="21" spans="1:3">
@@ -2705,7 +2705,7 @@
         <v>29</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" ht="21" spans="1:3">
@@ -2716,7 +2716,7 @@
         <v>30</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" ht="21" spans="1:3">
@@ -2727,7 +2727,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" ht="21" spans="1:3">
@@ -2738,7 +2738,7 @@
         <v>32</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" ht="21" spans="1:3">
@@ -2749,7 +2749,7 @@
         <v>33</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" ht="21" spans="1:3">
@@ -2760,7 +2760,7 @@
         <v>34</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" ht="21" spans="1:3">
@@ -2771,7 +2771,7 @@
         <v>35</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" ht="21" spans="1:3">
@@ -2782,7 +2782,7 @@
         <v>36</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" ht="21" spans="1:3">
@@ -2793,7 +2793,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" ht="21" spans="1:3">
@@ -2804,7 +2804,7 @@
         <v>38</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" ht="21" spans="1:3">
@@ -2815,7 +2815,7 @@
         <v>39</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" ht="21" spans="1:3">
@@ -2826,7 +2826,7 @@
         <v>40</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" ht="21" spans="1:3">
@@ -2837,7 +2837,7 @@
         <v>41</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" ht="21" spans="1:3">
@@ -2848,7 +2848,7 @@
         <v>42</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" ht="21" spans="1:3">
@@ -2859,7 +2859,7 @@
         <v>43</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" ht="21" spans="1:3">
@@ -2870,20 +2870,20 @@
         <v>44</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" ht="21" spans="2:3">
       <c r="B42" s="10"/>
       <c r="C42" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" ht="21" spans="1:3">
       <c r="A43" s="6"/>
       <c r="B43" s="10"/>
       <c r="C43" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" ht="21" spans="1:3">
@@ -2894,7 +2894,7 @@
         <v>46</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" ht="21" spans="1:3">
@@ -2905,7 +2905,7 @@
         <v>47</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" ht="21" spans="1:3">
@@ -2916,7 +2916,7 @@
         <v>48</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" ht="21" spans="1:3">
@@ -2927,7 +2927,7 @@
         <v>49</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" ht="21" spans="1:3">
@@ -2938,7 +2938,7 @@
         <v>50</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" ht="21" spans="1:3">
@@ -2949,7 +2949,7 @@
         <v>51</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" ht="21" spans="1:3">
@@ -2960,7 +2960,7 @@
         <v>52</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" ht="21" spans="1:3">
@@ -2971,7 +2971,7 @@
         <v>53</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" ht="21" spans="1:3">
@@ -2982,7 +2982,7 @@
         <v>54</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53" ht="21" spans="1:3">
@@ -2993,7 +2993,7 @@
         <v>55</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="55" ht="21" spans="1:3">
@@ -3009,7 +3009,7 @@
         <v>57</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="57" ht="21" spans="1:3">
@@ -3020,7 +3020,7 @@
         <v>58</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58" ht="21" spans="1:3">
@@ -3031,7 +3031,7 @@
         <v>59</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" ht="21" spans="1:3">
@@ -3042,7 +3042,7 @@
         <v>60</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60" ht="21" spans="1:3">
@@ -3053,7 +3053,7 @@
         <v>61</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="61" ht="21" spans="1:3">
@@ -3064,7 +3064,7 @@
         <v>62</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="62" ht="21" spans="1:3">
@@ -3075,7 +3075,7 @@
         <v>63</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" ht="21" spans="1:3">
@@ -3086,7 +3086,7 @@
         <v>64</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64" ht="21" spans="1:3">
@@ -3097,7 +3097,7 @@
         <v>65</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="65" ht="21" spans="1:3">
@@ -3108,7 +3108,7 @@
         <v>66</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="66" ht="21" spans="1:3">
@@ -3119,7 +3119,7 @@
         <v>67</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="67" ht="21" spans="1:3">
@@ -3130,7 +3130,7 @@
         <v>68</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="68" ht="21" spans="1:3">
@@ -3141,7 +3141,7 @@
         <v>69</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="69" ht="21" spans="1:3">
@@ -3152,7 +3152,7 @@
         <v>70</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="70" ht="21" spans="1:3">
@@ -3163,7 +3163,7 @@
         <v>71</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="71" ht="21" spans="1:3">
@@ -3174,7 +3174,7 @@
         <v>72</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="72" ht="21" spans="1:3">
@@ -3185,7 +3185,7 @@
         <v>73</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="73" ht="21" spans="1:3">
@@ -3196,7 +3196,7 @@
         <v>74</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="74" ht="21" spans="1:3">
@@ -3207,7 +3207,7 @@
         <v>75</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="75" ht="21" spans="1:3">
@@ -3218,7 +3218,7 @@
         <v>76</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="76" ht="21" spans="1:3">
@@ -3229,7 +3229,7 @@
         <v>77</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="77" ht="21" spans="1:3">
@@ -3240,7 +3240,7 @@
         <v>78</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="78" ht="21" spans="1:3">
@@ -3251,7 +3251,7 @@
         <v>79</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="79" ht="21" spans="1:3">
@@ -3262,7 +3262,7 @@
         <v>80</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="80" ht="21" spans="1:3">
@@ -3273,7 +3273,7 @@
         <v>81</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="81" ht="21" spans="1:3">
@@ -3284,7 +3284,7 @@
         <v>82</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="82" ht="21" spans="1:3">
@@ -3295,7 +3295,7 @@
         <v>83</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="83" ht="21" spans="1:3">
@@ -3306,7 +3306,7 @@
         <v>84</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="84" ht="21" spans="1:3">
@@ -3317,7 +3317,7 @@
         <v>85</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="85" ht="21" spans="1:3">
@@ -3328,7 +3328,7 @@
         <v>86</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="86" ht="21" spans="1:3">
@@ -3339,7 +3339,7 @@
         <v>87</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="87" ht="21" spans="1:3">
@@ -3350,7 +3350,7 @@
         <v>88</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="88" ht="21" spans="1:3">
@@ -3361,7 +3361,7 @@
         <v>89</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="89" ht="21" spans="1:3">
@@ -3372,7 +3372,7 @@
         <v>90</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="90" ht="21" spans="1:3">
@@ -3383,7 +3383,7 @@
         <v>91</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="91" ht="21" spans="1:3">
@@ -3394,7 +3394,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="92" ht="21" spans="1:3">
@@ -3405,7 +3405,7 @@
         <v>93</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="93" ht="21" spans="1:3">
@@ -3416,7 +3416,7 @@
         <v>94</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="94" ht="21" spans="1:3">
@@ -3427,7 +3427,7 @@
         <v>95</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="95" ht="21" spans="1:3">
@@ -3438,7 +3438,7 @@
         <v>96</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="96" ht="21" spans="1:3">
@@ -3449,7 +3449,7 @@
         <v>97</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="97" ht="21" spans="1:3">
@@ -3460,7 +3460,7 @@
         <v>98</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="98" ht="21" spans="1:3">
@@ -3471,7 +3471,7 @@
         <v>99</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="100" ht="21" spans="1:3">
@@ -3487,7 +3487,7 @@
         <v>101</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="102" ht="21" spans="1:3">
@@ -3498,7 +3498,7 @@
         <v>102</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="103" ht="21" spans="1:3">
@@ -3509,7 +3509,7 @@
         <v>103</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="104" ht="21" spans="1:3">
@@ -3520,7 +3520,7 @@
         <v>104</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="105" ht="21" spans="1:3">
@@ -3531,7 +3531,7 @@
         <v>105</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="106" ht="21" spans="1:3">
@@ -3542,7 +3542,7 @@
         <v>106</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="107" ht="21" spans="1:3">
@@ -3553,7 +3553,7 @@
         <v>107</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="108" ht="21" spans="1:3">
@@ -3564,7 +3564,7 @@
         <v>108</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="109" ht="21" spans="1:3">
@@ -3575,7 +3575,7 @@
         <v>109</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="110" ht="21" spans="1:3">
@@ -3586,7 +3586,7 @@
         <v>110</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="111" ht="21" spans="1:3">
@@ -3597,7 +3597,7 @@
         <v>111</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="112" ht="21" spans="1:3">
@@ -3608,7 +3608,7 @@
         <v>112</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="113" ht="21" spans="1:3">
@@ -3619,7 +3619,7 @@
         <v>113</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="114" ht="21" spans="1:3">
@@ -3630,7 +3630,7 @@
         <v>114</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="115" ht="21" spans="1:3">
@@ -3641,7 +3641,7 @@
         <v>115</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="116" ht="21" spans="1:3">
@@ -3652,7 +3652,7 @@
         <v>116</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="117" ht="21" spans="1:3">
@@ -3663,7 +3663,7 @@
         <v>117</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="118" ht="21" spans="1:3">
@@ -3674,7 +3674,7 @@
         <v>118</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="119" ht="21" spans="1:3">
@@ -3685,7 +3685,7 @@
         <v>119</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="120" ht="21" spans="1:3">
@@ -3696,7 +3696,7 @@
         <v>120</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="121" ht="21" spans="1:3">
@@ -3707,7 +3707,7 @@
         <v>121</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="122" ht="21" spans="1:3">
@@ -3718,7 +3718,7 @@
         <v>122</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="123" ht="21" spans="1:3">
@@ -3729,7 +3729,7 @@
         <v>123</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="124" ht="21" spans="1:3">
@@ -3740,7 +3740,7 @@
         <v>124</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="125" ht="21" spans="1:3">
@@ -3751,7 +3751,7 @@
         <v>125</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="126" ht="21" spans="1:3">
@@ -3762,7 +3762,7 @@
         <v>126</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="127" ht="21" spans="1:3">
@@ -3773,7 +3773,7 @@
         <v>127</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="128" ht="21" spans="1:3">
@@ -3784,7 +3784,7 @@
         <v>128</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="129" ht="21" spans="1:3">
@@ -3795,7 +3795,7 @@
         <v>129</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="130" ht="21" spans="1:3">
@@ -3806,7 +3806,7 @@
         <v>130</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="131" ht="21" spans="1:3">
@@ -3817,7 +3817,7 @@
         <v>131</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="132" ht="21" spans="1:3">
@@ -3828,7 +3828,7 @@
         <v>132</v>
       </c>
       <c r="C132" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="133" ht="21" spans="1:3">
@@ -3839,7 +3839,7 @@
         <v>133</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="134" ht="21" spans="1:3">
@@ -3850,7 +3850,7 @@
         <v>134</v>
       </c>
       <c r="C134" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="135" ht="21" spans="1:3">
@@ -3861,7 +3861,7 @@
         <v>135</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="136" ht="21" spans="1:3">
@@ -3872,7 +3872,7 @@
         <v>136</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="138" ht="21" spans="2:3">
@@ -3887,7 +3887,7 @@
         <v>138</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="140" ht="21" spans="1:3">
@@ -3898,7 +3898,7 @@
         <v>139</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="141" ht="21" spans="1:3">
@@ -3909,7 +3909,7 @@
         <v>140</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="142" ht="21" spans="1:3">
@@ -3920,7 +3920,7 @@
         <v>141</v>
       </c>
       <c r="C142" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="143" ht="21" spans="1:3">
@@ -3931,7 +3931,7 @@
         <v>142</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="144" ht="21" spans="1:3">
@@ -3942,7 +3942,7 @@
         <v>143</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="145" ht="21" spans="1:3">
@@ -3953,7 +3953,7 @@
         <v>144</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="146" ht="21" spans="1:3">
@@ -3964,7 +3964,7 @@
         <v>145</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="147" ht="21" spans="1:3">
@@ -3975,7 +3975,7 @@
         <v>146</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="148" ht="21" spans="1:3">
@@ -3986,7 +3986,7 @@
         <v>147</v>
       </c>
       <c r="C148" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="149" ht="21" spans="1:3">
@@ -3997,7 +3997,7 @@
         <v>148</v>
       </c>
       <c r="C149" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="150" ht="21" spans="1:3">
@@ -4008,7 +4008,7 @@
         <v>149</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="151" ht="21" spans="1:3">
@@ -4019,7 +4019,7 @@
         <v>150</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="152" ht="21" spans="1:3">
@@ -4030,7 +4030,7 @@
         <v>151</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="153" ht="21" spans="1:3">
@@ -4041,7 +4041,7 @@
         <v>152</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="154" ht="21" spans="1:3">
@@ -4052,7 +4052,7 @@
         <v>153</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="155" ht="21" spans="1:3">
@@ -4063,7 +4063,7 @@
         <v>154</v>
       </c>
       <c r="C155" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="156" ht="21" spans="1:3">
@@ -4074,7 +4074,7 @@
         <v>155</v>
       </c>
       <c r="C156" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="157" ht="21" spans="1:3">
@@ -4085,7 +4085,7 @@
         <v>156</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="158" ht="21" spans="1:3">
@@ -4096,7 +4096,7 @@
         <v>157</v>
       </c>
       <c r="C158" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="159" ht="21" spans="1:3">
@@ -4107,7 +4107,7 @@
         <v>158</v>
       </c>
       <c r="C159" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="160" ht="21" spans="1:3">
@@ -4118,7 +4118,7 @@
         <v>159</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="161" ht="21" spans="1:3">
@@ -4129,7 +4129,7 @@
         <v>160</v>
       </c>
       <c r="C161" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="162" ht="21" spans="1:3">
@@ -4140,7 +4140,7 @@
         <v>161</v>
       </c>
       <c r="C162" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="163" ht="21" spans="1:3">
@@ -4151,7 +4151,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="164" ht="21" spans="1:3">
@@ -4162,7 +4162,7 @@
         <v>163</v>
       </c>
       <c r="C164" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="165" ht="21" spans="1:3">
@@ -4173,7 +4173,7 @@
         <v>164</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="166" ht="21" spans="1:3">
@@ -4184,7 +4184,7 @@
         <v>165</v>
       </c>
       <c r="C166" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="167" ht="21" spans="1:3">
@@ -4195,7 +4195,7 @@
         <v>166</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="168" ht="21" spans="1:3">
@@ -4206,7 +4206,7 @@
         <v>167</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="169" ht="21" spans="1:3">
@@ -4217,7 +4217,7 @@
         <v>168</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="170" ht="21" spans="1:3">
@@ -4228,7 +4228,7 @@
         <v>169</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="171" ht="21" spans="1:3">
@@ -4239,7 +4239,7 @@
         <v>170</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="172" ht="21" spans="1:3">
@@ -4250,7 +4250,7 @@
         <v>171</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="173" ht="21" spans="1:3">
@@ -4261,7 +4261,7 @@
         <v>172</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="174" ht="21" spans="1:3">
@@ -4272,7 +4272,7 @@
         <v>173</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="176" ht="21" spans="2:3">
@@ -4463,7 +4463,7 @@
         <v>191</v>
       </c>
       <c r="C193" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="194" ht="21" spans="1:3">
@@ -4507,7 +4507,7 @@
         <v>196</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="198" ht="21" spans="1:3">
@@ -4518,7 +4518,7 @@
         <v>197</v>
       </c>
       <c r="C198" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="199" ht="21" spans="1:3">
@@ -4529,7 +4529,7 @@
         <v>198</v>
       </c>
       <c r="C199" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="200" ht="21" spans="1:3">
@@ -4540,7 +4540,7 @@
         <v>199</v>
       </c>
       <c r="C200" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="201" ht="21" spans="1:3">
@@ -4551,7 +4551,7 @@
         <v>200</v>
       </c>
       <c r="C201" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="202" ht="21" spans="1:3">
@@ -4562,7 +4562,7 @@
         <v>201</v>
       </c>
       <c r="C202" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="203" ht="21" spans="1:3">
@@ -4573,7 +4573,7 @@
         <v>202</v>
       </c>
       <c r="C203" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="204" ht="21" spans="1:3">
@@ -4584,7 +4584,7 @@
         <v>203</v>
       </c>
       <c r="C204" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="205" ht="21" spans="1:3">
@@ -4595,7 +4595,7 @@
         <v>204</v>
       </c>
       <c r="C205" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="206" ht="21" spans="1:3">
@@ -4606,7 +4606,7 @@
         <v>205</v>
       </c>
       <c r="C206" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="207" ht="21" spans="1:3">
@@ -4617,7 +4617,7 @@
         <v>206</v>
       </c>
       <c r="C207" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="208" ht="21" spans="1:3">
@@ -4628,7 +4628,7 @@
         <v>207</v>
       </c>
       <c r="C208" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="209" ht="21" spans="1:3">
@@ -4639,7 +4639,7 @@
         <v>208</v>
       </c>
       <c r="C209" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="210" ht="21" spans="1:3">
@@ -4650,7 +4650,7 @@
         <v>209</v>
       </c>
       <c r="C210" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="211" ht="21" spans="1:3">
@@ -4661,7 +4661,7 @@
         <v>210</v>
       </c>
       <c r="C211" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="212" ht="21" spans="1:3">
@@ -4682,7 +4682,7 @@
         <v>212</v>
       </c>
       <c r="C214" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="215" ht="21" spans="1:3">
@@ -4693,7 +4693,7 @@
         <v>213</v>
       </c>
       <c r="C215" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="216" ht="21" spans="1:3">
@@ -4704,7 +4704,7 @@
         <v>214</v>
       </c>
       <c r="C216" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="217" ht="21" spans="1:3">
@@ -4715,7 +4715,7 @@
         <v>215</v>
       </c>
       <c r="C217" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="218" ht="21" spans="1:3">
@@ -4726,7 +4726,7 @@
         <v>216</v>
       </c>
       <c r="C218" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="219" ht="21" spans="1:3">
@@ -4737,7 +4737,7 @@
         <v>217</v>
       </c>
       <c r="C219" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="220" ht="21" spans="1:3">
@@ -4748,7 +4748,7 @@
         <v>218</v>
       </c>
       <c r="C220" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="221" ht="21" spans="1:3">
@@ -4759,7 +4759,7 @@
         <v>219</v>
       </c>
       <c r="C221" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="222" ht="21" spans="1:3">
@@ -4770,7 +4770,7 @@
         <v>220</v>
       </c>
       <c r="C222" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="223" ht="21" spans="1:3">
@@ -4781,7 +4781,7 @@
         <v>221</v>
       </c>
       <c r="C223" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="224" ht="21" spans="1:3">
@@ -4792,7 +4792,7 @@
         <v>222</v>
       </c>
       <c r="C224" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="225" ht="21" spans="1:3">
@@ -4803,7 +4803,7 @@
         <v>223</v>
       </c>
       <c r="C225" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="226" ht="21" spans="1:3">
@@ -4814,7 +4814,7 @@
         <v>224</v>
       </c>
       <c r="C226" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="227" ht="21" spans="1:3">
@@ -4825,7 +4825,7 @@
         <v>225</v>
       </c>
       <c r="C227" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="228" ht="21" spans="1:3">
@@ -4836,7 +4836,7 @@
         <v>226</v>
       </c>
       <c r="C228" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="229" ht="21" spans="1:3">
@@ -4847,7 +4847,7 @@
         <v>227</v>
       </c>
       <c r="C229" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="230" ht="21" spans="1:3">
@@ -4858,7 +4858,7 @@
         <v>228</v>
       </c>
       <c r="C230" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="231" ht="21" spans="1:3">
@@ -4869,7 +4869,7 @@
         <v>229</v>
       </c>
       <c r="C231" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="232" ht="21" spans="1:3">
@@ -4880,7 +4880,7 @@
         <v>230</v>
       </c>
       <c r="C232" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="233" ht="21" spans="1:3">
@@ -4891,7 +4891,7 @@
         <v>231</v>
       </c>
       <c r="C233" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="234" ht="21" spans="1:3">
@@ -4902,7 +4902,7 @@
         <v>232</v>
       </c>
       <c r="C234" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="235" ht="21" spans="1:3">
@@ -4913,7 +4913,7 @@
         <v>233</v>
       </c>
       <c r="C235" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="236" ht="21" spans="2:3">
@@ -4932,7 +4932,7 @@
         <v>235</v>
       </c>
       <c r="C238" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="239" ht="21" spans="1:3">
@@ -4943,7 +4943,7 @@
         <v>236</v>
       </c>
       <c r="C239" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="240" ht="21" spans="1:3">
@@ -4954,7 +4954,7 @@
         <v>237</v>
       </c>
       <c r="C240" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="241" ht="21" spans="1:3">
@@ -4965,7 +4965,7 @@
         <v>238</v>
       </c>
       <c r="C241" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="242" ht="21" spans="1:3">
@@ -4987,7 +4987,7 @@
         <v>241</v>
       </c>
       <c r="C243" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="244" ht="21" spans="1:3">
@@ -4998,7 +4998,7 @@
         <v>242</v>
       </c>
       <c r="C244" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="245" ht="21" spans="1:3">
@@ -5009,7 +5009,7 @@
         <v>243</v>
       </c>
       <c r="C245" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="246" ht="21" spans="1:3">
@@ -5020,7 +5020,7 @@
         <v>244</v>
       </c>
       <c r="C246" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="247" ht="21" spans="1:3">
@@ -5031,7 +5031,7 @@
         <v>245</v>
       </c>
       <c r="C247" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="248" ht="21" spans="1:3">
@@ -5042,7 +5042,7 @@
         <v>246</v>
       </c>
       <c r="C248" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="249" ht="21" spans="1:3">
@@ -5053,7 +5053,7 @@
         <v>247</v>
       </c>
       <c r="C249" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="250" ht="21" spans="1:3">
@@ -5064,7 +5064,7 @@
         <v>248</v>
       </c>
       <c r="C250" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="251" ht="21" spans="1:3">
@@ -5075,7 +5075,7 @@
         <v>249</v>
       </c>
       <c r="C251" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="252" ht="21" spans="1:3">
@@ -5086,7 +5086,7 @@
         <v>250</v>
       </c>
       <c r="C252" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="253" ht="21" spans="1:3">
@@ -5097,7 +5097,7 @@
         <v>251</v>
       </c>
       <c r="C253" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="254" ht="21" spans="1:3">
@@ -5108,7 +5108,7 @@
         <v>252</v>
       </c>
       <c r="C254" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="255" ht="21" spans="1:3">
@@ -5119,7 +5119,7 @@
         <v>253</v>
       </c>
       <c r="C255" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="256" ht="21" spans="1:3">
@@ -5130,7 +5130,7 @@
         <v>254</v>
       </c>
       <c r="C256" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="257" ht="21" spans="1:3">
@@ -5141,7 +5141,7 @@
         <v>255</v>
       </c>
       <c r="C257" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="258" ht="21" spans="1:3">
@@ -5152,7 +5152,7 @@
         <v>256</v>
       </c>
       <c r="C258" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="259" ht="21" spans="1:3">
@@ -5163,7 +5163,7 @@
         <v>257</v>
       </c>
       <c r="C259" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="260" ht="21" spans="1:3">
@@ -5174,7 +5174,7 @@
         <v>258</v>
       </c>
       <c r="C260" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="261" ht="21" spans="1:3">
@@ -5185,7 +5185,7 @@
         <v>259</v>
       </c>
       <c r="C261" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="262" ht="21" spans="1:3">
@@ -5196,7 +5196,7 @@
         <v>260</v>
       </c>
       <c r="C262" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="263" ht="21" spans="1:3">
@@ -5207,7 +5207,7 @@
         <v>261</v>
       </c>
       <c r="C263" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="264" ht="21" spans="1:3">
@@ -5218,7 +5218,7 @@
         <v>262</v>
       </c>
       <c r="C264" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="265" ht="21" spans="1:3">
@@ -5229,7 +5229,7 @@
         <v>263</v>
       </c>
       <c r="C265" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="266" ht="21" spans="1:3">
@@ -5240,7 +5240,7 @@
         <v>264</v>
       </c>
       <c r="C266" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="267" ht="21" spans="1:3">
@@ -5251,7 +5251,7 @@
         <v>265</v>
       </c>
       <c r="C267" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="268" ht="21" spans="1:3">
@@ -5262,7 +5262,7 @@
         <v>266</v>
       </c>
       <c r="C268" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="269" ht="21" spans="1:3">
@@ -5273,7 +5273,7 @@
         <v>267</v>
       </c>
       <c r="C269" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="270" ht="21" spans="1:3">
@@ -5284,7 +5284,7 @@
         <v>268</v>
       </c>
       <c r="C270" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="271" ht="21" spans="1:3">
@@ -5295,7 +5295,7 @@
         <v>90</v>
       </c>
       <c r="C271" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="272" ht="21" spans="1:3">
@@ -5306,7 +5306,7 @@
         <v>269</v>
       </c>
       <c r="C272" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="273" ht="21" spans="2:3">
@@ -5325,7 +5325,7 @@
         <v>271</v>
       </c>
       <c r="C275" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="276" ht="21" spans="1:3">
@@ -5336,7 +5336,7 @@
         <v>272</v>
       </c>
       <c r="C276" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="277" ht="21" spans="1:3">
@@ -5347,7 +5347,7 @@
         <v>273</v>
       </c>
       <c r="C277" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="278" ht="21" spans="1:3">
@@ -5358,7 +5358,7 @@
         <v>274</v>
       </c>
       <c r="C278" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="279" ht="21" spans="1:3">
@@ -5369,7 +5369,7 @@
         <v>275</v>
       </c>
       <c r="C279" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="280" ht="21" spans="1:3">
@@ -5380,7 +5380,7 @@
         <v>276</v>
       </c>
       <c r="C280" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="281" ht="21" spans="1:3">
@@ -5391,7 +5391,7 @@
         <v>277</v>
       </c>
       <c r="C281" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="282" ht="21" spans="1:3">
@@ -5402,7 +5402,7 @@
         <v>278</v>
       </c>
       <c r="C282" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="283" ht="21" spans="1:3">
@@ -5413,7 +5413,7 @@
         <v>279</v>
       </c>
       <c r="C283" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="284" ht="21" spans="1:3">
@@ -5424,7 +5424,7 @@
         <v>280</v>
       </c>
       <c r="C284" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="285" ht="21" spans="1:3">
@@ -5435,7 +5435,7 @@
         <v>281</v>
       </c>
       <c r="C285" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="286" ht="21" spans="1:3">
@@ -5446,7 +5446,7 @@
         <v>282</v>
       </c>
       <c r="C286" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="287" ht="21" spans="1:3">
@@ -5457,7 +5457,7 @@
         <v>283</v>
       </c>
       <c r="C287" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="288" ht="21" spans="1:3">
@@ -5468,7 +5468,7 @@
         <v>284</v>
       </c>
       <c r="C288" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="289" ht="21" spans="1:3">
@@ -5479,7 +5479,7 @@
         <v>285</v>
       </c>
       <c r="C289" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="290" ht="21" spans="1:3">
@@ -5490,7 +5490,7 @@
         <v>286</v>
       </c>
       <c r="C290" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="291" ht="21" spans="1:3">
@@ -5501,7 +5501,7 @@
         <v>287</v>
       </c>
       <c r="C291" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="292" ht="21" spans="1:3">
@@ -5512,7 +5512,7 @@
         <v>288</v>
       </c>
       <c r="C292" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="293" ht="21" spans="1:3">
@@ -5523,7 +5523,7 @@
         <v>289</v>
       </c>
       <c r="C293" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="294" ht="21" spans="2:3">
@@ -5542,7 +5542,7 @@
         <v>291</v>
       </c>
       <c r="C296" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="297" ht="21" spans="1:3">
@@ -5553,7 +5553,7 @@
         <v>292</v>
       </c>
       <c r="C297" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="298" ht="21" spans="1:3">
@@ -5564,7 +5564,7 @@
         <v>293</v>
       </c>
       <c r="C298" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="299" ht="21" spans="1:3">
@@ -5575,7 +5575,7 @@
         <v>294</v>
       </c>
       <c r="C299" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="300" ht="21" spans="1:3">
@@ -5586,7 +5586,7 @@
         <v>295</v>
       </c>
       <c r="C300" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="301" ht="21" spans="1:3">
@@ -5597,7 +5597,7 @@
         <v>296</v>
       </c>
       <c r="C301" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="302" ht="21" spans="1:3">
@@ -5608,7 +5608,7 @@
         <v>297</v>
       </c>
       <c r="C302" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="303" ht="21" spans="1:3">
@@ -5619,7 +5619,7 @@
         <v>298</v>
       </c>
       <c r="C303" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="304" ht="21" spans="1:3">
@@ -5630,7 +5630,7 @@
         <v>299</v>
       </c>
       <c r="C304" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="305" ht="21" spans="1:3">
@@ -5641,7 +5641,7 @@
         <v>300</v>
       </c>
       <c r="C305" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="306" ht="21" spans="1:3">
@@ -5652,7 +5652,7 @@
         <v>301</v>
       </c>
       <c r="C306" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="307" ht="21" spans="1:3">
@@ -5663,7 +5663,7 @@
         <v>302</v>
       </c>
       <c r="C307" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="308" ht="21" spans="1:3">
@@ -5674,7 +5674,7 @@
         <v>303</v>
       </c>
       <c r="C308" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="309" ht="21" spans="1:3">
@@ -5685,7 +5685,7 @@
         <v>304</v>
       </c>
       <c r="C309" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="310" ht="21" spans="1:3">
@@ -5696,7 +5696,7 @@
         <v>305</v>
       </c>
       <c r="C310" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="311" ht="21" spans="1:3">
@@ -5707,7 +5707,7 @@
         <v>306</v>
       </c>
       <c r="C311" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="312" ht="21" spans="1:3">
@@ -5718,7 +5718,7 @@
         <v>307</v>
       </c>
       <c r="C312" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="313" ht="21" spans="1:3">
@@ -5729,7 +5729,7 @@
         <v>308</v>
       </c>
       <c r="C313" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="314" ht="21" spans="1:3">
@@ -5740,7 +5740,7 @@
         <v>309</v>
       </c>
       <c r="C314" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="315" ht="21" spans="1:3">
@@ -5751,7 +5751,7 @@
         <v>310</v>
       </c>
       <c r="C315" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="316" ht="21" spans="1:3">
@@ -5762,7 +5762,7 @@
         <v>311</v>
       </c>
       <c r="C316" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="317" ht="21" spans="1:3">
@@ -5773,7 +5773,7 @@
         <v>312</v>
       </c>
       <c r="C317" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="318" ht="21" spans="1:3">
@@ -5784,7 +5784,7 @@
         <v>313</v>
       </c>
       <c r="C318" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="319" ht="21" spans="1:3">
@@ -5795,7 +5795,7 @@
         <v>314</v>
       </c>
       <c r="C319" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="320" ht="21" spans="1:3">
@@ -5806,7 +5806,7 @@
         <v>315</v>
       </c>
       <c r="C320" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="321" ht="21" spans="1:3">
@@ -5817,7 +5817,7 @@
         <v>316</v>
       </c>
       <c r="C321" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="322" ht="21" spans="1:3">
@@ -5828,7 +5828,7 @@
         <v>317</v>
       </c>
       <c r="C322" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="323" ht="21" spans="1:3">
@@ -5839,7 +5839,7 @@
         <v>318</v>
       </c>
       <c r="C323" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="324" ht="21" spans="1:3">
@@ -5850,7 +5850,7 @@
         <v>319</v>
       </c>
       <c r="C324" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="325" ht="21" spans="1:3">
@@ -5861,7 +5861,7 @@
         <v>320</v>
       </c>
       <c r="C325" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="326" ht="21" spans="1:3">
@@ -5872,7 +5872,7 @@
         <v>321</v>
       </c>
       <c r="C326" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="327" ht="21" spans="1:3">
@@ -5883,7 +5883,7 @@
         <v>322</v>
       </c>
       <c r="C327" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="328" ht="21" spans="1:3">
@@ -5894,7 +5894,7 @@
         <v>323</v>
       </c>
       <c r="C328" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="329" ht="21" spans="1:3">
@@ -5905,7 +5905,7 @@
         <v>324</v>
       </c>
       <c r="C329" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="330" ht="21" spans="1:3">
@@ -5916,7 +5916,7 @@
         <v>325</v>
       </c>
       <c r="C330" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="331" ht="21" spans="1:3">
@@ -5927,7 +5927,7 @@
         <v>326</v>
       </c>
       <c r="C331" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="332" ht="21" spans="1:3">
@@ -5938,7 +5938,7 @@
         <v>327</v>
       </c>
       <c r="C332" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="333" ht="21" spans="1:3">
@@ -5949,7 +5949,7 @@
         <v>328</v>
       </c>
       <c r="C333" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="334" ht="21" spans="2:3">
@@ -5968,7 +5968,7 @@
         <v>330</v>
       </c>
       <c r="C336" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="337" ht="21" spans="1:3">
@@ -5979,7 +5979,7 @@
         <v>331</v>
       </c>
       <c r="C337" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="338" ht="21" spans="1:3">
@@ -5990,7 +5990,7 @@
         <v>332</v>
       </c>
       <c r="C338" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="339" ht="21" spans="1:3">
@@ -6001,7 +6001,7 @@
         <v>333</v>
       </c>
       <c r="C339" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="340" ht="21" spans="1:3">
@@ -6012,7 +6012,7 @@
         <v>334</v>
       </c>
       <c r="C340" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="341" ht="21" spans="1:3">
@@ -6023,7 +6023,7 @@
         <v>335</v>
       </c>
       <c r="C341" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="342" ht="21" spans="1:3">
@@ -6034,7 +6034,7 @@
         <v>336</v>
       </c>
       <c r="C342" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="343" ht="21" spans="1:3">
@@ -6045,7 +6045,7 @@
         <v>337</v>
       </c>
       <c r="C343" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="344" ht="21" spans="1:3">
@@ -6056,7 +6056,7 @@
         <v>338</v>
       </c>
       <c r="C344" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="345" ht="21" spans="1:3">
@@ -6067,7 +6067,7 @@
         <v>339</v>
       </c>
       <c r="C345" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="346" ht="21" spans="1:3">
@@ -6078,7 +6078,7 @@
         <v>340</v>
       </c>
       <c r="C346" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="347" ht="21" spans="1:3">
@@ -6089,7 +6089,7 @@
         <v>341</v>
       </c>
       <c r="C347" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="348" ht="21" spans="1:3">
@@ -6100,7 +6100,7 @@
         <v>342</v>
       </c>
       <c r="C348" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="349" ht="21" spans="1:3">
@@ -6111,7 +6111,7 @@
         <v>343</v>
       </c>
       <c r="C349" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="350" ht="21" spans="1:3">
@@ -6122,7 +6122,7 @@
         <v>344</v>
       </c>
       <c r="C350" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="351" ht="21" spans="1:3">
@@ -6133,7 +6133,7 @@
         <v>345</v>
       </c>
       <c r="C351" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="352" ht="21" spans="1:3">
@@ -6144,7 +6144,7 @@
         <v>346</v>
       </c>
       <c r="C352" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="353" ht="21" spans="1:3">
@@ -6155,7 +6155,7 @@
         <v>347</v>
       </c>
       <c r="C353" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="354" ht="21" spans="2:3">
@@ -6174,7 +6174,7 @@
         <v>349</v>
       </c>
       <c r="C356" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="357" ht="21" spans="1:3">
@@ -6251,7 +6251,7 @@
         <v>356</v>
       </c>
       <c r="C363" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="364" ht="21" spans="1:3">
@@ -6262,7 +6262,7 @@
         <v>357</v>
       </c>
       <c r="C364" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="365" ht="21" spans="1:3">
@@ -6273,7 +6273,7 @@
         <v>358</v>
       </c>
       <c r="C365" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="366" ht="21" spans="1:3">
@@ -6284,7 +6284,7 @@
         <v>359</v>
       </c>
       <c r="C366" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="367" ht="21" spans="1:3">
@@ -6295,7 +6295,7 @@
         <v>360</v>
       </c>
       <c r="C367" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="368" ht="21" spans="1:3">
@@ -6306,7 +6306,7 @@
         <v>361</v>
       </c>
       <c r="C368" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="369" ht="21" spans="1:3">
@@ -6317,7 +6317,7 @@
         <v>362</v>
       </c>
       <c r="C369" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="370" ht="21" spans="1:3">
@@ -6328,7 +6328,7 @@
         <v>363</v>
       </c>
       <c r="C370" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="371" ht="21" spans="1:3">
@@ -6339,7 +6339,7 @@
         <v>364</v>
       </c>
       <c r="C371" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="372" ht="21" spans="1:3">
@@ -6350,7 +6350,7 @@
         <v>365</v>
       </c>
       <c r="C372" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="373" ht="21" spans="1:3">
@@ -6361,7 +6361,7 @@
         <v>366</v>
       </c>
       <c r="C373" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="374" ht="21" spans="1:3">
@@ -6372,7 +6372,7 @@
         <v>367</v>
       </c>
       <c r="C374" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="375" ht="21" spans="1:3">
@@ -6383,7 +6383,7 @@
         <v>368</v>
       </c>
       <c r="C375" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="376" ht="21" spans="1:3">
@@ -6394,7 +6394,7 @@
         <v>369</v>
       </c>
       <c r="C376" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="377" ht="21" spans="1:3">
@@ -6405,7 +6405,7 @@
         <v>370</v>
       </c>
       <c r="C377" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="378" ht="21" spans="1:3">
@@ -6416,7 +6416,7 @@
         <v>371</v>
       </c>
       <c r="C378" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="379" ht="21" spans="1:3">
@@ -6427,7 +6427,7 @@
         <v>372</v>
       </c>
       <c r="C379" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="380" ht="21" spans="1:3">
@@ -6438,7 +6438,7 @@
         <v>373</v>
       </c>
       <c r="C380" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="381" ht="21" spans="1:3">
@@ -6449,7 +6449,7 @@
         <v>374</v>
       </c>
       <c r="C381" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="382" ht="21" spans="1:3">
@@ -6460,7 +6460,7 @@
         <v>375</v>
       </c>
       <c r="C382" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="383" ht="21" spans="1:3">
@@ -6471,7 +6471,7 @@
         <v>376</v>
       </c>
       <c r="C383" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="384" ht="21" spans="1:3">
@@ -6482,7 +6482,7 @@
         <v>377</v>
       </c>
       <c r="C384" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="385" ht="21" spans="1:3">
@@ -6493,7 +6493,7 @@
         <v>378</v>
       </c>
       <c r="C385" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="386" ht="21" spans="1:3">
@@ -6504,7 +6504,7 @@
         <v>379</v>
       </c>
       <c r="C386" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="387" ht="21" spans="1:3">
@@ -6515,7 +6515,7 @@
         <v>380</v>
       </c>
       <c r="C387" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="388" ht="21" spans="1:3">
@@ -6526,7 +6526,7 @@
         <v>381</v>
       </c>
       <c r="C388" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="389" ht="21" spans="1:3">
@@ -6537,7 +6537,7 @@
         <v>382</v>
       </c>
       <c r="C389" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="390" ht="21" spans="1:3">
@@ -6548,7 +6548,7 @@
         <v>382</v>
       </c>
       <c r="C390" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="391" ht="21" spans="1:3">
@@ -6559,7 +6559,7 @@
         <v>383</v>
       </c>
       <c r="C391" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="392" ht="21" spans="1:3">
@@ -6570,7 +6570,7 @@
         <v>384</v>
       </c>
       <c r="C392" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="393" ht="21" spans="1:3">
@@ -6581,7 +6581,7 @@
         <v>385</v>
       </c>
       <c r="C393" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="394" ht="21" spans="1:3">
@@ -6592,7 +6592,7 @@
         <v>386</v>
       </c>
       <c r="C394" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="395" ht="21" spans="1:3">
@@ -6603,7 +6603,7 @@
         <v>387</v>
       </c>
       <c r="C395" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="396" ht="21" spans="1:3">
@@ -6614,7 +6614,7 @@
         <v>388</v>
       </c>
       <c r="C396" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="397" ht="21" spans="1:3">
@@ -6625,7 +6625,7 @@
         <v>389</v>
       </c>
       <c r="C397" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="398" ht="21" spans="1:3">
@@ -6636,7 +6636,7 @@
         <v>390</v>
       </c>
       <c r="C398" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="399" ht="21" spans="1:3">
@@ -6647,7 +6647,7 @@
         <v>391</v>
       </c>
       <c r="C399" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="400" ht="21" spans="2:3">
@@ -6666,7 +6666,7 @@
         <v>393</v>
       </c>
       <c r="C402" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="403" ht="21" spans="1:3">
@@ -6677,7 +6677,7 @@
         <v>394</v>
       </c>
       <c r="C403" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="404" ht="21" spans="1:3">
@@ -6688,7 +6688,7 @@
         <v>395</v>
       </c>
       <c r="C404" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="405" ht="21" spans="1:3">
@@ -6699,7 +6699,7 @@
         <v>92</v>
       </c>
       <c r="C405" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="406" ht="21" spans="1:3">
@@ -6710,7 +6710,7 @@
         <v>396</v>
       </c>
       <c r="C406" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="407" ht="21" spans="1:3">
@@ -6721,7 +6721,7 @@
         <v>397</v>
       </c>
       <c r="C407" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="408" ht="21" spans="2:3">
@@ -6817,7 +6817,7 @@
         <v>278</v>
       </c>
       <c r="C417" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="418" ht="21" spans="1:3">
@@ -6828,7 +6828,7 @@
         <v>406</v>
       </c>
       <c r="C418" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="419" ht="21" spans="1:3">
@@ -6839,7 +6839,7 @@
         <v>407</v>
       </c>
       <c r="C419" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="420" ht="21" spans="1:3">
@@ -6850,7 +6850,7 @@
         <v>408</v>
       </c>
       <c r="C420" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="421" ht="21" spans="1:3">
@@ -6861,7 +6861,7 @@
         <v>409</v>
       </c>
       <c r="C421" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="422" ht="21" spans="1:3">
@@ -6872,7 +6872,7 @@
         <v>410</v>
       </c>
       <c r="C422" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="423" ht="21" spans="1:3">
@@ -6883,7 +6883,7 @@
         <v>411</v>
       </c>
       <c r="C423" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="424" ht="21" spans="1:3">
@@ -6894,7 +6894,7 @@
         <v>412</v>
       </c>
       <c r="C424" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="425" ht="21" spans="1:3">
@@ -6905,7 +6905,7 @@
         <v>413</v>
       </c>
       <c r="C425" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="426" ht="21" spans="1:3">
@@ -6916,7 +6916,7 @@
         <v>414</v>
       </c>
       <c r="C426" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="427" ht="21" spans="1:3">
@@ -6927,7 +6927,7 @@
         <v>415</v>
       </c>
       <c r="C427" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="428" ht="21" spans="1:3">
@@ -6938,7 +6938,7 @@
         <v>416</v>
       </c>
       <c r="C428" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="429" ht="21" spans="1:3">
@@ -6949,7 +6949,7 @@
         <v>417</v>
       </c>
       <c r="C429" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="430" ht="21" spans="1:3">
@@ -6960,7 +6960,7 @@
         <v>418</v>
       </c>
       <c r="C430" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="431" ht="21" spans="1:3">
@@ -6971,7 +6971,7 @@
         <v>419</v>
       </c>
       <c r="C431" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="432" ht="21" spans="1:3">
@@ -6982,7 +6982,7 @@
         <v>420</v>
       </c>
       <c r="C432" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="433" ht="21" spans="1:3">
@@ -6993,7 +6993,7 @@
         <v>421</v>
       </c>
       <c r="C433" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="434" ht="21" spans="1:3">
@@ -7004,7 +7004,7 @@
         <v>422</v>
       </c>
       <c r="C434" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="435" ht="21" spans="1:3">
@@ -7015,7 +7015,7 @@
         <v>423</v>
       </c>
       <c r="C435" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="436" ht="21" spans="1:3">
@@ -7026,7 +7026,7 @@
         <v>424</v>
       </c>
       <c r="C436" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="437" ht="21" spans="1:3">
@@ -7037,7 +7037,7 @@
         <v>425</v>
       </c>
       <c r="C437" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="438" ht="21" spans="1:3">
@@ -7048,7 +7048,7 @@
         <v>17</v>
       </c>
       <c r="C438" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="439" ht="21" spans="1:3">
@@ -7059,7 +7059,7 @@
         <v>426</v>
       </c>
       <c r="C439" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="440" ht="21" spans="1:3">
@@ -7070,7 +7070,7 @@
         <v>427</v>
       </c>
       <c r="C440" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="441" ht="21" spans="1:3">
@@ -7081,7 +7081,7 @@
         <v>428</v>
       </c>
       <c r="C441" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="442" ht="21" spans="1:3">
@@ -7092,7 +7092,7 @@
         <v>429</v>
       </c>
       <c r="C442" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="443" ht="21" spans="1:3">
@@ -7103,7 +7103,7 @@
         <v>430</v>
       </c>
       <c r="C443" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="444" ht="21" spans="1:3">
@@ -7114,7 +7114,7 @@
         <v>431</v>
       </c>
       <c r="C444" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="445" ht="21" spans="1:3">
@@ -7125,7 +7125,7 @@
         <v>432</v>
       </c>
       <c r="C445" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="446" ht="21" spans="1:3">
@@ -7136,7 +7136,7 @@
         <v>433</v>
       </c>
       <c r="C446" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="447" ht="21" spans="1:3">
@@ -7147,7 +7147,7 @@
         <v>434</v>
       </c>
       <c r="C447" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="448" ht="21" spans="1:3">
@@ -7158,7 +7158,7 @@
         <v>435</v>
       </c>
       <c r="C448" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="449" ht="21" spans="1:3">
@@ -7169,7 +7169,7 @@
         <v>436</v>
       </c>
       <c r="C449" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="450" ht="21" spans="1:3">
@@ -7180,7 +7180,7 @@
         <v>437</v>
       </c>
       <c r="C450" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="451" ht="21" spans="1:3">
@@ -7191,7 +7191,7 @@
         <v>438</v>
       </c>
       <c r="C451" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="452" ht="21" spans="1:3">
@@ -7202,7 +7202,7 @@
         <v>439</v>
       </c>
       <c r="C452" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="453" ht="21" spans="1:3">
@@ -7213,7 +7213,7 @@
         <v>440</v>
       </c>
       <c r="C453" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="454" ht="21" spans="1:3">
@@ -7224,7 +7224,7 @@
         <v>441</v>
       </c>
       <c r="C454" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="455" ht="21" spans="1:3">
@@ -7235,7 +7235,7 @@
         <v>442</v>
       </c>
       <c r="C455" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="456" ht="21" spans="1:3">
@@ -7246,7 +7246,7 @@
         <v>443</v>
       </c>
       <c r="C456" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="457" ht="21" spans="1:3">
@@ -7257,7 +7257,7 @@
         <v>444</v>
       </c>
       <c r="C457" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="458" ht="21" spans="1:3">
@@ -7268,7 +7268,7 @@
         <v>445</v>
       </c>
       <c r="C458" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="459" ht="21" spans="1:3">
@@ -7279,7 +7279,7 @@
         <v>446</v>
       </c>
       <c r="C459" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="460" ht="21" spans="1:3">
@@ -7290,7 +7290,7 @@
         <v>447</v>
       </c>
       <c r="C460" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="461" ht="21" spans="1:3">
@@ -7301,7 +7301,7 @@
         <v>448</v>
       </c>
       <c r="C461" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="462" ht="21" spans="1:3">
@@ -7312,7 +7312,7 @@
         <v>449</v>
       </c>
       <c r="C462" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="463" ht="21" spans="1:3">
@@ -7323,7 +7323,7 @@
         <v>450</v>
       </c>
       <c r="C463" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="464" ht="21" spans="1:3">
@@ -7334,7 +7334,7 @@
         <v>451</v>
       </c>
       <c r="C464" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="465" ht="21" spans="1:3">
@@ -7345,7 +7345,7 @@
         <v>452</v>
       </c>
       <c r="C465" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="466" ht="21" spans="1:3">
@@ -7356,7 +7356,7 @@
         <v>453</v>
       </c>
       <c r="C466" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="467" ht="21" spans="1:3">
@@ -7367,7 +7367,7 @@
         <v>454</v>
       </c>
       <c r="C467" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="468" ht="21" spans="1:3">
@@ -7378,7 +7378,7 @@
         <v>455</v>
       </c>
       <c r="C468" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="469" ht="21" spans="1:3">
@@ -7389,7 +7389,7 @@
         <v>456</v>
       </c>
       <c r="C469" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="470" ht="21" spans="2:3">
@@ -7409,7 +7409,7 @@
         <v>458</v>
       </c>
       <c r="C472" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="473" ht="21" spans="1:3">
@@ -7420,7 +7420,7 @@
         <v>459</v>
       </c>
       <c r="C473" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="474" ht="21" spans="1:3">
@@ -7431,7 +7431,7 @@
         <v>460</v>
       </c>
       <c r="C474" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="475" ht="21" spans="1:3">
@@ -7442,7 +7442,7 @@
         <v>461</v>
       </c>
       <c r="C475" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="476" ht="21" spans="1:3">
@@ -7453,7 +7453,7 @@
         <v>462</v>
       </c>
       <c r="C476" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="477" ht="21" spans="1:3">
@@ -7464,7 +7464,7 @@
         <v>463</v>
       </c>
       <c r="C477" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="478" ht="21" spans="1:3">
@@ -7475,7 +7475,7 @@
         <v>464</v>
       </c>
       <c r="C478" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="479" ht="21" spans="1:3">
@@ -7486,7 +7486,7 @@
         <v>465</v>
       </c>
       <c r="C479" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="480" ht="21" spans="1:3">
@@ -7497,7 +7497,7 @@
         <v>466</v>
       </c>
       <c r="C480" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="481" ht="21" spans="1:3">
@@ -7508,7 +7508,7 @@
         <v>467</v>
       </c>
       <c r="C481" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Best time to buy and sell stock leetcode
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8892"/>
+    <workbookView windowWidth="23040" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -91,10 +91,10 @@
     <t>Best time to buy and Sell stock</t>
   </si>
   <si>
+    <t>find all pairs on integer array whose sum is equal to given number</t>
+  </si>
+  <si>
     <t>&lt;-&gt;</t>
-  </si>
-  <si>
-    <t>find all pairs on integer array whose sum is equal to given number</t>
   </si>
   <si>
     <t>find common elements In 3 sorted arrays</t>
@@ -1425,9 +1425,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
@@ -1502,14 +1502,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1518,14 +1510,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1539,22 +1524,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1568,8 +1538,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1588,6 +1559,20 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1615,16 +1600,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1639,7 +1624,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1660,97 +1660,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1762,7 +1672,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1780,7 +1690,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1792,7 +1720,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1804,19 +1744,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1828,13 +1774,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1848,22 +1848,47 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1892,21 +1917,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1916,178 +1926,168 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2441,7 +2441,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2660,8 +2660,8 @@
       <c r="B22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>25</v>
+      <c r="C22" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="23" ht="21" spans="1:3">
@@ -2669,10 +2669,10 @@
         <v>6</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" ht="21" spans="1:3">
@@ -2683,7 +2683,7 @@
         <v>27</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" ht="21" spans="1:3">
@@ -2694,7 +2694,7 @@
         <v>28</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" ht="21" spans="1:3">
@@ -2705,7 +2705,7 @@
         <v>29</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" ht="21" spans="1:3">
@@ -2716,7 +2716,7 @@
         <v>30</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" ht="21" spans="1:3">
@@ -2727,7 +2727,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" ht="21" spans="1:3">
@@ -2738,7 +2738,7 @@
         <v>32</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" ht="21" spans="1:3">
@@ -2749,7 +2749,7 @@
         <v>33</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" ht="21" spans="1:3">
@@ -2760,7 +2760,7 @@
         <v>34</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" ht="21" spans="1:3">
@@ -2771,7 +2771,7 @@
         <v>35</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" ht="21" spans="1:3">
@@ -2782,7 +2782,7 @@
         <v>36</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" ht="21" spans="1:3">
@@ -2793,7 +2793,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" ht="21" spans="1:3">
@@ -2804,7 +2804,7 @@
         <v>38</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" ht="21" spans="1:3">
@@ -2815,7 +2815,7 @@
         <v>39</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" ht="21" spans="1:3">
@@ -2826,7 +2826,7 @@
         <v>40</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" ht="21" spans="1:3">
@@ -2837,7 +2837,7 @@
         <v>41</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" ht="21" spans="1:3">
@@ -2848,7 +2848,7 @@
         <v>42</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" ht="21" spans="1:3">
@@ -2859,7 +2859,7 @@
         <v>43</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" ht="21" spans="1:3">
@@ -2870,20 +2870,20 @@
         <v>44</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" ht="21" spans="2:3">
       <c r="B42" s="10"/>
       <c r="C42" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43" ht="21" spans="1:3">
       <c r="A43" s="6"/>
       <c r="B43" s="10"/>
       <c r="C43" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" ht="21" spans="1:3">
@@ -2894,7 +2894,7 @@
         <v>46</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" ht="21" spans="1:3">
@@ -2905,7 +2905,7 @@
         <v>47</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" ht="21" spans="1:3">
@@ -2916,7 +2916,7 @@
         <v>48</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" ht="21" spans="1:3">
@@ -2927,7 +2927,7 @@
         <v>49</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" ht="21" spans="1:3">
@@ -2938,7 +2938,7 @@
         <v>50</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" ht="21" spans="1:3">
@@ -2949,7 +2949,7 @@
         <v>51</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" ht="21" spans="1:3">
@@ -2960,7 +2960,7 @@
         <v>52</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" ht="21" spans="1:3">
@@ -2971,7 +2971,7 @@
         <v>53</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" ht="21" spans="1:3">
@@ -2982,7 +2982,7 @@
         <v>54</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53" ht="21" spans="1:3">
@@ -2993,7 +2993,7 @@
         <v>55</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="55" ht="21" spans="1:3">
@@ -3009,7 +3009,7 @@
         <v>57</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" ht="21" spans="1:3">
@@ -3020,7 +3020,7 @@
         <v>58</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" ht="21" spans="1:3">
@@ -3031,7 +3031,7 @@
         <v>59</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="59" ht="21" spans="1:3">
@@ -3042,7 +3042,7 @@
         <v>60</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" ht="21" spans="1:3">
@@ -3053,7 +3053,7 @@
         <v>61</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="61" ht="21" spans="1:3">
@@ -3064,7 +3064,7 @@
         <v>62</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" ht="21" spans="1:3">
@@ -3075,7 +3075,7 @@
         <v>63</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" ht="21" spans="1:3">
@@ -3086,7 +3086,7 @@
         <v>64</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64" ht="21" spans="1:3">
@@ -3097,7 +3097,7 @@
         <v>65</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" ht="21" spans="1:3">
@@ -3108,7 +3108,7 @@
         <v>66</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="66" ht="21" spans="1:3">
@@ -3119,7 +3119,7 @@
         <v>67</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67" ht="21" spans="1:3">
@@ -3130,7 +3130,7 @@
         <v>68</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68" ht="21" spans="1:3">
@@ -3141,7 +3141,7 @@
         <v>69</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="69" ht="21" spans="1:3">
@@ -3152,7 +3152,7 @@
         <v>70</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" ht="21" spans="1:3">
@@ -3163,7 +3163,7 @@
         <v>71</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" ht="21" spans="1:3">
@@ -3174,7 +3174,7 @@
         <v>72</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="72" ht="21" spans="1:3">
@@ -3185,7 +3185,7 @@
         <v>73</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" ht="21" spans="1:3">
@@ -3196,7 +3196,7 @@
         <v>74</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74" ht="21" spans="1:3">
@@ -3207,7 +3207,7 @@
         <v>75</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75" ht="21" spans="1:3">
@@ -3218,7 +3218,7 @@
         <v>76</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="76" ht="21" spans="1:3">
@@ -3229,7 +3229,7 @@
         <v>77</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="77" ht="21" spans="1:3">
@@ -3240,7 +3240,7 @@
         <v>78</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="78" ht="21" spans="1:3">
@@ -3251,7 +3251,7 @@
         <v>79</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79" ht="21" spans="1:3">
@@ -3262,7 +3262,7 @@
         <v>80</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80" ht="21" spans="1:3">
@@ -3273,7 +3273,7 @@
         <v>81</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="81" ht="21" spans="1:3">
@@ -3284,7 +3284,7 @@
         <v>82</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="82" ht="21" spans="1:3">
@@ -3295,7 +3295,7 @@
         <v>83</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="83" ht="21" spans="1:3">
@@ -3306,7 +3306,7 @@
         <v>84</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="84" ht="21" spans="1:3">
@@ -3317,7 +3317,7 @@
         <v>85</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="85" ht="21" spans="1:3">
@@ -3328,7 +3328,7 @@
         <v>86</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="86" ht="21" spans="1:3">
@@ -3339,7 +3339,7 @@
         <v>87</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="87" ht="21" spans="1:3">
@@ -3350,7 +3350,7 @@
         <v>88</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="88" ht="21" spans="1:3">
@@ -3361,7 +3361,7 @@
         <v>89</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="89" ht="21" spans="1:3">
@@ -3372,7 +3372,7 @@
         <v>90</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="90" ht="21" spans="1:3">
@@ -3383,7 +3383,7 @@
         <v>91</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="91" ht="21" spans="1:3">
@@ -3394,7 +3394,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="92" ht="21" spans="1:3">
@@ -3405,7 +3405,7 @@
         <v>93</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="93" ht="21" spans="1:3">
@@ -3416,7 +3416,7 @@
         <v>94</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="94" ht="21" spans="1:3">
@@ -3427,7 +3427,7 @@
         <v>95</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="95" ht="21" spans="1:3">
@@ -3438,7 +3438,7 @@
         <v>96</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="96" ht="21" spans="1:3">
@@ -3449,7 +3449,7 @@
         <v>97</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="97" ht="21" spans="1:3">
@@ -3460,7 +3460,7 @@
         <v>98</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="98" ht="21" spans="1:3">
@@ -3471,7 +3471,7 @@
         <v>99</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="100" ht="21" spans="1:3">
@@ -3487,7 +3487,7 @@
         <v>101</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="102" ht="21" spans="1:3">
@@ -3498,7 +3498,7 @@
         <v>102</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="103" ht="21" spans="1:3">
@@ -3509,7 +3509,7 @@
         <v>103</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="104" ht="21" spans="1:3">
@@ -3520,7 +3520,7 @@
         <v>104</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="105" ht="21" spans="1:3">
@@ -3531,7 +3531,7 @@
         <v>105</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="106" ht="21" spans="1:3">
@@ -3542,7 +3542,7 @@
         <v>106</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="107" ht="21" spans="1:3">
@@ -3553,7 +3553,7 @@
         <v>107</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="108" ht="21" spans="1:3">
@@ -3564,7 +3564,7 @@
         <v>108</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="109" ht="21" spans="1:3">
@@ -3575,7 +3575,7 @@
         <v>109</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="110" ht="21" spans="1:3">
@@ -3586,7 +3586,7 @@
         <v>110</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="111" ht="21" spans="1:3">
@@ -3597,7 +3597,7 @@
         <v>111</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="112" ht="21" spans="1:3">
@@ -3608,7 +3608,7 @@
         <v>112</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="113" ht="21" spans="1:3">
@@ -3619,7 +3619,7 @@
         <v>113</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="114" ht="21" spans="1:3">
@@ -3630,7 +3630,7 @@
         <v>114</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="115" ht="21" spans="1:3">
@@ -3641,7 +3641,7 @@
         <v>115</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="116" ht="21" spans="1:3">
@@ -3652,7 +3652,7 @@
         <v>116</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="117" ht="21" spans="1:3">
@@ -3663,7 +3663,7 @@
         <v>117</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="118" ht="21" spans="1:3">
@@ -3674,7 +3674,7 @@
         <v>118</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="119" ht="21" spans="1:3">
@@ -3685,7 +3685,7 @@
         <v>119</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="120" ht="21" spans="1:3">
@@ -3696,7 +3696,7 @@
         <v>120</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="121" ht="21" spans="1:3">
@@ -3707,7 +3707,7 @@
         <v>121</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="122" ht="21" spans="1:3">
@@ -3718,7 +3718,7 @@
         <v>122</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="123" ht="21" spans="1:3">
@@ -3729,7 +3729,7 @@
         <v>123</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="124" ht="21" spans="1:3">
@@ -3740,7 +3740,7 @@
         <v>124</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="125" ht="21" spans="1:3">
@@ -3751,7 +3751,7 @@
         <v>125</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="126" ht="21" spans="1:3">
@@ -3762,7 +3762,7 @@
         <v>126</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="127" ht="21" spans="1:3">
@@ -3773,7 +3773,7 @@
         <v>127</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="128" ht="21" spans="1:3">
@@ -3784,7 +3784,7 @@
         <v>128</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="129" ht="21" spans="1:3">
@@ -3795,7 +3795,7 @@
         <v>129</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="130" ht="21" spans="1:3">
@@ -3806,7 +3806,7 @@
         <v>130</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="131" ht="21" spans="1:3">
@@ -3817,7 +3817,7 @@
         <v>131</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="132" ht="21" spans="1:3">
@@ -3828,7 +3828,7 @@
         <v>132</v>
       </c>
       <c r="C132" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="133" ht="21" spans="1:3">
@@ -3839,7 +3839,7 @@
         <v>133</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="134" ht="21" spans="1:3">
@@ -3850,7 +3850,7 @@
         <v>134</v>
       </c>
       <c r="C134" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="135" ht="21" spans="1:3">
@@ -3861,7 +3861,7 @@
         <v>135</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="136" ht="21" spans="1:3">
@@ -3872,7 +3872,7 @@
         <v>136</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="138" ht="21" spans="2:3">
@@ -3887,7 +3887,7 @@
         <v>138</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="140" ht="21" spans="1:3">
@@ -3898,7 +3898,7 @@
         <v>139</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="141" ht="21" spans="1:3">
@@ -3909,7 +3909,7 @@
         <v>140</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="142" ht="21" spans="1:3">
@@ -3920,7 +3920,7 @@
         <v>141</v>
       </c>
       <c r="C142" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="143" ht="21" spans="1:3">
@@ -3931,7 +3931,7 @@
         <v>142</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="144" ht="21" spans="1:3">
@@ -3942,7 +3942,7 @@
         <v>143</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="145" ht="21" spans="1:3">
@@ -3953,7 +3953,7 @@
         <v>144</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="146" ht="21" spans="1:3">
@@ -3964,7 +3964,7 @@
         <v>145</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="147" ht="21" spans="1:3">
@@ -3975,7 +3975,7 @@
         <v>146</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="148" ht="21" spans="1:3">
@@ -3986,7 +3986,7 @@
         <v>147</v>
       </c>
       <c r="C148" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="149" ht="21" spans="1:3">
@@ -3997,7 +3997,7 @@
         <v>148</v>
       </c>
       <c r="C149" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="150" ht="21" spans="1:3">
@@ -4008,7 +4008,7 @@
         <v>149</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="151" ht="21" spans="1:3">
@@ -4019,7 +4019,7 @@
         <v>150</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="152" ht="21" spans="1:3">
@@ -4030,7 +4030,7 @@
         <v>151</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="153" ht="21" spans="1:3">
@@ -4041,7 +4041,7 @@
         <v>152</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="154" ht="21" spans="1:3">
@@ -4052,7 +4052,7 @@
         <v>153</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="155" ht="21" spans="1:3">
@@ -4063,7 +4063,7 @@
         <v>154</v>
       </c>
       <c r="C155" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="156" ht="21" spans="1:3">
@@ -4074,7 +4074,7 @@
         <v>155</v>
       </c>
       <c r="C156" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="157" ht="21" spans="1:3">
@@ -4085,7 +4085,7 @@
         <v>156</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="158" ht="21" spans="1:3">
@@ -4096,7 +4096,7 @@
         <v>157</v>
       </c>
       <c r="C158" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="159" ht="21" spans="1:3">
@@ -4107,7 +4107,7 @@
         <v>158</v>
       </c>
       <c r="C159" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="160" ht="21" spans="1:3">
@@ -4118,7 +4118,7 @@
         <v>159</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="161" ht="21" spans="1:3">
@@ -4129,7 +4129,7 @@
         <v>160</v>
       </c>
       <c r="C161" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="162" ht="21" spans="1:3">
@@ -4140,7 +4140,7 @@
         <v>161</v>
       </c>
       <c r="C162" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="163" ht="21" spans="1:3">
@@ -4151,7 +4151,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="164" ht="21" spans="1:3">
@@ -4162,7 +4162,7 @@
         <v>163</v>
       </c>
       <c r="C164" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="165" ht="21" spans="1:3">
@@ -4173,7 +4173,7 @@
         <v>164</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="166" ht="21" spans="1:3">
@@ -4184,7 +4184,7 @@
         <v>165</v>
       </c>
       <c r="C166" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="167" ht="21" spans="1:3">
@@ -4195,7 +4195,7 @@
         <v>166</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="168" ht="21" spans="1:3">
@@ -4206,7 +4206,7 @@
         <v>167</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="169" ht="21" spans="1:3">
@@ -4217,7 +4217,7 @@
         <v>168</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="170" ht="21" spans="1:3">
@@ -4228,7 +4228,7 @@
         <v>169</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="171" ht="21" spans="1:3">
@@ -4239,7 +4239,7 @@
         <v>170</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="172" ht="21" spans="1:3">
@@ -4250,7 +4250,7 @@
         <v>171</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="173" ht="21" spans="1:3">
@@ -4261,7 +4261,7 @@
         <v>172</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="174" ht="21" spans="1:3">
@@ -4272,7 +4272,7 @@
         <v>173</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="176" ht="21" spans="2:3">
@@ -4463,7 +4463,7 @@
         <v>191</v>
       </c>
       <c r="C193" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="194" ht="21" spans="1:3">
@@ -4507,7 +4507,7 @@
         <v>196</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="198" ht="21" spans="1:3">
@@ -4518,7 +4518,7 @@
         <v>197</v>
       </c>
       <c r="C198" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="199" ht="21" spans="1:3">
@@ -4529,7 +4529,7 @@
         <v>198</v>
       </c>
       <c r="C199" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="200" ht="21" spans="1:3">
@@ -4540,7 +4540,7 @@
         <v>199</v>
       </c>
       <c r="C200" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="201" ht="21" spans="1:3">
@@ -4551,7 +4551,7 @@
         <v>200</v>
       </c>
       <c r="C201" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="202" ht="21" spans="1:3">
@@ -4562,7 +4562,7 @@
         <v>201</v>
       </c>
       <c r="C202" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="203" ht="21" spans="1:3">
@@ -4573,7 +4573,7 @@
         <v>202</v>
       </c>
       <c r="C203" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="204" ht="21" spans="1:3">
@@ -4584,7 +4584,7 @@
         <v>203</v>
       </c>
       <c r="C204" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="205" ht="21" spans="1:3">
@@ -4595,7 +4595,7 @@
         <v>204</v>
       </c>
       <c r="C205" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="206" ht="21" spans="1:3">
@@ -4606,7 +4606,7 @@
         <v>205</v>
       </c>
       <c r="C206" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="207" ht="21" spans="1:3">
@@ -4617,7 +4617,7 @@
         <v>206</v>
       </c>
       <c r="C207" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="208" ht="21" spans="1:3">
@@ -4628,7 +4628,7 @@
         <v>207</v>
       </c>
       <c r="C208" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="209" ht="21" spans="1:3">
@@ -4639,7 +4639,7 @@
         <v>208</v>
       </c>
       <c r="C209" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="210" ht="21" spans="1:3">
@@ -4650,7 +4650,7 @@
         <v>209</v>
       </c>
       <c r="C210" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="211" ht="21" spans="1:3">
@@ -4661,7 +4661,7 @@
         <v>210</v>
       </c>
       <c r="C211" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="212" ht="21" spans="1:3">
@@ -4682,7 +4682,7 @@
         <v>212</v>
       </c>
       <c r="C214" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="215" ht="21" spans="1:3">
@@ -4693,7 +4693,7 @@
         <v>213</v>
       </c>
       <c r="C215" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="216" ht="21" spans="1:3">
@@ -4704,7 +4704,7 @@
         <v>214</v>
       </c>
       <c r="C216" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="217" ht="21" spans="1:3">
@@ -4715,7 +4715,7 @@
         <v>215</v>
       </c>
       <c r="C217" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="218" ht="21" spans="1:3">
@@ -4726,7 +4726,7 @@
         <v>216</v>
       </c>
       <c r="C218" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="219" ht="21" spans="1:3">
@@ -4737,7 +4737,7 @@
         <v>217</v>
       </c>
       <c r="C219" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="220" ht="21" spans="1:3">
@@ -4748,7 +4748,7 @@
         <v>218</v>
       </c>
       <c r="C220" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="221" ht="21" spans="1:3">
@@ -4759,7 +4759,7 @@
         <v>219</v>
       </c>
       <c r="C221" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="222" ht="21" spans="1:3">
@@ -4770,7 +4770,7 @@
         <v>220</v>
       </c>
       <c r="C222" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="223" ht="21" spans="1:3">
@@ -4781,7 +4781,7 @@
         <v>221</v>
       </c>
       <c r="C223" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="224" ht="21" spans="1:3">
@@ -4792,7 +4792,7 @@
         <v>222</v>
       </c>
       <c r="C224" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="225" ht="21" spans="1:3">
@@ -4803,7 +4803,7 @@
         <v>223</v>
       </c>
       <c r="C225" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="226" ht="21" spans="1:3">
@@ -4814,7 +4814,7 @@
         <v>224</v>
       </c>
       <c r="C226" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="227" ht="21" spans="1:3">
@@ -4825,7 +4825,7 @@
         <v>225</v>
       </c>
       <c r="C227" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="228" ht="21" spans="1:3">
@@ -4836,7 +4836,7 @@
         <v>226</v>
       </c>
       <c r="C228" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="229" ht="21" spans="1:3">
@@ -4847,7 +4847,7 @@
         <v>227</v>
       </c>
       <c r="C229" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="230" ht="21" spans="1:3">
@@ -4858,7 +4858,7 @@
         <v>228</v>
       </c>
       <c r="C230" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="231" ht="21" spans="1:3">
@@ -4869,7 +4869,7 @@
         <v>229</v>
       </c>
       <c r="C231" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="232" ht="21" spans="1:3">
@@ -4880,7 +4880,7 @@
         <v>230</v>
       </c>
       <c r="C232" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="233" ht="21" spans="1:3">
@@ -4891,7 +4891,7 @@
         <v>231</v>
       </c>
       <c r="C233" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="234" ht="21" spans="1:3">
@@ -4902,7 +4902,7 @@
         <v>232</v>
       </c>
       <c r="C234" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="235" ht="21" spans="1:3">
@@ -4913,7 +4913,7 @@
         <v>233</v>
       </c>
       <c r="C235" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="236" ht="21" spans="2:3">
@@ -4932,7 +4932,7 @@
         <v>235</v>
       </c>
       <c r="C238" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="239" ht="21" spans="1:3">
@@ -4943,7 +4943,7 @@
         <v>236</v>
       </c>
       <c r="C239" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="240" ht="21" spans="1:3">
@@ -4954,7 +4954,7 @@
         <v>237</v>
       </c>
       <c r="C240" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="241" ht="21" spans="1:3">
@@ -4965,7 +4965,7 @@
         <v>238</v>
       </c>
       <c r="C241" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="242" ht="21" spans="1:3">
@@ -4987,7 +4987,7 @@
         <v>241</v>
       </c>
       <c r="C243" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="244" ht="21" spans="1:3">
@@ -4998,7 +4998,7 @@
         <v>242</v>
       </c>
       <c r="C244" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="245" ht="21" spans="1:3">
@@ -5009,7 +5009,7 @@
         <v>243</v>
       </c>
       <c r="C245" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="246" ht="21" spans="1:3">
@@ -5020,7 +5020,7 @@
         <v>244</v>
       </c>
       <c r="C246" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="247" ht="21" spans="1:3">
@@ -5031,7 +5031,7 @@
         <v>245</v>
       </c>
       <c r="C247" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="248" ht="21" spans="1:3">
@@ -5042,7 +5042,7 @@
         <v>246</v>
       </c>
       <c r="C248" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="249" ht="21" spans="1:3">
@@ -5053,7 +5053,7 @@
         <v>247</v>
       </c>
       <c r="C249" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="250" ht="21" spans="1:3">
@@ -5064,7 +5064,7 @@
         <v>248</v>
       </c>
       <c r="C250" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="251" ht="21" spans="1:3">
@@ -5075,7 +5075,7 @@
         <v>249</v>
       </c>
       <c r="C251" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="252" ht="21" spans="1:3">
@@ -5086,7 +5086,7 @@
         <v>250</v>
       </c>
       <c r="C252" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="253" ht="21" spans="1:3">
@@ -5097,7 +5097,7 @@
         <v>251</v>
       </c>
       <c r="C253" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="254" ht="21" spans="1:3">
@@ -5108,7 +5108,7 @@
         <v>252</v>
       </c>
       <c r="C254" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="255" ht="21" spans="1:3">
@@ -5119,7 +5119,7 @@
         <v>253</v>
       </c>
       <c r="C255" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="256" ht="21" spans="1:3">
@@ -5130,7 +5130,7 @@
         <v>254</v>
       </c>
       <c r="C256" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="257" ht="21" spans="1:3">
@@ -5141,7 +5141,7 @@
         <v>255</v>
       </c>
       <c r="C257" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="258" ht="21" spans="1:3">
@@ -5152,7 +5152,7 @@
         <v>256</v>
       </c>
       <c r="C258" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="259" ht="21" spans="1:3">
@@ -5163,7 +5163,7 @@
         <v>257</v>
       </c>
       <c r="C259" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="260" ht="21" spans="1:3">
@@ -5174,7 +5174,7 @@
         <v>258</v>
       </c>
       <c r="C260" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="261" ht="21" spans="1:3">
@@ -5185,7 +5185,7 @@
         <v>259</v>
       </c>
       <c r="C261" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="262" ht="21" spans="1:3">
@@ -5196,7 +5196,7 @@
         <v>260</v>
       </c>
       <c r="C262" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="263" ht="21" spans="1:3">
@@ -5207,7 +5207,7 @@
         <v>261</v>
       </c>
       <c r="C263" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="264" ht="21" spans="1:3">
@@ -5218,7 +5218,7 @@
         <v>262</v>
       </c>
       <c r="C264" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="265" ht="21" spans="1:3">
@@ -5229,7 +5229,7 @@
         <v>263</v>
       </c>
       <c r="C265" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="266" ht="21" spans="1:3">
@@ -5240,7 +5240,7 @@
         <v>264</v>
       </c>
       <c r="C266" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="267" ht="21" spans="1:3">
@@ -5251,7 +5251,7 @@
         <v>265</v>
       </c>
       <c r="C267" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="268" ht="21" spans="1:3">
@@ -5262,7 +5262,7 @@
         <v>266</v>
       </c>
       <c r="C268" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="269" ht="21" spans="1:3">
@@ -5273,7 +5273,7 @@
         <v>267</v>
       </c>
       <c r="C269" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="270" ht="21" spans="1:3">
@@ -5284,7 +5284,7 @@
         <v>268</v>
       </c>
       <c r="C270" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="271" ht="21" spans="1:3">
@@ -5295,7 +5295,7 @@
         <v>90</v>
       </c>
       <c r="C271" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="272" ht="21" spans="1:3">
@@ -5306,7 +5306,7 @@
         <v>269</v>
       </c>
       <c r="C272" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="273" ht="21" spans="2:3">
@@ -5325,7 +5325,7 @@
         <v>271</v>
       </c>
       <c r="C275" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="276" ht="21" spans="1:3">
@@ -5336,7 +5336,7 @@
         <v>272</v>
       </c>
       <c r="C276" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="277" ht="21" spans="1:3">
@@ -5347,7 +5347,7 @@
         <v>273</v>
       </c>
       <c r="C277" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="278" ht="21" spans="1:3">
@@ -5358,7 +5358,7 @@
         <v>274</v>
       </c>
       <c r="C278" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="279" ht="21" spans="1:3">
@@ -5369,7 +5369,7 @@
         <v>275</v>
       </c>
       <c r="C279" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="280" ht="21" spans="1:3">
@@ -5380,7 +5380,7 @@
         <v>276</v>
       </c>
       <c r="C280" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="281" ht="21" spans="1:3">
@@ -5391,7 +5391,7 @@
         <v>277</v>
       </c>
       <c r="C281" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="282" ht="21" spans="1:3">
@@ -5402,7 +5402,7 @@
         <v>278</v>
       </c>
       <c r="C282" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="283" ht="21" spans="1:3">
@@ -5413,7 +5413,7 @@
         <v>279</v>
       </c>
       <c r="C283" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="284" ht="21" spans="1:3">
@@ -5424,7 +5424,7 @@
         <v>280</v>
       </c>
       <c r="C284" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="285" ht="21" spans="1:3">
@@ -5435,7 +5435,7 @@
         <v>281</v>
       </c>
       <c r="C285" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="286" ht="21" spans="1:3">
@@ -5446,7 +5446,7 @@
         <v>282</v>
       </c>
       <c r="C286" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="287" ht="21" spans="1:3">
@@ -5457,7 +5457,7 @@
         <v>283</v>
       </c>
       <c r="C287" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="288" ht="21" spans="1:3">
@@ -5468,7 +5468,7 @@
         <v>284</v>
       </c>
       <c r="C288" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="289" ht="21" spans="1:3">
@@ -5479,7 +5479,7 @@
         <v>285</v>
       </c>
       <c r="C289" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="290" ht="21" spans="1:3">
@@ -5490,7 +5490,7 @@
         <v>286</v>
       </c>
       <c r="C290" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="291" ht="21" spans="1:3">
@@ -5501,7 +5501,7 @@
         <v>287</v>
       </c>
       <c r="C291" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="292" ht="21" spans="1:3">
@@ -5512,7 +5512,7 @@
         <v>288</v>
       </c>
       <c r="C292" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="293" ht="21" spans="1:3">
@@ -5523,7 +5523,7 @@
         <v>289</v>
       </c>
       <c r="C293" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="294" ht="21" spans="2:3">
@@ -5542,7 +5542,7 @@
         <v>291</v>
       </c>
       <c r="C296" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="297" ht="21" spans="1:3">
@@ -5553,7 +5553,7 @@
         <v>292</v>
       </c>
       <c r="C297" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="298" ht="21" spans="1:3">
@@ -5564,7 +5564,7 @@
         <v>293</v>
       </c>
       <c r="C298" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="299" ht="21" spans="1:3">
@@ -5575,7 +5575,7 @@
         <v>294</v>
       </c>
       <c r="C299" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="300" ht="21" spans="1:3">
@@ -5586,7 +5586,7 @@
         <v>295</v>
       </c>
       <c r="C300" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="301" ht="21" spans="1:3">
@@ -5597,7 +5597,7 @@
         <v>296</v>
       </c>
       <c r="C301" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="302" ht="21" spans="1:3">
@@ -5608,7 +5608,7 @@
         <v>297</v>
       </c>
       <c r="C302" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="303" ht="21" spans="1:3">
@@ -5619,7 +5619,7 @@
         <v>298</v>
       </c>
       <c r="C303" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="304" ht="21" spans="1:3">
@@ -5630,7 +5630,7 @@
         <v>299</v>
       </c>
       <c r="C304" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="305" ht="21" spans="1:3">
@@ -5641,7 +5641,7 @@
         <v>300</v>
       </c>
       <c r="C305" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="306" ht="21" spans="1:3">
@@ -5652,7 +5652,7 @@
         <v>301</v>
       </c>
       <c r="C306" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="307" ht="21" spans="1:3">
@@ -5663,7 +5663,7 @@
         <v>302</v>
       </c>
       <c r="C307" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="308" ht="21" spans="1:3">
@@ -5674,7 +5674,7 @@
         <v>303</v>
       </c>
       <c r="C308" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="309" ht="21" spans="1:3">
@@ -5685,7 +5685,7 @@
         <v>304</v>
       </c>
       <c r="C309" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="310" ht="21" spans="1:3">
@@ -5696,7 +5696,7 @@
         <v>305</v>
       </c>
       <c r="C310" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="311" ht="21" spans="1:3">
@@ -5707,7 +5707,7 @@
         <v>306</v>
       </c>
       <c r="C311" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="312" ht="21" spans="1:3">
@@ -5718,7 +5718,7 @@
         <v>307</v>
       </c>
       <c r="C312" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="313" ht="21" spans="1:3">
@@ -5729,7 +5729,7 @@
         <v>308</v>
       </c>
       <c r="C313" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="314" ht="21" spans="1:3">
@@ -5740,7 +5740,7 @@
         <v>309</v>
       </c>
       <c r="C314" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="315" ht="21" spans="1:3">
@@ -5751,7 +5751,7 @@
         <v>310</v>
       </c>
       <c r="C315" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="316" ht="21" spans="1:3">
@@ -5762,7 +5762,7 @@
         <v>311</v>
       </c>
       <c r="C316" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="317" ht="21" spans="1:3">
@@ -5773,7 +5773,7 @@
         <v>312</v>
       </c>
       <c r="C317" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="318" ht="21" spans="1:3">
@@ -5784,7 +5784,7 @@
         <v>313</v>
       </c>
       <c r="C318" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="319" ht="21" spans="1:3">
@@ -5795,7 +5795,7 @@
         <v>314</v>
       </c>
       <c r="C319" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="320" ht="21" spans="1:3">
@@ -5806,7 +5806,7 @@
         <v>315</v>
       </c>
       <c r="C320" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="321" ht="21" spans="1:3">
@@ -5817,7 +5817,7 @@
         <v>316</v>
       </c>
       <c r="C321" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="322" ht="21" spans="1:3">
@@ -5828,7 +5828,7 @@
         <v>317</v>
       </c>
       <c r="C322" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="323" ht="21" spans="1:3">
@@ -5839,7 +5839,7 @@
         <v>318</v>
       </c>
       <c r="C323" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="324" ht="21" spans="1:3">
@@ -5850,7 +5850,7 @@
         <v>319</v>
       </c>
       <c r="C324" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="325" ht="21" spans="1:3">
@@ -5861,7 +5861,7 @@
         <v>320</v>
       </c>
       <c r="C325" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="326" ht="21" spans="1:3">
@@ -5872,7 +5872,7 @@
         <v>321</v>
       </c>
       <c r="C326" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="327" ht="21" spans="1:3">
@@ -5883,7 +5883,7 @@
         <v>322</v>
       </c>
       <c r="C327" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="328" ht="21" spans="1:3">
@@ -5894,7 +5894,7 @@
         <v>323</v>
       </c>
       <c r="C328" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="329" ht="21" spans="1:3">
@@ -5905,7 +5905,7 @@
         <v>324</v>
       </c>
       <c r="C329" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="330" ht="21" spans="1:3">
@@ -5916,7 +5916,7 @@
         <v>325</v>
       </c>
       <c r="C330" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="331" ht="21" spans="1:3">
@@ -5927,7 +5927,7 @@
         <v>326</v>
       </c>
       <c r="C331" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="332" ht="21" spans="1:3">
@@ -5938,7 +5938,7 @@
         <v>327</v>
       </c>
       <c r="C332" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="333" ht="21" spans="1:3">
@@ -5949,7 +5949,7 @@
         <v>328</v>
       </c>
       <c r="C333" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="334" ht="21" spans="2:3">
@@ -5968,7 +5968,7 @@
         <v>330</v>
       </c>
       <c r="C336" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="337" ht="21" spans="1:3">
@@ -5979,7 +5979,7 @@
         <v>331</v>
       </c>
       <c r="C337" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="338" ht="21" spans="1:3">
@@ -5990,7 +5990,7 @@
         <v>332</v>
       </c>
       <c r="C338" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="339" ht="21" spans="1:3">
@@ -6001,7 +6001,7 @@
         <v>333</v>
       </c>
       <c r="C339" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="340" ht="21" spans="1:3">
@@ -6012,7 +6012,7 @@
         <v>334</v>
       </c>
       <c r="C340" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="341" ht="21" spans="1:3">
@@ -6023,7 +6023,7 @@
         <v>335</v>
       </c>
       <c r="C341" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="342" ht="21" spans="1:3">
@@ -6034,7 +6034,7 @@
         <v>336</v>
       </c>
       <c r="C342" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="343" ht="21" spans="1:3">
@@ -6045,7 +6045,7 @@
         <v>337</v>
       </c>
       <c r="C343" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="344" ht="21" spans="1:3">
@@ -6056,7 +6056,7 @@
         <v>338</v>
       </c>
       <c r="C344" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="345" ht="21" spans="1:3">
@@ -6067,7 +6067,7 @@
         <v>339</v>
       </c>
       <c r="C345" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="346" ht="21" spans="1:3">
@@ -6078,7 +6078,7 @@
         <v>340</v>
       </c>
       <c r="C346" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="347" ht="21" spans="1:3">
@@ -6089,7 +6089,7 @@
         <v>341</v>
       </c>
       <c r="C347" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="348" ht="21" spans="1:3">
@@ -6100,7 +6100,7 @@
         <v>342</v>
       </c>
       <c r="C348" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="349" ht="21" spans="1:3">
@@ -6111,7 +6111,7 @@
         <v>343</v>
       </c>
       <c r="C349" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="350" ht="21" spans="1:3">
@@ -6122,7 +6122,7 @@
         <v>344</v>
       </c>
       <c r="C350" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="351" ht="21" spans="1:3">
@@ -6133,7 +6133,7 @@
         <v>345</v>
       </c>
       <c r="C351" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="352" ht="21" spans="1:3">
@@ -6144,7 +6144,7 @@
         <v>346</v>
       </c>
       <c r="C352" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="353" ht="21" spans="1:3">
@@ -6155,7 +6155,7 @@
         <v>347</v>
       </c>
       <c r="C353" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="354" ht="21" spans="2:3">
@@ -6174,7 +6174,7 @@
         <v>349</v>
       </c>
       <c r="C356" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="357" ht="21" spans="1:3">
@@ -6251,7 +6251,7 @@
         <v>356</v>
       </c>
       <c r="C363" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="364" ht="21" spans="1:3">
@@ -6262,7 +6262,7 @@
         <v>357</v>
       </c>
       <c r="C364" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="365" ht="21" spans="1:3">
@@ -6273,7 +6273,7 @@
         <v>358</v>
       </c>
       <c r="C365" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="366" ht="21" spans="1:3">
@@ -6284,7 +6284,7 @@
         <v>359</v>
       </c>
       <c r="C366" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="367" ht="21" spans="1:3">
@@ -6295,7 +6295,7 @@
         <v>360</v>
       </c>
       <c r="C367" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="368" ht="21" spans="1:3">
@@ -6306,7 +6306,7 @@
         <v>361</v>
       </c>
       <c r="C368" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="369" ht="21" spans="1:3">
@@ -6317,7 +6317,7 @@
         <v>362</v>
       </c>
       <c r="C369" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="370" ht="21" spans="1:3">
@@ -6328,7 +6328,7 @@
         <v>363</v>
       </c>
       <c r="C370" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="371" ht="21" spans="1:3">
@@ -6339,7 +6339,7 @@
         <v>364</v>
       </c>
       <c r="C371" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="372" ht="21" spans="1:3">
@@ -6350,7 +6350,7 @@
         <v>365</v>
       </c>
       <c r="C372" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="373" ht="21" spans="1:3">
@@ -6361,7 +6361,7 @@
         <v>366</v>
       </c>
       <c r="C373" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="374" ht="21" spans="1:3">
@@ -6372,7 +6372,7 @@
         <v>367</v>
       </c>
       <c r="C374" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="375" ht="21" spans="1:3">
@@ -6383,7 +6383,7 @@
         <v>368</v>
       </c>
       <c r="C375" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="376" ht="21" spans="1:3">
@@ -6394,7 +6394,7 @@
         <v>369</v>
       </c>
       <c r="C376" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="377" ht="21" spans="1:3">
@@ -6405,7 +6405,7 @@
         <v>370</v>
       </c>
       <c r="C377" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="378" ht="21" spans="1:3">
@@ -6416,7 +6416,7 @@
         <v>371</v>
       </c>
       <c r="C378" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="379" ht="21" spans="1:3">
@@ -6427,7 +6427,7 @@
         <v>372</v>
       </c>
       <c r="C379" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="380" ht="21" spans="1:3">
@@ -6438,7 +6438,7 @@
         <v>373</v>
       </c>
       <c r="C380" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="381" ht="21" spans="1:3">
@@ -6449,7 +6449,7 @@
         <v>374</v>
       </c>
       <c r="C381" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="382" ht="21" spans="1:3">
@@ -6460,7 +6460,7 @@
         <v>375</v>
       </c>
       <c r="C382" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="383" ht="21" spans="1:3">
@@ -6471,7 +6471,7 @@
         <v>376</v>
       </c>
       <c r="C383" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="384" ht="21" spans="1:3">
@@ -6482,7 +6482,7 @@
         <v>377</v>
       </c>
       <c r="C384" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="385" ht="21" spans="1:3">
@@ -6493,7 +6493,7 @@
         <v>378</v>
       </c>
       <c r="C385" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="386" ht="21" spans="1:3">
@@ -6504,7 +6504,7 @@
         <v>379</v>
       </c>
       <c r="C386" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="387" ht="21" spans="1:3">
@@ -6515,7 +6515,7 @@
         <v>380</v>
       </c>
       <c r="C387" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="388" ht="21" spans="1:3">
@@ -6526,7 +6526,7 @@
         <v>381</v>
       </c>
       <c r="C388" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="389" ht="21" spans="1:3">
@@ -6537,7 +6537,7 @@
         <v>382</v>
       </c>
       <c r="C389" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="390" ht="21" spans="1:3">
@@ -6548,7 +6548,7 @@
         <v>382</v>
       </c>
       <c r="C390" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="391" ht="21" spans="1:3">
@@ -6559,7 +6559,7 @@
         <v>383</v>
       </c>
       <c r="C391" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="392" ht="21" spans="1:3">
@@ -6570,7 +6570,7 @@
         <v>384</v>
       </c>
       <c r="C392" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="393" ht="21" spans="1:3">
@@ -6581,7 +6581,7 @@
         <v>385</v>
       </c>
       <c r="C393" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="394" ht="21" spans="1:3">
@@ -6592,7 +6592,7 @@
         <v>386</v>
       </c>
       <c r="C394" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="395" ht="21" spans="1:3">
@@ -6603,7 +6603,7 @@
         <v>387</v>
       </c>
       <c r="C395" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="396" ht="21" spans="1:3">
@@ -6614,7 +6614,7 @@
         <v>388</v>
       </c>
       <c r="C396" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="397" ht="21" spans="1:3">
@@ -6625,7 +6625,7 @@
         <v>389</v>
       </c>
       <c r="C397" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="398" ht="21" spans="1:3">
@@ -6636,7 +6636,7 @@
         <v>390</v>
       </c>
       <c r="C398" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="399" ht="21" spans="1:3">
@@ -6647,7 +6647,7 @@
         <v>391</v>
       </c>
       <c r="C399" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="400" ht="21" spans="2:3">
@@ -6666,7 +6666,7 @@
         <v>393</v>
       </c>
       <c r="C402" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="403" ht="21" spans="1:3">
@@ -6677,7 +6677,7 @@
         <v>394</v>
       </c>
       <c r="C403" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="404" ht="21" spans="1:3">
@@ -6688,7 +6688,7 @@
         <v>395</v>
       </c>
       <c r="C404" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="405" ht="21" spans="1:3">
@@ -6699,7 +6699,7 @@
         <v>92</v>
       </c>
       <c r="C405" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="406" ht="21" spans="1:3">
@@ -6710,7 +6710,7 @@
         <v>396</v>
       </c>
       <c r="C406" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="407" ht="21" spans="1:3">
@@ -6721,7 +6721,7 @@
         <v>397</v>
       </c>
       <c r="C407" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="408" ht="21" spans="2:3">
@@ -6817,7 +6817,7 @@
         <v>278</v>
       </c>
       <c r="C417" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="418" ht="21" spans="1:3">
@@ -6828,7 +6828,7 @@
         <v>406</v>
       </c>
       <c r="C418" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="419" ht="21" spans="1:3">
@@ -6839,7 +6839,7 @@
         <v>407</v>
       </c>
       <c r="C419" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="420" ht="21" spans="1:3">
@@ -6850,7 +6850,7 @@
         <v>408</v>
       </c>
       <c r="C420" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="421" ht="21" spans="1:3">
@@ -6861,7 +6861,7 @@
         <v>409</v>
       </c>
       <c r="C421" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="422" ht="21" spans="1:3">
@@ -6872,7 +6872,7 @@
         <v>410</v>
       </c>
       <c r="C422" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="423" ht="21" spans="1:3">
@@ -6883,7 +6883,7 @@
         <v>411</v>
       </c>
       <c r="C423" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="424" ht="21" spans="1:3">
@@ -6894,7 +6894,7 @@
         <v>412</v>
       </c>
       <c r="C424" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="425" ht="21" spans="1:3">
@@ -6905,7 +6905,7 @@
         <v>413</v>
       </c>
       <c r="C425" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="426" ht="21" spans="1:3">
@@ -6916,7 +6916,7 @@
         <v>414</v>
       </c>
       <c r="C426" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="427" ht="21" spans="1:3">
@@ -6927,7 +6927,7 @@
         <v>415</v>
       </c>
       <c r="C427" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="428" ht="21" spans="1:3">
@@ -6938,7 +6938,7 @@
         <v>416</v>
       </c>
       <c r="C428" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="429" ht="21" spans="1:3">
@@ -6949,7 +6949,7 @@
         <v>417</v>
       </c>
       <c r="C429" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="430" ht="21" spans="1:3">
@@ -6960,7 +6960,7 @@
         <v>418</v>
       </c>
       <c r="C430" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="431" ht="21" spans="1:3">
@@ -6971,7 +6971,7 @@
         <v>419</v>
       </c>
       <c r="C431" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="432" ht="21" spans="1:3">
@@ -6982,7 +6982,7 @@
         <v>420</v>
       </c>
       <c r="C432" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="433" ht="21" spans="1:3">
@@ -6993,7 +6993,7 @@
         <v>421</v>
       </c>
       <c r="C433" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="434" ht="21" spans="1:3">
@@ -7004,7 +7004,7 @@
         <v>422</v>
       </c>
       <c r="C434" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="435" ht="21" spans="1:3">
@@ -7015,7 +7015,7 @@
         <v>423</v>
       </c>
       <c r="C435" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="436" ht="21" spans="1:3">
@@ -7026,7 +7026,7 @@
         <v>424</v>
       </c>
       <c r="C436" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="437" ht="21" spans="1:3">
@@ -7037,7 +7037,7 @@
         <v>425</v>
       </c>
       <c r="C437" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="438" ht="21" spans="1:3">
@@ -7048,7 +7048,7 @@
         <v>17</v>
       </c>
       <c r="C438" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="439" ht="21" spans="1:3">
@@ -7059,7 +7059,7 @@
         <v>426</v>
       </c>
       <c r="C439" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="440" ht="21" spans="1:3">
@@ -7070,7 +7070,7 @@
         <v>427</v>
       </c>
       <c r="C440" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="441" ht="21" spans="1:3">
@@ -7081,7 +7081,7 @@
         <v>428</v>
       </c>
       <c r="C441" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="442" ht="21" spans="1:3">
@@ -7092,7 +7092,7 @@
         <v>429</v>
       </c>
       <c r="C442" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="443" ht="21" spans="1:3">
@@ -7103,7 +7103,7 @@
         <v>430</v>
       </c>
       <c r="C443" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="444" ht="21" spans="1:3">
@@ -7114,7 +7114,7 @@
         <v>431</v>
       </c>
       <c r="C444" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="445" ht="21" spans="1:3">
@@ -7125,7 +7125,7 @@
         <v>432</v>
       </c>
       <c r="C445" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="446" ht="21" spans="1:3">
@@ -7136,7 +7136,7 @@
         <v>433</v>
       </c>
       <c r="C446" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="447" ht="21" spans="1:3">
@@ -7147,7 +7147,7 @@
         <v>434</v>
       </c>
       <c r="C447" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="448" ht="21" spans="1:3">
@@ -7158,7 +7158,7 @@
         <v>435</v>
       </c>
       <c r="C448" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="449" ht="21" spans="1:3">
@@ -7169,7 +7169,7 @@
         <v>436</v>
       </c>
       <c r="C449" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="450" ht="21" spans="1:3">
@@ -7180,7 +7180,7 @@
         <v>437</v>
       </c>
       <c r="C450" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="451" ht="21" spans="1:3">
@@ -7191,7 +7191,7 @@
         <v>438</v>
       </c>
       <c r="C451" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="452" ht="21" spans="1:3">
@@ -7202,7 +7202,7 @@
         <v>439</v>
       </c>
       <c r="C452" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="453" ht="21" spans="1:3">
@@ -7213,7 +7213,7 @@
         <v>440</v>
       </c>
       <c r="C453" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="454" ht="21" spans="1:3">
@@ -7224,7 +7224,7 @@
         <v>441</v>
       </c>
       <c r="C454" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="455" ht="21" spans="1:3">
@@ -7235,7 +7235,7 @@
         <v>442</v>
       </c>
       <c r="C455" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="456" ht="21" spans="1:3">
@@ -7246,7 +7246,7 @@
         <v>443</v>
       </c>
       <c r="C456" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="457" ht="21" spans="1:3">
@@ -7257,7 +7257,7 @@
         <v>444</v>
       </c>
       <c r="C457" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="458" ht="21" spans="1:3">
@@ -7268,7 +7268,7 @@
         <v>445</v>
       </c>
       <c r="C458" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="459" ht="21" spans="1:3">
@@ -7279,7 +7279,7 @@
         <v>446</v>
       </c>
       <c r="C459" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="460" ht="21" spans="1:3">
@@ -7290,7 +7290,7 @@
         <v>447</v>
       </c>
       <c r="C460" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="461" ht="21" spans="1:3">
@@ -7301,7 +7301,7 @@
         <v>448</v>
       </c>
       <c r="C461" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="462" ht="21" spans="1:3">
@@ -7312,7 +7312,7 @@
         <v>449</v>
       </c>
       <c r="C462" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="463" ht="21" spans="1:3">
@@ -7323,7 +7323,7 @@
         <v>450</v>
       </c>
       <c r="C463" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="464" ht="21" spans="1:3">
@@ -7334,7 +7334,7 @@
         <v>451</v>
       </c>
       <c r="C464" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="465" ht="21" spans="1:3">
@@ -7345,7 +7345,7 @@
         <v>452</v>
       </c>
       <c r="C465" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="466" ht="21" spans="1:3">
@@ -7356,7 +7356,7 @@
         <v>453</v>
       </c>
       <c r="C466" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="467" ht="21" spans="1:3">
@@ -7367,7 +7367,7 @@
         <v>454</v>
       </c>
       <c r="C467" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="468" ht="21" spans="1:3">
@@ -7378,7 +7378,7 @@
         <v>455</v>
       </c>
       <c r="C468" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="469" ht="21" spans="1:3">
@@ -7389,7 +7389,7 @@
         <v>456</v>
       </c>
       <c r="C469" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="470" ht="21" spans="2:3">
@@ -7409,7 +7409,7 @@
         <v>458</v>
       </c>
       <c r="C472" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="473" ht="21" spans="1:3">
@@ -7420,7 +7420,7 @@
         <v>459</v>
       </c>
       <c r="C473" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="474" ht="21" spans="1:3">
@@ -7431,7 +7431,7 @@
         <v>460</v>
       </c>
       <c r="C474" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="475" ht="21" spans="1:3">
@@ -7442,7 +7442,7 @@
         <v>461</v>
       </c>
       <c r="C475" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="476" ht="21" spans="1:3">
@@ -7453,7 +7453,7 @@
         <v>462</v>
       </c>
       <c r="C476" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="477" ht="21" spans="1:3">
@@ -7464,7 +7464,7 @@
         <v>463</v>
       </c>
       <c r="C477" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="478" ht="21" spans="1:3">
@@ -7475,7 +7475,7 @@
         <v>464</v>
       </c>
       <c r="C478" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="479" ht="21" spans="1:3">
@@ -7486,7 +7486,7 @@
         <v>465</v>
       </c>
       <c r="C479" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="480" ht="21" spans="1:3">
@@ -7497,7 +7497,7 @@
         <v>466</v>
       </c>
       <c r="C480" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="481" ht="21" spans="1:3">
@@ -7508,7 +7508,7 @@
         <v>467</v>
       </c>
       <c r="C481" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
common elements in two arrays
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -94,13 +94,13 @@
     <t>find all pairs on integer array whose sum is equal to given number</t>
   </si>
   <si>
+    <t>find common elements In 3 sorted arrays</t>
+  </si>
+  <si>
+    <t>Rearrange the array in alternating positive and negative items with O(1) extra space</t>
+  </si>
+  <si>
     <t>&lt;-&gt;</t>
-  </si>
-  <si>
-    <t>find common elements In 3 sorted arrays</t>
-  </si>
-  <si>
-    <t>Rearrange the array in alternating positive and negative items with O(1) extra space</t>
   </si>
   <si>
     <t>Find if there is any subarray with sum equal to 0</t>
@@ -1425,9 +1425,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
@@ -1505,13 +1505,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1519,12 +1512,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1563,13 +1564,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1602,14 +1596,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1624,15 +1618,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1660,49 +1660,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1726,19 +1696,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1750,7 +1708,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1762,19 +1756,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1798,7 +1780,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1810,31 +1810,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1848,32 +1848,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1917,20 +1896,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1945,149 +1921,173 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2441,7 +2441,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2671,8 +2671,8 @@
       <c r="B23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>26</v>
+      <c r="C23" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="24" ht="21" spans="1:3">
@@ -2680,10 +2680,10 @@
         <v>6</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="9" t="s">
         <v>26</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="25" ht="21" spans="1:3">
@@ -2691,10 +2691,10 @@
         <v>6</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" ht="21" spans="1:3">
@@ -2705,7 +2705,7 @@
         <v>29</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" ht="21" spans="1:3">
@@ -2716,7 +2716,7 @@
         <v>30</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" ht="21" spans="1:3">
@@ -2727,7 +2727,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" ht="21" spans="1:3">
@@ -2738,7 +2738,7 @@
         <v>32</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" ht="21" spans="1:3">
@@ -2749,7 +2749,7 @@
         <v>33</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" ht="21" spans="1:3">
@@ -2760,7 +2760,7 @@
         <v>34</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" ht="21" spans="1:3">
@@ -2771,7 +2771,7 @@
         <v>35</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" ht="21" spans="1:3">
@@ -2782,7 +2782,7 @@
         <v>36</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" ht="21" spans="1:3">
@@ -2793,7 +2793,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" ht="21" spans="1:3">
@@ -2804,7 +2804,7 @@
         <v>38</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" ht="21" spans="1:3">
@@ -2815,7 +2815,7 @@
         <v>39</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" ht="21" spans="1:3">
@@ -2826,7 +2826,7 @@
         <v>40</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" ht="21" spans="1:3">
@@ -2837,7 +2837,7 @@
         <v>41</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" ht="21" spans="1:3">
@@ -2848,7 +2848,7 @@
         <v>42</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" ht="21" spans="1:3">
@@ -2859,7 +2859,7 @@
         <v>43</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" ht="21" spans="1:3">
@@ -2870,20 +2870,20 @@
         <v>44</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" ht="21" spans="2:3">
       <c r="B42" s="10"/>
       <c r="C42" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" ht="21" spans="1:3">
       <c r="A43" s="6"/>
       <c r="B43" s="10"/>
       <c r="C43" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" ht="21" spans="1:3">
@@ -2894,7 +2894,7 @@
         <v>46</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" ht="21" spans="1:3">
@@ -2905,7 +2905,7 @@
         <v>47</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" ht="21" spans="1:3">
@@ -2916,7 +2916,7 @@
         <v>48</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" ht="21" spans="1:3">
@@ -2927,7 +2927,7 @@
         <v>49</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" ht="21" spans="1:3">
@@ -2938,7 +2938,7 @@
         <v>50</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" ht="21" spans="1:3">
@@ -2949,7 +2949,7 @@
         <v>51</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" ht="21" spans="1:3">
@@ -2960,7 +2960,7 @@
         <v>52</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="51" ht="21" spans="1:3">
@@ -2971,7 +2971,7 @@
         <v>53</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" ht="21" spans="1:3">
@@ -2982,7 +2982,7 @@
         <v>54</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" ht="21" spans="1:3">
@@ -2993,7 +2993,7 @@
         <v>55</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" ht="21" spans="1:3">
@@ -3009,7 +3009,7 @@
         <v>57</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="57" ht="21" spans="1:3">
@@ -3020,7 +3020,7 @@
         <v>58</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="58" ht="21" spans="1:3">
@@ -3031,7 +3031,7 @@
         <v>59</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="59" ht="21" spans="1:3">
@@ -3042,7 +3042,7 @@
         <v>60</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="60" ht="21" spans="1:3">
@@ -3053,7 +3053,7 @@
         <v>61</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="61" ht="21" spans="1:3">
@@ -3064,7 +3064,7 @@
         <v>62</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="62" ht="21" spans="1:3">
@@ -3075,7 +3075,7 @@
         <v>63</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="63" ht="21" spans="1:3">
@@ -3086,7 +3086,7 @@
         <v>64</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" ht="21" spans="1:3">
@@ -3097,7 +3097,7 @@
         <v>65</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="65" ht="21" spans="1:3">
@@ -3108,7 +3108,7 @@
         <v>66</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="66" ht="21" spans="1:3">
@@ -3119,7 +3119,7 @@
         <v>67</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67" ht="21" spans="1:3">
@@ -3130,7 +3130,7 @@
         <v>68</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="68" ht="21" spans="1:3">
@@ -3141,7 +3141,7 @@
         <v>69</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="69" ht="21" spans="1:3">
@@ -3152,7 +3152,7 @@
         <v>70</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="70" ht="21" spans="1:3">
@@ -3163,7 +3163,7 @@
         <v>71</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="71" ht="21" spans="1:3">
@@ -3174,7 +3174,7 @@
         <v>72</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="72" ht="21" spans="1:3">
@@ -3185,7 +3185,7 @@
         <v>73</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="73" ht="21" spans="1:3">
@@ -3196,7 +3196,7 @@
         <v>74</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="74" ht="21" spans="1:3">
@@ -3207,7 +3207,7 @@
         <v>75</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="75" ht="21" spans="1:3">
@@ -3218,7 +3218,7 @@
         <v>76</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="76" ht="21" spans="1:3">
@@ -3229,7 +3229,7 @@
         <v>77</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="77" ht="21" spans="1:3">
@@ -3240,7 +3240,7 @@
         <v>78</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="78" ht="21" spans="1:3">
@@ -3251,7 +3251,7 @@
         <v>79</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="79" ht="21" spans="1:3">
@@ -3262,7 +3262,7 @@
         <v>80</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="80" ht="21" spans="1:3">
@@ -3273,7 +3273,7 @@
         <v>81</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="81" ht="21" spans="1:3">
@@ -3284,7 +3284,7 @@
         <v>82</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="82" ht="21" spans="1:3">
@@ -3295,7 +3295,7 @@
         <v>83</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="83" ht="21" spans="1:3">
@@ -3306,7 +3306,7 @@
         <v>84</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="84" ht="21" spans="1:3">
@@ -3317,7 +3317,7 @@
         <v>85</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="85" ht="21" spans="1:3">
@@ -3328,7 +3328,7 @@
         <v>86</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="86" ht="21" spans="1:3">
@@ -3339,7 +3339,7 @@
         <v>87</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="87" ht="21" spans="1:3">
@@ -3350,7 +3350,7 @@
         <v>88</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="88" ht="21" spans="1:3">
@@ -3361,7 +3361,7 @@
         <v>89</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="89" ht="21" spans="1:3">
@@ -3372,7 +3372,7 @@
         <v>90</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="90" ht="21" spans="1:3">
@@ -3383,7 +3383,7 @@
         <v>91</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="91" ht="21" spans="1:3">
@@ -3394,7 +3394,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="92" ht="21" spans="1:3">
@@ -3405,7 +3405,7 @@
         <v>93</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="93" ht="21" spans="1:3">
@@ -3416,7 +3416,7 @@
         <v>94</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="94" ht="21" spans="1:3">
@@ -3427,7 +3427,7 @@
         <v>95</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="95" ht="21" spans="1:3">
@@ -3438,7 +3438,7 @@
         <v>96</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="96" ht="21" spans="1:3">
@@ -3449,7 +3449,7 @@
         <v>97</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="97" ht="21" spans="1:3">
@@ -3460,7 +3460,7 @@
         <v>98</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="98" ht="21" spans="1:3">
@@ -3471,7 +3471,7 @@
         <v>99</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="100" ht="21" spans="1:3">
@@ -3487,7 +3487,7 @@
         <v>101</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="102" ht="21" spans="1:3">
@@ -3498,7 +3498,7 @@
         <v>102</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="103" ht="21" spans="1:3">
@@ -3509,7 +3509,7 @@
         <v>103</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="104" ht="21" spans="1:3">
@@ -3520,7 +3520,7 @@
         <v>104</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="105" ht="21" spans="1:3">
@@ -3531,7 +3531,7 @@
         <v>105</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="106" ht="21" spans="1:3">
@@ -3542,7 +3542,7 @@
         <v>106</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="107" ht="21" spans="1:3">
@@ -3553,7 +3553,7 @@
         <v>107</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="108" ht="21" spans="1:3">
@@ -3564,7 +3564,7 @@
         <v>108</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="109" ht="21" spans="1:3">
@@ -3575,7 +3575,7 @@
         <v>109</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="110" ht="21" spans="1:3">
@@ -3586,7 +3586,7 @@
         <v>110</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="111" ht="21" spans="1:3">
@@ -3597,7 +3597,7 @@
         <v>111</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="112" ht="21" spans="1:3">
@@ -3608,7 +3608,7 @@
         <v>112</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="113" ht="21" spans="1:3">
@@ -3619,7 +3619,7 @@
         <v>113</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="114" ht="21" spans="1:3">
@@ -3630,7 +3630,7 @@
         <v>114</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="115" ht="21" spans="1:3">
@@ -3641,7 +3641,7 @@
         <v>115</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="116" ht="21" spans="1:3">
@@ -3652,7 +3652,7 @@
         <v>116</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="117" ht="21" spans="1:3">
@@ -3663,7 +3663,7 @@
         <v>117</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="118" ht="21" spans="1:3">
@@ -3674,7 +3674,7 @@
         <v>118</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="119" ht="21" spans="1:3">
@@ -3685,7 +3685,7 @@
         <v>119</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="120" ht="21" spans="1:3">
@@ -3696,7 +3696,7 @@
         <v>120</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="121" ht="21" spans="1:3">
@@ -3707,7 +3707,7 @@
         <v>121</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="122" ht="21" spans="1:3">
@@ -3718,7 +3718,7 @@
         <v>122</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="123" ht="21" spans="1:3">
@@ -3729,7 +3729,7 @@
         <v>123</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="124" ht="21" spans="1:3">
@@ -3740,7 +3740,7 @@
         <v>124</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="125" ht="21" spans="1:3">
@@ -3751,7 +3751,7 @@
         <v>125</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="126" ht="21" spans="1:3">
@@ -3762,7 +3762,7 @@
         <v>126</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="127" ht="21" spans="1:3">
@@ -3773,7 +3773,7 @@
         <v>127</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="128" ht="21" spans="1:3">
@@ -3784,7 +3784,7 @@
         <v>128</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="129" ht="21" spans="1:3">
@@ -3795,7 +3795,7 @@
         <v>129</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="130" ht="21" spans="1:3">
@@ -3806,7 +3806,7 @@
         <v>130</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="131" ht="21" spans="1:3">
@@ -3817,7 +3817,7 @@
         <v>131</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="132" ht="21" spans="1:3">
@@ -3828,7 +3828,7 @@
         <v>132</v>
       </c>
       <c r="C132" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="133" ht="21" spans="1:3">
@@ -3839,7 +3839,7 @@
         <v>133</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="134" ht="21" spans="1:3">
@@ -3850,7 +3850,7 @@
         <v>134</v>
       </c>
       <c r="C134" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="135" ht="21" spans="1:3">
@@ -3861,7 +3861,7 @@
         <v>135</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="136" ht="21" spans="1:3">
@@ -3872,7 +3872,7 @@
         <v>136</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="138" ht="21" spans="2:3">
@@ -3887,7 +3887,7 @@
         <v>138</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="140" ht="21" spans="1:3">
@@ -3898,7 +3898,7 @@
         <v>139</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="141" ht="21" spans="1:3">
@@ -3909,7 +3909,7 @@
         <v>140</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="142" ht="21" spans="1:3">
@@ -3920,7 +3920,7 @@
         <v>141</v>
       </c>
       <c r="C142" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="143" ht="21" spans="1:3">
@@ -3931,7 +3931,7 @@
         <v>142</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="144" ht="21" spans="1:3">
@@ -3942,7 +3942,7 @@
         <v>143</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="145" ht="21" spans="1:3">
@@ -3953,7 +3953,7 @@
         <v>144</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="146" ht="21" spans="1:3">
@@ -3964,7 +3964,7 @@
         <v>145</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="147" ht="21" spans="1:3">
@@ -3975,7 +3975,7 @@
         <v>146</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="148" ht="21" spans="1:3">
@@ -3986,7 +3986,7 @@
         <v>147</v>
       </c>
       <c r="C148" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="149" ht="21" spans="1:3">
@@ -3997,7 +3997,7 @@
         <v>148</v>
       </c>
       <c r="C149" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="150" ht="21" spans="1:3">
@@ -4008,7 +4008,7 @@
         <v>149</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="151" ht="21" spans="1:3">
@@ -4019,7 +4019,7 @@
         <v>150</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="152" ht="21" spans="1:3">
@@ -4030,7 +4030,7 @@
         <v>151</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="153" ht="21" spans="1:3">
@@ -4041,7 +4041,7 @@
         <v>152</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="154" ht="21" spans="1:3">
@@ -4052,7 +4052,7 @@
         <v>153</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="155" ht="21" spans="1:3">
@@ -4063,7 +4063,7 @@
         <v>154</v>
       </c>
       <c r="C155" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="156" ht="21" spans="1:3">
@@ -4074,7 +4074,7 @@
         <v>155</v>
       </c>
       <c r="C156" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="157" ht="21" spans="1:3">
@@ -4085,7 +4085,7 @@
         <v>156</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="158" ht="21" spans="1:3">
@@ -4096,7 +4096,7 @@
         <v>157</v>
       </c>
       <c r="C158" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="159" ht="21" spans="1:3">
@@ -4107,7 +4107,7 @@
         <v>158</v>
       </c>
       <c r="C159" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="160" ht="21" spans="1:3">
@@ -4118,7 +4118,7 @@
         <v>159</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="161" ht="21" spans="1:3">
@@ -4129,7 +4129,7 @@
         <v>160</v>
       </c>
       <c r="C161" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="162" ht="21" spans="1:3">
@@ -4140,7 +4140,7 @@
         <v>161</v>
       </c>
       <c r="C162" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="163" ht="21" spans="1:3">
@@ -4151,7 +4151,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="164" ht="21" spans="1:3">
@@ -4162,7 +4162,7 @@
         <v>163</v>
       </c>
       <c r="C164" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="165" ht="21" spans="1:3">
@@ -4173,7 +4173,7 @@
         <v>164</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="166" ht="21" spans="1:3">
@@ -4184,7 +4184,7 @@
         <v>165</v>
       </c>
       <c r="C166" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="167" ht="21" spans="1:3">
@@ -4195,7 +4195,7 @@
         <v>166</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="168" ht="21" spans="1:3">
@@ -4206,7 +4206,7 @@
         <v>167</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="169" ht="21" spans="1:3">
@@ -4217,7 +4217,7 @@
         <v>168</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="170" ht="21" spans="1:3">
@@ -4228,7 +4228,7 @@
         <v>169</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="171" ht="21" spans="1:3">
@@ -4239,7 +4239,7 @@
         <v>170</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="172" ht="21" spans="1:3">
@@ -4250,7 +4250,7 @@
         <v>171</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="173" ht="21" spans="1:3">
@@ -4261,7 +4261,7 @@
         <v>172</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="174" ht="21" spans="1:3">
@@ -4272,7 +4272,7 @@
         <v>173</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="176" ht="21" spans="2:3">
@@ -4463,7 +4463,7 @@
         <v>191</v>
       </c>
       <c r="C193" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="194" ht="21" spans="1:3">
@@ -4507,7 +4507,7 @@
         <v>196</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="198" ht="21" spans="1:3">
@@ -4518,7 +4518,7 @@
         <v>197</v>
       </c>
       <c r="C198" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="199" ht="21" spans="1:3">
@@ -4529,7 +4529,7 @@
         <v>198</v>
       </c>
       <c r="C199" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="200" ht="21" spans="1:3">
@@ -4540,7 +4540,7 @@
         <v>199</v>
       </c>
       <c r="C200" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="201" ht="21" spans="1:3">
@@ -4551,7 +4551,7 @@
         <v>200</v>
       </c>
       <c r="C201" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="202" ht="21" spans="1:3">
@@ -4562,7 +4562,7 @@
         <v>201</v>
       </c>
       <c r="C202" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="203" ht="21" spans="1:3">
@@ -4573,7 +4573,7 @@
         <v>202</v>
       </c>
       <c r="C203" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="204" ht="21" spans="1:3">
@@ -4584,7 +4584,7 @@
         <v>203</v>
       </c>
       <c r="C204" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="205" ht="21" spans="1:3">
@@ -4595,7 +4595,7 @@
         <v>204</v>
       </c>
       <c r="C205" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="206" ht="21" spans="1:3">
@@ -4606,7 +4606,7 @@
         <v>205</v>
       </c>
       <c r="C206" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="207" ht="21" spans="1:3">
@@ -4617,7 +4617,7 @@
         <v>206</v>
       </c>
       <c r="C207" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="208" ht="21" spans="1:3">
@@ -4628,7 +4628,7 @@
         <v>207</v>
       </c>
       <c r="C208" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="209" ht="21" spans="1:3">
@@ -4639,7 +4639,7 @@
         <v>208</v>
       </c>
       <c r="C209" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="210" ht="21" spans="1:3">
@@ -4650,7 +4650,7 @@
         <v>209</v>
       </c>
       <c r="C210" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="211" ht="21" spans="1:3">
@@ -4661,7 +4661,7 @@
         <v>210</v>
       </c>
       <c r="C211" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="212" ht="21" spans="1:3">
@@ -4682,7 +4682,7 @@
         <v>212</v>
       </c>
       <c r="C214" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="215" ht="21" spans="1:3">
@@ -4693,7 +4693,7 @@
         <v>213</v>
       </c>
       <c r="C215" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="216" ht="21" spans="1:3">
@@ -4704,7 +4704,7 @@
         <v>214</v>
       </c>
       <c r="C216" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="217" ht="21" spans="1:3">
@@ -4715,7 +4715,7 @@
         <v>215</v>
       </c>
       <c r="C217" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="218" ht="21" spans="1:3">
@@ -4726,7 +4726,7 @@
         <v>216</v>
       </c>
       <c r="C218" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="219" ht="21" spans="1:3">
@@ -4737,7 +4737,7 @@
         <v>217</v>
       </c>
       <c r="C219" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="220" ht="21" spans="1:3">
@@ -4748,7 +4748,7 @@
         <v>218</v>
       </c>
       <c r="C220" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="221" ht="21" spans="1:3">
@@ -4759,7 +4759,7 @@
         <v>219</v>
       </c>
       <c r="C221" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="222" ht="21" spans="1:3">
@@ -4770,7 +4770,7 @@
         <v>220</v>
       </c>
       <c r="C222" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="223" ht="21" spans="1:3">
@@ -4781,7 +4781,7 @@
         <v>221</v>
       </c>
       <c r="C223" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="224" ht="21" spans="1:3">
@@ -4792,7 +4792,7 @@
         <v>222</v>
       </c>
       <c r="C224" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="225" ht="21" spans="1:3">
@@ -4803,7 +4803,7 @@
         <v>223</v>
       </c>
       <c r="C225" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="226" ht="21" spans="1:3">
@@ -4814,7 +4814,7 @@
         <v>224</v>
       </c>
       <c r="C226" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="227" ht="21" spans="1:3">
@@ -4825,7 +4825,7 @@
         <v>225</v>
       </c>
       <c r="C227" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="228" ht="21" spans="1:3">
@@ -4836,7 +4836,7 @@
         <v>226</v>
       </c>
       <c r="C228" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="229" ht="21" spans="1:3">
@@ -4847,7 +4847,7 @@
         <v>227</v>
       </c>
       <c r="C229" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="230" ht="21" spans="1:3">
@@ -4858,7 +4858,7 @@
         <v>228</v>
       </c>
       <c r="C230" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="231" ht="21" spans="1:3">
@@ -4869,7 +4869,7 @@
         <v>229</v>
       </c>
       <c r="C231" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="232" ht="21" spans="1:3">
@@ -4880,7 +4880,7 @@
         <v>230</v>
       </c>
       <c r="C232" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="233" ht="21" spans="1:3">
@@ -4891,7 +4891,7 @@
         <v>231</v>
       </c>
       <c r="C233" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="234" ht="21" spans="1:3">
@@ -4902,7 +4902,7 @@
         <v>232</v>
       </c>
       <c r="C234" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="235" ht="21" spans="1:3">
@@ -4913,7 +4913,7 @@
         <v>233</v>
       </c>
       <c r="C235" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="236" ht="21" spans="2:3">
@@ -4932,7 +4932,7 @@
         <v>235</v>
       </c>
       <c r="C238" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="239" ht="21" spans="1:3">
@@ -4943,7 +4943,7 @@
         <v>236</v>
       </c>
       <c r="C239" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="240" ht="21" spans="1:3">
@@ -4954,7 +4954,7 @@
         <v>237</v>
       </c>
       <c r="C240" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="241" ht="21" spans="1:3">
@@ -4965,7 +4965,7 @@
         <v>238</v>
       </c>
       <c r="C241" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="242" ht="21" spans="1:3">
@@ -4987,7 +4987,7 @@
         <v>241</v>
       </c>
       <c r="C243" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="244" ht="21" spans="1:3">
@@ -4998,7 +4998,7 @@
         <v>242</v>
       </c>
       <c r="C244" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="245" ht="21" spans="1:3">
@@ -5009,7 +5009,7 @@
         <v>243</v>
       </c>
       <c r="C245" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="246" ht="21" spans="1:3">
@@ -5020,7 +5020,7 @@
         <v>244</v>
       </c>
       <c r="C246" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="247" ht="21" spans="1:3">
@@ -5031,7 +5031,7 @@
         <v>245</v>
       </c>
       <c r="C247" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="248" ht="21" spans="1:3">
@@ -5042,7 +5042,7 @@
         <v>246</v>
       </c>
       <c r="C248" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="249" ht="21" spans="1:3">
@@ -5053,7 +5053,7 @@
         <v>247</v>
       </c>
       <c r="C249" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="250" ht="21" spans="1:3">
@@ -5064,7 +5064,7 @@
         <v>248</v>
       </c>
       <c r="C250" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="251" ht="21" spans="1:3">
@@ -5075,7 +5075,7 @@
         <v>249</v>
       </c>
       <c r="C251" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="252" ht="21" spans="1:3">
@@ -5086,7 +5086,7 @@
         <v>250</v>
       </c>
       <c r="C252" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="253" ht="21" spans="1:3">
@@ -5097,7 +5097,7 @@
         <v>251</v>
       </c>
       <c r="C253" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="254" ht="21" spans="1:3">
@@ -5108,7 +5108,7 @@
         <v>252</v>
       </c>
       <c r="C254" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="255" ht="21" spans="1:3">
@@ -5119,7 +5119,7 @@
         <v>253</v>
       </c>
       <c r="C255" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="256" ht="21" spans="1:3">
@@ -5130,7 +5130,7 @@
         <v>254</v>
       </c>
       <c r="C256" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="257" ht="21" spans="1:3">
@@ -5141,7 +5141,7 @@
         <v>255</v>
       </c>
       <c r="C257" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="258" ht="21" spans="1:3">
@@ -5152,7 +5152,7 @@
         <v>256</v>
       </c>
       <c r="C258" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="259" ht="21" spans="1:3">
@@ -5163,7 +5163,7 @@
         <v>257</v>
       </c>
       <c r="C259" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="260" ht="21" spans="1:3">
@@ -5174,7 +5174,7 @@
         <v>258</v>
       </c>
       <c r="C260" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="261" ht="21" spans="1:3">
@@ -5185,7 +5185,7 @@
         <v>259</v>
       </c>
       <c r="C261" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="262" ht="21" spans="1:3">
@@ -5196,7 +5196,7 @@
         <v>260</v>
       </c>
       <c r="C262" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="263" ht="21" spans="1:3">
@@ -5207,7 +5207,7 @@
         <v>261</v>
       </c>
       <c r="C263" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="264" ht="21" spans="1:3">
@@ -5218,7 +5218,7 @@
         <v>262</v>
       </c>
       <c r="C264" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="265" ht="21" spans="1:3">
@@ -5229,7 +5229,7 @@
         <v>263</v>
       </c>
       <c r="C265" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="266" ht="21" spans="1:3">
@@ -5240,7 +5240,7 @@
         <v>264</v>
       </c>
       <c r="C266" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="267" ht="21" spans="1:3">
@@ -5251,7 +5251,7 @@
         <v>265</v>
       </c>
       <c r="C267" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="268" ht="21" spans="1:3">
@@ -5262,7 +5262,7 @@
         <v>266</v>
       </c>
       <c r="C268" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="269" ht="21" spans="1:3">
@@ -5273,7 +5273,7 @@
         <v>267</v>
       </c>
       <c r="C269" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="270" ht="21" spans="1:3">
@@ -5284,7 +5284,7 @@
         <v>268</v>
       </c>
       <c r="C270" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="271" ht="21" spans="1:3">
@@ -5295,7 +5295,7 @@
         <v>90</v>
       </c>
       <c r="C271" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="272" ht="21" spans="1:3">
@@ -5306,7 +5306,7 @@
         <v>269</v>
       </c>
       <c r="C272" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="273" ht="21" spans="2:3">
@@ -5325,7 +5325,7 @@
         <v>271</v>
       </c>
       <c r="C275" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="276" ht="21" spans="1:3">
@@ -5336,7 +5336,7 @@
         <v>272</v>
       </c>
       <c r="C276" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="277" ht="21" spans="1:3">
@@ -5347,7 +5347,7 @@
         <v>273</v>
       </c>
       <c r="C277" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="278" ht="21" spans="1:3">
@@ -5358,7 +5358,7 @@
         <v>274</v>
       </c>
       <c r="C278" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="279" ht="21" spans="1:3">
@@ -5369,7 +5369,7 @@
         <v>275</v>
       </c>
       <c r="C279" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="280" ht="21" spans="1:3">
@@ -5380,7 +5380,7 @@
         <v>276</v>
       </c>
       <c r="C280" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="281" ht="21" spans="1:3">
@@ -5391,7 +5391,7 @@
         <v>277</v>
       </c>
       <c r="C281" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="282" ht="21" spans="1:3">
@@ -5402,7 +5402,7 @@
         <v>278</v>
       </c>
       <c r="C282" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="283" ht="21" spans="1:3">
@@ -5413,7 +5413,7 @@
         <v>279</v>
       </c>
       <c r="C283" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="284" ht="21" spans="1:3">
@@ -5424,7 +5424,7 @@
         <v>280</v>
       </c>
       <c r="C284" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="285" ht="21" spans="1:3">
@@ -5435,7 +5435,7 @@
         <v>281</v>
       </c>
       <c r="C285" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="286" ht="21" spans="1:3">
@@ -5446,7 +5446,7 @@
         <v>282</v>
       </c>
       <c r="C286" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="287" ht="21" spans="1:3">
@@ -5457,7 +5457,7 @@
         <v>283</v>
       </c>
       <c r="C287" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="288" ht="21" spans="1:3">
@@ -5468,7 +5468,7 @@
         <v>284</v>
       </c>
       <c r="C288" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="289" ht="21" spans="1:3">
@@ -5479,7 +5479,7 @@
         <v>285</v>
       </c>
       <c r="C289" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="290" ht="21" spans="1:3">
@@ -5490,7 +5490,7 @@
         <v>286</v>
       </c>
       <c r="C290" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="291" ht="21" spans="1:3">
@@ -5501,7 +5501,7 @@
         <v>287</v>
       </c>
       <c r="C291" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="292" ht="21" spans="1:3">
@@ -5512,7 +5512,7 @@
         <v>288</v>
       </c>
       <c r="C292" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="293" ht="21" spans="1:3">
@@ -5523,7 +5523,7 @@
         <v>289</v>
       </c>
       <c r="C293" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="294" ht="21" spans="2:3">
@@ -5542,7 +5542,7 @@
         <v>291</v>
       </c>
       <c r="C296" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="297" ht="21" spans="1:3">
@@ -5553,7 +5553,7 @@
         <v>292</v>
       </c>
       <c r="C297" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="298" ht="21" spans="1:3">
@@ -5564,7 +5564,7 @@
         <v>293</v>
       </c>
       <c r="C298" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="299" ht="21" spans="1:3">
@@ -5575,7 +5575,7 @@
         <v>294</v>
       </c>
       <c r="C299" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="300" ht="21" spans="1:3">
@@ -5586,7 +5586,7 @@
         <v>295</v>
       </c>
       <c r="C300" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="301" ht="21" spans="1:3">
@@ -5597,7 +5597,7 @@
         <v>296</v>
       </c>
       <c r="C301" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="302" ht="21" spans="1:3">
@@ -5608,7 +5608,7 @@
         <v>297</v>
       </c>
       <c r="C302" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="303" ht="21" spans="1:3">
@@ -5619,7 +5619,7 @@
         <v>298</v>
       </c>
       <c r="C303" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="304" ht="21" spans="1:3">
@@ -5630,7 +5630,7 @@
         <v>299</v>
       </c>
       <c r="C304" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="305" ht="21" spans="1:3">
@@ -5641,7 +5641,7 @@
         <v>300</v>
       </c>
       <c r="C305" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="306" ht="21" spans="1:3">
@@ -5652,7 +5652,7 @@
         <v>301</v>
       </c>
       <c r="C306" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="307" ht="21" spans="1:3">
@@ -5663,7 +5663,7 @@
         <v>302</v>
       </c>
       <c r="C307" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="308" ht="21" spans="1:3">
@@ -5674,7 +5674,7 @@
         <v>303</v>
       </c>
       <c r="C308" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="309" ht="21" spans="1:3">
@@ -5685,7 +5685,7 @@
         <v>304</v>
       </c>
       <c r="C309" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="310" ht="21" spans="1:3">
@@ -5696,7 +5696,7 @@
         <v>305</v>
       </c>
       <c r="C310" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="311" ht="21" spans="1:3">
@@ -5707,7 +5707,7 @@
         <v>306</v>
       </c>
       <c r="C311" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="312" ht="21" spans="1:3">
@@ -5718,7 +5718,7 @@
         <v>307</v>
       </c>
       <c r="C312" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="313" ht="21" spans="1:3">
@@ -5729,7 +5729,7 @@
         <v>308</v>
       </c>
       <c r="C313" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="314" ht="21" spans="1:3">
@@ -5740,7 +5740,7 @@
         <v>309</v>
       </c>
       <c r="C314" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="315" ht="21" spans="1:3">
@@ -5751,7 +5751,7 @@
         <v>310</v>
       </c>
       <c r="C315" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="316" ht="21" spans="1:3">
@@ -5762,7 +5762,7 @@
         <v>311</v>
       </c>
       <c r="C316" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="317" ht="21" spans="1:3">
@@ -5773,7 +5773,7 @@
         <v>312</v>
       </c>
       <c r="C317" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="318" ht="21" spans="1:3">
@@ -5784,7 +5784,7 @@
         <v>313</v>
       </c>
       <c r="C318" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="319" ht="21" spans="1:3">
@@ -5795,7 +5795,7 @@
         <v>314</v>
       </c>
       <c r="C319" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="320" ht="21" spans="1:3">
@@ -5806,7 +5806,7 @@
         <v>315</v>
       </c>
       <c r="C320" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="321" ht="21" spans="1:3">
@@ -5817,7 +5817,7 @@
         <v>316</v>
       </c>
       <c r="C321" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="322" ht="21" spans="1:3">
@@ -5828,7 +5828,7 @@
         <v>317</v>
       </c>
       <c r="C322" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="323" ht="21" spans="1:3">
@@ -5839,7 +5839,7 @@
         <v>318</v>
       </c>
       <c r="C323" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="324" ht="21" spans="1:3">
@@ -5850,7 +5850,7 @@
         <v>319</v>
       </c>
       <c r="C324" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="325" ht="21" spans="1:3">
@@ -5861,7 +5861,7 @@
         <v>320</v>
       </c>
       <c r="C325" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="326" ht="21" spans="1:3">
@@ -5872,7 +5872,7 @@
         <v>321</v>
       </c>
       <c r="C326" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="327" ht="21" spans="1:3">
@@ -5883,7 +5883,7 @@
         <v>322</v>
       </c>
       <c r="C327" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="328" ht="21" spans="1:3">
@@ -5894,7 +5894,7 @@
         <v>323</v>
       </c>
       <c r="C328" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="329" ht="21" spans="1:3">
@@ -5905,7 +5905,7 @@
         <v>324</v>
       </c>
       <c r="C329" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="330" ht="21" spans="1:3">
@@ -5916,7 +5916,7 @@
         <v>325</v>
       </c>
       <c r="C330" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="331" ht="21" spans="1:3">
@@ -5927,7 +5927,7 @@
         <v>326</v>
       </c>
       <c r="C331" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="332" ht="21" spans="1:3">
@@ -5938,7 +5938,7 @@
         <v>327</v>
       </c>
       <c r="C332" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="333" ht="21" spans="1:3">
@@ -5949,7 +5949,7 @@
         <v>328</v>
       </c>
       <c r="C333" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="334" ht="21" spans="2:3">
@@ -5968,7 +5968,7 @@
         <v>330</v>
       </c>
       <c r="C336" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="337" ht="21" spans="1:3">
@@ -5979,7 +5979,7 @@
         <v>331</v>
       </c>
       <c r="C337" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="338" ht="21" spans="1:3">
@@ -5990,7 +5990,7 @@
         <v>332</v>
       </c>
       <c r="C338" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="339" ht="21" spans="1:3">
@@ -6001,7 +6001,7 @@
         <v>333</v>
       </c>
       <c r="C339" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="340" ht="21" spans="1:3">
@@ -6012,7 +6012,7 @@
         <v>334</v>
       </c>
       <c r="C340" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="341" ht="21" spans="1:3">
@@ -6023,7 +6023,7 @@
         <v>335</v>
       </c>
       <c r="C341" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="342" ht="21" spans="1:3">
@@ -6034,7 +6034,7 @@
         <v>336</v>
       </c>
       <c r="C342" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="343" ht="21" spans="1:3">
@@ -6045,7 +6045,7 @@
         <v>337</v>
       </c>
       <c r="C343" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="344" ht="21" spans="1:3">
@@ -6056,7 +6056,7 @@
         <v>338</v>
       </c>
       <c r="C344" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="345" ht="21" spans="1:3">
@@ -6067,7 +6067,7 @@
         <v>339</v>
       </c>
       <c r="C345" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="346" ht="21" spans="1:3">
@@ -6078,7 +6078,7 @@
         <v>340</v>
       </c>
       <c r="C346" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="347" ht="21" spans="1:3">
@@ -6089,7 +6089,7 @@
         <v>341</v>
       </c>
       <c r="C347" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="348" ht="21" spans="1:3">
@@ -6100,7 +6100,7 @@
         <v>342</v>
       </c>
       <c r="C348" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="349" ht="21" spans="1:3">
@@ -6111,7 +6111,7 @@
         <v>343</v>
       </c>
       <c r="C349" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="350" ht="21" spans="1:3">
@@ -6122,7 +6122,7 @@
         <v>344</v>
       </c>
       <c r="C350" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="351" ht="21" spans="1:3">
@@ -6133,7 +6133,7 @@
         <v>345</v>
       </c>
       <c r="C351" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="352" ht="21" spans="1:3">
@@ -6144,7 +6144,7 @@
         <v>346</v>
       </c>
       <c r="C352" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="353" ht="21" spans="1:3">
@@ -6155,7 +6155,7 @@
         <v>347</v>
       </c>
       <c r="C353" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="354" ht="21" spans="2:3">
@@ -6174,7 +6174,7 @@
         <v>349</v>
       </c>
       <c r="C356" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="357" ht="21" spans="1:3">
@@ -6251,7 +6251,7 @@
         <v>356</v>
       </c>
       <c r="C363" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="364" ht="21" spans="1:3">
@@ -6262,7 +6262,7 @@
         <v>357</v>
       </c>
       <c r="C364" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="365" ht="21" spans="1:3">
@@ -6273,7 +6273,7 @@
         <v>358</v>
       </c>
       <c r="C365" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="366" ht="21" spans="1:3">
@@ -6284,7 +6284,7 @@
         <v>359</v>
       </c>
       <c r="C366" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="367" ht="21" spans="1:3">
@@ -6295,7 +6295,7 @@
         <v>360</v>
       </c>
       <c r="C367" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="368" ht="21" spans="1:3">
@@ -6306,7 +6306,7 @@
         <v>361</v>
       </c>
       <c r="C368" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="369" ht="21" spans="1:3">
@@ -6317,7 +6317,7 @@
         <v>362</v>
       </c>
       <c r="C369" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="370" ht="21" spans="1:3">
@@ -6328,7 +6328,7 @@
         <v>363</v>
       </c>
       <c r="C370" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="371" ht="21" spans="1:3">
@@ -6339,7 +6339,7 @@
         <v>364</v>
       </c>
       <c r="C371" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="372" ht="21" spans="1:3">
@@ -6350,7 +6350,7 @@
         <v>365</v>
       </c>
       <c r="C372" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="373" ht="21" spans="1:3">
@@ -6361,7 +6361,7 @@
         <v>366</v>
       </c>
       <c r="C373" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="374" ht="21" spans="1:3">
@@ -6372,7 +6372,7 @@
         <v>367</v>
       </c>
       <c r="C374" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="375" ht="21" spans="1:3">
@@ -6383,7 +6383,7 @@
         <v>368</v>
       </c>
       <c r="C375" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="376" ht="21" spans="1:3">
@@ -6394,7 +6394,7 @@
         <v>369</v>
       </c>
       <c r="C376" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="377" ht="21" spans="1:3">
@@ -6405,7 +6405,7 @@
         <v>370</v>
       </c>
       <c r="C377" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="378" ht="21" spans="1:3">
@@ -6416,7 +6416,7 @@
         <v>371</v>
       </c>
       <c r="C378" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="379" ht="21" spans="1:3">
@@ -6427,7 +6427,7 @@
         <v>372</v>
       </c>
       <c r="C379" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="380" ht="21" spans="1:3">
@@ -6438,7 +6438,7 @@
         <v>373</v>
       </c>
       <c r="C380" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="381" ht="21" spans="1:3">
@@ -6449,7 +6449,7 @@
         <v>374</v>
       </c>
       <c r="C381" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="382" ht="21" spans="1:3">
@@ -6460,7 +6460,7 @@
         <v>375</v>
       </c>
       <c r="C382" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="383" ht="21" spans="1:3">
@@ -6471,7 +6471,7 @@
         <v>376</v>
       </c>
       <c r="C383" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="384" ht="21" spans="1:3">
@@ -6482,7 +6482,7 @@
         <v>377</v>
       </c>
       <c r="C384" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="385" ht="21" spans="1:3">
@@ -6493,7 +6493,7 @@
         <v>378</v>
       </c>
       <c r="C385" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="386" ht="21" spans="1:3">
@@ -6504,7 +6504,7 @@
         <v>379</v>
       </c>
       <c r="C386" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="387" ht="21" spans="1:3">
@@ -6515,7 +6515,7 @@
         <v>380</v>
       </c>
       <c r="C387" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="388" ht="21" spans="1:3">
@@ -6526,7 +6526,7 @@
         <v>381</v>
       </c>
       <c r="C388" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="389" ht="21" spans="1:3">
@@ -6537,7 +6537,7 @@
         <v>382</v>
       </c>
       <c r="C389" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="390" ht="21" spans="1:3">
@@ -6548,7 +6548,7 @@
         <v>382</v>
       </c>
       <c r="C390" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="391" ht="21" spans="1:3">
@@ -6559,7 +6559,7 @@
         <v>383</v>
       </c>
       <c r="C391" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="392" ht="21" spans="1:3">
@@ -6570,7 +6570,7 @@
         <v>384</v>
       </c>
       <c r="C392" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="393" ht="21" spans="1:3">
@@ -6581,7 +6581,7 @@
         <v>385</v>
       </c>
       <c r="C393" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="394" ht="21" spans="1:3">
@@ -6592,7 +6592,7 @@
         <v>386</v>
       </c>
       <c r="C394" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="395" ht="21" spans="1:3">
@@ -6603,7 +6603,7 @@
         <v>387</v>
       </c>
       <c r="C395" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="396" ht="21" spans="1:3">
@@ -6614,7 +6614,7 @@
         <v>388</v>
       </c>
       <c r="C396" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="397" ht="21" spans="1:3">
@@ -6625,7 +6625,7 @@
         <v>389</v>
       </c>
       <c r="C397" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="398" ht="21" spans="1:3">
@@ -6636,7 +6636,7 @@
         <v>390</v>
       </c>
       <c r="C398" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="399" ht="21" spans="1:3">
@@ -6647,7 +6647,7 @@
         <v>391</v>
       </c>
       <c r="C399" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="400" ht="21" spans="2:3">
@@ -6666,7 +6666,7 @@
         <v>393</v>
       </c>
       <c r="C402" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="403" ht="21" spans="1:3">
@@ -6677,7 +6677,7 @@
         <v>394</v>
       </c>
       <c r="C403" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="404" ht="21" spans="1:3">
@@ -6688,7 +6688,7 @@
         <v>395</v>
       </c>
       <c r="C404" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="405" ht="21" spans="1:3">
@@ -6699,7 +6699,7 @@
         <v>92</v>
       </c>
       <c r="C405" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="406" ht="21" spans="1:3">
@@ -6710,7 +6710,7 @@
         <v>396</v>
       </c>
       <c r="C406" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="407" ht="21" spans="1:3">
@@ -6721,7 +6721,7 @@
         <v>397</v>
       </c>
       <c r="C407" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="408" ht="21" spans="2:3">
@@ -6817,7 +6817,7 @@
         <v>278</v>
       </c>
       <c r="C417" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="418" ht="21" spans="1:3">
@@ -6828,7 +6828,7 @@
         <v>406</v>
       </c>
       <c r="C418" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="419" ht="21" spans="1:3">
@@ -6839,7 +6839,7 @@
         <v>407</v>
       </c>
       <c r="C419" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="420" ht="21" spans="1:3">
@@ -6850,7 +6850,7 @@
         <v>408</v>
       </c>
       <c r="C420" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="421" ht="21" spans="1:3">
@@ -6861,7 +6861,7 @@
         <v>409</v>
       </c>
       <c r="C421" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="422" ht="21" spans="1:3">
@@ -6872,7 +6872,7 @@
         <v>410</v>
       </c>
       <c r="C422" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="423" ht="21" spans="1:3">
@@ -6883,7 +6883,7 @@
         <v>411</v>
       </c>
       <c r="C423" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="424" ht="21" spans="1:3">
@@ -6894,7 +6894,7 @@
         <v>412</v>
       </c>
       <c r="C424" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="425" ht="21" spans="1:3">
@@ -6905,7 +6905,7 @@
         <v>413</v>
       </c>
       <c r="C425" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="426" ht="21" spans="1:3">
@@ -6916,7 +6916,7 @@
         <v>414</v>
       </c>
       <c r="C426" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="427" ht="21" spans="1:3">
@@ -6927,7 +6927,7 @@
         <v>415</v>
       </c>
       <c r="C427" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="428" ht="21" spans="1:3">
@@ -6938,7 +6938,7 @@
         <v>416</v>
       </c>
       <c r="C428" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="429" ht="21" spans="1:3">
@@ -6949,7 +6949,7 @@
         <v>417</v>
       </c>
       <c r="C429" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="430" ht="21" spans="1:3">
@@ -6960,7 +6960,7 @@
         <v>418</v>
       </c>
       <c r="C430" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="431" ht="21" spans="1:3">
@@ -6971,7 +6971,7 @@
         <v>419</v>
       </c>
       <c r="C431" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="432" ht="21" spans="1:3">
@@ -6982,7 +6982,7 @@
         <v>420</v>
       </c>
       <c r="C432" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="433" ht="21" spans="1:3">
@@ -6993,7 +6993,7 @@
         <v>421</v>
       </c>
       <c r="C433" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="434" ht="21" spans="1:3">
@@ -7004,7 +7004,7 @@
         <v>422</v>
       </c>
       <c r="C434" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="435" ht="21" spans="1:3">
@@ -7015,7 +7015,7 @@
         <v>423</v>
       </c>
       <c r="C435" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="436" ht="21" spans="1:3">
@@ -7026,7 +7026,7 @@
         <v>424</v>
       </c>
       <c r="C436" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="437" ht="21" spans="1:3">
@@ -7037,7 +7037,7 @@
         <v>425</v>
       </c>
       <c r="C437" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="438" ht="21" spans="1:3">
@@ -7048,7 +7048,7 @@
         <v>17</v>
       </c>
       <c r="C438" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="439" ht="21" spans="1:3">
@@ -7059,7 +7059,7 @@
         <v>426</v>
       </c>
       <c r="C439" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="440" ht="21" spans="1:3">
@@ -7070,7 +7070,7 @@
         <v>427</v>
       </c>
       <c r="C440" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="441" ht="21" spans="1:3">
@@ -7081,7 +7081,7 @@
         <v>428</v>
       </c>
       <c r="C441" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="442" ht="21" spans="1:3">
@@ -7092,7 +7092,7 @@
         <v>429</v>
       </c>
       <c r="C442" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="443" ht="21" spans="1:3">
@@ -7103,7 +7103,7 @@
         <v>430</v>
       </c>
       <c r="C443" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="444" ht="21" spans="1:3">
@@ -7114,7 +7114,7 @@
         <v>431</v>
       </c>
       <c r="C444" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="445" ht="21" spans="1:3">
@@ -7125,7 +7125,7 @@
         <v>432</v>
       </c>
       <c r="C445" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="446" ht="21" spans="1:3">
@@ -7136,7 +7136,7 @@
         <v>433</v>
       </c>
       <c r="C446" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="447" ht="21" spans="1:3">
@@ -7147,7 +7147,7 @@
         <v>434</v>
       </c>
       <c r="C447" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="448" ht="21" spans="1:3">
@@ -7158,7 +7158,7 @@
         <v>435</v>
       </c>
       <c r="C448" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="449" ht="21" spans="1:3">
@@ -7169,7 +7169,7 @@
         <v>436</v>
       </c>
       <c r="C449" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="450" ht="21" spans="1:3">
@@ -7180,7 +7180,7 @@
         <v>437</v>
       </c>
       <c r="C450" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="451" ht="21" spans="1:3">
@@ -7191,7 +7191,7 @@
         <v>438</v>
       </c>
       <c r="C451" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="452" ht="21" spans="1:3">
@@ -7202,7 +7202,7 @@
         <v>439</v>
       </c>
       <c r="C452" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="453" ht="21" spans="1:3">
@@ -7213,7 +7213,7 @@
         <v>440</v>
       </c>
       <c r="C453" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="454" ht="21" spans="1:3">
@@ -7224,7 +7224,7 @@
         <v>441</v>
       </c>
       <c r="C454" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="455" ht="21" spans="1:3">
@@ -7235,7 +7235,7 @@
         <v>442</v>
       </c>
       <c r="C455" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="456" ht="21" spans="1:3">
@@ -7246,7 +7246,7 @@
         <v>443</v>
       </c>
       <c r="C456" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="457" ht="21" spans="1:3">
@@ -7257,7 +7257,7 @@
         <v>444</v>
       </c>
       <c r="C457" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="458" ht="21" spans="1:3">
@@ -7268,7 +7268,7 @@
         <v>445</v>
       </c>
       <c r="C458" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="459" ht="21" spans="1:3">
@@ -7279,7 +7279,7 @@
         <v>446</v>
       </c>
       <c r="C459" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="460" ht="21" spans="1:3">
@@ -7290,7 +7290,7 @@
         <v>447</v>
       </c>
       <c r="C460" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="461" ht="21" spans="1:3">
@@ -7301,7 +7301,7 @@
         <v>448</v>
       </c>
       <c r="C461" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="462" ht="21" spans="1:3">
@@ -7312,7 +7312,7 @@
         <v>449</v>
       </c>
       <c r="C462" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="463" ht="21" spans="1:3">
@@ -7323,7 +7323,7 @@
         <v>450</v>
       </c>
       <c r="C463" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="464" ht="21" spans="1:3">
@@ -7334,7 +7334,7 @@
         <v>451</v>
       </c>
       <c r="C464" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="465" ht="21" spans="1:3">
@@ -7345,7 +7345,7 @@
         <v>452</v>
       </c>
       <c r="C465" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="466" ht="21" spans="1:3">
@@ -7356,7 +7356,7 @@
         <v>453</v>
       </c>
       <c r="C466" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="467" ht="21" spans="1:3">
@@ -7367,7 +7367,7 @@
         <v>454</v>
       </c>
       <c r="C467" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="468" ht="21" spans="1:3">
@@ -7378,7 +7378,7 @@
         <v>455</v>
       </c>
       <c r="C468" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="469" ht="21" spans="1:3">
@@ -7389,7 +7389,7 @@
         <v>456</v>
       </c>
       <c r="C469" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="470" ht="21" spans="2:3">
@@ -7409,7 +7409,7 @@
         <v>458</v>
       </c>
       <c r="C472" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="473" ht="21" spans="1:3">
@@ -7420,7 +7420,7 @@
         <v>459</v>
       </c>
       <c r="C473" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="474" ht="21" spans="1:3">
@@ -7431,7 +7431,7 @@
         <v>460</v>
       </c>
       <c r="C474" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="475" ht="21" spans="1:3">
@@ -7442,7 +7442,7 @@
         <v>461</v>
       </c>
       <c r="C475" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="476" ht="21" spans="1:3">
@@ -7453,7 +7453,7 @@
         <v>462</v>
       </c>
       <c r="C476" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="477" ht="21" spans="1:3">
@@ -7464,7 +7464,7 @@
         <v>463</v>
       </c>
       <c r="C477" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="478" ht="21" spans="1:3">
@@ -7475,7 +7475,7 @@
         <v>464</v>
       </c>
       <c r="C478" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="479" ht="21" spans="1:3">
@@ -7486,7 +7486,7 @@
         <v>465</v>
       </c>
       <c r="C479" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="480" ht="21" spans="1:3">
@@ -7497,7 +7497,7 @@
         <v>466</v>
       </c>
       <c r="C480" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="481" ht="21" spans="1:3">
@@ -7508,7 +7508,7 @@
         <v>467</v>
       </c>
       <c r="C481" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rearrange array element in alternating pos and neg position using 0(1) space
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -100,10 +100,10 @@
     <t>Rearrange the array in alternating positive and negative items with O(1) extra space</t>
   </si>
   <si>
+    <t>Find if there is any subarray with sum equal to 0</t>
+  </si>
+  <si>
     <t>&lt;-&gt;</t>
-  </si>
-  <si>
-    <t>Find if there is any subarray with sum equal to 0</t>
   </si>
   <si>
     <t>Find factorial of a large number</t>
@@ -1425,10 +1425,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1503,7 +1503,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1516,6 +1524,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -1524,24 +1546,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1594,16 +1601,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1612,13 +1618,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1638,8 +1637,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1660,19 +1660,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1690,6 +1684,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1702,7 +1720,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1714,13 +1792,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1732,109 +1834,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1845,15 +1845,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1913,11 +1904,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1945,149 +1934,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2440,8 +2440,8 @@
   <sheetPr/>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2693,8 +2693,8 @@
       <c r="B25" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>28</v>
+      <c r="C25" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="26" ht="21" spans="1:3">
@@ -2702,10 +2702,10 @@
         <v>6</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" ht="21" spans="1:3">
@@ -2716,7 +2716,7 @@
         <v>30</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" ht="21" spans="1:3">
@@ -2727,7 +2727,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" ht="21" spans="1:3">
@@ -2738,7 +2738,7 @@
         <v>32</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" ht="21" spans="1:3">
@@ -2749,7 +2749,7 @@
         <v>33</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" ht="21" spans="1:3">
@@ -2760,7 +2760,7 @@
         <v>34</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" ht="21" spans="1:3">
@@ -2771,7 +2771,7 @@
         <v>35</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" ht="21" spans="1:3">
@@ -2782,7 +2782,7 @@
         <v>36</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" ht="21" spans="1:3">
@@ -2793,7 +2793,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" ht="21" spans="1:3">
@@ -2804,7 +2804,7 @@
         <v>38</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" ht="21" spans="1:3">
@@ -2815,7 +2815,7 @@
         <v>39</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" ht="21" spans="1:3">
@@ -2826,7 +2826,7 @@
         <v>40</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" ht="21" spans="1:3">
@@ -2837,7 +2837,7 @@
         <v>41</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" ht="21" spans="1:3">
@@ -2848,7 +2848,7 @@
         <v>42</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" ht="21" spans="1:3">
@@ -2859,7 +2859,7 @@
         <v>43</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" ht="21" spans="1:3">
@@ -2870,20 +2870,20 @@
         <v>44</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" ht="21" spans="2:3">
       <c r="B42" s="10"/>
       <c r="C42" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" ht="21" spans="1:3">
       <c r="A43" s="6"/>
       <c r="B43" s="10"/>
       <c r="C43" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" ht="21" spans="1:3">
@@ -2894,7 +2894,7 @@
         <v>46</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" ht="21" spans="1:3">
@@ -2905,7 +2905,7 @@
         <v>47</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" ht="21" spans="1:3">
@@ -2916,7 +2916,7 @@
         <v>48</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" ht="21" spans="1:3">
@@ -2927,7 +2927,7 @@
         <v>49</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" ht="21" spans="1:3">
@@ -2938,7 +2938,7 @@
         <v>50</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" ht="21" spans="1:3">
@@ -2949,7 +2949,7 @@
         <v>51</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" ht="21" spans="1:3">
@@ -2960,7 +2960,7 @@
         <v>52</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" ht="21" spans="1:3">
@@ -2971,7 +2971,7 @@
         <v>53</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" ht="21" spans="1:3">
@@ -2982,7 +2982,7 @@
         <v>54</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" ht="21" spans="1:3">
@@ -2993,7 +2993,7 @@
         <v>55</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="55" ht="21" spans="1:3">
@@ -3009,7 +3009,7 @@
         <v>57</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="57" ht="21" spans="1:3">
@@ -3020,7 +3020,7 @@
         <v>58</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="58" ht="21" spans="1:3">
@@ -3031,7 +3031,7 @@
         <v>59</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59" ht="21" spans="1:3">
@@ -3042,7 +3042,7 @@
         <v>60</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="60" ht="21" spans="1:3">
@@ -3053,7 +3053,7 @@
         <v>61</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="61" ht="21" spans="1:3">
@@ -3064,7 +3064,7 @@
         <v>62</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="62" ht="21" spans="1:3">
@@ -3075,7 +3075,7 @@
         <v>63</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="63" ht="21" spans="1:3">
@@ -3086,7 +3086,7 @@
         <v>64</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="64" ht="21" spans="1:3">
@@ -3097,7 +3097,7 @@
         <v>65</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65" ht="21" spans="1:3">
@@ -3108,7 +3108,7 @@
         <v>66</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66" ht="21" spans="1:3">
@@ -3119,7 +3119,7 @@
         <v>67</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67" ht="21" spans="1:3">
@@ -3130,7 +3130,7 @@
         <v>68</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="68" ht="21" spans="1:3">
@@ -3141,7 +3141,7 @@
         <v>69</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="69" ht="21" spans="1:3">
@@ -3152,7 +3152,7 @@
         <v>70</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="70" ht="21" spans="1:3">
@@ -3163,7 +3163,7 @@
         <v>71</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="71" ht="21" spans="1:3">
@@ -3174,7 +3174,7 @@
         <v>72</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="72" ht="21" spans="1:3">
@@ -3185,7 +3185,7 @@
         <v>73</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="73" ht="21" spans="1:3">
@@ -3196,7 +3196,7 @@
         <v>74</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="74" ht="21" spans="1:3">
@@ -3207,7 +3207,7 @@
         <v>75</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="75" ht="21" spans="1:3">
@@ -3218,7 +3218,7 @@
         <v>76</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="76" ht="21" spans="1:3">
@@ -3229,7 +3229,7 @@
         <v>77</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="77" ht="21" spans="1:3">
@@ -3240,7 +3240,7 @@
         <v>78</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="78" ht="21" spans="1:3">
@@ -3251,7 +3251,7 @@
         <v>79</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="79" ht="21" spans="1:3">
@@ -3262,7 +3262,7 @@
         <v>80</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="80" ht="21" spans="1:3">
@@ -3273,7 +3273,7 @@
         <v>81</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="81" ht="21" spans="1:3">
@@ -3284,7 +3284,7 @@
         <v>82</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="82" ht="21" spans="1:3">
@@ -3295,7 +3295,7 @@
         <v>83</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="83" ht="21" spans="1:3">
@@ -3306,7 +3306,7 @@
         <v>84</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="84" ht="21" spans="1:3">
@@ -3317,7 +3317,7 @@
         <v>85</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="85" ht="21" spans="1:3">
@@ -3328,7 +3328,7 @@
         <v>86</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="86" ht="21" spans="1:3">
@@ -3339,7 +3339,7 @@
         <v>87</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="87" ht="21" spans="1:3">
@@ -3350,7 +3350,7 @@
         <v>88</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="88" ht="21" spans="1:3">
@@ -3361,7 +3361,7 @@
         <v>89</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="89" ht="21" spans="1:3">
@@ -3372,7 +3372,7 @@
         <v>90</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="90" ht="21" spans="1:3">
@@ -3383,7 +3383,7 @@
         <v>91</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="91" ht="21" spans="1:3">
@@ -3394,7 +3394,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="92" ht="21" spans="1:3">
@@ -3405,7 +3405,7 @@
         <v>93</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="93" ht="21" spans="1:3">
@@ -3416,7 +3416,7 @@
         <v>94</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="94" ht="21" spans="1:3">
@@ -3427,7 +3427,7 @@
         <v>95</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="95" ht="21" spans="1:3">
@@ -3438,7 +3438,7 @@
         <v>96</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="96" ht="21" spans="1:3">
@@ -3449,7 +3449,7 @@
         <v>97</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="97" ht="21" spans="1:3">
@@ -3460,7 +3460,7 @@
         <v>98</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="98" ht="21" spans="1:3">
@@ -3471,7 +3471,7 @@
         <v>99</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="100" ht="21" spans="1:3">
@@ -3487,7 +3487,7 @@
         <v>101</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="102" ht="21" spans="1:3">
@@ -3498,7 +3498,7 @@
         <v>102</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="103" ht="21" spans="1:3">
@@ -3509,7 +3509,7 @@
         <v>103</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="104" ht="21" spans="1:3">
@@ -3520,7 +3520,7 @@
         <v>104</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="105" ht="21" spans="1:3">
@@ -3531,7 +3531,7 @@
         <v>105</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="106" ht="21" spans="1:3">
@@ -3542,7 +3542,7 @@
         <v>106</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="107" ht="21" spans="1:3">
@@ -3553,7 +3553,7 @@
         <v>107</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="108" ht="21" spans="1:3">
@@ -3564,7 +3564,7 @@
         <v>108</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="109" ht="21" spans="1:3">
@@ -3575,7 +3575,7 @@
         <v>109</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="110" ht="21" spans="1:3">
@@ -3586,7 +3586,7 @@
         <v>110</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="111" ht="21" spans="1:3">
@@ -3597,7 +3597,7 @@
         <v>111</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="112" ht="21" spans="1:3">
@@ -3608,7 +3608,7 @@
         <v>112</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="113" ht="21" spans="1:3">
@@ -3619,7 +3619,7 @@
         <v>113</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="114" ht="21" spans="1:3">
@@ -3630,7 +3630,7 @@
         <v>114</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="115" ht="21" spans="1:3">
@@ -3641,7 +3641,7 @@
         <v>115</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="116" ht="21" spans="1:3">
@@ -3652,7 +3652,7 @@
         <v>116</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="117" ht="21" spans="1:3">
@@ -3663,7 +3663,7 @@
         <v>117</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="118" ht="21" spans="1:3">
@@ -3674,7 +3674,7 @@
         <v>118</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="119" ht="21" spans="1:3">
@@ -3685,7 +3685,7 @@
         <v>119</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="120" ht="21" spans="1:3">
@@ -3696,7 +3696,7 @@
         <v>120</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="121" ht="21" spans="1:3">
@@ -3707,7 +3707,7 @@
         <v>121</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="122" ht="21" spans="1:3">
@@ -3718,7 +3718,7 @@
         <v>122</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="123" ht="21" spans="1:3">
@@ -3729,7 +3729,7 @@
         <v>123</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="124" ht="21" spans="1:3">
@@ -3740,7 +3740,7 @@
         <v>124</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="125" ht="21" spans="1:3">
@@ -3751,7 +3751,7 @@
         <v>125</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="126" ht="21" spans="1:3">
@@ -3762,7 +3762,7 @@
         <v>126</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="127" ht="21" spans="1:3">
@@ -3773,7 +3773,7 @@
         <v>127</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="128" ht="21" spans="1:3">
@@ -3784,7 +3784,7 @@
         <v>128</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="129" ht="21" spans="1:3">
@@ -3795,7 +3795,7 @@
         <v>129</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="130" ht="21" spans="1:3">
@@ -3806,7 +3806,7 @@
         <v>130</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="131" ht="21" spans="1:3">
@@ -3817,7 +3817,7 @@
         <v>131</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="132" ht="21" spans="1:3">
@@ -3828,7 +3828,7 @@
         <v>132</v>
       </c>
       <c r="C132" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="133" ht="21" spans="1:3">
@@ -3839,7 +3839,7 @@
         <v>133</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="134" ht="21" spans="1:3">
@@ -3850,7 +3850,7 @@
         <v>134</v>
       </c>
       <c r="C134" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="135" ht="21" spans="1:3">
@@ -3861,7 +3861,7 @@
         <v>135</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="136" ht="21" spans="1:3">
@@ -3872,7 +3872,7 @@
         <v>136</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="138" ht="21" spans="2:3">
@@ -3887,7 +3887,7 @@
         <v>138</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="140" ht="21" spans="1:3">
@@ -3898,7 +3898,7 @@
         <v>139</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="141" ht="21" spans="1:3">
@@ -3909,7 +3909,7 @@
         <v>140</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="142" ht="21" spans="1:3">
@@ -3920,7 +3920,7 @@
         <v>141</v>
       </c>
       <c r="C142" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="143" ht="21" spans="1:3">
@@ -3931,7 +3931,7 @@
         <v>142</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="144" ht="21" spans="1:3">
@@ -3942,7 +3942,7 @@
         <v>143</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="145" ht="21" spans="1:3">
@@ -3953,7 +3953,7 @@
         <v>144</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="146" ht="21" spans="1:3">
@@ -3964,7 +3964,7 @@
         <v>145</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="147" ht="21" spans="1:3">
@@ -3975,7 +3975,7 @@
         <v>146</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="148" ht="21" spans="1:3">
@@ -3986,7 +3986,7 @@
         <v>147</v>
       </c>
       <c r="C148" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="149" ht="21" spans="1:3">
@@ -3997,7 +3997,7 @@
         <v>148</v>
       </c>
       <c r="C149" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="150" ht="21" spans="1:3">
@@ -4008,7 +4008,7 @@
         <v>149</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="151" ht="21" spans="1:3">
@@ -4019,7 +4019,7 @@
         <v>150</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="152" ht="21" spans="1:3">
@@ -4030,7 +4030,7 @@
         <v>151</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="153" ht="21" spans="1:3">
@@ -4041,7 +4041,7 @@
         <v>152</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="154" ht="21" spans="1:3">
@@ -4052,7 +4052,7 @@
         <v>153</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="155" ht="21" spans="1:3">
@@ -4063,7 +4063,7 @@
         <v>154</v>
       </c>
       <c r="C155" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="156" ht="21" spans="1:3">
@@ -4074,7 +4074,7 @@
         <v>155</v>
       </c>
       <c r="C156" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="157" ht="21" spans="1:3">
@@ -4085,7 +4085,7 @@
         <v>156</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="158" ht="21" spans="1:3">
@@ -4096,7 +4096,7 @@
         <v>157</v>
       </c>
       <c r="C158" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="159" ht="21" spans="1:3">
@@ -4107,7 +4107,7 @@
         <v>158</v>
       </c>
       <c r="C159" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="160" ht="21" spans="1:3">
@@ -4118,7 +4118,7 @@
         <v>159</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="161" ht="21" spans="1:3">
@@ -4129,7 +4129,7 @@
         <v>160</v>
       </c>
       <c r="C161" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="162" ht="21" spans="1:3">
@@ -4140,7 +4140,7 @@
         <v>161</v>
       </c>
       <c r="C162" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="163" ht="21" spans="1:3">
@@ -4151,7 +4151,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="164" ht="21" spans="1:3">
@@ -4162,7 +4162,7 @@
         <v>163</v>
       </c>
       <c r="C164" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="165" ht="21" spans="1:3">
@@ -4173,7 +4173,7 @@
         <v>164</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="166" ht="21" spans="1:3">
@@ -4184,7 +4184,7 @@
         <v>165</v>
       </c>
       <c r="C166" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="167" ht="21" spans="1:3">
@@ -4195,7 +4195,7 @@
         <v>166</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="168" ht="21" spans="1:3">
@@ -4206,7 +4206,7 @@
         <v>167</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="169" ht="21" spans="1:3">
@@ -4217,7 +4217,7 @@
         <v>168</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="170" ht="21" spans="1:3">
@@ -4228,7 +4228,7 @@
         <v>169</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="171" ht="21" spans="1:3">
@@ -4239,7 +4239,7 @@
         <v>170</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="172" ht="21" spans="1:3">
@@ -4250,7 +4250,7 @@
         <v>171</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="173" ht="21" spans="1:3">
@@ -4261,7 +4261,7 @@
         <v>172</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="174" ht="21" spans="1:3">
@@ -4272,7 +4272,7 @@
         <v>173</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="176" ht="21" spans="2:3">
@@ -4463,7 +4463,7 @@
         <v>191</v>
       </c>
       <c r="C193" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="194" ht="21" spans="1:3">
@@ -4507,7 +4507,7 @@
         <v>196</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="198" ht="21" spans="1:3">
@@ -4518,7 +4518,7 @@
         <v>197</v>
       </c>
       <c r="C198" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="199" ht="21" spans="1:3">
@@ -4529,7 +4529,7 @@
         <v>198</v>
       </c>
       <c r="C199" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="200" ht="21" spans="1:3">
@@ -4540,7 +4540,7 @@
         <v>199</v>
       </c>
       <c r="C200" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="201" ht="21" spans="1:3">
@@ -4551,7 +4551,7 @@
         <v>200</v>
       </c>
       <c r="C201" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="202" ht="21" spans="1:3">
@@ -4562,7 +4562,7 @@
         <v>201</v>
       </c>
       <c r="C202" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="203" ht="21" spans="1:3">
@@ -4573,7 +4573,7 @@
         <v>202</v>
       </c>
       <c r="C203" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="204" ht="21" spans="1:3">
@@ -4584,7 +4584,7 @@
         <v>203</v>
       </c>
       <c r="C204" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="205" ht="21" spans="1:3">
@@ -4595,7 +4595,7 @@
         <v>204</v>
       </c>
       <c r="C205" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="206" ht="21" spans="1:3">
@@ -4606,7 +4606,7 @@
         <v>205</v>
       </c>
       <c r="C206" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="207" ht="21" spans="1:3">
@@ -4617,7 +4617,7 @@
         <v>206</v>
       </c>
       <c r="C207" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="208" ht="21" spans="1:3">
@@ -4628,7 +4628,7 @@
         <v>207</v>
       </c>
       <c r="C208" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="209" ht="21" spans="1:3">
@@ -4639,7 +4639,7 @@
         <v>208</v>
       </c>
       <c r="C209" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="210" ht="21" spans="1:3">
@@ -4650,7 +4650,7 @@
         <v>209</v>
       </c>
       <c r="C210" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="211" ht="21" spans="1:3">
@@ -4661,7 +4661,7 @@
         <v>210</v>
       </c>
       <c r="C211" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="212" ht="21" spans="1:3">
@@ -4682,7 +4682,7 @@
         <v>212</v>
       </c>
       <c r="C214" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="215" ht="21" spans="1:3">
@@ -4693,7 +4693,7 @@
         <v>213</v>
       </c>
       <c r="C215" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="216" ht="21" spans="1:3">
@@ -4704,7 +4704,7 @@
         <v>214</v>
       </c>
       <c r="C216" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="217" ht="21" spans="1:3">
@@ -4715,7 +4715,7 @@
         <v>215</v>
       </c>
       <c r="C217" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="218" ht="21" spans="1:3">
@@ -4726,7 +4726,7 @@
         <v>216</v>
       </c>
       <c r="C218" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="219" ht="21" spans="1:3">
@@ -4737,7 +4737,7 @@
         <v>217</v>
       </c>
       <c r="C219" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="220" ht="21" spans="1:3">
@@ -4748,7 +4748,7 @@
         <v>218</v>
       </c>
       <c r="C220" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="221" ht="21" spans="1:3">
@@ -4759,7 +4759,7 @@
         <v>219</v>
       </c>
       <c r="C221" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="222" ht="21" spans="1:3">
@@ -4770,7 +4770,7 @@
         <v>220</v>
       </c>
       <c r="C222" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="223" ht="21" spans="1:3">
@@ -4781,7 +4781,7 @@
         <v>221</v>
       </c>
       <c r="C223" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="224" ht="21" spans="1:3">
@@ -4792,7 +4792,7 @@
         <v>222</v>
       </c>
       <c r="C224" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="225" ht="21" spans="1:3">
@@ -4803,7 +4803,7 @@
         <v>223</v>
       </c>
       <c r="C225" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="226" ht="21" spans="1:3">
@@ -4814,7 +4814,7 @@
         <v>224</v>
       </c>
       <c r="C226" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="227" ht="21" spans="1:3">
@@ -4825,7 +4825,7 @@
         <v>225</v>
       </c>
       <c r="C227" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="228" ht="21" spans="1:3">
@@ -4836,7 +4836,7 @@
         <v>226</v>
       </c>
       <c r="C228" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="229" ht="21" spans="1:3">
@@ -4847,7 +4847,7 @@
         <v>227</v>
       </c>
       <c r="C229" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="230" ht="21" spans="1:3">
@@ -4858,7 +4858,7 @@
         <v>228</v>
       </c>
       <c r="C230" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="231" ht="21" spans="1:3">
@@ -4869,7 +4869,7 @@
         <v>229</v>
       </c>
       <c r="C231" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="232" ht="21" spans="1:3">
@@ -4880,7 +4880,7 @@
         <v>230</v>
       </c>
       <c r="C232" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="233" ht="21" spans="1:3">
@@ -4891,7 +4891,7 @@
         <v>231</v>
       </c>
       <c r="C233" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="234" ht="21" spans="1:3">
@@ -4902,7 +4902,7 @@
         <v>232</v>
       </c>
       <c r="C234" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="235" ht="21" spans="1:3">
@@ -4913,7 +4913,7 @@
         <v>233</v>
       </c>
       <c r="C235" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="236" ht="21" spans="2:3">
@@ -4932,7 +4932,7 @@
         <v>235</v>
       </c>
       <c r="C238" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="239" ht="21" spans="1:3">
@@ -4943,7 +4943,7 @@
         <v>236</v>
       </c>
       <c r="C239" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="240" ht="21" spans="1:3">
@@ -4954,7 +4954,7 @@
         <v>237</v>
       </c>
       <c r="C240" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="241" ht="21" spans="1:3">
@@ -4965,7 +4965,7 @@
         <v>238</v>
       </c>
       <c r="C241" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="242" ht="21" spans="1:3">
@@ -4987,7 +4987,7 @@
         <v>241</v>
       </c>
       <c r="C243" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="244" ht="21" spans="1:3">
@@ -4998,7 +4998,7 @@
         <v>242</v>
       </c>
       <c r="C244" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="245" ht="21" spans="1:3">
@@ -5009,7 +5009,7 @@
         <v>243</v>
       </c>
       <c r="C245" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="246" ht="21" spans="1:3">
@@ -5020,7 +5020,7 @@
         <v>244</v>
       </c>
       <c r="C246" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="247" ht="21" spans="1:3">
@@ -5031,7 +5031,7 @@
         <v>245</v>
       </c>
       <c r="C247" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="248" ht="21" spans="1:3">
@@ -5042,7 +5042,7 @@
         <v>246</v>
       </c>
       <c r="C248" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="249" ht="21" spans="1:3">
@@ -5053,7 +5053,7 @@
         <v>247</v>
       </c>
       <c r="C249" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="250" ht="21" spans="1:3">
@@ -5064,7 +5064,7 @@
         <v>248</v>
       </c>
       <c r="C250" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="251" ht="21" spans="1:3">
@@ -5075,7 +5075,7 @@
         <v>249</v>
       </c>
       <c r="C251" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="252" ht="21" spans="1:3">
@@ -5086,7 +5086,7 @@
         <v>250</v>
       </c>
       <c r="C252" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="253" ht="21" spans="1:3">
@@ -5097,7 +5097,7 @@
         <v>251</v>
       </c>
       <c r="C253" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="254" ht="21" spans="1:3">
@@ -5108,7 +5108,7 @@
         <v>252</v>
       </c>
       <c r="C254" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="255" ht="21" spans="1:3">
@@ -5119,7 +5119,7 @@
         <v>253</v>
       </c>
       <c r="C255" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="256" ht="21" spans="1:3">
@@ -5130,7 +5130,7 @@
         <v>254</v>
       </c>
       <c r="C256" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="257" ht="21" spans="1:3">
@@ -5141,7 +5141,7 @@
         <v>255</v>
       </c>
       <c r="C257" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="258" ht="21" spans="1:3">
@@ -5152,7 +5152,7 @@
         <v>256</v>
       </c>
       <c r="C258" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="259" ht="21" spans="1:3">
@@ -5163,7 +5163,7 @@
         <v>257</v>
       </c>
       <c r="C259" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="260" ht="21" spans="1:3">
@@ -5174,7 +5174,7 @@
         <v>258</v>
       </c>
       <c r="C260" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="261" ht="21" spans="1:3">
@@ -5185,7 +5185,7 @@
         <v>259</v>
       </c>
       <c r="C261" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="262" ht="21" spans="1:3">
@@ -5196,7 +5196,7 @@
         <v>260</v>
       </c>
       <c r="C262" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="263" ht="21" spans="1:3">
@@ -5207,7 +5207,7 @@
         <v>261</v>
       </c>
       <c r="C263" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="264" ht="21" spans="1:3">
@@ -5218,7 +5218,7 @@
         <v>262</v>
       </c>
       <c r="C264" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="265" ht="21" spans="1:3">
@@ -5229,7 +5229,7 @@
         <v>263</v>
       </c>
       <c r="C265" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="266" ht="21" spans="1:3">
@@ -5240,7 +5240,7 @@
         <v>264</v>
       </c>
       <c r="C266" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="267" ht="21" spans="1:3">
@@ -5251,7 +5251,7 @@
         <v>265</v>
       </c>
       <c r="C267" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="268" ht="21" spans="1:3">
@@ -5262,7 +5262,7 @@
         <v>266</v>
       </c>
       <c r="C268" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="269" ht="21" spans="1:3">
@@ -5273,7 +5273,7 @@
         <v>267</v>
       </c>
       <c r="C269" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="270" ht="21" spans="1:3">
@@ -5284,7 +5284,7 @@
         <v>268</v>
       </c>
       <c r="C270" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="271" ht="21" spans="1:3">
@@ -5295,7 +5295,7 @@
         <v>90</v>
       </c>
       <c r="C271" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="272" ht="21" spans="1:3">
@@ -5306,7 +5306,7 @@
         <v>269</v>
       </c>
       <c r="C272" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="273" ht="21" spans="2:3">
@@ -5325,7 +5325,7 @@
         <v>271</v>
       </c>
       <c r="C275" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="276" ht="21" spans="1:3">
@@ -5336,7 +5336,7 @@
         <v>272</v>
       </c>
       <c r="C276" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="277" ht="21" spans="1:3">
@@ -5347,7 +5347,7 @@
         <v>273</v>
       </c>
       <c r="C277" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="278" ht="21" spans="1:3">
@@ -5358,7 +5358,7 @@
         <v>274</v>
       </c>
       <c r="C278" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="279" ht="21" spans="1:3">
@@ -5369,7 +5369,7 @@
         <v>275</v>
       </c>
       <c r="C279" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="280" ht="21" spans="1:3">
@@ -5380,7 +5380,7 @@
         <v>276</v>
       </c>
       <c r="C280" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="281" ht="21" spans="1:3">
@@ -5391,7 +5391,7 @@
         <v>277</v>
       </c>
       <c r="C281" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="282" ht="21" spans="1:3">
@@ -5402,7 +5402,7 @@
         <v>278</v>
       </c>
       <c r="C282" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="283" ht="21" spans="1:3">
@@ -5413,7 +5413,7 @@
         <v>279</v>
       </c>
       <c r="C283" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="284" ht="21" spans="1:3">
@@ -5424,7 +5424,7 @@
         <v>280</v>
       </c>
       <c r="C284" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="285" ht="21" spans="1:3">
@@ -5435,7 +5435,7 @@
         <v>281</v>
       </c>
       <c r="C285" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="286" ht="21" spans="1:3">
@@ -5446,7 +5446,7 @@
         <v>282</v>
       </c>
       <c r="C286" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="287" ht="21" spans="1:3">
@@ -5457,7 +5457,7 @@
         <v>283</v>
       </c>
       <c r="C287" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="288" ht="21" spans="1:3">
@@ -5468,7 +5468,7 @@
         <v>284</v>
       </c>
       <c r="C288" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="289" ht="21" spans="1:3">
@@ -5479,7 +5479,7 @@
         <v>285</v>
       </c>
       <c r="C289" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="290" ht="21" spans="1:3">
@@ -5490,7 +5490,7 @@
         <v>286</v>
       </c>
       <c r="C290" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="291" ht="21" spans="1:3">
@@ -5501,7 +5501,7 @@
         <v>287</v>
       </c>
       <c r="C291" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="292" ht="21" spans="1:3">
@@ -5512,7 +5512,7 @@
         <v>288</v>
       </c>
       <c r="C292" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="293" ht="21" spans="1:3">
@@ -5523,7 +5523,7 @@
         <v>289</v>
       </c>
       <c r="C293" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="294" ht="21" spans="2:3">
@@ -5542,7 +5542,7 @@
         <v>291</v>
       </c>
       <c r="C296" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="297" ht="21" spans="1:3">
@@ -5553,7 +5553,7 @@
         <v>292</v>
       </c>
       <c r="C297" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="298" ht="21" spans="1:3">
@@ -5564,7 +5564,7 @@
         <v>293</v>
       </c>
       <c r="C298" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="299" ht="21" spans="1:3">
@@ -5575,7 +5575,7 @@
         <v>294</v>
       </c>
       <c r="C299" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="300" ht="21" spans="1:3">
@@ -5586,7 +5586,7 @@
         <v>295</v>
       </c>
       <c r="C300" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="301" ht="21" spans="1:3">
@@ -5597,7 +5597,7 @@
         <v>296</v>
       </c>
       <c r="C301" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="302" ht="21" spans="1:3">
@@ -5608,7 +5608,7 @@
         <v>297</v>
       </c>
       <c r="C302" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="303" ht="21" spans="1:3">
@@ -5619,7 +5619,7 @@
         <v>298</v>
       </c>
       <c r="C303" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="304" ht="21" spans="1:3">
@@ -5630,7 +5630,7 @@
         <v>299</v>
       </c>
       <c r="C304" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="305" ht="21" spans="1:3">
@@ -5641,7 +5641,7 @@
         <v>300</v>
       </c>
       <c r="C305" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="306" ht="21" spans="1:3">
@@ -5652,7 +5652,7 @@
         <v>301</v>
       </c>
       <c r="C306" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="307" ht="21" spans="1:3">
@@ -5663,7 +5663,7 @@
         <v>302</v>
       </c>
       <c r="C307" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="308" ht="21" spans="1:3">
@@ -5674,7 +5674,7 @@
         <v>303</v>
       </c>
       <c r="C308" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="309" ht="21" spans="1:3">
@@ -5685,7 +5685,7 @@
         <v>304</v>
       </c>
       <c r="C309" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="310" ht="21" spans="1:3">
@@ -5696,7 +5696,7 @@
         <v>305</v>
       </c>
       <c r="C310" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="311" ht="21" spans="1:3">
@@ -5707,7 +5707,7 @@
         <v>306</v>
       </c>
       <c r="C311" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="312" ht="21" spans="1:3">
@@ -5718,7 +5718,7 @@
         <v>307</v>
       </c>
       <c r="C312" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="313" ht="21" spans="1:3">
@@ -5729,7 +5729,7 @@
         <v>308</v>
       </c>
       <c r="C313" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="314" ht="21" spans="1:3">
@@ -5740,7 +5740,7 @@
         <v>309</v>
       </c>
       <c r="C314" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="315" ht="21" spans="1:3">
@@ -5751,7 +5751,7 @@
         <v>310</v>
       </c>
       <c r="C315" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="316" ht="21" spans="1:3">
@@ -5762,7 +5762,7 @@
         <v>311</v>
       </c>
       <c r="C316" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="317" ht="21" spans="1:3">
@@ -5773,7 +5773,7 @@
         <v>312</v>
       </c>
       <c r="C317" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="318" ht="21" spans="1:3">
@@ -5784,7 +5784,7 @@
         <v>313</v>
       </c>
       <c r="C318" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="319" ht="21" spans="1:3">
@@ -5795,7 +5795,7 @@
         <v>314</v>
       </c>
       <c r="C319" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="320" ht="21" spans="1:3">
@@ -5806,7 +5806,7 @@
         <v>315</v>
       </c>
       <c r="C320" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="321" ht="21" spans="1:3">
@@ -5817,7 +5817,7 @@
         <v>316</v>
       </c>
       <c r="C321" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="322" ht="21" spans="1:3">
@@ -5828,7 +5828,7 @@
         <v>317</v>
       </c>
       <c r="C322" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="323" ht="21" spans="1:3">
@@ -5839,7 +5839,7 @@
         <v>318</v>
       </c>
       <c r="C323" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="324" ht="21" spans="1:3">
@@ -5850,7 +5850,7 @@
         <v>319</v>
       </c>
       <c r="C324" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="325" ht="21" spans="1:3">
@@ -5861,7 +5861,7 @@
         <v>320</v>
       </c>
       <c r="C325" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="326" ht="21" spans="1:3">
@@ -5872,7 +5872,7 @@
         <v>321</v>
       </c>
       <c r="C326" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="327" ht="21" spans="1:3">
@@ -5883,7 +5883,7 @@
         <v>322</v>
       </c>
       <c r="C327" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="328" ht="21" spans="1:3">
@@ -5894,7 +5894,7 @@
         <v>323</v>
       </c>
       <c r="C328" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="329" ht="21" spans="1:3">
@@ -5905,7 +5905,7 @@
         <v>324</v>
       </c>
       <c r="C329" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="330" ht="21" spans="1:3">
@@ -5916,7 +5916,7 @@
         <v>325</v>
       </c>
       <c r="C330" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="331" ht="21" spans="1:3">
@@ -5927,7 +5927,7 @@
         <v>326</v>
       </c>
       <c r="C331" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="332" ht="21" spans="1:3">
@@ -5938,7 +5938,7 @@
         <v>327</v>
       </c>
       <c r="C332" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="333" ht="21" spans="1:3">
@@ -5949,7 +5949,7 @@
         <v>328</v>
       </c>
       <c r="C333" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="334" ht="21" spans="2:3">
@@ -5968,7 +5968,7 @@
         <v>330</v>
       </c>
       <c r="C336" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="337" ht="21" spans="1:3">
@@ -5979,7 +5979,7 @@
         <v>331</v>
       </c>
       <c r="C337" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="338" ht="21" spans="1:3">
@@ -5990,7 +5990,7 @@
         <v>332</v>
       </c>
       <c r="C338" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="339" ht="21" spans="1:3">
@@ -6001,7 +6001,7 @@
         <v>333</v>
       </c>
       <c r="C339" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="340" ht="21" spans="1:3">
@@ -6012,7 +6012,7 @@
         <v>334</v>
       </c>
       <c r="C340" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="341" ht="21" spans="1:3">
@@ -6023,7 +6023,7 @@
         <v>335</v>
       </c>
       <c r="C341" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="342" ht="21" spans="1:3">
@@ -6034,7 +6034,7 @@
         <v>336</v>
       </c>
       <c r="C342" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="343" ht="21" spans="1:3">
@@ -6045,7 +6045,7 @@
         <v>337</v>
       </c>
       <c r="C343" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="344" ht="21" spans="1:3">
@@ -6056,7 +6056,7 @@
         <v>338</v>
       </c>
       <c r="C344" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="345" ht="21" spans="1:3">
@@ -6067,7 +6067,7 @@
         <v>339</v>
       </c>
       <c r="C345" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="346" ht="21" spans="1:3">
@@ -6078,7 +6078,7 @@
         <v>340</v>
       </c>
       <c r="C346" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="347" ht="21" spans="1:3">
@@ -6089,7 +6089,7 @@
         <v>341</v>
       </c>
       <c r="C347" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="348" ht="21" spans="1:3">
@@ -6100,7 +6100,7 @@
         <v>342</v>
       </c>
       <c r="C348" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="349" ht="21" spans="1:3">
@@ -6111,7 +6111,7 @@
         <v>343</v>
       </c>
       <c r="C349" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="350" ht="21" spans="1:3">
@@ -6122,7 +6122,7 @@
         <v>344</v>
       </c>
       <c r="C350" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="351" ht="21" spans="1:3">
@@ -6133,7 +6133,7 @@
         <v>345</v>
       </c>
       <c r="C351" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="352" ht="21" spans="1:3">
@@ -6144,7 +6144,7 @@
         <v>346</v>
       </c>
       <c r="C352" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="353" ht="21" spans="1:3">
@@ -6155,7 +6155,7 @@
         <v>347</v>
       </c>
       <c r="C353" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="354" ht="21" spans="2:3">
@@ -6174,7 +6174,7 @@
         <v>349</v>
       </c>
       <c r="C356" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="357" ht="21" spans="1:3">
@@ -6251,7 +6251,7 @@
         <v>356</v>
       </c>
       <c r="C363" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="364" ht="21" spans="1:3">
@@ -6262,7 +6262,7 @@
         <v>357</v>
       </c>
       <c r="C364" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="365" ht="21" spans="1:3">
@@ -6273,7 +6273,7 @@
         <v>358</v>
       </c>
       <c r="C365" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="366" ht="21" spans="1:3">
@@ -6284,7 +6284,7 @@
         <v>359</v>
       </c>
       <c r="C366" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="367" ht="21" spans="1:3">
@@ -6295,7 +6295,7 @@
         <v>360</v>
       </c>
       <c r="C367" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="368" ht="21" spans="1:3">
@@ -6306,7 +6306,7 @@
         <v>361</v>
       </c>
       <c r="C368" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="369" ht="21" spans="1:3">
@@ -6317,7 +6317,7 @@
         <v>362</v>
       </c>
       <c r="C369" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="370" ht="21" spans="1:3">
@@ -6328,7 +6328,7 @@
         <v>363</v>
       </c>
       <c r="C370" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="371" ht="21" spans="1:3">
@@ -6339,7 +6339,7 @@
         <v>364</v>
       </c>
       <c r="C371" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="372" ht="21" spans="1:3">
@@ -6350,7 +6350,7 @@
         <v>365</v>
       </c>
       <c r="C372" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="373" ht="21" spans="1:3">
@@ -6361,7 +6361,7 @@
         <v>366</v>
       </c>
       <c r="C373" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="374" ht="21" spans="1:3">
@@ -6372,7 +6372,7 @@
         <v>367</v>
       </c>
       <c r="C374" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="375" ht="21" spans="1:3">
@@ -6383,7 +6383,7 @@
         <v>368</v>
       </c>
       <c r="C375" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="376" ht="21" spans="1:3">
@@ -6394,7 +6394,7 @@
         <v>369</v>
       </c>
       <c r="C376" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="377" ht="21" spans="1:3">
@@ -6405,7 +6405,7 @@
         <v>370</v>
       </c>
       <c r="C377" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="378" ht="21" spans="1:3">
@@ -6416,7 +6416,7 @@
         <v>371</v>
       </c>
       <c r="C378" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="379" ht="21" spans="1:3">
@@ -6427,7 +6427,7 @@
         <v>372</v>
       </c>
       <c r="C379" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="380" ht="21" spans="1:3">
@@ -6438,7 +6438,7 @@
         <v>373</v>
       </c>
       <c r="C380" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="381" ht="21" spans="1:3">
@@ -6449,7 +6449,7 @@
         <v>374</v>
       </c>
       <c r="C381" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="382" ht="21" spans="1:3">
@@ -6460,7 +6460,7 @@
         <v>375</v>
       </c>
       <c r="C382" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="383" ht="21" spans="1:3">
@@ -6471,7 +6471,7 @@
         <v>376</v>
       </c>
       <c r="C383" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="384" ht="21" spans="1:3">
@@ -6482,7 +6482,7 @@
         <v>377</v>
       </c>
       <c r="C384" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="385" ht="21" spans="1:3">
@@ -6493,7 +6493,7 @@
         <v>378</v>
       </c>
       <c r="C385" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="386" ht="21" spans="1:3">
@@ -6504,7 +6504,7 @@
         <v>379</v>
       </c>
       <c r="C386" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="387" ht="21" spans="1:3">
@@ -6515,7 +6515,7 @@
         <v>380</v>
       </c>
       <c r="C387" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="388" ht="21" spans="1:3">
@@ -6526,7 +6526,7 @@
         <v>381</v>
       </c>
       <c r="C388" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="389" ht="21" spans="1:3">
@@ -6537,7 +6537,7 @@
         <v>382</v>
       </c>
       <c r="C389" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="390" ht="21" spans="1:3">
@@ -6548,7 +6548,7 @@
         <v>382</v>
       </c>
       <c r="C390" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="391" ht="21" spans="1:3">
@@ -6559,7 +6559,7 @@
         <v>383</v>
       </c>
       <c r="C391" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="392" ht="21" spans="1:3">
@@ -6570,7 +6570,7 @@
         <v>384</v>
       </c>
       <c r="C392" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="393" ht="21" spans="1:3">
@@ -6581,7 +6581,7 @@
         <v>385</v>
       </c>
       <c r="C393" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="394" ht="21" spans="1:3">
@@ -6592,7 +6592,7 @@
         <v>386</v>
       </c>
       <c r="C394" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="395" ht="21" spans="1:3">
@@ -6603,7 +6603,7 @@
         <v>387</v>
       </c>
       <c r="C395" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="396" ht="21" spans="1:3">
@@ -6614,7 +6614,7 @@
         <v>388</v>
       </c>
       <c r="C396" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="397" ht="21" spans="1:3">
@@ -6625,7 +6625,7 @@
         <v>389</v>
       </c>
       <c r="C397" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="398" ht="21" spans="1:3">
@@ -6636,7 +6636,7 @@
         <v>390</v>
       </c>
       <c r="C398" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="399" ht="21" spans="1:3">
@@ -6647,7 +6647,7 @@
         <v>391</v>
       </c>
       <c r="C399" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="400" ht="21" spans="2:3">
@@ -6666,7 +6666,7 @@
         <v>393</v>
       </c>
       <c r="C402" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="403" ht="21" spans="1:3">
@@ -6677,7 +6677,7 @@
         <v>394</v>
       </c>
       <c r="C403" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="404" ht="21" spans="1:3">
@@ -6688,7 +6688,7 @@
         <v>395</v>
       </c>
       <c r="C404" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="405" ht="21" spans="1:3">
@@ -6699,7 +6699,7 @@
         <v>92</v>
       </c>
       <c r="C405" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="406" ht="21" spans="1:3">
@@ -6710,7 +6710,7 @@
         <v>396</v>
       </c>
       <c r="C406" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="407" ht="21" spans="1:3">
@@ -6721,7 +6721,7 @@
         <v>397</v>
       </c>
       <c r="C407" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="408" ht="21" spans="2:3">
@@ -6817,7 +6817,7 @@
         <v>278</v>
       </c>
       <c r="C417" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="418" ht="21" spans="1:3">
@@ -6828,7 +6828,7 @@
         <v>406</v>
       </c>
       <c r="C418" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="419" ht="21" spans="1:3">
@@ -6839,7 +6839,7 @@
         <v>407</v>
       </c>
       <c r="C419" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="420" ht="21" spans="1:3">
@@ -6850,7 +6850,7 @@
         <v>408</v>
       </c>
       <c r="C420" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="421" ht="21" spans="1:3">
@@ -6861,7 +6861,7 @@
         <v>409</v>
       </c>
       <c r="C421" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="422" ht="21" spans="1:3">
@@ -6872,7 +6872,7 @@
         <v>410</v>
       </c>
       <c r="C422" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="423" ht="21" spans="1:3">
@@ -6883,7 +6883,7 @@
         <v>411</v>
       </c>
       <c r="C423" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="424" ht="21" spans="1:3">
@@ -6894,7 +6894,7 @@
         <v>412</v>
       </c>
       <c r="C424" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="425" ht="21" spans="1:3">
@@ -6905,7 +6905,7 @@
         <v>413</v>
       </c>
       <c r="C425" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="426" ht="21" spans="1:3">
@@ -6916,7 +6916,7 @@
         <v>414</v>
       </c>
       <c r="C426" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="427" ht="21" spans="1:3">
@@ -6927,7 +6927,7 @@
         <v>415</v>
       </c>
       <c r="C427" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="428" ht="21" spans="1:3">
@@ -6938,7 +6938,7 @@
         <v>416</v>
       </c>
       <c r="C428" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="429" ht="21" spans="1:3">
@@ -6949,7 +6949,7 @@
         <v>417</v>
       </c>
       <c r="C429" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="430" ht="21" spans="1:3">
@@ -6960,7 +6960,7 @@
         <v>418</v>
       </c>
       <c r="C430" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="431" ht="21" spans="1:3">
@@ -6971,7 +6971,7 @@
         <v>419</v>
       </c>
       <c r="C431" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="432" ht="21" spans="1:3">
@@ -6982,7 +6982,7 @@
         <v>420</v>
       </c>
       <c r="C432" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="433" ht="21" spans="1:3">
@@ -6993,7 +6993,7 @@
         <v>421</v>
       </c>
       <c r="C433" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="434" ht="21" spans="1:3">
@@ -7004,7 +7004,7 @@
         <v>422</v>
       </c>
       <c r="C434" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="435" ht="21" spans="1:3">
@@ -7015,7 +7015,7 @@
         <v>423</v>
       </c>
       <c r="C435" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="436" ht="21" spans="1:3">
@@ -7026,7 +7026,7 @@
         <v>424</v>
       </c>
       <c r="C436" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="437" ht="21" spans="1:3">
@@ -7037,7 +7037,7 @@
         <v>425</v>
       </c>
       <c r="C437" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="438" ht="21" spans="1:3">
@@ -7048,7 +7048,7 @@
         <v>17</v>
       </c>
       <c r="C438" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="439" ht="21" spans="1:3">
@@ -7059,7 +7059,7 @@
         <v>426</v>
       </c>
       <c r="C439" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="440" ht="21" spans="1:3">
@@ -7070,7 +7070,7 @@
         <v>427</v>
       </c>
       <c r="C440" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="441" ht="21" spans="1:3">
@@ -7081,7 +7081,7 @@
         <v>428</v>
       </c>
       <c r="C441" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="442" ht="21" spans="1:3">
@@ -7092,7 +7092,7 @@
         <v>429</v>
       </c>
       <c r="C442" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="443" ht="21" spans="1:3">
@@ -7103,7 +7103,7 @@
         <v>430</v>
       </c>
       <c r="C443" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="444" ht="21" spans="1:3">
@@ -7114,7 +7114,7 @@
         <v>431</v>
       </c>
       <c r="C444" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="445" ht="21" spans="1:3">
@@ -7125,7 +7125,7 @@
         <v>432</v>
       </c>
       <c r="C445" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="446" ht="21" spans="1:3">
@@ -7136,7 +7136,7 @@
         <v>433</v>
       </c>
       <c r="C446" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="447" ht="21" spans="1:3">
@@ -7147,7 +7147,7 @@
         <v>434</v>
       </c>
       <c r="C447" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="448" ht="21" spans="1:3">
@@ -7158,7 +7158,7 @@
         <v>435</v>
       </c>
       <c r="C448" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="449" ht="21" spans="1:3">
@@ -7169,7 +7169,7 @@
         <v>436</v>
       </c>
       <c r="C449" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="450" ht="21" spans="1:3">
@@ -7180,7 +7180,7 @@
         <v>437</v>
       </c>
       <c r="C450" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="451" ht="21" spans="1:3">
@@ -7191,7 +7191,7 @@
         <v>438</v>
       </c>
       <c r="C451" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="452" ht="21" spans="1:3">
@@ -7202,7 +7202,7 @@
         <v>439</v>
       </c>
       <c r="C452" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="453" ht="21" spans="1:3">
@@ -7213,7 +7213,7 @@
         <v>440</v>
       </c>
       <c r="C453" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="454" ht="21" spans="1:3">
@@ -7224,7 +7224,7 @@
         <v>441</v>
       </c>
       <c r="C454" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="455" ht="21" spans="1:3">
@@ -7235,7 +7235,7 @@
         <v>442</v>
       </c>
       <c r="C455" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="456" ht="21" spans="1:3">
@@ -7246,7 +7246,7 @@
         <v>443</v>
       </c>
       <c r="C456" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="457" ht="21" spans="1:3">
@@ -7257,7 +7257,7 @@
         <v>444</v>
       </c>
       <c r="C457" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="458" ht="21" spans="1:3">
@@ -7268,7 +7268,7 @@
         <v>445</v>
       </c>
       <c r="C458" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="459" ht="21" spans="1:3">
@@ -7279,7 +7279,7 @@
         <v>446</v>
       </c>
       <c r="C459" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="460" ht="21" spans="1:3">
@@ -7290,7 +7290,7 @@
         <v>447</v>
       </c>
       <c r="C460" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="461" ht="21" spans="1:3">
@@ -7301,7 +7301,7 @@
         <v>448</v>
       </c>
       <c r="C461" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="462" ht="21" spans="1:3">
@@ -7312,7 +7312,7 @@
         <v>449</v>
       </c>
       <c r="C462" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="463" ht="21" spans="1:3">
@@ -7323,7 +7323,7 @@
         <v>450</v>
       </c>
       <c r="C463" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="464" ht="21" spans="1:3">
@@ -7334,7 +7334,7 @@
         <v>451</v>
       </c>
       <c r="C464" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="465" ht="21" spans="1:3">
@@ -7345,7 +7345,7 @@
         <v>452</v>
       </c>
       <c r="C465" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="466" ht="21" spans="1:3">
@@ -7356,7 +7356,7 @@
         <v>453</v>
       </c>
       <c r="C466" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="467" ht="21" spans="1:3">
@@ -7367,7 +7367,7 @@
         <v>454</v>
       </c>
       <c r="C467" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="468" ht="21" spans="1:3">
@@ -7378,7 +7378,7 @@
         <v>455</v>
       </c>
       <c r="C468" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="469" ht="21" spans="1:3">
@@ -7389,7 +7389,7 @@
         <v>456</v>
       </c>
       <c r="C469" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="470" ht="21" spans="2:3">
@@ -7409,7 +7409,7 @@
         <v>458</v>
       </c>
       <c r="C472" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="473" ht="21" spans="1:3">
@@ -7420,7 +7420,7 @@
         <v>459</v>
       </c>
       <c r="C473" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="474" ht="21" spans="1:3">
@@ -7431,7 +7431,7 @@
         <v>460</v>
       </c>
       <c r="C474" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="475" ht="21" spans="1:3">
@@ -7442,7 +7442,7 @@
         <v>461</v>
       </c>
       <c r="C475" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="476" ht="21" spans="1:3">
@@ -7453,7 +7453,7 @@
         <v>462</v>
       </c>
       <c r="C476" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="477" ht="21" spans="1:3">
@@ -7464,7 +7464,7 @@
         <v>463</v>
       </c>
       <c r="C477" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="478" ht="21" spans="1:3">
@@ -7475,7 +7475,7 @@
         <v>464</v>
       </c>
       <c r="C478" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="479" ht="21" spans="1:3">
@@ -7486,7 +7486,7 @@
         <v>465</v>
       </c>
       <c r="C479" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="480" ht="21" spans="1:3">
@@ -7497,7 +7497,7 @@
         <v>466</v>
       </c>
       <c r="C480" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="481" ht="21" spans="1:3">
@@ -7508,7 +7508,7 @@
         <v>467</v>
       </c>
       <c r="C481" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Subarray with sum 0
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -103,10 +103,10 @@
     <t>Find if there is any subarray with sum equal to 0</t>
   </si>
   <si>
+    <t>Find factorial of a large number</t>
+  </si>
+  <si>
     <t>&lt;-&gt;</t>
-  </si>
-  <si>
-    <t>Find factorial of a large number</t>
   </si>
   <si>
     <t xml:space="preserve">find maximum product subarray </t>
@@ -1425,10 +1425,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1503,9 +1503,77 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1518,21 +1586,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1546,90 +1631,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -1637,9 +1638,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1660,13 +1660,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1684,13 +1714,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1702,97 +1816,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1804,37 +1828,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1845,21 +1845,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1880,9 +1865,59 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1910,184 +1945,149 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2440,8 +2440,8 @@
   <sheetPr/>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2701,11 +2701,11 @@
       <c r="A26" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>29</v>
+      <c r="C26" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="27" ht="21" spans="1:3">
@@ -2713,10 +2713,10 @@
         <v>6</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" ht="21" spans="1:3">
@@ -2727,7 +2727,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" ht="21" spans="1:3">
@@ -2738,7 +2738,7 @@
         <v>32</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" ht="21" spans="1:3">
@@ -2749,7 +2749,7 @@
         <v>33</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" ht="21" spans="1:3">
@@ -2760,7 +2760,7 @@
         <v>34</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" ht="21" spans="1:3">
@@ -2771,7 +2771,7 @@
         <v>35</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" ht="21" spans="1:3">
@@ -2782,7 +2782,7 @@
         <v>36</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" ht="21" spans="1:3">
@@ -2793,7 +2793,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" ht="21" spans="1:3">
@@ -2804,7 +2804,7 @@
         <v>38</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" ht="21" spans="1:3">
@@ -2815,7 +2815,7 @@
         <v>39</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" ht="21" spans="1:3">
@@ -2826,7 +2826,7 @@
         <v>40</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" ht="21" spans="1:3">
@@ -2837,7 +2837,7 @@
         <v>41</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" ht="21" spans="1:3">
@@ -2848,7 +2848,7 @@
         <v>42</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" ht="21" spans="1:3">
@@ -2859,7 +2859,7 @@
         <v>43</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" ht="21" spans="1:3">
@@ -2870,20 +2870,20 @@
         <v>44</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" ht="21" spans="2:3">
       <c r="B42" s="10"/>
       <c r="C42" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" ht="21" spans="1:3">
       <c r="A43" s="6"/>
       <c r="B43" s="10"/>
       <c r="C43" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" ht="21" spans="1:3">
@@ -2894,7 +2894,7 @@
         <v>46</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" ht="21" spans="1:3">
@@ -2905,7 +2905,7 @@
         <v>47</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" ht="21" spans="1:3">
@@ -2916,7 +2916,7 @@
         <v>48</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" ht="21" spans="1:3">
@@ -2927,7 +2927,7 @@
         <v>49</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" ht="21" spans="1:3">
@@ -2938,7 +2938,7 @@
         <v>50</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" ht="21" spans="1:3">
@@ -2949,7 +2949,7 @@
         <v>51</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" ht="21" spans="1:3">
@@ -2960,7 +2960,7 @@
         <v>52</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" ht="21" spans="1:3">
@@ -2971,7 +2971,7 @@
         <v>53</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" ht="21" spans="1:3">
@@ -2982,7 +2982,7 @@
         <v>54</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" ht="21" spans="1:3">
@@ -2993,7 +2993,7 @@
         <v>55</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" ht="21" spans="1:3">
@@ -3009,7 +3009,7 @@
         <v>57</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="57" ht="21" spans="1:3">
@@ -3020,7 +3020,7 @@
         <v>58</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="58" ht="21" spans="1:3">
@@ -3031,7 +3031,7 @@
         <v>59</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="59" ht="21" spans="1:3">
@@ -3042,7 +3042,7 @@
         <v>60</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" ht="21" spans="1:3">
@@ -3053,7 +3053,7 @@
         <v>61</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="61" ht="21" spans="1:3">
@@ -3064,7 +3064,7 @@
         <v>62</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="62" ht="21" spans="1:3">
@@ -3075,7 +3075,7 @@
         <v>63</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="63" ht="21" spans="1:3">
@@ -3086,7 +3086,7 @@
         <v>64</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" ht="21" spans="1:3">
@@ -3097,7 +3097,7 @@
         <v>65</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65" ht="21" spans="1:3">
@@ -3108,7 +3108,7 @@
         <v>66</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66" ht="21" spans="1:3">
@@ -3119,7 +3119,7 @@
         <v>67</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" ht="21" spans="1:3">
@@ -3130,7 +3130,7 @@
         <v>68</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" ht="21" spans="1:3">
@@ -3141,7 +3141,7 @@
         <v>69</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="69" ht="21" spans="1:3">
@@ -3152,7 +3152,7 @@
         <v>70</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" ht="21" spans="1:3">
@@ -3163,7 +3163,7 @@
         <v>71</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71" ht="21" spans="1:3">
@@ -3174,7 +3174,7 @@
         <v>72</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" ht="21" spans="1:3">
@@ -3185,7 +3185,7 @@
         <v>73</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="73" ht="21" spans="1:3">
@@ -3196,7 +3196,7 @@
         <v>74</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="74" ht="21" spans="1:3">
@@ -3207,7 +3207,7 @@
         <v>75</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="75" ht="21" spans="1:3">
@@ -3218,7 +3218,7 @@
         <v>76</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="76" ht="21" spans="1:3">
@@ -3229,7 +3229,7 @@
         <v>77</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="77" ht="21" spans="1:3">
@@ -3240,7 +3240,7 @@
         <v>78</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="78" ht="21" spans="1:3">
@@ -3251,7 +3251,7 @@
         <v>79</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="79" ht="21" spans="1:3">
@@ -3262,7 +3262,7 @@
         <v>80</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="80" ht="21" spans="1:3">
@@ -3273,7 +3273,7 @@
         <v>81</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="81" ht="21" spans="1:3">
@@ -3284,7 +3284,7 @@
         <v>82</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="82" ht="21" spans="1:3">
@@ -3295,7 +3295,7 @@
         <v>83</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="83" ht="21" spans="1:3">
@@ -3306,7 +3306,7 @@
         <v>84</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="84" ht="21" spans="1:3">
@@ -3317,7 +3317,7 @@
         <v>85</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="85" ht="21" spans="1:3">
@@ -3328,7 +3328,7 @@
         <v>86</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="86" ht="21" spans="1:3">
@@ -3339,7 +3339,7 @@
         <v>87</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="87" ht="21" spans="1:3">
@@ -3350,7 +3350,7 @@
         <v>88</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="88" ht="21" spans="1:3">
@@ -3361,7 +3361,7 @@
         <v>89</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="89" ht="21" spans="1:3">
@@ -3372,7 +3372,7 @@
         <v>90</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="90" ht="21" spans="1:3">
@@ -3383,7 +3383,7 @@
         <v>91</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="91" ht="21" spans="1:3">
@@ -3394,7 +3394,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="92" ht="21" spans="1:3">
@@ -3405,7 +3405,7 @@
         <v>93</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="93" ht="21" spans="1:3">
@@ -3416,7 +3416,7 @@
         <v>94</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="94" ht="21" spans="1:3">
@@ -3427,7 +3427,7 @@
         <v>95</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="95" ht="21" spans="1:3">
@@ -3438,7 +3438,7 @@
         <v>96</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="96" ht="21" spans="1:3">
@@ -3449,7 +3449,7 @@
         <v>97</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="97" ht="21" spans="1:3">
@@ -3460,7 +3460,7 @@
         <v>98</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="98" ht="21" spans="1:3">
@@ -3471,7 +3471,7 @@
         <v>99</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="100" ht="21" spans="1:3">
@@ -3487,7 +3487,7 @@
         <v>101</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="102" ht="21" spans="1:3">
@@ -3498,7 +3498,7 @@
         <v>102</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="103" ht="21" spans="1:3">
@@ -3509,7 +3509,7 @@
         <v>103</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="104" ht="21" spans="1:3">
@@ -3520,7 +3520,7 @@
         <v>104</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="105" ht="21" spans="1:3">
@@ -3531,7 +3531,7 @@
         <v>105</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="106" ht="21" spans="1:3">
@@ -3542,7 +3542,7 @@
         <v>106</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="107" ht="21" spans="1:3">
@@ -3553,7 +3553,7 @@
         <v>107</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="108" ht="21" spans="1:3">
@@ -3564,7 +3564,7 @@
         <v>108</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="109" ht="21" spans="1:3">
@@ -3575,7 +3575,7 @@
         <v>109</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="110" ht="21" spans="1:3">
@@ -3586,7 +3586,7 @@
         <v>110</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="111" ht="21" spans="1:3">
@@ -3597,7 +3597,7 @@
         <v>111</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="112" ht="21" spans="1:3">
@@ -3608,7 +3608,7 @@
         <v>112</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="113" ht="21" spans="1:3">
@@ -3619,7 +3619,7 @@
         <v>113</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="114" ht="21" spans="1:3">
@@ -3630,7 +3630,7 @@
         <v>114</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="115" ht="21" spans="1:3">
@@ -3641,7 +3641,7 @@
         <v>115</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="116" ht="21" spans="1:3">
@@ -3652,7 +3652,7 @@
         <v>116</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="117" ht="21" spans="1:3">
@@ -3663,7 +3663,7 @@
         <v>117</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="118" ht="21" spans="1:3">
@@ -3674,7 +3674,7 @@
         <v>118</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="119" ht="21" spans="1:3">
@@ -3685,7 +3685,7 @@
         <v>119</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="120" ht="21" spans="1:3">
@@ -3696,7 +3696,7 @@
         <v>120</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="121" ht="21" spans="1:3">
@@ -3707,7 +3707,7 @@
         <v>121</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="122" ht="21" spans="1:3">
@@ -3718,7 +3718,7 @@
         <v>122</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="123" ht="21" spans="1:3">
@@ -3729,7 +3729,7 @@
         <v>123</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="124" ht="21" spans="1:3">
@@ -3740,7 +3740,7 @@
         <v>124</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="125" ht="21" spans="1:3">
@@ -3751,7 +3751,7 @@
         <v>125</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="126" ht="21" spans="1:3">
@@ -3762,7 +3762,7 @@
         <v>126</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="127" ht="21" spans="1:3">
@@ -3773,7 +3773,7 @@
         <v>127</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="128" ht="21" spans="1:3">
@@ -3784,7 +3784,7 @@
         <v>128</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="129" ht="21" spans="1:3">
@@ -3795,7 +3795,7 @@
         <v>129</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="130" ht="21" spans="1:3">
@@ -3806,7 +3806,7 @@
         <v>130</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="131" ht="21" spans="1:3">
@@ -3817,7 +3817,7 @@
         <v>131</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="132" ht="21" spans="1:3">
@@ -3828,7 +3828,7 @@
         <v>132</v>
       </c>
       <c r="C132" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="133" ht="21" spans="1:3">
@@ -3839,7 +3839,7 @@
         <v>133</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="134" ht="21" spans="1:3">
@@ -3850,7 +3850,7 @@
         <v>134</v>
       </c>
       <c r="C134" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="135" ht="21" spans="1:3">
@@ -3861,7 +3861,7 @@
         <v>135</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="136" ht="21" spans="1:3">
@@ -3872,7 +3872,7 @@
         <v>136</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="138" ht="21" spans="2:3">
@@ -3887,7 +3887,7 @@
         <v>138</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="140" ht="21" spans="1:3">
@@ -3898,7 +3898,7 @@
         <v>139</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="141" ht="21" spans="1:3">
@@ -3909,7 +3909,7 @@
         <v>140</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="142" ht="21" spans="1:3">
@@ -3920,7 +3920,7 @@
         <v>141</v>
       </c>
       <c r="C142" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="143" ht="21" spans="1:3">
@@ -3931,7 +3931,7 @@
         <v>142</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="144" ht="21" spans="1:3">
@@ -3942,7 +3942,7 @@
         <v>143</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="145" ht="21" spans="1:3">
@@ -3953,7 +3953,7 @@
         <v>144</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="146" ht="21" spans="1:3">
@@ -3964,7 +3964,7 @@
         <v>145</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="147" ht="21" spans="1:3">
@@ -3975,7 +3975,7 @@
         <v>146</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="148" ht="21" spans="1:3">
@@ -3986,7 +3986,7 @@
         <v>147</v>
       </c>
       <c r="C148" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="149" ht="21" spans="1:3">
@@ -3997,7 +3997,7 @@
         <v>148</v>
       </c>
       <c r="C149" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="150" ht="21" spans="1:3">
@@ -4008,7 +4008,7 @@
         <v>149</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="151" ht="21" spans="1:3">
@@ -4019,7 +4019,7 @@
         <v>150</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="152" ht="21" spans="1:3">
@@ -4030,7 +4030,7 @@
         <v>151</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="153" ht="21" spans="1:3">
@@ -4041,7 +4041,7 @@
         <v>152</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="154" ht="21" spans="1:3">
@@ -4052,7 +4052,7 @@
         <v>153</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="155" ht="21" spans="1:3">
@@ -4063,7 +4063,7 @@
         <v>154</v>
       </c>
       <c r="C155" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="156" ht="21" spans="1:3">
@@ -4074,7 +4074,7 @@
         <v>155</v>
       </c>
       <c r="C156" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="157" ht="21" spans="1:3">
@@ -4085,7 +4085,7 @@
         <v>156</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="158" ht="21" spans="1:3">
@@ -4096,7 +4096,7 @@
         <v>157</v>
       </c>
       <c r="C158" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="159" ht="21" spans="1:3">
@@ -4107,7 +4107,7 @@
         <v>158</v>
       </c>
       <c r="C159" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="160" ht="21" spans="1:3">
@@ -4118,7 +4118,7 @@
         <v>159</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="161" ht="21" spans="1:3">
@@ -4129,7 +4129,7 @@
         <v>160</v>
       </c>
       <c r="C161" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="162" ht="21" spans="1:3">
@@ -4140,7 +4140,7 @@
         <v>161</v>
       </c>
       <c r="C162" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="163" ht="21" spans="1:3">
@@ -4151,7 +4151,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="164" ht="21" spans="1:3">
@@ -4162,7 +4162,7 @@
         <v>163</v>
       </c>
       <c r="C164" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="165" ht="21" spans="1:3">
@@ -4173,7 +4173,7 @@
         <v>164</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="166" ht="21" spans="1:3">
@@ -4184,7 +4184,7 @@
         <v>165</v>
       </c>
       <c r="C166" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="167" ht="21" spans="1:3">
@@ -4195,7 +4195,7 @@
         <v>166</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="168" ht="21" spans="1:3">
@@ -4206,7 +4206,7 @@
         <v>167</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="169" ht="21" spans="1:3">
@@ -4217,7 +4217,7 @@
         <v>168</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="170" ht="21" spans="1:3">
@@ -4228,7 +4228,7 @@
         <v>169</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="171" ht="21" spans="1:3">
@@ -4239,7 +4239,7 @@
         <v>170</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="172" ht="21" spans="1:3">
@@ -4250,7 +4250,7 @@
         <v>171</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="173" ht="21" spans="1:3">
@@ -4261,7 +4261,7 @@
         <v>172</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="174" ht="21" spans="1:3">
@@ -4272,7 +4272,7 @@
         <v>173</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="176" ht="21" spans="2:3">
@@ -4463,7 +4463,7 @@
         <v>191</v>
       </c>
       <c r="C193" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="194" ht="21" spans="1:3">
@@ -4507,7 +4507,7 @@
         <v>196</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="198" ht="21" spans="1:3">
@@ -4518,7 +4518,7 @@
         <v>197</v>
       </c>
       <c r="C198" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="199" ht="21" spans="1:3">
@@ -4529,7 +4529,7 @@
         <v>198</v>
       </c>
       <c r="C199" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="200" ht="21" spans="1:3">
@@ -4540,7 +4540,7 @@
         <v>199</v>
       </c>
       <c r="C200" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="201" ht="21" spans="1:3">
@@ -4551,7 +4551,7 @@
         <v>200</v>
       </c>
       <c r="C201" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="202" ht="21" spans="1:3">
@@ -4562,7 +4562,7 @@
         <v>201</v>
       </c>
       <c r="C202" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="203" ht="21" spans="1:3">
@@ -4573,7 +4573,7 @@
         <v>202</v>
       </c>
       <c r="C203" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="204" ht="21" spans="1:3">
@@ -4584,7 +4584,7 @@
         <v>203</v>
       </c>
       <c r="C204" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="205" ht="21" spans="1:3">
@@ -4595,7 +4595,7 @@
         <v>204</v>
       </c>
       <c r="C205" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="206" ht="21" spans="1:3">
@@ -4606,7 +4606,7 @@
         <v>205</v>
       </c>
       <c r="C206" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="207" ht="21" spans="1:3">
@@ -4617,7 +4617,7 @@
         <v>206</v>
       </c>
       <c r="C207" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="208" ht="21" spans="1:3">
@@ -4628,7 +4628,7 @@
         <v>207</v>
       </c>
       <c r="C208" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="209" ht="21" spans="1:3">
@@ -4639,7 +4639,7 @@
         <v>208</v>
       </c>
       <c r="C209" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="210" ht="21" spans="1:3">
@@ -4650,7 +4650,7 @@
         <v>209</v>
       </c>
       <c r="C210" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="211" ht="21" spans="1:3">
@@ -4661,7 +4661,7 @@
         <v>210</v>
       </c>
       <c r="C211" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="212" ht="21" spans="1:3">
@@ -4682,7 +4682,7 @@
         <v>212</v>
       </c>
       <c r="C214" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="215" ht="21" spans="1:3">
@@ -4693,7 +4693,7 @@
         <v>213</v>
       </c>
       <c r="C215" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="216" ht="21" spans="1:3">
@@ -4704,7 +4704,7 @@
         <v>214</v>
       </c>
       <c r="C216" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="217" ht="21" spans="1:3">
@@ -4715,7 +4715,7 @@
         <v>215</v>
       </c>
       <c r="C217" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="218" ht="21" spans="1:3">
@@ -4726,7 +4726,7 @@
         <v>216</v>
       </c>
       <c r="C218" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="219" ht="21" spans="1:3">
@@ -4737,7 +4737,7 @@
         <v>217</v>
       </c>
       <c r="C219" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="220" ht="21" spans="1:3">
@@ -4748,7 +4748,7 @@
         <v>218</v>
       </c>
       <c r="C220" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="221" ht="21" spans="1:3">
@@ -4759,7 +4759,7 @@
         <v>219</v>
       </c>
       <c r="C221" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="222" ht="21" spans="1:3">
@@ -4770,7 +4770,7 @@
         <v>220</v>
       </c>
       <c r="C222" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="223" ht="21" spans="1:3">
@@ -4781,7 +4781,7 @@
         <v>221</v>
       </c>
       <c r="C223" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="224" ht="21" spans="1:3">
@@ -4792,7 +4792,7 @@
         <v>222</v>
       </c>
       <c r="C224" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="225" ht="21" spans="1:3">
@@ -4803,7 +4803,7 @@
         <v>223</v>
       </c>
       <c r="C225" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="226" ht="21" spans="1:3">
@@ -4814,7 +4814,7 @@
         <v>224</v>
       </c>
       <c r="C226" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="227" ht="21" spans="1:3">
@@ -4825,7 +4825,7 @@
         <v>225</v>
       </c>
       <c r="C227" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="228" ht="21" spans="1:3">
@@ -4836,7 +4836,7 @@
         <v>226</v>
       </c>
       <c r="C228" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="229" ht="21" spans="1:3">
@@ -4847,7 +4847,7 @@
         <v>227</v>
       </c>
       <c r="C229" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="230" ht="21" spans="1:3">
@@ -4858,7 +4858,7 @@
         <v>228</v>
       </c>
       <c r="C230" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="231" ht="21" spans="1:3">
@@ -4869,7 +4869,7 @@
         <v>229</v>
       </c>
       <c r="C231" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="232" ht="21" spans="1:3">
@@ -4880,7 +4880,7 @@
         <v>230</v>
       </c>
       <c r="C232" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="233" ht="21" spans="1:3">
@@ -4891,7 +4891,7 @@
         <v>231</v>
       </c>
       <c r="C233" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="234" ht="21" spans="1:3">
@@ -4902,7 +4902,7 @@
         <v>232</v>
       </c>
       <c r="C234" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="235" ht="21" spans="1:3">
@@ -4913,7 +4913,7 @@
         <v>233</v>
       </c>
       <c r="C235" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="236" ht="21" spans="2:3">
@@ -4932,7 +4932,7 @@
         <v>235</v>
       </c>
       <c r="C238" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="239" ht="21" spans="1:3">
@@ -4943,7 +4943,7 @@
         <v>236</v>
       </c>
       <c r="C239" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="240" ht="21" spans="1:3">
@@ -4954,7 +4954,7 @@
         <v>237</v>
       </c>
       <c r="C240" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="241" ht="21" spans="1:3">
@@ -4965,7 +4965,7 @@
         <v>238</v>
       </c>
       <c r="C241" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="242" ht="21" spans="1:3">
@@ -4987,7 +4987,7 @@
         <v>241</v>
       </c>
       <c r="C243" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="244" ht="21" spans="1:3">
@@ -4998,7 +4998,7 @@
         <v>242</v>
       </c>
       <c r="C244" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="245" ht="21" spans="1:3">
@@ -5009,7 +5009,7 @@
         <v>243</v>
       </c>
       <c r="C245" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="246" ht="21" spans="1:3">
@@ -5020,7 +5020,7 @@
         <v>244</v>
       </c>
       <c r="C246" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="247" ht="21" spans="1:3">
@@ -5031,7 +5031,7 @@
         <v>245</v>
       </c>
       <c r="C247" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="248" ht="21" spans="1:3">
@@ -5042,7 +5042,7 @@
         <v>246</v>
       </c>
       <c r="C248" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="249" ht="21" spans="1:3">
@@ -5053,7 +5053,7 @@
         <v>247</v>
       </c>
       <c r="C249" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="250" ht="21" spans="1:3">
@@ -5064,7 +5064,7 @@
         <v>248</v>
       </c>
       <c r="C250" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="251" ht="21" spans="1:3">
@@ -5075,7 +5075,7 @@
         <v>249</v>
       </c>
       <c r="C251" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="252" ht="21" spans="1:3">
@@ -5086,7 +5086,7 @@
         <v>250</v>
       </c>
       <c r="C252" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="253" ht="21" spans="1:3">
@@ -5097,7 +5097,7 @@
         <v>251</v>
       </c>
       <c r="C253" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="254" ht="21" spans="1:3">
@@ -5108,7 +5108,7 @@
         <v>252</v>
       </c>
       <c r="C254" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="255" ht="21" spans="1:3">
@@ -5119,7 +5119,7 @@
         <v>253</v>
       </c>
       <c r="C255" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="256" ht="21" spans="1:3">
@@ -5130,7 +5130,7 @@
         <v>254</v>
       </c>
       <c r="C256" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="257" ht="21" spans="1:3">
@@ -5141,7 +5141,7 @@
         <v>255</v>
       </c>
       <c r="C257" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="258" ht="21" spans="1:3">
@@ -5152,7 +5152,7 @@
         <v>256</v>
       </c>
       <c r="C258" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="259" ht="21" spans="1:3">
@@ -5163,7 +5163,7 @@
         <v>257</v>
       </c>
       <c r="C259" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="260" ht="21" spans="1:3">
@@ -5174,7 +5174,7 @@
         <v>258</v>
       </c>
       <c r="C260" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="261" ht="21" spans="1:3">
@@ -5185,7 +5185,7 @@
         <v>259</v>
       </c>
       <c r="C261" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="262" ht="21" spans="1:3">
@@ -5196,7 +5196,7 @@
         <v>260</v>
       </c>
       <c r="C262" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="263" ht="21" spans="1:3">
@@ -5207,7 +5207,7 @@
         <v>261</v>
       </c>
       <c r="C263" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="264" ht="21" spans="1:3">
@@ -5218,7 +5218,7 @@
         <v>262</v>
       </c>
       <c r="C264" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="265" ht="21" spans="1:3">
@@ -5229,7 +5229,7 @@
         <v>263</v>
       </c>
       <c r="C265" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="266" ht="21" spans="1:3">
@@ -5240,7 +5240,7 @@
         <v>264</v>
       </c>
       <c r="C266" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="267" ht="21" spans="1:3">
@@ -5251,7 +5251,7 @@
         <v>265</v>
       </c>
       <c r="C267" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="268" ht="21" spans="1:3">
@@ -5262,7 +5262,7 @@
         <v>266</v>
       </c>
       <c r="C268" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="269" ht="21" spans="1:3">
@@ -5273,7 +5273,7 @@
         <v>267</v>
       </c>
       <c r="C269" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="270" ht="21" spans="1:3">
@@ -5284,7 +5284,7 @@
         <v>268</v>
       </c>
       <c r="C270" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="271" ht="21" spans="1:3">
@@ -5295,7 +5295,7 @@
         <v>90</v>
       </c>
       <c r="C271" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="272" ht="21" spans="1:3">
@@ -5306,7 +5306,7 @@
         <v>269</v>
       </c>
       <c r="C272" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="273" ht="21" spans="2:3">
@@ -5325,7 +5325,7 @@
         <v>271</v>
       </c>
       <c r="C275" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="276" ht="21" spans="1:3">
@@ -5336,7 +5336,7 @@
         <v>272</v>
       </c>
       <c r="C276" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="277" ht="21" spans="1:3">
@@ -5347,7 +5347,7 @@
         <v>273</v>
       </c>
       <c r="C277" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="278" ht="21" spans="1:3">
@@ -5358,7 +5358,7 @@
         <v>274</v>
       </c>
       <c r="C278" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="279" ht="21" spans="1:3">
@@ -5369,7 +5369,7 @@
         <v>275</v>
       </c>
       <c r="C279" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="280" ht="21" spans="1:3">
@@ -5380,7 +5380,7 @@
         <v>276</v>
       </c>
       <c r="C280" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="281" ht="21" spans="1:3">
@@ -5391,7 +5391,7 @@
         <v>277</v>
       </c>
       <c r="C281" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="282" ht="21" spans="1:3">
@@ -5402,7 +5402,7 @@
         <v>278</v>
       </c>
       <c r="C282" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="283" ht="21" spans="1:3">
@@ -5413,7 +5413,7 @@
         <v>279</v>
       </c>
       <c r="C283" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="284" ht="21" spans="1:3">
@@ -5424,7 +5424,7 @@
         <v>280</v>
       </c>
       <c r="C284" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="285" ht="21" spans="1:3">
@@ -5435,7 +5435,7 @@
         <v>281</v>
       </c>
       <c r="C285" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="286" ht="21" spans="1:3">
@@ -5446,7 +5446,7 @@
         <v>282</v>
       </c>
       <c r="C286" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="287" ht="21" spans="1:3">
@@ -5457,7 +5457,7 @@
         <v>283</v>
       </c>
       <c r="C287" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="288" ht="21" spans="1:3">
@@ -5468,7 +5468,7 @@
         <v>284</v>
       </c>
       <c r="C288" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="289" ht="21" spans="1:3">
@@ -5479,7 +5479,7 @@
         <v>285</v>
       </c>
       <c r="C289" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="290" ht="21" spans="1:3">
@@ -5490,7 +5490,7 @@
         <v>286</v>
       </c>
       <c r="C290" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="291" ht="21" spans="1:3">
@@ -5501,7 +5501,7 @@
         <v>287</v>
       </c>
       <c r="C291" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="292" ht="21" spans="1:3">
@@ -5512,7 +5512,7 @@
         <v>288</v>
       </c>
       <c r="C292" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="293" ht="21" spans="1:3">
@@ -5523,7 +5523,7 @@
         <v>289</v>
       </c>
       <c r="C293" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="294" ht="21" spans="2:3">
@@ -5542,7 +5542,7 @@
         <v>291</v>
       </c>
       <c r="C296" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="297" ht="21" spans="1:3">
@@ -5553,7 +5553,7 @@
         <v>292</v>
       </c>
       <c r="C297" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="298" ht="21" spans="1:3">
@@ -5564,7 +5564,7 @@
         <v>293</v>
       </c>
       <c r="C298" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="299" ht="21" spans="1:3">
@@ -5575,7 +5575,7 @@
         <v>294</v>
       </c>
       <c r="C299" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="300" ht="21" spans="1:3">
@@ -5586,7 +5586,7 @@
         <v>295</v>
       </c>
       <c r="C300" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="301" ht="21" spans="1:3">
@@ -5597,7 +5597,7 @@
         <v>296</v>
       </c>
       <c r="C301" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="302" ht="21" spans="1:3">
@@ -5608,7 +5608,7 @@
         <v>297</v>
       </c>
       <c r="C302" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="303" ht="21" spans="1:3">
@@ -5619,7 +5619,7 @@
         <v>298</v>
       </c>
       <c r="C303" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="304" ht="21" spans="1:3">
@@ -5630,7 +5630,7 @@
         <v>299</v>
       </c>
       <c r="C304" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="305" ht="21" spans="1:3">
@@ -5641,7 +5641,7 @@
         <v>300</v>
       </c>
       <c r="C305" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="306" ht="21" spans="1:3">
@@ -5652,7 +5652,7 @@
         <v>301</v>
       </c>
       <c r="C306" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="307" ht="21" spans="1:3">
@@ -5663,7 +5663,7 @@
         <v>302</v>
       </c>
       <c r="C307" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="308" ht="21" spans="1:3">
@@ -5674,7 +5674,7 @@
         <v>303</v>
       </c>
       <c r="C308" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="309" ht="21" spans="1:3">
@@ -5685,7 +5685,7 @@
         <v>304</v>
       </c>
       <c r="C309" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="310" ht="21" spans="1:3">
@@ -5696,7 +5696,7 @@
         <v>305</v>
       </c>
       <c r="C310" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="311" ht="21" spans="1:3">
@@ -5707,7 +5707,7 @@
         <v>306</v>
       </c>
       <c r="C311" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="312" ht="21" spans="1:3">
@@ -5718,7 +5718,7 @@
         <v>307</v>
       </c>
       <c r="C312" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="313" ht="21" spans="1:3">
@@ -5729,7 +5729,7 @@
         <v>308</v>
       </c>
       <c r="C313" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="314" ht="21" spans="1:3">
@@ -5740,7 +5740,7 @@
         <v>309</v>
       </c>
       <c r="C314" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="315" ht="21" spans="1:3">
@@ -5751,7 +5751,7 @@
         <v>310</v>
       </c>
       <c r="C315" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="316" ht="21" spans="1:3">
@@ -5762,7 +5762,7 @@
         <v>311</v>
       </c>
       <c r="C316" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="317" ht="21" spans="1:3">
@@ -5773,7 +5773,7 @@
         <v>312</v>
       </c>
       <c r="C317" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="318" ht="21" spans="1:3">
@@ -5784,7 +5784,7 @@
         <v>313</v>
       </c>
       <c r="C318" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="319" ht="21" spans="1:3">
@@ -5795,7 +5795,7 @@
         <v>314</v>
       </c>
       <c r="C319" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="320" ht="21" spans="1:3">
@@ -5806,7 +5806,7 @@
         <v>315</v>
       </c>
       <c r="C320" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="321" ht="21" spans="1:3">
@@ -5817,7 +5817,7 @@
         <v>316</v>
       </c>
       <c r="C321" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="322" ht="21" spans="1:3">
@@ -5828,7 +5828,7 @@
         <v>317</v>
       </c>
       <c r="C322" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="323" ht="21" spans="1:3">
@@ -5839,7 +5839,7 @@
         <v>318</v>
       </c>
       <c r="C323" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="324" ht="21" spans="1:3">
@@ -5850,7 +5850,7 @@
         <v>319</v>
       </c>
       <c r="C324" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="325" ht="21" spans="1:3">
@@ -5861,7 +5861,7 @@
         <v>320</v>
       </c>
       <c r="C325" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="326" ht="21" spans="1:3">
@@ -5872,7 +5872,7 @@
         <v>321</v>
       </c>
       <c r="C326" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="327" ht="21" spans="1:3">
@@ -5883,7 +5883,7 @@
         <v>322</v>
       </c>
       <c r="C327" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="328" ht="21" spans="1:3">
@@ -5894,7 +5894,7 @@
         <v>323</v>
       </c>
       <c r="C328" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="329" ht="21" spans="1:3">
@@ -5905,7 +5905,7 @@
         <v>324</v>
       </c>
       <c r="C329" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="330" ht="21" spans="1:3">
@@ -5916,7 +5916,7 @@
         <v>325</v>
       </c>
       <c r="C330" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="331" ht="21" spans="1:3">
@@ -5927,7 +5927,7 @@
         <v>326</v>
       </c>
       <c r="C331" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="332" ht="21" spans="1:3">
@@ -5938,7 +5938,7 @@
         <v>327</v>
       </c>
       <c r="C332" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="333" ht="21" spans="1:3">
@@ -5949,7 +5949,7 @@
         <v>328</v>
       </c>
       <c r="C333" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="334" ht="21" spans="2:3">
@@ -5968,7 +5968,7 @@
         <v>330</v>
       </c>
       <c r="C336" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="337" ht="21" spans="1:3">
@@ -5979,7 +5979,7 @@
         <v>331</v>
       </c>
       <c r="C337" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="338" ht="21" spans="1:3">
@@ -5990,7 +5990,7 @@
         <v>332</v>
       </c>
       <c r="C338" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="339" ht="21" spans="1:3">
@@ -6001,7 +6001,7 @@
         <v>333</v>
       </c>
       <c r="C339" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="340" ht="21" spans="1:3">
@@ -6012,7 +6012,7 @@
         <v>334</v>
       </c>
       <c r="C340" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="341" ht="21" spans="1:3">
@@ -6023,7 +6023,7 @@
         <v>335</v>
       </c>
       <c r="C341" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="342" ht="21" spans="1:3">
@@ -6034,7 +6034,7 @@
         <v>336</v>
       </c>
       <c r="C342" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="343" ht="21" spans="1:3">
@@ -6045,7 +6045,7 @@
         <v>337</v>
       </c>
       <c r="C343" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="344" ht="21" spans="1:3">
@@ -6056,7 +6056,7 @@
         <v>338</v>
       </c>
       <c r="C344" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="345" ht="21" spans="1:3">
@@ -6067,7 +6067,7 @@
         <v>339</v>
       </c>
       <c r="C345" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="346" ht="21" spans="1:3">
@@ -6078,7 +6078,7 @@
         <v>340</v>
       </c>
       <c r="C346" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="347" ht="21" spans="1:3">
@@ -6089,7 +6089,7 @@
         <v>341</v>
       </c>
       <c r="C347" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="348" ht="21" spans="1:3">
@@ -6100,7 +6100,7 @@
         <v>342</v>
       </c>
       <c r="C348" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="349" ht="21" spans="1:3">
@@ -6111,7 +6111,7 @@
         <v>343</v>
       </c>
       <c r="C349" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="350" ht="21" spans="1:3">
@@ -6122,7 +6122,7 @@
         <v>344</v>
       </c>
       <c r="C350" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="351" ht="21" spans="1:3">
@@ -6133,7 +6133,7 @@
         <v>345</v>
       </c>
       <c r="C351" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="352" ht="21" spans="1:3">
@@ -6144,7 +6144,7 @@
         <v>346</v>
       </c>
       <c r="C352" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="353" ht="21" spans="1:3">
@@ -6155,7 +6155,7 @@
         <v>347</v>
       </c>
       <c r="C353" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="354" ht="21" spans="2:3">
@@ -6174,7 +6174,7 @@
         <v>349</v>
       </c>
       <c r="C356" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="357" ht="21" spans="1:3">
@@ -6251,7 +6251,7 @@
         <v>356</v>
       </c>
       <c r="C363" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="364" ht="21" spans="1:3">
@@ -6262,7 +6262,7 @@
         <v>357</v>
       </c>
       <c r="C364" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="365" ht="21" spans="1:3">
@@ -6273,7 +6273,7 @@
         <v>358</v>
       </c>
       <c r="C365" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="366" ht="21" spans="1:3">
@@ -6284,7 +6284,7 @@
         <v>359</v>
       </c>
       <c r="C366" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="367" ht="21" spans="1:3">
@@ -6295,7 +6295,7 @@
         <v>360</v>
       </c>
       <c r="C367" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="368" ht="21" spans="1:3">
@@ -6306,7 +6306,7 @@
         <v>361</v>
       </c>
       <c r="C368" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="369" ht="21" spans="1:3">
@@ -6317,7 +6317,7 @@
         <v>362</v>
       </c>
       <c r="C369" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="370" ht="21" spans="1:3">
@@ -6328,7 +6328,7 @@
         <v>363</v>
       </c>
       <c r="C370" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="371" ht="21" spans="1:3">
@@ -6339,7 +6339,7 @@
         <v>364</v>
       </c>
       <c r="C371" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="372" ht="21" spans="1:3">
@@ -6350,7 +6350,7 @@
         <v>365</v>
       </c>
       <c r="C372" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="373" ht="21" spans="1:3">
@@ -6361,7 +6361,7 @@
         <v>366</v>
       </c>
       <c r="C373" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="374" ht="21" spans="1:3">
@@ -6372,7 +6372,7 @@
         <v>367</v>
       </c>
       <c r="C374" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="375" ht="21" spans="1:3">
@@ -6383,7 +6383,7 @@
         <v>368</v>
       </c>
       <c r="C375" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="376" ht="21" spans="1:3">
@@ -6394,7 +6394,7 @@
         <v>369</v>
       </c>
       <c r="C376" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="377" ht="21" spans="1:3">
@@ -6405,7 +6405,7 @@
         <v>370</v>
       </c>
       <c r="C377" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="378" ht="21" spans="1:3">
@@ -6416,7 +6416,7 @@
         <v>371</v>
       </c>
       <c r="C378" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="379" ht="21" spans="1:3">
@@ -6427,7 +6427,7 @@
         <v>372</v>
       </c>
       <c r="C379" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="380" ht="21" spans="1:3">
@@ -6438,7 +6438,7 @@
         <v>373</v>
       </c>
       <c r="C380" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="381" ht="21" spans="1:3">
@@ -6449,7 +6449,7 @@
         <v>374</v>
       </c>
       <c r="C381" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="382" ht="21" spans="1:3">
@@ -6460,7 +6460,7 @@
         <v>375</v>
       </c>
       <c r="C382" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="383" ht="21" spans="1:3">
@@ -6471,7 +6471,7 @@
         <v>376</v>
       </c>
       <c r="C383" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="384" ht="21" spans="1:3">
@@ -6482,7 +6482,7 @@
         <v>377</v>
       </c>
       <c r="C384" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="385" ht="21" spans="1:3">
@@ -6493,7 +6493,7 @@
         <v>378</v>
       </c>
       <c r="C385" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="386" ht="21" spans="1:3">
@@ -6504,7 +6504,7 @@
         <v>379</v>
       </c>
       <c r="C386" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="387" ht="21" spans="1:3">
@@ -6515,7 +6515,7 @@
         <v>380</v>
       </c>
       <c r="C387" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="388" ht="21" spans="1:3">
@@ -6526,7 +6526,7 @@
         <v>381</v>
       </c>
       <c r="C388" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="389" ht="21" spans="1:3">
@@ -6537,7 +6537,7 @@
         <v>382</v>
       </c>
       <c r="C389" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="390" ht="21" spans="1:3">
@@ -6548,7 +6548,7 @@
         <v>382</v>
       </c>
       <c r="C390" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="391" ht="21" spans="1:3">
@@ -6559,7 +6559,7 @@
         <v>383</v>
       </c>
       <c r="C391" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="392" ht="21" spans="1:3">
@@ -6570,7 +6570,7 @@
         <v>384</v>
       </c>
       <c r="C392" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="393" ht="21" spans="1:3">
@@ -6581,7 +6581,7 @@
         <v>385</v>
       </c>
       <c r="C393" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="394" ht="21" spans="1:3">
@@ -6592,7 +6592,7 @@
         <v>386</v>
       </c>
       <c r="C394" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="395" ht="21" spans="1:3">
@@ -6603,7 +6603,7 @@
         <v>387</v>
       </c>
       <c r="C395" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="396" ht="21" spans="1:3">
@@ -6614,7 +6614,7 @@
         <v>388</v>
       </c>
       <c r="C396" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="397" ht="21" spans="1:3">
@@ -6625,7 +6625,7 @@
         <v>389</v>
       </c>
       <c r="C397" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="398" ht="21" spans="1:3">
@@ -6636,7 +6636,7 @@
         <v>390</v>
       </c>
       <c r="C398" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="399" ht="21" spans="1:3">
@@ -6647,7 +6647,7 @@
         <v>391</v>
       </c>
       <c r="C399" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="400" ht="21" spans="2:3">
@@ -6666,7 +6666,7 @@
         <v>393</v>
       </c>
       <c r="C402" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="403" ht="21" spans="1:3">
@@ -6677,7 +6677,7 @@
         <v>394</v>
       </c>
       <c r="C403" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="404" ht="21" spans="1:3">
@@ -6688,7 +6688,7 @@
         <v>395</v>
       </c>
       <c r="C404" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="405" ht="21" spans="1:3">
@@ -6699,7 +6699,7 @@
         <v>92</v>
       </c>
       <c r="C405" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="406" ht="21" spans="1:3">
@@ -6710,7 +6710,7 @@
         <v>396</v>
       </c>
       <c r="C406" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="407" ht="21" spans="1:3">
@@ -6721,7 +6721,7 @@
         <v>397</v>
       </c>
       <c r="C407" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="408" ht="21" spans="2:3">
@@ -6817,7 +6817,7 @@
         <v>278</v>
       </c>
       <c r="C417" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="418" ht="21" spans="1:3">
@@ -6828,7 +6828,7 @@
         <v>406</v>
       </c>
       <c r="C418" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="419" ht="21" spans="1:3">
@@ -6839,7 +6839,7 @@
         <v>407</v>
       </c>
       <c r="C419" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="420" ht="21" spans="1:3">
@@ -6850,7 +6850,7 @@
         <v>408</v>
       </c>
       <c r="C420" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="421" ht="21" spans="1:3">
@@ -6861,7 +6861,7 @@
         <v>409</v>
       </c>
       <c r="C421" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="422" ht="21" spans="1:3">
@@ -6872,7 +6872,7 @@
         <v>410</v>
       </c>
       <c r="C422" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="423" ht="21" spans="1:3">
@@ -6883,7 +6883,7 @@
         <v>411</v>
       </c>
       <c r="C423" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="424" ht="21" spans="1:3">
@@ -6894,7 +6894,7 @@
         <v>412</v>
       </c>
       <c r="C424" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="425" ht="21" spans="1:3">
@@ -6905,7 +6905,7 @@
         <v>413</v>
       </c>
       <c r="C425" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="426" ht="21" spans="1:3">
@@ -6916,7 +6916,7 @@
         <v>414</v>
       </c>
       <c r="C426" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="427" ht="21" spans="1:3">
@@ -6927,7 +6927,7 @@
         <v>415</v>
       </c>
       <c r="C427" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="428" ht="21" spans="1:3">
@@ -6938,7 +6938,7 @@
         <v>416</v>
       </c>
       <c r="C428" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="429" ht="21" spans="1:3">
@@ -6949,7 +6949,7 @@
         <v>417</v>
       </c>
       <c r="C429" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="430" ht="21" spans="1:3">
@@ -6960,7 +6960,7 @@
         <v>418</v>
       </c>
       <c r="C430" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="431" ht="21" spans="1:3">
@@ -6971,7 +6971,7 @@
         <v>419</v>
       </c>
       <c r="C431" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="432" ht="21" spans="1:3">
@@ -6982,7 +6982,7 @@
         <v>420</v>
       </c>
       <c r="C432" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="433" ht="21" spans="1:3">
@@ -6993,7 +6993,7 @@
         <v>421</v>
       </c>
       <c r="C433" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="434" ht="21" spans="1:3">
@@ -7004,7 +7004,7 @@
         <v>422</v>
       </c>
       <c r="C434" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="435" ht="21" spans="1:3">
@@ -7015,7 +7015,7 @@
         <v>423</v>
       </c>
       <c r="C435" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="436" ht="21" spans="1:3">
@@ -7026,7 +7026,7 @@
         <v>424</v>
       </c>
       <c r="C436" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="437" ht="21" spans="1:3">
@@ -7037,7 +7037,7 @@
         <v>425</v>
       </c>
       <c r="C437" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="438" ht="21" spans="1:3">
@@ -7048,7 +7048,7 @@
         <v>17</v>
       </c>
       <c r="C438" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="439" ht="21" spans="1:3">
@@ -7059,7 +7059,7 @@
         <v>426</v>
       </c>
       <c r="C439" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="440" ht="21" spans="1:3">
@@ -7070,7 +7070,7 @@
         <v>427</v>
       </c>
       <c r="C440" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="441" ht="21" spans="1:3">
@@ -7081,7 +7081,7 @@
         <v>428</v>
       </c>
       <c r="C441" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="442" ht="21" spans="1:3">
@@ -7092,7 +7092,7 @@
         <v>429</v>
       </c>
       <c r="C442" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="443" ht="21" spans="1:3">
@@ -7103,7 +7103,7 @@
         <v>430</v>
       </c>
       <c r="C443" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="444" ht="21" spans="1:3">
@@ -7114,7 +7114,7 @@
         <v>431</v>
       </c>
       <c r="C444" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="445" ht="21" spans="1:3">
@@ -7125,7 +7125,7 @@
         <v>432</v>
       </c>
       <c r="C445" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="446" ht="21" spans="1:3">
@@ -7136,7 +7136,7 @@
         <v>433</v>
       </c>
       <c r="C446" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="447" ht="21" spans="1:3">
@@ -7147,7 +7147,7 @@
         <v>434</v>
       </c>
       <c r="C447" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="448" ht="21" spans="1:3">
@@ -7158,7 +7158,7 @@
         <v>435</v>
       </c>
       <c r="C448" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="449" ht="21" spans="1:3">
@@ -7169,7 +7169,7 @@
         <v>436</v>
       </c>
       <c r="C449" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="450" ht="21" spans="1:3">
@@ -7180,7 +7180,7 @@
         <v>437</v>
       </c>
       <c r="C450" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="451" ht="21" spans="1:3">
@@ -7191,7 +7191,7 @@
         <v>438</v>
       </c>
       <c r="C451" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="452" ht="21" spans="1:3">
@@ -7202,7 +7202,7 @@
         <v>439</v>
       </c>
       <c r="C452" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="453" ht="21" spans="1:3">
@@ -7213,7 +7213,7 @@
         <v>440</v>
       </c>
       <c r="C453" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="454" ht="21" spans="1:3">
@@ -7224,7 +7224,7 @@
         <v>441</v>
       </c>
       <c r="C454" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="455" ht="21" spans="1:3">
@@ -7235,7 +7235,7 @@
         <v>442</v>
       </c>
       <c r="C455" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="456" ht="21" spans="1:3">
@@ -7246,7 +7246,7 @@
         <v>443</v>
       </c>
       <c r="C456" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="457" ht="21" spans="1:3">
@@ -7257,7 +7257,7 @@
         <v>444</v>
       </c>
       <c r="C457" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="458" ht="21" spans="1:3">
@@ -7268,7 +7268,7 @@
         <v>445</v>
       </c>
       <c r="C458" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="459" ht="21" spans="1:3">
@@ -7279,7 +7279,7 @@
         <v>446</v>
       </c>
       <c r="C459" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="460" ht="21" spans="1:3">
@@ -7290,7 +7290,7 @@
         <v>447</v>
       </c>
       <c r="C460" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="461" ht="21" spans="1:3">
@@ -7301,7 +7301,7 @@
         <v>448</v>
       </c>
       <c r="C461" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="462" ht="21" spans="1:3">
@@ -7312,7 +7312,7 @@
         <v>449</v>
       </c>
       <c r="C462" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="463" ht="21" spans="1:3">
@@ -7323,7 +7323,7 @@
         <v>450</v>
       </c>
       <c r="C463" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="464" ht="21" spans="1:3">
@@ -7334,7 +7334,7 @@
         <v>451</v>
       </c>
       <c r="C464" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="465" ht="21" spans="1:3">
@@ -7345,7 +7345,7 @@
         <v>452</v>
       </c>
       <c r="C465" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="466" ht="21" spans="1:3">
@@ -7356,7 +7356,7 @@
         <v>453</v>
       </c>
       <c r="C466" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="467" ht="21" spans="1:3">
@@ -7367,7 +7367,7 @@
         <v>454</v>
       </c>
       <c r="C467" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="468" ht="21" spans="1:3">
@@ -7378,7 +7378,7 @@
         <v>455</v>
       </c>
       <c r="C468" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="469" ht="21" spans="1:3">
@@ -7389,7 +7389,7 @@
         <v>456</v>
       </c>
       <c r="C469" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="470" ht="21" spans="2:3">
@@ -7409,7 +7409,7 @@
         <v>458</v>
       </c>
       <c r="C472" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="473" ht="21" spans="1:3">
@@ -7420,7 +7420,7 @@
         <v>459</v>
       </c>
       <c r="C473" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="474" ht="21" spans="1:3">
@@ -7431,7 +7431,7 @@
         <v>460</v>
       </c>
       <c r="C474" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="475" ht="21" spans="1:3">
@@ -7442,7 +7442,7 @@
         <v>461</v>
       </c>
       <c r="C475" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="476" ht="21" spans="1:3">
@@ -7453,7 +7453,7 @@
         <v>462</v>
       </c>
       <c r="C476" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="477" ht="21" spans="1:3">
@@ -7464,7 +7464,7 @@
         <v>463</v>
       </c>
       <c r="C477" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="478" ht="21" spans="1:3">
@@ -7475,7 +7475,7 @@
         <v>464</v>
       </c>
       <c r="C478" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="479" ht="21" spans="1:3">
@@ -7486,7 +7486,7 @@
         <v>465</v>
       </c>
       <c r="C479" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="480" ht="21" spans="1:3">
@@ -7497,7 +7497,7 @@
         <v>466</v>
       </c>
       <c r="C480" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="481" ht="21" spans="1:3">
@@ -7508,7 +7508,7 @@
         <v>467</v>
       </c>
       <c r="C481" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reverse a string with 0(1) space
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1425,10 +1425,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1509,9 +1509,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1527,23 +1562,32 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1555,22 +1599,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1586,32 +1616,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1623,23 +1630,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1660,7 +1660,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1672,7 +1672,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1684,73 +1810,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1762,79 +1828,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1865,20 +1865,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1887,7 +1891,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1922,33 +1926,29 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1967,127 +1967,127 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2440,8 +2440,8 @@
   <sheetPr/>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2712,7 +2712,7 @@
       <c r="A27" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C27" s="9" t="s">
@@ -3005,18 +3005,18 @@
       <c r="A56" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C56" s="9" t="s">
-        <v>30</v>
+      <c r="C56" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="57" ht="21" spans="1:3">
       <c r="A57" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C57" s="9" t="s">

</xml_diff>

<commit_message>
Check a stirng is pallindrome or  not
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1426,8 +1426,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
@@ -1509,8 +1509,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1524,14 +1525,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1539,9 +1533,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1555,14 +1549,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1609,14 +1595,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1637,9 +1631,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1660,7 +1660,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1672,7 +1672,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1684,7 +1762,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1696,145 +1834,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1845,6 +1845,36 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1896,32 +1926,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1934,27 +1945,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1967,127 +1967,127 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2441,7 +2441,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -3020,7 +3020,7 @@
         <v>58</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Longest consecutive subsequence 0nlogn
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1427,8 +1427,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1503,7 +1503,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1516,37 +1516,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1561,10 +1556,18 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1575,11 +1578,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1607,9 +1609,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1622,16 +1623,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1639,7 +1632,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1660,19 +1660,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1690,31 +1786,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1726,115 +1834,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1863,6 +1863,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1874,15 +1894,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1911,6 +1922,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1925,30 +1945,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1967,127 +1967,127 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2440,8 +2440,8 @@
   <sheetPr/>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2734,11 +2734,11 @@
       <c r="A29" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>30</v>
+      <c r="C29" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="30" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Triplet sum in array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1425,10 +1425,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1503,16 +1503,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1525,7 +1532,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1539,27 +1546,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1578,10 +1569,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1610,14 +1602,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1639,7 +1624,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1660,7 +1660,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1672,13 +1684,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1696,13 +1810,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1714,121 +1828,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1867,17 +1867,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1922,15 +1911,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1945,149 +1925,169 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2441,7 +2441,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2781,8 +2781,8 @@
       <c r="B33" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>30</v>
+      <c r="C33" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="34" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Count more than n/k occurrances of an element(map solution)
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1425,10 +1425,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1510,6 +1510,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1517,7 +1524,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1531,8 +1546,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1543,22 +1559,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1602,7 +1602,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1624,6 +1624,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1633,13 +1640,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1660,13 +1660,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1678,13 +1672,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1702,13 +1738,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1720,25 +1810,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1750,91 +1834,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1863,15 +1863,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1883,6 +1874,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1948,7 +1948,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1967,28 +1967,28 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1997,7 +1997,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -2006,88 +2006,88 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2441,7 +2441,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2745,11 +2745,11 @@
       <c r="A30" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>30</v>
+      <c r="C30" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="31" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Max profit by buying selling stock Leetcode
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1426,8 +1426,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
@@ -1502,15 +1502,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1524,23 +1526,36 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1562,26 +1577,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1602,7 +1602,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1617,14 +1617,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1639,7 +1639,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1660,13 +1660,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1678,7 +1678,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1690,7 +1768,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1702,91 +1816,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1798,43 +1834,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1848,17 +1848,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1912,6 +1908,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1925,76 +1945,56 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -2006,88 +2006,88 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2441,7 +2441,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2756,18 +2756,18 @@
       <c r="A31" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>30</v>
+      <c r="C31" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="32" ht="21" spans="1:3">
       <c r="A32" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="9" t="s">

</xml_diff>

<commit_message>
Array subset of another array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1502,17 +1502,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1520,35 +1527,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1563,7 +1541,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1577,6 +1570,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -1585,26 +1592,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1617,14 +1617,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1632,14 +1640,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1660,37 +1660,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1702,13 +1678,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1726,7 +1720,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1738,7 +1768,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1750,61 +1822,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1816,25 +1834,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1845,17 +1845,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1870,6 +1859,21 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1908,30 +1912,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1945,149 +1925,169 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2441,7 +2441,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2770,8 +2770,8 @@
       <c r="B32" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>30</v>
+      <c r="C32" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="33" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Search a 2d matrix
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1426,9 +1426,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1502,38 +1502,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1547,7 +1524,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1560,9 +1560,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1615,31 +1630,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1666,13 +1666,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1690,13 +1732,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1714,7 +1750,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1726,19 +1762,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1756,7 +1816,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1768,67 +1828,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1840,7 +1840,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1856,9 +1856,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1878,6 +1880,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1889,15 +1900,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1943,157 +1945,155 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2450,7 +2450,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2910,11 +2910,11 @@
       <c r="A45" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="9" t="s">
-        <v>30</v>
+      <c r="C45" s="12" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="46" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Median of a 2d matrix with sorted rows
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1425,10 +1425,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1503,14 +1503,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1524,45 +1525,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1571,13 +1541,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1596,6 +1559,14 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1639,7 +1610,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1666,43 +1666,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1714,25 +1720,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1750,13 +1738,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1768,13 +1756,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1786,19 +1792,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1810,37 +1822,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1851,17 +1851,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1876,15 +1865,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1951,149 +1931,169 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2450,7 +2450,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2921,11 +2921,11 @@
       <c r="A46" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C46" s="9" t="s">
-        <v>30</v>
+      <c r="C46" s="12" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="47" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Row with max 1s
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1425,10 +1425,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1503,17 +1503,16 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1532,7 +1531,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1541,6 +1563,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1559,6 +1588,13 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1585,14 +1621,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -1606,34 +1634,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1666,7 +1666,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1678,7 +1714,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1690,61 +1792,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1756,91 +1834,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1855,6 +1855,36 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1865,21 +1895,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1908,17 +1923,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1928,15 +1937,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1954,146 +1954,146 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2450,7 +2450,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2935,8 +2935,8 @@
       <c r="B47" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C47" s="9" t="s">
-        <v>30</v>
+      <c r="C47" s="12" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="48" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Two strings are rotation of each other?
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1502,8 +1502,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1517,7 +1541,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1538,48 +1585,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1602,22 +1610,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1625,7 +1625,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1639,7 +1639,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1666,13 +1666,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1684,79 +1762,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1774,7 +1780,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1786,31 +1798,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1822,25 +1816,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1851,60 +1851,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1932,13 +1878,56 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1951,149 +1940,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2449,8 +2449,8 @@
   <sheetPr/>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -2954,7 +2954,7 @@
       <c r="A49" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="7" t="s">
         <v>51</v>
       </c>
       <c r="C49" s="9" t="s">
@@ -3061,15 +3061,15 @@
       <c r="B60" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C60" s="9" t="s">
-        <v>30</v>
+      <c r="C60" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="61" ht="21" spans="1:3">
       <c r="A61" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="7" t="s">
         <v>62</v>
       </c>
       <c r="C61" s="9" t="s">
@@ -4295,7 +4295,7 @@
       <c r="B177" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="C177" s="9" t="s">
+      <c r="C177" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4306,7 +4306,7 @@
       <c r="B178" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="C178" s="9" t="s">
+      <c r="C178" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4317,7 +4317,7 @@
       <c r="B179" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="C179" s="9" t="s">
+      <c r="C179" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4328,7 +4328,7 @@
       <c r="B180" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="C180" s="9" t="s">
+      <c r="C180" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4339,7 +4339,7 @@
       <c r="B181" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="C181" s="9" t="s">
+      <c r="C181" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4350,7 +4350,7 @@
       <c r="B182" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="C182" s="9" t="s">
+      <c r="C182" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4361,7 +4361,7 @@
       <c r="B183" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="C183" s="9" t="s">
+      <c r="C183" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4372,7 +4372,7 @@
       <c r="B184" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="C184" s="9" t="s">
+      <c r="C184" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4383,7 +4383,7 @@
       <c r="B185" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="C185" s="9" t="s">
+      <c r="C185" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4394,7 +4394,7 @@
       <c r="B186" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="C186" s="9" t="s">
+      <c r="C186" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4405,7 +4405,7 @@
       <c r="B187" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="C187" s="9" t="s">
+      <c r="C187" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4416,7 +4416,7 @@
       <c r="B188" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="C188" s="9" t="s">
+      <c r="C188" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4427,7 +4427,7 @@
       <c r="B189" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="C189" s="9" t="s">
+      <c r="C189" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4438,7 +4438,7 @@
       <c r="B190" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="C190" s="9" t="s">
+      <c r="C190" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4449,7 +4449,7 @@
       <c r="B191" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="C191" s="9" t="s">
+      <c r="C191" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4460,7 +4460,7 @@
       <c r="B192" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="C192" s="9" t="s">
+      <c r="C192" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4482,7 +4482,7 @@
       <c r="B194" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="C194" s="9" t="s">
+      <c r="C194" s="12" t="s">
         <v>193</v>
       </c>
     </row>
@@ -4493,7 +4493,7 @@
       <c r="B195" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="C195" s="9" t="s">
+      <c r="C195" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4504,7 +4504,7 @@
       <c r="B196" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="C196" s="9" t="s">
+      <c r="C196" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -6193,7 +6193,7 @@
       <c r="B357" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="C357" s="9" t="s">
+      <c r="C357" s="12" t="s">
         <v>240</v>
       </c>
     </row>
@@ -6204,7 +6204,7 @@
       <c r="B358" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="C358" s="9" t="s">
+      <c r="C358" s="12" t="s">
         <v>240</v>
       </c>
     </row>
@@ -6215,7 +6215,7 @@
       <c r="B359" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="C359" s="9" t="s">
+      <c r="C359" s="12" t="s">
         <v>240</v>
       </c>
     </row>
@@ -6226,7 +6226,7 @@
       <c r="B360" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="C360" s="9" t="s">
+      <c r="C360" s="12" t="s">
         <v>240</v>
       </c>
     </row>
@@ -6237,7 +6237,7 @@
       <c r="B361" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="C361" s="9" t="s">
+      <c r="C361" s="12" t="s">
         <v>240</v>
       </c>
     </row>
@@ -6248,7 +6248,7 @@
       <c r="B362" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="C362" s="9" t="s">
+      <c r="C362" s="12" t="s">
         <v>240</v>
       </c>
     </row>
@@ -6748,7 +6748,7 @@
       <c r="B410" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="C410" s="9" t="s">
+      <c r="C410" s="12" t="s">
         <v>5</v>
       </c>
     </row>
@@ -6759,7 +6759,7 @@
       <c r="B411" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="C411" s="9" t="s">
+      <c r="C411" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -6770,7 +6770,7 @@
       <c r="B412" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="C412" s="9" t="s">
+      <c r="C412" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -6781,7 +6781,7 @@
       <c r="B413" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="C413" s="9" t="s">
+      <c r="C413" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -6792,7 +6792,7 @@
       <c r="B414" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="C414" s="9" t="s">
+      <c r="C414" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -6803,7 +6803,7 @@
       <c r="B415" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="C415" s="9" t="s">
+      <c r="C415" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -6814,7 +6814,7 @@
       <c r="B416" s="8" t="s">
         <v>405</v>
       </c>
-      <c r="C416" s="9" t="s">
+      <c r="C416" s="12" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Count and say leetcode
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1425,10 +1425,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1502,14 +1502,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1517,17 +1509,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1541,14 +1532,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1601,8 +1600,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1616,30 +1637,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1666,7 +1666,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1678,7 +1678,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1690,55 +1708,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1756,79 +1726,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1844,6 +1748,102 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -1854,17 +1854,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1872,8 +1868,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1917,6 +1913,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1931,70 +1951,50 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2006,94 +2006,94 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2450,7 +2450,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -3083,15 +3083,15 @@
       <c r="B62" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C62" s="9" t="s">
-        <v>30</v>
+      <c r="C62" s="12" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="63" ht="21" spans="1:3">
       <c r="A63" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="B63" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C63" s="9" t="s">

</xml_diff>

<commit_message>
split string with same number of 0s 1s
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1434,10 +1434,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -1525,6 +1525,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1532,7 +1539,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1540,22 +1547,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1570,6 +1577,14 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -1577,38 +1592,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1624,15 +1610,36 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1648,13 +1655,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1688,7 +1688,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1700,13 +1700,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1718,13 +1712,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1736,31 +1748,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1778,13 +1772,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1796,25 +1790,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1826,43 +1862,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1876,20 +1876,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1924,17 +1921,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1976,146 +1976,146 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2477,8 +2477,8 @@
   <sheetPr/>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -3163,18 +3163,18 @@
       <c r="A67" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="B67" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C67" s="9" t="s">
-        <v>30</v>
+      <c r="C67" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="68" ht="21" spans="1:3">
       <c r="A68" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B68" s="7" t="s">
         <v>72</v>
       </c>
       <c r="C68" s="9" t="s">

</xml_diff>

<commit_message>
Clone a graph leetcode
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1434,10 +1434,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -1524,15 +1524,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1545,11 +1547,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1562,6 +1563,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1582,17 +1598,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1606,9 +1622,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1623,29 +1646,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1659,9 +1660,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1694,7 +1694,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1706,37 +1808,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1748,25 +1838,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1778,97 +1862,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1879,15 +1879,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1917,6 +1908,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1932,6 +1941,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1943,24 +1961,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1982,7 +1982,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2001,127 +2001,127 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2487,7 +2487,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A353" workbookViewId="0">
-      <selection activeCell="C363" sqref="C363"/>
+      <selection activeCell="C364" sqref="C364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -6304,11 +6304,11 @@
       <c r="A364" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="B364" s="8" t="s">
+      <c r="B364" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="C364" s="9" t="s">
-        <v>30</v>
+      <c r="C364" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="365" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Making wired connections leetcode
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1435,9 +1435,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -1532,9 +1532,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1548,16 +1561,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1569,7 +1583,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1584,6 +1598,29 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -1592,7 +1629,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1606,64 +1659,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1694,6 +1694,66 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1706,37 +1766,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1748,7 +1790,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1766,7 +1814,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1778,97 +1868,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1893,6 +1893,39 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1908,11 +1941,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1940,188 +1979,149 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2487,7 +2487,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A353" workbookViewId="0">
-      <selection activeCell="C364" sqref="C364"/>
+      <selection activeCell="C365" sqref="C365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -6315,11 +6315,11 @@
       <c r="A365" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="B365" s="8" t="s">
+      <c r="B365" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="C365" s="9" t="s">
-        <v>30</v>
+      <c r="C365" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="366" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Min time taken by each job (topological sort problem)
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1434,10 +1434,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -1524,23 +1524,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1560,8 +1545,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1569,21 +1562,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1599,7 +1578,60 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1614,30 +1646,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1651,19 +1660,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1694,19 +1694,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1724,7 +1766,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1736,7 +1790,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1748,127 +1868,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1884,11 +1884,59 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1904,39 +1952,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1959,169 +1974,154 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2486,8 +2486,8 @@
   <sheetPr/>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A353" workbookViewId="0">
-      <selection activeCell="C365" sqref="C365"/>
+    <sheetView tabSelected="1" topLeftCell="A358" workbookViewId="0">
+      <selection activeCell="B375" sqref="B375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -6351,19 +6351,19 @@
       <c r="B368" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="C368" s="9" t="s">
-        <v>30</v>
+      <c r="C368" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="369" ht="21" spans="1:3">
       <c r="A369" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="B369" s="8" t="s">
+      <c r="B369" s="7" t="s">
         <v>365</v>
       </c>
-      <c r="C369" s="9" t="s">
-        <v>30</v>
+      <c r="C369" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="370" ht="21" spans="1:3">

</xml_diff>

<commit_message>
Alien dictionary toposort problem
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1114,7 +1114,7 @@
     <t>Minimum time taken by each job to be completed given by a Directed Acyclic Graph</t>
   </si>
   <si>
-    <t>Find whether it is possible to finish all tasks or not from given dependencies</t>
+    <t>Find whether it is possible to finish all tasks or not from given dependencies (Cycle detection)</t>
   </si>
   <si>
     <t>Find the no. of Isalnds</t>
@@ -1434,10 +1434,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -1525,9 +1525,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1539,30 +1539,28 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1578,16 +1576,25 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1630,23 +1637,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1655,6 +1648,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1694,6 +1694,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1706,25 +1748,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1736,19 +1772,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1766,13 +1814,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1784,19 +1850,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1808,67 +1868,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1885,58 +1885,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1971,157 +1921,207 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2487,7 +2487,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A358" workbookViewId="0">
-      <selection activeCell="B375" sqref="B375"/>
+      <selection activeCell="C372" sqref="C372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -6370,11 +6370,11 @@
       <c r="A370" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="B370" s="8" t="s">
+      <c r="B370" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="C370" s="9" t="s">
-        <v>30</v>
+      <c r="C370" s="12" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="371" ht="21" spans="1:3">
@@ -6384,19 +6384,19 @@
       <c r="B371" s="8" t="s">
         <v>367</v>
       </c>
-      <c r="C371" s="9" t="s">
-        <v>30</v>
+      <c r="C371" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="372" ht="21" spans="1:3">
       <c r="A372" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="B372" s="8" t="s">
+      <c r="B372" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="C372" s="9" t="s">
-        <v>30</v>
+      <c r="C372" s="12" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="373" ht="21" spans="1:3">
@@ -7896,7 +7896,7 @@
     <hyperlink ref="B367" r:id="rId322" display="Dijkstra algo"/>
     <hyperlink ref="B368" r:id="rId323" display="Implement Topological Sort "/>
     <hyperlink ref="B369" r:id="rId324" display="Minimum time taken by each job to be completed given by a Directed Acyclic Graph"/>
-    <hyperlink ref="B370" r:id="rId325" display="Find whether it is possible to finish all tasks or not from given dependencies"/>
+    <hyperlink ref="B370" r:id="rId325" display="Find whether it is possible to finish all tasks or not from given dependencies (Cycle detection)"/>
     <hyperlink ref="B371" r:id="rId326" display="Find the no. of Isalnds"/>
     <hyperlink ref="B372" r:id="rId327" display="Given a sorted Dictionary of an Alien Language, find order of characters"/>
     <hyperlink ref="B373" r:id="rId328" display="Implement Kruksal’sAlgorithm"/>

</xml_diff>

<commit_message>
Number of subsets using recursion
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1434,10 +1434,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -1525,12 +1525,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1546,9 +1554,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1564,20 +1571,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1599,8 +1592,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1614,14 +1623,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -1631,13 +1632,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1700,25 +1700,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1730,7 +1724,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1748,13 +1742,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1766,43 +1778,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1820,7 +1796,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1832,19 +1808,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1856,19 +1838,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1882,26 +1882,26 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1945,26 +1945,26 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1982,83 +1982,83 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -2067,61 +2067,61 @@
     <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2487,7 +2487,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A372" workbookViewId="0">
-      <selection activeCell="C379" sqref="C379"/>
+      <selection activeCell="B380" sqref="B380"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -6480,7 +6480,7 @@
       <c r="A380" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="B380" s="8" t="s">
+      <c r="B380" s="7" t="s">
         <v>376</v>
       </c>
       <c r="C380" s="9" t="s">

</xml_diff>